<commit_message>
Update to tracking sheet
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ell-vsvr1\RedirectedFolders\bras3130\Desktop\digital-anon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2637E86-DA17-4630-9C18-5E6AD70C02C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E079D50A-A970-4D04-B220-3D73B0847DF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="349">
   <si>
     <t>M-Number</t>
   </si>
@@ -113,9 +113,6 @@
     <t>M113</t>
   </si>
   <si>
-    <t>[Anon] Typescript fragment, with the author's ms. corrections, unsigned, and undated. 8p. Paginated 3-10. On verso of p. 8-9 her: People one would have liked to have met. Holograph fragment. 2p.</t>
-  </si>
-  <si>
     <t>m48</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>m51</t>
   </si>
   <si>
-    <t>Anon. Typescript fragment, with the author's ms. corrections, unsigned and undated. 2p.</t>
-  </si>
-  <si>
     <t>Anon</t>
   </si>
   <si>
@@ -701,9 +695,6 @@
     <t>Find way to render blank lines on p. 2 and p. 9</t>
   </si>
   <si>
-    <t>Anon. Typescript fragment, with the author's ms. correction on p. 3, unsigned and undated. 9p. Wanting p. 1. Paginated 2-10.</t>
-  </si>
-  <si>
     <t>Find way to render blank lines on p. 1</t>
   </si>
   <si>
@@ -879,6 +870,213 @@
   </si>
   <si>
     <t>Home to Bess of Hardwick</t>
+  </si>
+  <si>
+    <t>Michelangelo</t>
+  </si>
+  <si>
+    <t>psn-mich</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-mich</t>
+  </si>
+  <si>
+    <t>Raphael</t>
+  </si>
+  <si>
+    <t>psn-raph</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-raph</t>
+  </si>
+  <si>
+    <t>lit-past</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-past</t>
+  </si>
+  <si>
+    <t>cf. psn-past</t>
+  </si>
+  <si>
+    <t>Paston Letters</t>
+  </si>
+  <si>
+    <t>Pilliwinks</t>
+  </si>
+  <si>
+    <t>obj-pill</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#obj-pill</t>
+  </si>
+  <si>
+    <t>Thumbscrews???</t>
+  </si>
+  <si>
+    <t>pla-keni</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-keni</t>
+  </si>
+  <si>
+    <t>Henslowe, Philip</t>
+  </si>
+  <si>
+    <t>psn-phen</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-phen</t>
+  </si>
+  <si>
+    <t>Philip Henslowe (1550-1616)</t>
+  </si>
+  <si>
+    <t>Kenilworth</t>
+  </si>
+  <si>
+    <t>Latimer, Hugh</t>
+  </si>
+  <si>
+    <t>psn-hlat</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-hlat</t>
+  </si>
+  <si>
+    <t>Lord's Prayer</t>
+  </si>
+  <si>
+    <t>lit-lord</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-lord</t>
+  </si>
+  <si>
+    <t>Globe, The</t>
+  </si>
+  <si>
+    <t>pla-glob</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-glob</t>
+  </si>
+  <si>
+    <t>Rose, The</t>
+  </si>
+  <si>
+    <t>pla-rose</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-rose</t>
+  </si>
+  <si>
+    <t>Crown, The</t>
+  </si>
+  <si>
+    <t>pla-crow</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-crow</t>
+  </si>
+  <si>
+    <t>Southwark</t>
+  </si>
+  <si>
+    <t>pla-sout</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-sout</t>
+  </si>
+  <si>
+    <t>Hood, Robin</t>
+  </si>
+  <si>
+    <t>psn-rhoo</t>
+  </si>
+  <si>
+    <t>Everyman</t>
+  </si>
+  <si>
+    <t>lit-ever</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-rhoo</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-ever</t>
+  </si>
+  <si>
+    <t>St George</t>
+  </si>
+  <si>
+    <t>psn-stge</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-stge</t>
+  </si>
+  <si>
+    <t>Faust</t>
+  </si>
+  <si>
+    <t>lit-faus</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-faus</t>
+  </si>
+  <si>
+    <t>lit-tamb</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-tamb</t>
+  </si>
+  <si>
+    <t>Hamlet</t>
+  </si>
+  <si>
+    <t>lit-haml</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-haml</t>
+  </si>
+  <si>
+    <t>King Lear</t>
+  </si>
+  <si>
+    <t>lit-lear</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-lear</t>
+  </si>
+  <si>
+    <t>Antony and Cleopatra</t>
+  </si>
+  <si>
+    <t>lit-ancl</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-ancl</t>
+  </si>
+  <si>
+    <t>Tamburlaine</t>
+  </si>
+  <si>
+    <t>M52. Anon. Typescript fragment with the author's ms. corrections, unsigned and undated. 19p. Paginated [1]-19, wanting p. 5, 14 (two p. 15).</t>
+  </si>
+  <si>
+    <t>M51. Anon. Typescript fragment, with the author's ms. correction on p. 3, unsigned and undated. 9p. Wanting p. 1. Paginated 2-10.</t>
+  </si>
+  <si>
+    <t>m52</t>
+  </si>
+  <si>
+    <t>transcriptions/m52.xml</t>
+  </si>
+  <si>
+    <t>M48. Anon. Typescript fragment, with the author's ms. corrections, unsigned and undated. 2p.</t>
+  </si>
+  <si>
+    <t>M49. [Anon] Typescript fragment, with the author's ms. corrections, unsigned, and undated. 8p. Paginated 3-10. On verso of p. 8-9 her: People one would have liked to have met. Holograph fragment. 2p.</t>
   </si>
 </sst>
 </file>
@@ -1276,9 +1474,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B11" sqref="B11"/>
+      <selection pane="topRight" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,7 +1506,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>11</v>
@@ -1339,19 +1537,19 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>347</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1359,19 +1557,19 @@
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>348</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1379,19 +1577,19 @@
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1399,24 +1597,36 @@
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>223</v>
+        <v>344</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1472,11 +1682,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,137 +1710,137 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>188</v>
+        <v>339</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>189</v>
+        <v>340</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>190</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>116</v>
+        <v>186</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>117</v>
+        <v>187</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>219</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>205</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>206</v>
+        <v>115</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>207</v>
+        <v>116</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>138</v>
+        <v>203</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>139</v>
+        <v>204</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>140</v>
+        <v>205</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>92</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>239</v>
+        <v>87</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>240</v>
+        <v>88</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>241</v>
+        <v>89</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1638,7 +1848,7 @@
         <v>236</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>237</v>
@@ -1649,915 +1859,1204 @@
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>148</v>
+        <v>234</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>147</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>146</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>182</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>183</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>186</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>152</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>148</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>149</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>69</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>242</v>
+        <v>84</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>243</v>
+        <v>85</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>244</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>245</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>58</v>
+        <v>246</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>100</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>165</v>
+        <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>166</v>
+        <v>56</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>167</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>270</v>
+        <v>313</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>271</v>
+        <v>314</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>272</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>75</v>
+        <v>163</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>76</v>
+        <v>164</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>78</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>144</v>
+        <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>146</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>198</v>
+        <v>253</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>170</v>
+        <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>199</v>
+        <v>251</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>200</v>
+        <v>252</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>259</v>
+        <v>142</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>163</v>
+        <v>321</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>164</v>
+        <v>322</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>168</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>113</v>
+        <v>196</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>51</v>
+        <v>168</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>114</v>
+        <v>197</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>115</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>256</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>48</v>
+        <v>328</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>63</v>
+        <v>329</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>49</v>
+        <v>330</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>233</v>
+        <v>161</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>234</v>
+        <v>162</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>235</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>225</v>
+        <v>307</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>226</v>
+        <v>308</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>228</v>
+        <v>309</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>229</v>
+        <v>111</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>230</v>
+        <v>112</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>232</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>110</v>
+        <v>38</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>111</v>
+        <v>57</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>160</v>
+        <v>333</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>161</v>
+        <v>334</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>162</v>
+        <v>335</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>180</v>
+        <v>276</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>196</v>
+        <v>277</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>181</v>
+        <v>278</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>201</v>
+        <v>46</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>202</v>
+        <v>61</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>203</v>
+        <v>93</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>204</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>153</v>
+        <v>230</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>154</v>
+        <v>231</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>155</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>104</v>
+        <v>296</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>105</v>
+        <v>297</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>106</v>
+        <v>298</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>66</v>
+        <v>222</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>67</v>
+        <v>223</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>70</v>
+        <v>224</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>68</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>156</v>
+        <v>226</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>157</v>
+        <v>227</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>158</v>
+        <v>228</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>159</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>54</v>
+        <v>319</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>65</v>
+        <v>320</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>96</v>
+        <v>323</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>251</v>
+        <v>108</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>253</v>
+        <v>109</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>258</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>194</v>
+        <v>300</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>195</v>
+        <v>294</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>197</v>
+        <v>295</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>246</v>
+        <v>159</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>247</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>43</v>
+        <v>336</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>60</v>
+        <v>337</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>97</v>
+        <v>338</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>135</v>
+        <v>178</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>136</v>
+        <v>194</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>137</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>131</v>
+        <v>301</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>132</v>
+        <v>302</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>134</v>
+        <v>303</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>263</v>
+        <v>102</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>264</v>
+        <v>103</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>265</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>260</v>
+        <v>304</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>261</v>
+        <v>305</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>262</v>
+        <v>306</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>170</v>
+        <v>32</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>175</v>
+        <v>156</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>50</v>
+        <v>280</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>77</v>
+        <v>281</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>52</v>
+        <v>282</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>169</v>
+        <v>248</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>170</v>
+        <v>32</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>171</v>
+        <v>250</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>172</v>
+        <v>249</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>53</v>
+        <v>242</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>64</v>
+        <v>243</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>101</v>
+        <v>244</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>266</v>
+        <v>41</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>267</v>
+        <v>58</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>269</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>184</v>
+        <v>209</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>187</v>
+        <v>211</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>191</v>
+        <v>289</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>192</v>
+        <v>286</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>193</v>
+        <v>287</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>214</v>
+        <v>129</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>215</v>
+        <v>130</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>217</v>
+        <v>131</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>221</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>41</v>
+        <v>139</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>42</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>177</v>
+        <v>260</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>178</v>
+        <v>261</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>179</v>
+        <v>262</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>71</v>
+        <v>257</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>72</v>
+        <v>258</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>74</v>
+        <v>259</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>273</v>
+        <v>290</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>34</v>
+        <v>168</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>274</v>
+        <v>291</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>275</v>
+        <v>292</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>278</v>
+        <v>80</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>276</v>
+        <v>81</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>277</v>
+        <v>82</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>279</v>
+        <v>171</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>282</v>
+      <c r="B78" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState ref="A2:F68">
+    <sortState ref="A2:F91">
       <sortCondition ref="A1:A27"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Updates to tracking sheet
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ell-vsvr1\RedirectedFolders\bras3130\Desktop\digital-anon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E079D50A-A970-4D04-B220-3D73B0847DF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CC35C3-319E-4E6E-9ABB-C79553524523}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Annotations!$A$1:$F$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="371">
   <si>
     <t>M-Number</t>
   </si>
@@ -251,9 +250,6 @@
     <t>Bible Guy</t>
   </si>
   <si>
-    <t>English Channel</t>
-  </si>
-  <si>
     <t>pla-chan</t>
   </si>
   <si>
@@ -1070,13 +1066,82 @@
     <t>m52</t>
   </si>
   <si>
+    <t>m53</t>
+  </si>
+  <si>
     <t>transcriptions/m52.xml</t>
   </si>
   <si>
+    <t>transcriptions/m53.xml</t>
+  </si>
+  <si>
     <t>M48. Anon. Typescript fragment, with the author's ms. corrections, unsigned and undated. 2p.</t>
   </si>
   <si>
     <t>M49. [Anon] Typescript fragment, with the author's ms. corrections, unsigned, and undated. 8p. Paginated 3-10. On verso of p. 8-9 her: People one would have liked to have met. Holograph fragment. 2p.</t>
+  </si>
+  <si>
+    <t>M53. Anon. Typescript fragment, unsigned, dated Nov. 24, 1940. With the author's ms corrections. 26p. Paginated 1-25. Two pages paginated 22.</t>
+  </si>
+  <si>
+    <t>Trevelyan, George</t>
+  </si>
+  <si>
+    <t>psn-gtre</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-gtre</t>
+  </si>
+  <si>
+    <t>G. M. Trevelyan, History of England - note, go back and add references</t>
+  </si>
+  <si>
+    <t>History of England</t>
+  </si>
+  <si>
+    <t>lit-hist</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-hist</t>
+  </si>
+  <si>
+    <t>Channel, English</t>
+  </si>
+  <si>
+    <t>Lea, River</t>
+  </si>
+  <si>
+    <t>pla-rlea</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-rlea</t>
+  </si>
+  <si>
+    <t>Rome</t>
+  </si>
+  <si>
+    <t>pla-rome</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-rome</t>
+  </si>
+  <si>
+    <t>Palestine</t>
+  </si>
+  <si>
+    <t>pla-pale</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-pale</t>
+  </si>
+  <si>
+    <t>Description of England</t>
+  </si>
+  <si>
+    <t>lit-desc</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-desc</t>
   </si>
 </sst>
 </file>
@@ -1474,9 +1539,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B37" sqref="B37"/>
+      <selection pane="topRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,13 +1602,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>36</v>
@@ -1557,19 +1622,19 @@
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1577,19 +1642,19 @@
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>36</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1597,19 +1662,19 @@
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1617,10 +1682,10 @@
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>346</v>
@@ -1629,9 +1694,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1682,11 +1756,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,7 +1784,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -1721,19 +1795,19 @@
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1747,142 +1821,142 @@
         <v>53</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>340</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1896,307 +1970,307 @@
         <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>358</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>239</v>
+        <v>83</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>240</v>
+        <v>84</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>241</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="E20" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>313</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>314</v>
+        <v>56</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>315</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>163</v>
+        <v>312</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>164</v>
+        <v>313</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>165</v>
+        <v>314</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>267</v>
+        <v>162</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>268</v>
+        <v>163</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>269</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>266</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>74</v>
+        <v>267</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>76</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>252</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="D32" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2210,38 +2284,38 @@
         <v>57</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>334</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2255,7 +2329,7 @@
         <v>61</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>47</v>
@@ -2263,800 +2337,887 @@
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>222</v>
+        <v>355</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>223</v>
+        <v>356</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>225</v>
+        <v>357</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>319</v>
+        <v>225</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>320</v>
+        <v>226</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>323</v>
+        <v>227</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>108</v>
+        <v>318</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>109</v>
+        <v>319</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>110</v>
+        <v>322</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>300</v>
+        <v>107</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>294</v>
+        <v>108</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>295</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>158</v>
+        <v>299</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>159</v>
+        <v>293</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>160</v>
+        <v>294</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>336</v>
+        <v>157</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>337</v>
+        <v>158</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>338</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>178</v>
+        <v>335</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>194</v>
+        <v>336</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>179</v>
+        <v>337</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>301</v>
+        <v>198</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>302</v>
+        <v>199</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>303</v>
+        <v>200</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>151</v>
+        <v>300</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>152</v>
+        <v>301</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>153</v>
+        <v>302</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>304</v>
+        <v>101</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>305</v>
+        <v>102</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>306</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>64</v>
+        <v>303</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>65</v>
+        <v>304</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>66</v>
+        <v>305</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>154</v>
+        <v>64</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>155</v>
+        <v>65</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>156</v>
+        <v>68</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>157</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>52</v>
+        <v>153</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>63</v>
+        <v>154</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>94</v>
+        <v>155</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>280</v>
+        <v>52</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>281</v>
+        <v>63</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>282</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>248</v>
+        <v>279</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>250</v>
+        <v>280</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>255</v>
+        <v>281</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>192</v>
+        <v>247</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>193</v>
+        <v>249</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>195</v>
+        <v>248</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>242</v>
+        <v>191</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>243</v>
+        <v>192</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>244</v>
+        <v>194</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>41</v>
+        <v>241</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>58</v>
+        <v>242</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>95</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>133</v>
+        <v>41</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>134</v>
+        <v>58</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>209</v>
+        <v>132</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>210</v>
+        <v>133</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>214</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>289</v>
+        <v>208</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>286</v>
+        <v>209</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>287</v>
+        <v>210</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>288</v>
+        <v>213</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>129</v>
+        <v>288</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>130</v>
+        <v>285</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>131</v>
+        <v>286</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>132</v>
+        <v>287</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>260</v>
+        <v>138</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>261</v>
+        <v>139</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>262</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>290</v>
+        <v>256</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>168</v>
+        <v>32</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>80</v>
+        <v>289</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>32</v>
+        <v>167</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>81</v>
+        <v>290</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>82</v>
+        <v>291</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>83</v>
+        <v>292</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>171</v>
+        <v>79</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>168</v>
+        <v>32</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>172</v>
+        <v>80</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>173</v>
+        <v>81</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>43</v>
+        <v>170</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>32</v>
+        <v>167</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>59</v>
+        <v>171</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>283</v>
+        <v>48</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>284</v>
+        <v>74</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>285</v>
+        <v>96</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>310</v>
+        <v>282</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>311</v>
+        <v>283</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>167</v>
+        <v>309</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>168</v>
+        <v>49</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>169</v>
+        <v>310</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>170</v>
+        <v>311</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>206</v>
+        <v>166</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>32</v>
+        <v>167</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>207</v>
+        <v>168</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>208</v>
+        <v>169</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>51</v>
+        <v>205</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>62</v>
+        <v>206</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>99</v>
+        <v>207</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>263</v>
+        <v>51</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>264</v>
+        <v>62</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>266</v>
+        <v>98</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>316</v>
+        <v>262</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>317</v>
+        <v>263</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>318</v>
+        <v>264</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>119</v>
+        <v>315</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>120</v>
+        <v>316</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>121</v>
+        <v>317</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>182</v>
+        <v>118</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>183</v>
+        <v>119</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>185</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>325</v>
+        <v>181</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>326</v>
+        <v>182</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>327</v>
+        <v>184</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>189</v>
+        <v>324</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>190</v>
+        <v>325</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>191</v>
+        <v>326</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>270</v>
+        <v>188</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>271</v>
+        <v>189</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>272</v>
+        <v>190</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>212</v>
+        <v>269</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>213</v>
+        <v>270</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>219</v>
+        <v>271</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>342</v>
+        <v>211</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>331</v>
+        <v>212</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>332</v>
+        <v>214</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>39</v>
+        <v>341</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>60</v>
+        <v>330</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>40</v>
+        <v>331</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>275</v>
+        <v>351</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>273</v>
+        <v>352</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>274</v>
+        <v>353</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>175</v>
+        <v>39</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>176</v>
+        <v>60</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>177</v>
+        <v>99</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C91" s="1" t="s">
+      <c r="B93" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D93" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E93" s="1" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState ref="A2:F91">
+    <sortState ref="A2:F93">
       <sortCondition ref="A1:A27"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Update to title of m54.xml
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ell-vsvr1\RedirectedFolders\bras3130\Desktop\digital-anon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E47574F-7D75-4124-AB77-1E70CA34134C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396E3BAE-5A8D-4780-86D2-871301202D32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="413">
   <si>
     <t>M-Number</t>
   </si>
@@ -1256,6 +1256,18 @@
   </si>
   <si>
     <t>../resources/annotations.xml#pla-fort</t>
+  </si>
+  <si>
+    <t>m54</t>
+  </si>
+  <si>
+    <t>transcriptions/m54.xml</t>
+  </si>
+  <si>
+    <t>Page Count</t>
+  </si>
+  <si>
+    <t>M54. [Anon] Typescript fragments, unsigned and undated, 33p. Fragmentary pagination and not consecutive with the other typescript fragments. On verso of p. 11  unidentified holograph fragment.</t>
   </si>
 </sst>
 </file>
@@ -1651,11 +1663,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G36" sqref="G36"/>
+      <selection pane="topRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,11 +1676,12 @@
     <col min="2" max="2" width="63.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" style="1" customWidth="1"/>
     <col min="4" max="5" width="13.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="54.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="54.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1685,33 +1698,36 @@
         <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1724,14 +1740,17 @@
       <c r="D7" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="5">
+        <v>2</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1744,14 +1763,17 @@
       <c r="D8" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="5">
+        <v>8</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1764,14 +1786,17 @@
       <c r="D9" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="5">
+        <v>9</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1784,14 +1809,17 @@
       <c r="D10" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="5">
+        <v>9</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1804,11 +1832,14 @@
       <c r="D11" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="5">
+        <v>19</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1821,26 +1852,44 @@
       <c r="D12" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="F12" s="5">
+        <v>26</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="F13" s="5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1861,7 +1910,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F1048576">
+  <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -1875,9 +1924,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D109" sqref="D109"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2019,1493 +2068,1493 @@
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>135</v>
+        <v>393</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>136</v>
+        <v>394</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>137</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>369</v>
+        <v>384</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>370</v>
+        <v>385</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>371</v>
+        <v>386</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>375</v>
+        <v>387</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>89</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>234</v>
+        <v>369</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>235</v>
+        <v>370</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>236</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>231</v>
+        <v>86</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>232</v>
+        <v>87</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>233</v>
+        <v>88</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>146</v>
+        <v>234</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>145</v>
+        <v>235</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>144</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>372</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>373</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>100</v>
+        <v>374</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>178</v>
+        <v>231</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>179</v>
+        <v>232</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>182</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>356</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>178</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>55</v>
+        <v>179</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>67</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>83</v>
+        <v>147</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>84</v>
+        <v>148</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>85</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>237</v>
+        <v>356</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>238</v>
+        <v>73</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>239</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>243</v>
+        <v>83</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>244</v>
+        <v>84</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>245</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>237</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>56</v>
+        <v>238</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>97</v>
+        <v>239</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>311</v>
+        <v>104</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>312</v>
+        <v>105</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>313</v>
+        <v>106</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>366</v>
+        <v>390</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>162</v>
+        <v>244</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>163</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>265</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>266</v>
+        <v>56</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>267</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>251</v>
+        <v>311</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>249</v>
+        <v>312</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>252</v>
+        <v>313</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>141</v>
+        <v>366</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>142</v>
+        <v>367</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>143</v>
+        <v>368</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>319</v>
+        <v>161</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>320</v>
+        <v>162</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>322</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>194</v>
+        <v>265</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>195</v>
+        <v>266</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>196</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>116</v>
+        <v>249</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>117</v>
+        <v>250</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>326</v>
+        <v>141</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>327</v>
+        <v>142</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>328</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>159</v>
+        <v>319</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>164</v>
+        <v>322</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>305</v>
+        <v>194</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>306</v>
+        <v>195</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>307</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>110</v>
+        <v>254</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>326</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>57</v>
+        <v>327</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>91</v>
+        <v>328</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>331</v>
+        <v>406</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>332</v>
+        <v>407</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>333</v>
+        <v>408</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>274</v>
+        <v>159</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>275</v>
+        <v>160</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>277</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>46</v>
+        <v>305</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>61</v>
+        <v>306</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>47</v>
+        <v>307</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>228</v>
+        <v>110</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>229</v>
+        <v>111</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>230</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>294</v>
+        <v>38</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>295</v>
+        <v>57</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>297</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>353</v>
+        <v>399</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>354</v>
+        <v>400</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>355</v>
+        <v>401</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>220</v>
+        <v>331</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>221</v>
+        <v>332</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>223</v>
+        <v>333</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>224</v>
+        <v>274</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>225</v>
+        <v>275</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>226</v>
+        <v>276</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>227</v>
+        <v>277</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>317</v>
+        <v>46</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>318</v>
+        <v>61</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>321</v>
+        <v>92</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>107</v>
+        <v>228</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>108</v>
+        <v>229</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>293</v>
+        <v>296</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>176</v>
+        <v>353</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>192</v>
+        <v>354</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>177</v>
+        <v>355</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>299</v>
+        <v>224</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>300</v>
+        <v>225</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>301</v>
+        <v>226</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>150</v>
+        <v>317</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>151</v>
+        <v>318</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>152</v>
+        <v>321</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>357</v>
+        <v>107</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>358</v>
+        <v>108</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>359</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>383</v>
+        <v>298</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>334</v>
+        <v>292</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>335</v>
+        <v>293</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>101</v>
+        <v>176</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>102</v>
+        <v>192</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>103</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>302</v>
+        <v>197</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>303</v>
+        <v>198</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>304</v>
+        <v>199</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>64</v>
+        <v>299</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>65</v>
+        <v>300</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>66</v>
+        <v>301</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>52</v>
+        <v>357</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>63</v>
+        <v>358</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>93</v>
+        <v>359</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>278</v>
+        <v>383</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>279</v>
+        <v>334</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>280</v>
+        <v>335</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>246</v>
+        <v>101</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>248</v>
+        <v>102</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>253</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>190</v>
+        <v>403</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>191</v>
+        <v>404</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>193</v>
+        <v>405</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>240</v>
+        <v>302</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>241</v>
+        <v>303</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>242</v>
+        <v>304</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>94</v>
+        <v>68</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>134</v>
+        <v>155</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>207</v>
+        <v>52</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>208</v>
+        <v>63</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>212</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>378</v>
+        <v>278</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>379</v>
+        <v>279</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>380</v>
+        <v>280</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>363</v>
+        <v>246</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>364</v>
+        <v>248</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>365</v>
+        <v>247</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>287</v>
+        <v>190</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>284</v>
+        <v>191</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>286</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>128</v>
+        <v>240</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>129</v>
+        <v>241</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>131</v>
+        <v>242</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>138</v>
+        <v>41</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>139</v>
+        <v>58</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>258</v>
+        <v>396</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>259</v>
+        <v>397</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>260</v>
+        <v>398</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>255</v>
+        <v>132</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>256</v>
+        <v>133</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>257</v>
+        <v>134</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>288</v>
+        <v>207</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>289</v>
+        <v>208</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>290</v>
+        <v>209</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>291</v>
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>79</v>
+        <v>378</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>80</v>
+        <v>379</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>82</v>
+        <v>380</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>169</v>
+        <v>363</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>166</v>
+        <v>49</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>170</v>
+        <v>364</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>171</v>
+        <v>365</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>43</v>
+        <v>287</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>59</v>
+        <v>284</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>95</v>
+        <v>285</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>74</v>
+        <v>129</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>50</v>
+        <v>131</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>281</v>
+        <v>138</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>282</v>
+        <v>139</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>283</v>
+        <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>360</v>
+        <v>258</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>361</v>
+        <v>259</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>362</v>
+        <v>260</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>308</v>
+        <v>255</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>309</v>
+        <v>256</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>310</v>
+        <v>257</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>165</v>
+        <v>288</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>166</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>167</v>
+        <v>289</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>168</v>
+        <v>290</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>204</v>
+        <v>79</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>205</v>
+        <v>80</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>206</v>
+        <v>81</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>51</v>
+        <v>169</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>32</v>
+        <v>166</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>62</v>
+        <v>170</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>98</v>
+        <v>171</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>261</v>
+        <v>43</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>262</v>
+        <v>59</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>264</v>
+        <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>314</v>
+        <v>48</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>315</v>
+        <v>74</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>316</v>
+        <v>96</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>118</v>
+        <v>281</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>119</v>
+        <v>282</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>120</v>
+        <v>283</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>181</v>
+        <v>361</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>183</v>
+        <v>362</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>268</v>
+        <v>204</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>269</v>
+        <v>205</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>270</v>
+        <v>206</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>210</v>
+        <v>51</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>211</v>
+        <v>62</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>217</v>
+        <v>98</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>339</v>
+        <v>261</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>329</v>
+        <v>262</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>330</v>
+        <v>263</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>349</v>
+        <v>314</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>350</v>
+        <v>315</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>352</v>
+        <v>316</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>273</v>
+        <v>180</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>271</v>
+        <v>181</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>272</v>
+        <v>183</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>173</v>
+        <v>323</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>174</v>
+        <v>324</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>175</v>
+        <v>325</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>69</v>
+        <v>187</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>70</v>
+        <v>188</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>72</v>
+        <v>189</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>384</v>
+        <v>268</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>385</v>
+        <v>269</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>386</v>
+        <v>270</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>387</v>
+        <v>210</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>388</v>
+        <v>211</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>389</v>
+        <v>213</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>390</v>
+        <v>339</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>391</v>
+        <v>329</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>392</v>
+        <v>330</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>393</v>
+        <v>349</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>394</v>
+        <v>350</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>395</v>
+        <v>351</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>396</v>
+        <v>39</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>397</v>
+        <v>60</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>398</v>
+        <v>99</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>399</v>
+        <v>273</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>400</v>
+        <v>271</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>402</v>
+        <v>272</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>403</v>
+        <v>173</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>404</v>
+        <v>174</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>405</v>
+        <v>175</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>406</v>
+        <v>69</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>407</v>
+        <v>70</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>408</v>
+        <v>71</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState ref="A2:F101">
+    <sortState ref="A2:F109">
       <sortCondition ref="A1:A27"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Further updates to tracking sheet
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ell-vsvr1\RedirectedFolders\bras3130\Desktop\digital-anon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396E3BAE-5A8D-4780-86D2-871301202D32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B5101E-C604-48BE-A449-06A0DAE23E94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="423">
   <si>
     <t>M-Number</t>
   </si>
@@ -1268,6 +1268,36 @@
   </si>
   <si>
     <t>M54. [Anon] Typescript fragments, unsigned and undated, 33p. Fragmentary pagination and not consecutive with the other typescript fragments. On verso of p. 11  unidentified holograph fragment.</t>
+  </si>
+  <si>
+    <t>Golden Bowl, The</t>
+  </si>
+  <si>
+    <t>lit-gold</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-gold</t>
+  </si>
+  <si>
+    <t>Ambassadors, The</t>
+  </si>
+  <si>
+    <t>lit-amba</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-amba</t>
+  </si>
+  <si>
+    <t>Edward IV</t>
+  </si>
+  <si>
+    <t>psn-edw4</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-edw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is this actually Edward IV??? I'm guessing based on Latimer and the c16th but then again… Check against quotes! </t>
   </si>
 </sst>
 </file>
@@ -1665,9 +1695,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B13" sqref="B13"/>
+      <selection pane="topRight" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,11 +1952,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F109"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3552,6 +3582,51 @@
         <v>72</v>
       </c>
     </row>
+    <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
     <sortState ref="A2:F109">

</xml_diff>

<commit_message>
initial commit for m108.xml
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537385ED-9F22-6C4B-9E30-6255DC4BE4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442B7CC9-58AB-B24B-B3D6-E545F8283252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12220" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="429">
   <si>
     <t>M-Number</t>
   </si>
@@ -1318,6 +1318,15 @@
   </si>
   <si>
     <t>../resources/annotations.xml#lit-shep</t>
+  </si>
+  <si>
+    <t>Leland, John</t>
+  </si>
+  <si>
+    <t>psn-jlel</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-jlel</t>
   </si>
 </sst>
 </file>
@@ -1972,11 +1981,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F113"/>
+  <dimension ref="A1:F114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3661,6 +3670,20 @@
         <v>72</v>
       </c>
     </row>
+    <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F113">

</xml_diff>

<commit_message>
Yet more updates to tracking sheet
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A9D590-3277-9A41-B5E9-971170092CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B748704-DDDB-B142-A2AB-09EF5423BCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41200" yWindow="0" windowWidth="10000" windowHeight="28800" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="37120" yWindow="0" windowWidth="14080" windowHeight="28800" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="488">
   <si>
     <t>M-Number</t>
   </si>
@@ -1542,6 +1542,12 @@
   </si>
   <si>
     <t>../resources/annotations.xml#pla-lund</t>
+  </si>
+  <si>
+    <t>heheheheheheh</t>
+  </si>
+  <si>
+    <t>trac</t>
   </si>
 </sst>
 </file>
@@ -1947,9 +1953,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B14" sqref="B14"/>
+      <selection pane="topRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2158,7 +2164,10 @@
         <v>409</v>
       </c>
       <c r="F13" s="5">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2181,6 +2190,9 @@
     <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2218,9 +2230,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
   <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E125" sqref="E125"/>
+    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2286,1936 +2298,1939 @@
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>415</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>416</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>90</v>
+        <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>336</v>
+        <v>477</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>337</v>
+        <v>478</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>338</v>
+        <v>479</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>184</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>185</v>
+        <v>53</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>382</v>
+        <v>336</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>157</v>
+        <v>337</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>158</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>113</v>
+        <v>184</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>114</v>
+        <v>185</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>201</v>
+        <v>382</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>216</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>393</v>
+        <v>113</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>394</v>
+        <v>114</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>395</v>
+        <v>115</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>384</v>
+        <v>201</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>385</v>
+        <v>202</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>386</v>
+        <v>203</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>453</v>
+        <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>135</v>
+        <v>384</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>136</v>
+        <v>385</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>137</v>
+        <v>386</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>369</v>
+        <v>451</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>370</v>
+        <v>452</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>371</v>
+        <v>453</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>375</v>
+        <v>387</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>234</v>
+        <v>369</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>235</v>
+        <v>370</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>236</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>231</v>
+        <v>86</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>232</v>
+        <v>87</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>146</v>
+        <v>234</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>145</v>
+        <v>235</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>144</v>
+        <v>236</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>372</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>54</v>
+        <v>373</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>100</v>
+        <v>374</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>178</v>
+        <v>231</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>179</v>
+        <v>232</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>182</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>356</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>178</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>55</v>
+        <v>179</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>67</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>83</v>
+        <v>147</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>84</v>
+        <v>148</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>85</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>237</v>
+        <v>356</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>238</v>
+        <v>73</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>239</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>214</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>390</v>
+        <v>83</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>391</v>
+        <v>84</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>392</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>243</v>
+        <v>461</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>244</v>
+        <v>462</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>245</v>
+        <v>463</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>237</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>56</v>
+        <v>238</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>97</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>311</v>
+        <v>104</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>312</v>
+        <v>105</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>313</v>
+        <v>106</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>366</v>
+        <v>390</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>367</v>
+        <v>391</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>368</v>
+        <v>392</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>161</v>
+        <v>243</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>162</v>
+        <v>244</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>163</v>
+        <v>245</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>418</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>419</v>
+        <v>56</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>421</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>265</v>
+        <v>311</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>266</v>
+        <v>312</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>267</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>251</v>
+        <v>366</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>249</v>
+        <v>367</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>252</v>
+        <v>368</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>319</v>
+        <v>418</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>320</v>
+        <v>419</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>322</v>
+        <v>420</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>194</v>
+        <v>418</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>195</v>
+        <v>419</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>196</v>
+        <v>420</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>116</v>
+        <v>266</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>117</v>
+        <v>267</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>326</v>
+        <v>251</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>327</v>
+        <v>249</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>328</v>
+        <v>250</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>405</v>
+        <v>464</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>306</v>
+        <v>320</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>307</v>
+        <v>322</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>412</v>
+        <v>194</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>45</v>
+        <v>166</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>413</v>
+        <v>195</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>414</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>110</v>
+        <v>254</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>38</v>
+        <v>326</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>57</v>
+        <v>327</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>91</v>
+        <v>328</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>457</v>
+        <v>405</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>331</v>
+        <v>159</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>332</v>
+        <v>160</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>333</v>
+        <v>164</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>274</v>
+        <v>305</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>275</v>
+        <v>306</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>277</v>
+        <v>307</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>46</v>
+        <v>412</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>61</v>
+        <v>413</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>47</v>
+        <v>414</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>228</v>
+        <v>412</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>229</v>
+        <v>413</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>230</v>
+        <v>414</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>294</v>
+        <v>110</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>295</v>
+        <v>111</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>297</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>353</v>
+        <v>38</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>354</v>
+        <v>57</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>355</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>220</v>
+        <v>457</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>221</v>
+        <v>399</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>222</v>
+        <v>400</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>223</v>
+        <v>401</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>224</v>
+        <v>331</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>225</v>
+        <v>332</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>227</v>
+        <v>333</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>317</v>
+        <v>274</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>321</v>
+        <v>276</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>109</v>
+        <v>92</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>298</v>
+        <v>472</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>292</v>
+        <v>473</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>293</v>
+        <v>474</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>454</v>
+        <v>228</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>455</v>
+        <v>229</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>456</v>
+        <v>230</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>176</v>
+        <v>294</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>192</v>
+        <v>295</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>177</v>
+        <v>296</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>197</v>
+        <v>353</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>198</v>
+        <v>354</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>299</v>
+        <v>220</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>300</v>
+        <v>221</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>301</v>
+        <v>222</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>150</v>
+        <v>224</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>151</v>
+        <v>225</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>152</v>
+        <v>226</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>357</v>
+        <v>317</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>359</v>
+        <v>321</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>383</v>
+        <v>107</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>334</v>
+        <v>108</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>335</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>425</v>
+        <v>298</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>426</v>
+        <v>292</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>427</v>
+        <v>293</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>101</v>
+        <v>454</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>102</v>
+        <v>455</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>103</v>
+        <v>456</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>402</v>
+        <v>176</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>403</v>
+        <v>192</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>404</v>
+        <v>177</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>302</v>
+        <v>197</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>303</v>
+        <v>198</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>304</v>
+        <v>199</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>64</v>
+        <v>299</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>65</v>
+        <v>300</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>66</v>
+        <v>301</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>432</v>
+        <v>357</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>433</v>
+        <v>358</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>435</v>
+        <v>359</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>52</v>
+        <v>383</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>63</v>
+        <v>334</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>93</v>
+        <v>335</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>278</v>
+        <v>425</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>279</v>
+        <v>426</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>280</v>
+        <v>427</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>246</v>
+        <v>101</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>248</v>
+        <v>102</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>253</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>190</v>
+        <v>402</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>191</v>
+        <v>403</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>193</v>
+        <v>404</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>446</v>
+        <v>302</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>445</v>
+        <v>303</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>444</v>
+        <v>304</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>240</v>
+        <v>483</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>241</v>
+        <v>484</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>242</v>
+        <v>485</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>94</v>
+        <v>68</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>396</v>
+        <v>153</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>397</v>
+        <v>154</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>398</v>
+        <v>155</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>132</v>
+        <v>432</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>133</v>
+        <v>433</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>134</v>
+        <v>434</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>207</v>
+        <v>52</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>208</v>
+        <v>63</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>212</v>
+        <v>93</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>378</v>
+        <v>278</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>379</v>
+        <v>279</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>380</v>
+        <v>280</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>363</v>
+        <v>246</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>364</v>
+        <v>248</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>365</v>
+        <v>247</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>287</v>
+        <v>190</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>284</v>
+        <v>191</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>286</v>
+        <v>193</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>128</v>
+        <v>446</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>129</v>
+        <v>445</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>130</v>
+        <v>447</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>131</v>
+        <v>444</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>138</v>
+        <v>240</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>139</v>
+        <v>241</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>140</v>
+        <v>242</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>258</v>
+        <v>41</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>259</v>
+        <v>58</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>260</v>
+        <v>94</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>255</v>
+        <v>396</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>32</v>
+        <v>166</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>256</v>
+        <v>397</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>257</v>
+        <v>398</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>288</v>
+        <v>132</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>166</v>
+        <v>49</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>289</v>
+        <v>133</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>291</v>
+        <v>134</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>79</v>
+        <v>207</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>80</v>
+        <v>208</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>81</v>
+        <v>209</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>82</v>
+        <v>212</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>169</v>
+        <v>467</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>166</v>
+        <v>45</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>170</v>
+        <v>468</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>171</v>
+        <v>469</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>43</v>
+        <v>378</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>59</v>
+        <v>379</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>95</v>
+        <v>380</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>48</v>
+        <v>363</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>74</v>
+        <v>364</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>50</v>
+        <v>365</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>360</v>
+        <v>128</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>361</v>
+        <v>129</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>362</v>
+        <v>130</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>308</v>
+        <v>138</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>309</v>
+        <v>139</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>310</v>
+        <v>140</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>165</v>
+        <v>258</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>166</v>
+        <v>49</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>167</v>
+        <v>259</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>168</v>
+        <v>260</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>204</v>
+        <v>255</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>205</v>
+        <v>256</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>206</v>
+        <v>257</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>51</v>
+        <v>288</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>32</v>
+        <v>166</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>62</v>
+        <v>289</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>98</v>
+        <v>290</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>422</v>
+        <v>79</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>423</v>
+        <v>80</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>424</v>
+        <v>81</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>261</v>
+        <v>169</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>32</v>
+        <v>166</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>262</v>
+        <v>170</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>264</v>
+        <v>171</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>440</v>
+        <v>43</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>441</v>
+        <v>59</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>443</v>
+        <v>95</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>314</v>
+        <v>48</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>315</v>
+        <v>74</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>316</v>
+        <v>96</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>118</v>
+        <v>281</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>119</v>
+        <v>282</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>120</v>
+        <v>283</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>181</v>
+        <v>361</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>183</v>
+        <v>362</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>268</v>
+        <v>204</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>269</v>
+        <v>205</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>270</v>
+        <v>206</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>210</v>
+        <v>51</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>211</v>
+        <v>62</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>217</v>
+        <v>98</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>339</v>
+        <v>422</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>329</v>
+        <v>423</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>330</v>
+        <v>424</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>349</v>
+        <v>422</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>350</v>
+        <v>423</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>352</v>
+        <v>424</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>39</v>
+        <v>261</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>60</v>
+        <v>262</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>99</v>
+        <v>263</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>40</v>
+        <v>264</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>273</v>
+        <v>314</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>271</v>
+        <v>315</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>272</v>
+        <v>316</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>173</v>
+        <v>118</v>
       </c>
       <c r="B119" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C120" s="1" t="s">
-        <v>429</v>
+        <v>181</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>431</v>
+        <v>183</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>69</v>
+        <v>323</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>70</v>
+        <v>324</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>72</v>
+        <v>325</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>460</v>
+        <v>187</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>458</v>
+        <v>188</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>459</v>
+        <v>189</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>461</v>
+        <v>480</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>462</v>
+        <v>481</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>463</v>
+        <v>482</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>464</v>
+        <v>268</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>465</v>
+        <v>269</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>471</v>
+        <v>270</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>467</v>
+        <v>210</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>468</v>
+        <v>211</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>469</v>
+        <v>213</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>470</v>
+        <v>217</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>472</v>
+        <v>339</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>473</v>
+        <v>329</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>475</v>
+        <v>330</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>412</v>
+        <v>349</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>413</v>
+        <v>350</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>414</v>
+        <v>351</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>415</v>
+        <v>39</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>416</v>
+        <v>60</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>417</v>
+        <v>99</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>418</v>
+        <v>436</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>419</v>
+        <v>437</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>420</v>
+        <v>438</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>476</v>
+        <v>439</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>422</v>
+        <v>273</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>423</v>
+        <v>271</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>424</v>
+        <v>272</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>477</v>
+        <v>173</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>478</v>
+        <v>174</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>480</v>
+        <v>428</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>481</v>
+        <v>429</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>482</v>
+        <v>430</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>483</v>
+        <v>69</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>484</v>
+        <v>70</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>485</v>
+        <v>71</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F121">
-      <sortCondition ref="A1:A121"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F133">
+      <sortCondition ref="A1:A133"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="F1:F1048576">

</xml_diff>

<commit_message>
further additions to tracking sheet
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B748704-DDDB-B142-A2AB-09EF5423BCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56C54E7-1C62-AE40-9882-16063BAF975A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37120" yWindow="0" windowWidth="14080" windowHeight="28800" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="519">
   <si>
     <t>M-Number</t>
   </si>
@@ -1547,7 +1547,100 @@
     <t>heheheheheheh</t>
   </si>
   <si>
-    <t>trac</t>
+    <t>Deptford</t>
+  </si>
+  <si>
+    <t>pla-dept</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-dept</t>
+  </si>
+  <si>
+    <t>Frizer, Ingram</t>
+  </si>
+  <si>
+    <t>psn-ifriz</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-ifriz</t>
+  </si>
+  <si>
+    <t>Jonson, Ben</t>
+  </si>
+  <si>
+    <t>psn-bjon</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-bjon</t>
+  </si>
+  <si>
+    <t>Spenser, Gabriel</t>
+  </si>
+  <si>
+    <t>psn-gspe</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-gspe</t>
+  </si>
+  <si>
+    <t>Kempe, William</t>
+  </si>
+  <si>
+    <t>psn-wkem</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-wkem</t>
+  </si>
+  <si>
+    <t>Norwich</t>
+  </si>
+  <si>
+    <t>pla-norw</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-norw</t>
+  </si>
+  <si>
+    <t>Tennyson, Arthur</t>
+  </si>
+  <si>
+    <t>Browning, Robert</t>
+  </si>
+  <si>
+    <t>psn-aten</t>
+  </si>
+  <si>
+    <t>psn-rbro</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-aten</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-rbro</t>
+  </si>
+  <si>
+    <t>Hobbes, Thomas</t>
+  </si>
+  <si>
+    <t>psn-thob</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-thob</t>
+  </si>
+  <si>
+    <t>Thoby?</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-gard</t>
+  </si>
+  <si>
+    <t>lit-gard</t>
+  </si>
+  <si>
+    <t>Garden, The</t>
+  </si>
+  <si>
+    <t>Marvell</t>
   </si>
 </sst>
 </file>
@@ -1953,7 +2046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B15" sqref="B15"/>
     </sheetView>
@@ -2191,9 +2284,6 @@
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>487</v>
-      </c>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -2228,11 +2318,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E143" sqref="E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4227,6 +4317,152 @@
         <v>72</v>
       </c>
     </row>
+    <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F133">

</xml_diff>

<commit_message>
Further additions to tracking sheet concerning m111.xml
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879CB1F6-80FC-7D49-839C-2ACFBAB2C403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B8B72A-9F85-094F-BC07-C76964B13A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="551">
   <si>
     <t>M-Number</t>
   </si>
@@ -1719,6 +1719,24 @@
   </si>
   <si>
     <t>../resources/annotations.xml#lit-stra</t>
+  </si>
+  <si>
+    <t>Grenwich</t>
+  </si>
+  <si>
+    <t>pla-gren</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-gren</t>
+  </si>
+  <si>
+    <t>Whitehall</t>
+  </si>
+  <si>
+    <t>pla-whit</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-whit</t>
   </si>
 </sst>
 </file>
@@ -2411,11 +2429,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F151"/>
+  <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E151" sqref="E151"/>
+      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4665,6 +4683,34 @@
         <v>544</v>
       </c>
     </row>
+    <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F150">

</xml_diff>

<commit_message>
Further updates to tracking sheet, fixing an embarrassing typo
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joshua/Documents/digital-anon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B8B72A-9F85-094F-BC07-C76964B13A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EC38CF-B033-B34C-9C04-1458B1AF60F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -1721,9 +1721,6 @@
     <t>../resources/annotations.xml#lit-stra</t>
   </si>
   <si>
-    <t>Grenwich</t>
-  </si>
-  <si>
     <t>pla-gren</t>
   </si>
   <si>
@@ -1737,6 +1734,9 @@
   </si>
   <si>
     <t>../resources/annotations.xml#pla-whit</t>
+  </si>
+  <si>
+    <t>Greenwich</t>
   </si>
 </sst>
 </file>
@@ -2433,7 +2433,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E153" sqref="E153"/>
+      <selection pane="bottomLeft" activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4685,30 +4685,30 @@
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C152" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D152" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C153" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="D153" s="1" t="s">
         <v>549</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to tracking sheet with details of m110.xml
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EC38CF-B033-B34C-9C04-1458B1AF60F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8056DADB-28A5-DE43-8F17-75DA1E48EA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="38360" yWindow="0" windowWidth="12840" windowHeight="28800" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="554">
   <si>
     <t>M-Number</t>
   </si>
@@ -1333,6 +1333,363 @@
   </si>
   <si>
     <t>../resources/annotations.xml#psn-hwri</t>
+  </si>
+  <si>
+    <t>Manners, Francis</t>
+  </si>
+  <si>
+    <t>psn-fmann</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-fmann</t>
+  </si>
+  <si>
+    <t>Sixth Earl of Rutland, probably. Employed Shakespeare and Richard Burbage to paint his emblem.</t>
+  </si>
+  <si>
+    <t>Whyte, Roland</t>
+  </si>
+  <si>
+    <t>psn-rwhy</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-rwhy</t>
+  </si>
+  <si>
+    <t>https://www.jstor.org/stable/2856997</t>
+  </si>
+  <si>
+    <t>Sidney, Sir Robert</t>
+  </si>
+  <si>
+    <t>psn-rsid</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-rsid</t>
+  </si>
+  <si>
+    <t>Younger brother to #psn-psid</t>
+  </si>
+  <si>
+    <t>Mysterious dedicatee of Shakespeare's Sonnets</t>
+  </si>
+  <si>
+    <t>psn-mrwh</t>
+  </si>
+  <si>
+    <t>Mr. W. H</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-mrwh</t>
+  </si>
+  <si>
+    <t>m108</t>
+  </si>
+  <si>
+    <t>transcriptions/m108.xml</t>
+  </si>
+  <si>
+    <t>M108 [The Reader]. Typescript fragment, with the author's ms. corrections, unsigned and undated. 7p. Paginated 23-28, with an unpaginated page at end.</t>
+  </si>
+  <si>
+    <t>Beaumont, Francis</t>
+  </si>
+  <si>
+    <t>psn-fbea</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-fbea</t>
+  </si>
+  <si>
+    <t>Kyd, Thomas</t>
+  </si>
+  <si>
+    <t>psn-tkyd</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-tkyd</t>
+  </si>
+  <si>
+    <t>Greg, Dr W. W.</t>
+  </si>
+  <si>
+    <t>lit-balle</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-balle</t>
+  </si>
+  <si>
+    <t>Ballet Russes</t>
+  </si>
+  <si>
+    <t>Cinema</t>
+  </si>
+  <si>
+    <t>lit-cine</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-cine</t>
+  </si>
+  <si>
+    <t>Essays (Bacon)</t>
+  </si>
+  <si>
+    <t>lit-baes</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-baes</t>
+  </si>
+  <si>
+    <t>Of Masques and Triumphs</t>
+  </si>
+  <si>
+    <t>lit-masq</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-masq</t>
+  </si>
+  <si>
+    <t>One of psn-fbac essays (cf. lit-baes)</t>
+  </si>
+  <si>
+    <t>cf. psn-fbac, lit-masq</t>
+  </si>
+  <si>
+    <t>Heart of Darkness</t>
+  </si>
+  <si>
+    <t>lit-hear</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-hear</t>
+  </si>
+  <si>
+    <t>A pun at end of m108.4, cf. psn-cmar</t>
+  </si>
+  <si>
+    <t>Is this actually Edward IV??? I'm guessing based on Latimer and the c16th but then again… Check against quotes! </t>
+  </si>
+  <si>
+    <t>Amesbury</t>
+  </si>
+  <si>
+    <t>pla-ames</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-ames</t>
+  </si>
+  <si>
+    <t>Stonehenge</t>
+  </si>
+  <si>
+    <t>pla-ston</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-ston</t>
+  </si>
+  <si>
+    <t>Lundy, Isle of</t>
+  </si>
+  <si>
+    <t>pla-lund</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-lund</t>
+  </si>
+  <si>
+    <t>heheheheheheh</t>
+  </si>
+  <si>
+    <t>Deptford</t>
+  </si>
+  <si>
+    <t>pla-dept</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-dept</t>
+  </si>
+  <si>
+    <t>Frizer, Ingram</t>
+  </si>
+  <si>
+    <t>psn-ifriz</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-ifriz</t>
+  </si>
+  <si>
+    <t>Jonson, Ben</t>
+  </si>
+  <si>
+    <t>psn-bjon</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-bjon</t>
+  </si>
+  <si>
+    <t>Spenser, Gabriel</t>
+  </si>
+  <si>
+    <t>psn-gspe</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-gspe</t>
+  </si>
+  <si>
+    <t>Kempe, William</t>
+  </si>
+  <si>
+    <t>psn-wkem</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-wkem</t>
+  </si>
+  <si>
+    <t>Norwich</t>
+  </si>
+  <si>
+    <t>pla-norw</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-norw</t>
+  </si>
+  <si>
+    <t>Tennyson, Arthur</t>
+  </si>
+  <si>
+    <t>Browning, Robert</t>
+  </si>
+  <si>
+    <t>psn-aten</t>
+  </si>
+  <si>
+    <t>psn-rbro</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-aten</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-rbro</t>
+  </si>
+  <si>
+    <t>Hobbes, Thomas</t>
+  </si>
+  <si>
+    <t>psn-thob</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-thob</t>
+  </si>
+  <si>
+    <t>Thoby?</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-gard</t>
+  </si>
+  <si>
+    <t>lit-gard</t>
+  </si>
+  <si>
+    <t>Garden, The</t>
+  </si>
+  <si>
+    <t>Marvell</t>
+  </si>
+  <si>
+    <t>Fytton, Sir Edward</t>
+  </si>
+  <si>
+    <t>psn-efyt</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-efyt</t>
+  </si>
+  <si>
+    <t>Gawsworth</t>
+  </si>
+  <si>
+    <t>Cheshire</t>
+  </si>
+  <si>
+    <t>pla-gaws</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-gaws</t>
+  </si>
+  <si>
+    <t>pla-ches</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-ches</t>
+  </si>
+  <si>
+    <t>Fytton, Mary</t>
+  </si>
+  <si>
+    <t>psn-mfyt</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-mfyt</t>
+  </si>
+  <si>
+    <t>Knollys, Sir William</t>
+  </si>
+  <si>
+    <t>psn-wkno</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-wkno</t>
+  </si>
+  <si>
+    <t>Chopping Knife near Ludgate</t>
+  </si>
+  <si>
+    <t>pla-chop</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml/pla-chop</t>
+  </si>
+  <si>
+    <t>Pembroke, Lord William</t>
+  </si>
+  <si>
+    <t>psn-wpem</t>
+  </si>
+  <si>
+    <t>M109 [The Reader]. Typescript, fragment, with the author's ms. corrections, unsigned and undated. 9p.</t>
+  </si>
+  <si>
+    <t>m109</t>
+  </si>
+  <si>
+    <t>transcriptions/m109.xml</t>
+  </si>
+  <si>
+    <t>Elizabeth and Essex</t>
+  </si>
+  <si>
+    <t>lit-stra</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-stra</t>
+  </si>
+  <si>
+    <t>pla-gren</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-gren</t>
+  </si>
+  <si>
+    <t>Whitehall</t>
+  </si>
+  <si>
+    <t>pla-whit</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-whit</t>
+  </si>
+  <si>
+    <t>Greenwich</t>
   </si>
   <si>
     <r>
@@ -1378,365 +1735,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> to him and he has been identified as Fair Youth of Sonnets. Son of Call-Me-Wrisley from Wolf Hall...</t>
+      <t xml:space="preserve"> to him and he has been identified as Fair Youth of Sonnets. Son of Call-Me-Risley from Wolf Hall...</t>
     </r>
   </si>
   <si>
-    <t>Manners, Francis</t>
-  </si>
-  <si>
-    <t>psn-fmann</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-fmann</t>
-  </si>
-  <si>
-    <t>Sixth Earl of Rutland, probably. Employed Shakespeare and Richard Burbage to paint his emblem.</t>
-  </si>
-  <si>
-    <t>Whyte, Roland</t>
-  </si>
-  <si>
-    <t>psn-rwhy</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-rwhy</t>
-  </si>
-  <si>
-    <t>https://www.jstor.org/stable/2856997</t>
-  </si>
-  <si>
-    <t>Sidney, Sir Robert</t>
-  </si>
-  <si>
-    <t>psn-rsid</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-rsid</t>
-  </si>
-  <si>
-    <t>Younger brother to #psn-psid</t>
-  </si>
-  <si>
-    <t>Mysterious dedicatee of Shakespeare's Sonnets</t>
-  </si>
-  <si>
-    <t>psn-mrwh</t>
-  </si>
-  <si>
-    <t>Mr. W. H</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-mrwh</t>
-  </si>
-  <si>
-    <t>m108</t>
-  </si>
-  <si>
-    <t>transcriptions/m108.xml</t>
-  </si>
-  <si>
-    <t>M108 [The Reader]. Typescript fragment, with the author's ms. corrections, unsigned and undated. 7p. Paginated 23-28, with an unpaginated page at end.</t>
-  </si>
-  <si>
-    <t>Beaumont, Francis</t>
-  </si>
-  <si>
-    <t>psn-fbea</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-fbea</t>
-  </si>
-  <si>
-    <t>Kyd, Thomas</t>
-  </si>
-  <si>
-    <t>psn-tkyd</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-tkyd</t>
-  </si>
-  <si>
-    <t>Greg, Dr W. W.</t>
-  </si>
-  <si>
-    <t>lit-balle</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#lit-balle</t>
-  </si>
-  <si>
-    <t>Ballet Russes</t>
-  </si>
-  <si>
-    <t>Cinema</t>
-  </si>
-  <si>
-    <t>lit-cine</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#lit-cine</t>
-  </si>
-  <si>
-    <t>Essays (Bacon)</t>
-  </si>
-  <si>
-    <t>lit-baes</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#lit-baes</t>
-  </si>
-  <si>
-    <t>Of Masques and Triumphs</t>
-  </si>
-  <si>
-    <t>lit-masq</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#lit-masq</t>
-  </si>
-  <si>
-    <t>One of psn-fbac essays (cf. lit-baes)</t>
-  </si>
-  <si>
-    <t>cf. psn-fbac, lit-masq</t>
-  </si>
-  <si>
-    <t>Heart of Darkness</t>
-  </si>
-  <si>
-    <t>lit-hear</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#lit-hear</t>
-  </si>
-  <si>
-    <t>A pun at end of m108.4, cf. psn-cmar</t>
-  </si>
-  <si>
-    <t>Is this actually Edward IV??? I'm guessing based on Latimer and the c16th but then again… Check against quotes! </t>
-  </si>
-  <si>
-    <t>Amesbury</t>
-  </si>
-  <si>
-    <t>pla-ames</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#pla-ames</t>
-  </si>
-  <si>
-    <t>Stonehenge</t>
-  </si>
-  <si>
-    <t>pla-ston</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#pla-ston</t>
-  </si>
-  <si>
-    <t>Lundy, Isle of</t>
-  </si>
-  <si>
-    <t>pla-lund</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#pla-lund</t>
-  </si>
-  <si>
-    <t>heheheheheheh</t>
-  </si>
-  <si>
-    <t>Deptford</t>
-  </si>
-  <si>
-    <t>pla-dept</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#pla-dept</t>
-  </si>
-  <si>
-    <t>Frizer, Ingram</t>
-  </si>
-  <si>
-    <t>psn-ifriz</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-ifriz</t>
-  </si>
-  <si>
-    <t>Jonson, Ben</t>
-  </si>
-  <si>
-    <t>psn-bjon</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-bjon</t>
-  </si>
-  <si>
-    <t>Spenser, Gabriel</t>
-  </si>
-  <si>
-    <t>psn-gspe</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-gspe</t>
-  </si>
-  <si>
-    <t>Kempe, William</t>
-  </si>
-  <si>
-    <t>psn-wkem</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-wkem</t>
-  </si>
-  <si>
-    <t>Norwich</t>
-  </si>
-  <si>
-    <t>pla-norw</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#pla-norw</t>
-  </si>
-  <si>
-    <t>Tennyson, Arthur</t>
-  </si>
-  <si>
-    <t>Browning, Robert</t>
-  </si>
-  <si>
-    <t>psn-aten</t>
-  </si>
-  <si>
-    <t>psn-rbro</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-aten</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-rbro</t>
-  </si>
-  <si>
-    <t>Hobbes, Thomas</t>
-  </si>
-  <si>
-    <t>psn-thob</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-thob</t>
-  </si>
-  <si>
-    <t>Thoby?</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#lit-gard</t>
-  </si>
-  <si>
-    <t>lit-gard</t>
-  </si>
-  <si>
-    <t>Garden, The</t>
-  </si>
-  <si>
-    <t>Marvell</t>
-  </si>
-  <si>
-    <t>Fytton, Sir Edward</t>
-  </si>
-  <si>
-    <t>psn-efyt</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-efyt</t>
-  </si>
-  <si>
-    <t>Gawsworth</t>
-  </si>
-  <si>
-    <t>Cheshire</t>
-  </si>
-  <si>
-    <t>pla-gaws</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#pla-gaws</t>
-  </si>
-  <si>
-    <t>pla-ches</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#pla-ches</t>
-  </si>
-  <si>
-    <t>Fytton, Mary</t>
-  </si>
-  <si>
-    <t>psn-mfyt</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-mfyt</t>
-  </si>
-  <si>
-    <t>Knollys, Sir William</t>
-  </si>
-  <si>
-    <t>psn-wkno</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-wkno</t>
-  </si>
-  <si>
-    <t>Chopping Knife near Ludgate</t>
-  </si>
-  <si>
-    <t>pla-chop</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml/pla-chop</t>
-  </si>
-  <si>
-    <t>Pembroke, Lord William</t>
-  </si>
-  <si>
-    <t>psn-wpem</t>
-  </si>
-  <si>
-    <t>M109 [The Reader]. Typescript, fragment, with the author's ms. corrections, unsigned and undated. 9p.</t>
-  </si>
-  <si>
-    <t>m109</t>
-  </si>
-  <si>
-    <t>transcriptions/m109.xml</t>
-  </si>
-  <si>
-    <t>Elizabeth and Essex</t>
-  </si>
-  <si>
-    <t>lit-stra</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#lit-stra</t>
-  </si>
-  <si>
-    <t>pla-gren</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#pla-gren</t>
-  </si>
-  <si>
-    <t>Whitehall</t>
-  </si>
-  <si>
-    <t>pla-whit</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#pla-whit</t>
-  </si>
-  <si>
-    <t>Greenwich</t>
+    <t>Unfortunate Traveller, The</t>
+  </si>
+  <si>
+    <t>lit-trav</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-trav</t>
   </si>
 </sst>
 </file>
@@ -2364,13 +2373,13 @@
         <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F14" s="5">
         <v>7</v>
@@ -2384,13 +2393,13 @@
         <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>541</v>
       </c>
       <c r="F15" s="5">
         <v>9</v>
@@ -2429,11 +2438,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F153"/>
+  <dimension ref="A1:F154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A152" sqref="A152"/>
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2513,16 +2522,16 @@
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -2617,16 +2626,16 @@
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -2659,16 +2668,16 @@
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -2746,16 +2755,16 @@
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2886,30 +2895,30 @@
     </row>
     <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>526</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>535</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -2928,16 +2937,16 @@
     </row>
     <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>462</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -2985,7 +2994,7 @@
         <v>392</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3032,16 +3041,16 @@
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3103,7 +3112,7 @@
         <v>420</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3139,19 +3148,19 @@
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>466</v>
-      </c>
       <c r="E48" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3240,61 +3249,61 @@
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>529</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>520</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -3313,16 +3322,16 @@
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3397,7 +3406,7 @@
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>32</v>
@@ -3462,19 +3471,19 @@
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="E70" s="1" t="s">
         <v>474</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3524,19 +3533,19 @@
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C74" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="E74" s="1" t="s">
         <v>513</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3603,30 +3612,30 @@
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C79" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C80" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>500</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3645,30 +3654,30 @@
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C82" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>532</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C83" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3816,16 +3825,16 @@
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C94" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>484</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3864,19 +3873,19 @@
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C97" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="E97" s="1" t="s">
         <v>434</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3940,19 +3949,19 @@
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>447</v>
-      </c>
       <c r="E102" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4030,33 +4039,33 @@
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C108" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>503</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C109" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="E109" s="1" t="s">
         <v>469</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4137,13 +4146,13 @@
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>537</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4384,19 +4393,19 @@
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C132" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="B132" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C132" s="1" t="s">
+      <c r="D132" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="E132" s="1" t="s">
         <v>442</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4429,16 +4438,16 @@
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C135" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C135" s="1" t="s">
+      <c r="D135" s="1" t="s">
         <v>497</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4485,16 +4494,16 @@
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C139" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="D139" s="1" t="s">
         <v>481</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4544,16 +4553,16 @@
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4592,19 +4601,19 @@
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C146" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="B146" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C146" s="1" t="s">
+      <c r="D146" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="E146" s="1" t="s">
         <v>438</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4635,7 +4644,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>428</v>
       </c>
@@ -4649,7 +4658,7 @@
         <v>430</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>431</v>
+        <v>550</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4671,44 +4680,58 @@
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C151" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D151" s="1" t="s">
         <v>543</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C152" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D152" s="1" t="s">
         <v>545</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C153" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="D153" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="D153" s="1" t="s">
-        <v>549</v>
+    </row>
+    <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>553</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further additions to tracking sheet pertaining to references in m110
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8056DADB-28A5-DE43-8F17-75DA1E48EA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751D2FE5-7E0E-9B45-BBD0-696ABCEEDF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38360" yWindow="0" windowWidth="12840" windowHeight="28800" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="39360" yWindow="0" windowWidth="11840" windowHeight="28800" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="558">
   <si>
     <t>M-Number</t>
   </si>
@@ -1746,6 +1746,18 @@
   </si>
   <si>
     <t>../resources/annotations.xml#lit-trav</t>
+  </si>
+  <si>
+    <t>Look at final few folios once the facsimiles arrive or when I get to the archive in person, as the microfilm just doesn't make any sense…</t>
+  </si>
+  <si>
+    <t>m110</t>
+  </si>
+  <si>
+    <t>M110 [The Reader]. Typescript fragment, with the author's ms. corrections, unsigned and undated. 5p.</t>
+  </si>
+  <si>
+    <t>transcriptions/m110.xml</t>
   </si>
 </sst>
 </file>
@@ -2153,7 +2165,7 @@
   <sheetViews>
     <sheetView topLeftCell="A8" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G15" sqref="G15"/>
+      <selection pane="topRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2404,10 +2416,28 @@
       <c r="F15" s="5">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="G15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="F16" s="5">
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -2441,7 +2471,7 @@
   <dimension ref="A1:F154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
@@ -3117,249 +3147,249 @@
     </row>
     <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>265</v>
+        <v>541</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>266</v>
+        <v>542</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>267</v>
+        <v>543</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>463</v>
+        <v>251</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>464</v>
+        <v>249</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>465</v>
+        <v>250</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>470</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>141</v>
+        <v>463</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>142</v>
+        <v>464</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>143</v>
+        <v>465</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>319</v>
+        <v>141</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>320</v>
+        <v>142</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>322</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>194</v>
+        <v>319</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>166</v>
+        <v>45</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>195</v>
+        <v>320</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>196</v>
+        <v>322</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>45</v>
+        <v>166</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>116</v>
+        <v>195</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>117</v>
+        <v>196</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>326</v>
+        <v>254</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>327</v>
+        <v>116</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>328</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>405</v>
+        <v>326</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>406</v>
+        <v>327</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>407</v>
+        <v>328</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>489</v>
+        <v>405</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>490</v>
+        <v>406</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>491</v>
+        <v>407</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>527</v>
+        <v>489</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>528</v>
+        <v>490</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>529</v>
+        <v>491</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>518</v>
+        <v>527</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>519</v>
+        <v>528</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" s="1" t="s">
+      <c r="B60" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>305</v>
+        <v>521</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>306</v>
+        <v>523</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>307</v>
+        <v>524</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>412</v>
+        <v>305</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>413</v>
+        <v>306</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>414</v>
+        <v>307</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3378,1366 +3408,1366 @@
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>110</v>
+        <v>412</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>111</v>
+        <v>413</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>112</v>
+        <v>414</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>456</v>
+        <v>38</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>399</v>
+        <v>57</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>401</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>331</v>
+        <v>549</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>332</v>
+        <v>544</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>333</v>
+        <v>545</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>274</v>
+        <v>456</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>275</v>
+        <v>399</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>276</v>
+        <v>400</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>277</v>
+        <v>401</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>46</v>
+        <v>331</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>61</v>
+        <v>332</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>47</v>
+        <v>333</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>471</v>
+        <v>274</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>472</v>
+        <v>275</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>473</v>
+        <v>276</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>474</v>
+        <v>277</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>228</v>
+        <v>46</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>229</v>
+        <v>61</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>230</v>
+        <v>92</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>294</v>
+        <v>471</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>295</v>
+        <v>472</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>296</v>
+        <v>473</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>297</v>
+        <v>474</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>353</v>
+        <v>228</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>354</v>
+        <v>229</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>355</v>
+        <v>230</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>510</v>
+        <v>294</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>511</v>
+        <v>295</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>512</v>
+        <v>296</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>513</v>
+        <v>297</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>220</v>
+        <v>353</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>221</v>
+        <v>354</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>223</v>
+        <v>355</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>224</v>
+        <v>510</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>225</v>
+        <v>511</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>226</v>
+        <v>512</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>227</v>
+        <v>513</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>317</v>
+        <v>220</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>318</v>
+        <v>221</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>321</v>
+        <v>222</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>107</v>
+        <v>224</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>108</v>
+        <v>225</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>109</v>
+        <v>226</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>492</v>
+        <v>317</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>493</v>
+        <v>318</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>494</v>
+        <v>321</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>498</v>
+        <v>107</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>499</v>
+        <v>108</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>500</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>298</v>
+        <v>492</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>292</v>
+        <v>493</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>293</v>
+        <v>494</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>530</v>
+        <v>498</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>531</v>
+        <v>499</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>532</v>
+        <v>500</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>453</v>
+        <v>298</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>454</v>
+        <v>292</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>455</v>
+        <v>293</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>176</v>
+        <v>530</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>192</v>
+        <v>531</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>177</v>
+        <v>532</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>197</v>
+        <v>453</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>198</v>
+        <v>454</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>200</v>
+        <v>455</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>299</v>
+        <v>176</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>300</v>
+        <v>192</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>301</v>
+        <v>177</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>150</v>
+        <v>197</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>151</v>
+        <v>198</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>152</v>
+        <v>199</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>357</v>
+        <v>299</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>358</v>
+        <v>300</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>359</v>
+        <v>301</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>383</v>
+        <v>150</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>334</v>
+        <v>151</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>335</v>
+        <v>152</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>425</v>
+        <v>357</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>426</v>
+        <v>358</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>427</v>
+        <v>359</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>101</v>
+        <v>383</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>102</v>
+        <v>334</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>103</v>
+        <v>335</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>402</v>
+        <v>425</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>403</v>
+        <v>426</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>404</v>
+        <v>427</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>302</v>
+        <v>101</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>303</v>
+        <v>102</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>304</v>
+        <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>482</v>
+        <v>402</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>483</v>
+        <v>403</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>484</v>
+        <v>404</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>64</v>
+        <v>302</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>65</v>
+        <v>303</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>66</v>
+        <v>304</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>153</v>
+        <v>482</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>154</v>
+        <v>483</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>156</v>
+        <v>484</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>431</v>
+        <v>64</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>432</v>
+        <v>65</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>433</v>
+        <v>68</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>434</v>
+        <v>66</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>52</v>
+        <v>153</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>63</v>
+        <v>154</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>93</v>
+        <v>155</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>278</v>
+        <v>431</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>279</v>
+        <v>432</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>280</v>
+        <v>433</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>246</v>
+        <v>52</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>248</v>
+        <v>63</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>253</v>
+        <v>93</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>190</v>
+        <v>278</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>191</v>
+        <v>279</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>193</v>
+        <v>280</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>445</v>
+        <v>246</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>444</v>
+        <v>248</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>446</v>
+        <v>247</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>443</v>
+        <v>253</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>240</v>
+        <v>190</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>241</v>
+        <v>191</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>242</v>
+        <v>193</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>41</v>
+        <v>445</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>58</v>
+        <v>444</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>94</v>
+        <v>446</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>396</v>
+        <v>240</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>397</v>
+        <v>241</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>398</v>
+        <v>242</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>133</v>
+        <v>58</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>207</v>
+        <v>396</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>32</v>
+        <v>166</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>208</v>
+        <v>397</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>212</v>
+        <v>398</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>501</v>
+        <v>132</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>502</v>
+        <v>133</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>503</v>
+        <v>134</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>466</v>
+        <v>207</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>467</v>
+        <v>208</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>468</v>
+        <v>209</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>469</v>
+        <v>212</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>378</v>
+        <v>501</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>379</v>
+        <v>502</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>380</v>
+        <v>503</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>363</v>
+        <v>466</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>364</v>
+        <v>467</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>365</v>
+        <v>468</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>287</v>
+        <v>378</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>284</v>
+        <v>379</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>286</v>
+        <v>380</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>128</v>
+        <v>363</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>129</v>
+        <v>364</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>131</v>
+        <v>365</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>138</v>
+        <v>287</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>139</v>
+        <v>284</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>140</v>
+        <v>285</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>536</v>
+        <v>128</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>537</v>
+        <v>129</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>258</v>
+        <v>138</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>259</v>
+        <v>139</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>260</v>
+        <v>140</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>255</v>
+        <v>536</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>257</v>
+        <v>537</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>288</v>
+        <v>258</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>166</v>
+        <v>49</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>289</v>
+        <v>259</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>291</v>
+        <v>260</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>79</v>
+        <v>255</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>80</v>
+        <v>256</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>82</v>
+        <v>257</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>169</v>
+        <v>288</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>166</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>170</v>
+        <v>289</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>171</v>
+        <v>290</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>48</v>
+        <v>169</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>74</v>
+        <v>170</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>50</v>
+        <v>171</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>281</v>
+        <v>43</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>282</v>
+        <v>59</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>283</v>
+        <v>95</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>360</v>
+        <v>48</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>361</v>
+        <v>74</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>362</v>
+        <v>96</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>309</v>
+        <v>282</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>310</v>
+        <v>283</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>165</v>
+        <v>360</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>166</v>
+        <v>49</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>167</v>
+        <v>361</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>168</v>
+        <v>362</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>204</v>
+        <v>308</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>205</v>
+        <v>309</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>206</v>
+        <v>310</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>51</v>
+        <v>165</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>32</v>
+        <v>166</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>62</v>
+        <v>167</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>98</v>
+        <v>168</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>422</v>
+        <v>204</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>423</v>
+        <v>205</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>424</v>
+        <v>206</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>422</v>
+        <v>51</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>423</v>
+        <v>62</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>424</v>
+        <v>98</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>261</v>
+        <v>422</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>262</v>
+        <v>423</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>264</v>
+        <v>424</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>439</v>
+        <v>422</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>440</v>
+        <v>423</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>442</v>
+        <v>424</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>314</v>
+        <v>261</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>315</v>
+        <v>262</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>316</v>
+        <v>263</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>118</v>
+        <v>439</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>119</v>
+        <v>440</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>120</v>
+        <v>441</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>495</v>
+        <v>314</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>496</v>
+        <v>315</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>497</v>
+        <v>316</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>180</v>
+        <v>118</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>181</v>
+        <v>119</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>183</v>
+        <v>120</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>323</v>
+        <v>495</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>324</v>
+        <v>496</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>325</v>
+        <v>497</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>479</v>
+        <v>323</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>480</v>
+        <v>324</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>481</v>
+        <v>325</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>268</v>
+        <v>187</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>269</v>
+        <v>188</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>270</v>
+        <v>189</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>210</v>
+        <v>479</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>211</v>
+        <v>480</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>217</v>
+        <v>481</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>339</v>
+        <v>268</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>329</v>
+        <v>269</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>330</v>
+        <v>270</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>504</v>
+        <v>210</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>506</v>
+        <v>211</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>508</v>
+        <v>213</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>350</v>
+        <v>329</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>39</v>
+        <v>504</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>60</v>
+        <v>506</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>40</v>
+        <v>508</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>435</v>
+        <v>349</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>436</v>
+        <v>350</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>437</v>
+        <v>351</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>438</v>
+        <v>352</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>273</v>
+        <v>551</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>271</v>
+        <v>552</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>272</v>
+        <v>553</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>173</v>
+        <v>39</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>174</v>
+        <v>60</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>175</v>
+        <v>99</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>428</v>
+        <v>546</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>429</v>
+        <v>547</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>69</v>
+        <v>435</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>70</v>
+        <v>436</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>71</v>
+        <v>437</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>72</v>
+        <v>438</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>541</v>
+        <v>273</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>542</v>
+        <v>271</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>543</v>
+        <v>272</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>549</v>
+        <v>173</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>544</v>
+        <v>174</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>545</v>
+        <v>175</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>546</v>
+        <v>428</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>547</v>
+        <v>429</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>548</v>
+        <v>430</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>551</v>
+        <v>69</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>552</v>
+        <v>70</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>553</v>
+        <v>71</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F150">
-      <sortCondition ref="A1:A150"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F154">
+      <sortCondition ref="A1:A154"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="F1:F1048576">

</xml_diff>

<commit_message>
Updated to include m111 info
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C17C5D-FCEA-DC43-9AC5-DC3342D2D100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73FF3E7-1876-F64A-9BE7-CC60379EED3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39360" yWindow="0" windowWidth="11840" windowHeight="28800" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="39360" yWindow="0" windowWidth="11840" windowHeight="28800" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="585">
   <si>
     <t>M-Number</t>
   </si>
@@ -1758,6 +1758,87 @@
   </si>
   <si>
     <t>transcriptions/m110.xml</t>
+  </si>
+  <si>
+    <t>psn-lucy</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-lucy</t>
+  </si>
+  <si>
+    <t>BA character</t>
+  </si>
+  <si>
+    <t>psn-bart</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-bart</t>
+  </si>
+  <si>
+    <t>Outline of History</t>
+  </si>
+  <si>
+    <t>lit-outl</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-outl</t>
+  </si>
+  <si>
+    <t>From BA</t>
+  </si>
+  <si>
+    <t>Swithin, Lucy</t>
+  </si>
+  <si>
+    <t>Oliver, Bartholomew</t>
+  </si>
+  <si>
+    <t>Sohrab</t>
+  </si>
+  <si>
+    <t>psn-sohr</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-sohr</t>
+  </si>
+  <si>
+    <t>Dog from BA. Use monster thesis footnote?</t>
+  </si>
+  <si>
+    <t>Cleopatra</t>
+  </si>
+  <si>
+    <t>Falstaff</t>
+  </si>
+  <si>
+    <t>Macbeth</t>
+  </si>
+  <si>
+    <t>Tempest, The</t>
+  </si>
+  <si>
+    <t>psn-cleo</t>
+  </si>
+  <si>
+    <t>psn-fals</t>
+  </si>
+  <si>
+    <t>psn-macb</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-cleo</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-fals</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-macb</t>
+  </si>
+  <si>
+    <t>lit-temp</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-temp</t>
   </si>
 </sst>
 </file>
@@ -2163,9 +2244,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2439,6 +2520,9 @@
       <c r="F16" s="5">
         <v>5</v>
       </c>
+      <c r="G16" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -2468,11 +2552,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F154"/>
+  <dimension ref="A1:F162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A146" sqref="A146"/>
+    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4764,6 +4848,130 @@
         <v>72</v>
       </c>
     </row>
+    <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A159" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A160" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A161" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A162" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>584</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F154">

</xml_diff>

<commit_message>
tracking sheet: added m111-2.xml info
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73FF3E7-1876-F64A-9BE7-CC60379EED3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D4C878-F9B2-9E4B-8ABA-2264EA30C346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39360" yWindow="0" windowWidth="11840" windowHeight="28800" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="36040" yWindow="0" windowWidth="15160" windowHeight="28800" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="599">
   <si>
     <t>M-Number</t>
   </si>
@@ -114,9 +114,6 @@
     <t>M110</t>
   </si>
   <si>
-    <t>M111</t>
-  </si>
-  <si>
     <t>M112</t>
   </si>
   <si>
@@ -1375,9 +1372,6 @@
   </si>
   <si>
     <t>psn-mrwh</t>
-  </si>
-  <si>
-    <t>Mr. W. H</t>
   </si>
   <si>
     <t>../resources/annotations.xml#psn-mrwh</t>
@@ -1840,12 +1834,60 @@
   <si>
     <t>../resources/annotations.xml#lit-temp</t>
   </si>
+  <si>
+    <t>M111-1</t>
+  </si>
+  <si>
+    <t>M111-2</t>
+  </si>
+  <si>
+    <t>M111-3</t>
+  </si>
+  <si>
+    <t>m111-1</t>
+  </si>
+  <si>
+    <t>transcriptions/m111-1.xml</t>
+  </si>
+  <si>
+    <t>W. H., Mr.</t>
+  </si>
+  <si>
+    <t>Stationers' Office</t>
+  </si>
+  <si>
+    <t>psn-stat</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-stat</t>
+  </si>
+  <si>
+    <t>Ibsen, Henrik</t>
+  </si>
+  <si>
+    <t>psn-hibs</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-hibs</t>
+  </si>
+  <si>
+    <t>M111-1 [The Reader]. Set 1 of 3. Typescript fragment, with the author's ms. corrections, unsigned and undated. 8p.</t>
+  </si>
+  <si>
+    <t>M111-2 [The Reader]. Set 2 of 3. Typescript fragment, unsigned and undated. 4p.</t>
+  </si>
+  <si>
+    <t>m111-2</t>
+  </si>
+  <si>
+    <t>transcriptions/m111-2.xml</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1865,6 +1907,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2242,11 +2290,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2277,10 +2325,10 @@
         <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>11</v>
@@ -2311,22 +2359,22 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F7" s="5">
         <v>2</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -2334,22 +2382,22 @@
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F8" s="5">
         <v>8</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2357,22 +2405,22 @@
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="F9" s="5">
         <v>9</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2380,22 +2428,22 @@
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F10" s="5">
         <v>9</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2403,19 +2451,19 @@
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F11" s="5">
         <v>19</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -2423,22 +2471,22 @@
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F12" s="5">
         <v>26</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -2446,19 +2494,19 @@
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>409</v>
       </c>
       <c r="F13" s="5">
         <v>35</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2466,19 +2514,19 @@
         <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F14" s="5">
         <v>7</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2486,22 +2534,22 @@
         <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>538</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>540</v>
       </c>
       <c r="F15" s="5">
         <v>9</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2509,37 +2557,75 @@
         <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>555</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>557</v>
       </c>
       <c r="F16" s="5">
         <v>5</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="F17" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="F18" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="F19" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Y"</formula>
@@ -2552,11 +2638,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F162"/>
+  <dimension ref="A1:F164"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A162" sqref="A162"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2580,2402 +2666,2430 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>476</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>450</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>507</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>373</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="D27" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>533</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>460</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>237</v>
+        <v>571</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>238</v>
+        <v>575</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>239</v>
+        <v>578</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>104</v>
+        <v>236</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>105</v>
+        <v>237</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>390</v>
+        <v>103</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>391</v>
+        <v>104</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>392</v>
+        <v>105</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>485</v>
+        <v>213</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>243</v>
+        <v>389</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>244</v>
+        <v>390</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>245</v>
+        <v>391</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>42</v>
+        <v>242</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>56</v>
+        <v>243</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>97</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>311</v>
+        <v>41</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>312</v>
+        <v>55</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>313</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>486</v>
+        <v>310</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>487</v>
+        <v>311</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>488</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>366</v>
+        <v>484</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>367</v>
+        <v>485</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>368</v>
+        <v>486</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>161</v>
+        <v>365</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>162</v>
+        <v>366</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>163</v>
+        <v>367</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>418</v>
+        <v>160</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>419</v>
+        <v>161</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>421</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>541</v>
+        <v>417</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>542</v>
+        <v>418</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>543</v>
+        <v>419</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>265</v>
+        <v>539</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>266</v>
+        <v>540</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>267</v>
+        <v>541</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>463</v>
+        <v>250</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>464</v>
+        <v>248</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>465</v>
+        <v>249</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>470</v>
+        <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>141</v>
+        <v>461</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>142</v>
+        <v>462</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>143</v>
+        <v>463</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>319</v>
+        <v>140</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>320</v>
+        <v>141</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>322</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>194</v>
+        <v>318</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>166</v>
+        <v>44</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>195</v>
+        <v>319</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>196</v>
+        <v>321</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>254</v>
+        <v>193</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>116</v>
+        <v>194</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>117</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>326</v>
+        <v>253</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>327</v>
+        <v>115</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>328</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>405</v>
+        <v>572</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>406</v>
+        <v>576</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>407</v>
+        <v>579</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>489</v>
+        <v>325</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>490</v>
+        <v>326</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>491</v>
+        <v>327</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>527</v>
+        <v>404</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>528</v>
+        <v>405</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>529</v>
+        <v>406</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>518</v>
+        <v>487</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>519</v>
+        <v>488</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>520</v>
+        <v>489</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="E59" s="1" t="s">
+      <c r="B60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="D60" s="1" t="s">
-        <v>164</v>
+        <v>518</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>512</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>305</v>
+        <v>158</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>306</v>
+        <v>159</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>307</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>412</v>
+        <v>519</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>413</v>
+        <v>521</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>414</v>
+        <v>522</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>412</v>
+        <v>304</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>413</v>
+        <v>305</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>414</v>
+        <v>306</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>110</v>
+        <v>411</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>111</v>
+        <v>412</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>112</v>
+        <v>413</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>38</v>
+        <v>411</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>57</v>
+        <v>412</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>91</v>
+        <v>413</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>549</v>
+        <v>109</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>544</v>
+        <v>110</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>545</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>456</v>
+        <v>37</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>399</v>
+        <v>56</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>401</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>331</v>
+        <v>547</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>332</v>
+        <v>542</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>333</v>
+        <v>543</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>274</v>
+        <v>454</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>275</v>
+        <v>398</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>276</v>
+        <v>399</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>277</v>
+        <v>400</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>46</v>
+        <v>330</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>61</v>
+        <v>331</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>47</v>
+        <v>332</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>471</v>
+        <v>273</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>472</v>
+        <v>274</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>473</v>
+        <v>275</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>474</v>
+        <v>276</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>228</v>
+        <v>45</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>229</v>
+        <v>60</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>230</v>
+        <v>91</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>294</v>
+        <v>469</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>295</v>
+        <v>470</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>296</v>
+        <v>471</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>297</v>
+        <v>472</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>353</v>
+        <v>227</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>354</v>
+        <v>228</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>355</v>
+        <v>229</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>510</v>
+        <v>293</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>511</v>
+        <v>294</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>512</v>
+        <v>295</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>513</v>
+        <v>296</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>220</v>
+        <v>352</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>221</v>
+        <v>353</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>223</v>
+        <v>354</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>224</v>
+        <v>508</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>225</v>
+        <v>509</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>226</v>
+        <v>510</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>227</v>
+        <v>511</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>317</v>
+        <v>219</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>318</v>
+        <v>220</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>321</v>
+        <v>221</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>107</v>
+        <v>223</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>108</v>
+        <v>224</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>109</v>
+        <v>225</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>492</v>
+        <v>316</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>493</v>
+        <v>317</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>494</v>
+        <v>320</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>498</v>
+        <v>106</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>499</v>
+        <v>107</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>500</v>
+        <v>108</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>298</v>
+        <v>490</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>292</v>
+        <v>491</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>293</v>
+        <v>492</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>530</v>
+        <v>496</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>531</v>
+        <v>497</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>532</v>
+        <v>498</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>453</v>
+        <v>297</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>454</v>
+        <v>291</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>455</v>
+        <v>292</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>176</v>
+        <v>528</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>192</v>
+        <v>529</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>177</v>
+        <v>530</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>197</v>
+        <v>451</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>198</v>
+        <v>452</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>200</v>
+        <v>453</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>299</v>
+        <v>175</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>300</v>
+        <v>191</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>301</v>
+        <v>176</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>150</v>
+        <v>196</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>151</v>
+        <v>197</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>152</v>
+        <v>198</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>357</v>
+        <v>298</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>358</v>
+        <v>299</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>359</v>
+        <v>300</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>383</v>
+        <v>149</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>334</v>
+        <v>150</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>335</v>
+        <v>151</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>425</v>
+        <v>356</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>426</v>
+        <v>357</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>427</v>
+        <v>358</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>101</v>
+        <v>382</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>102</v>
+        <v>333</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>103</v>
+        <v>334</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>402</v>
+        <v>424</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>403</v>
+        <v>425</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>404</v>
+        <v>426</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>302</v>
+        <v>100</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>303</v>
+        <v>101</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>304</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>482</v>
+        <v>401</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>483</v>
+        <v>402</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>484</v>
+        <v>403</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>64</v>
+        <v>301</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>65</v>
+        <v>302</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>66</v>
+        <v>303</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>153</v>
+        <v>480</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>154</v>
+        <v>481</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>156</v>
+        <v>482</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>431</v>
+        <v>63</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>432</v>
+        <v>64</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>433</v>
+        <v>67</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>434</v>
+        <v>65</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>52</v>
+        <v>573</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>63</v>
+        <v>577</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>93</v>
+        <v>580</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>278</v>
+        <v>152</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>279</v>
+        <v>153</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>280</v>
+        <v>154</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>246</v>
+        <v>430</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>248</v>
+        <v>431</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>247</v>
+        <v>432</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>253</v>
+        <v>433</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>190</v>
+        <v>51</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>191</v>
+        <v>62</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>193</v>
+        <v>92</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>445</v>
+        <v>277</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>444</v>
+        <v>278</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>443</v>
+        <v>279</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>242</v>
+        <v>246</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>41</v>
+        <v>189</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>58</v>
+        <v>190</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>94</v>
+        <v>192</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>396</v>
+        <v>239</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>166</v>
+        <v>31</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>397</v>
+        <v>240</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>398</v>
+        <v>241</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>132</v>
+        <v>40</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>133</v>
+        <v>57</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>207</v>
+        <v>395</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>32</v>
+        <v>165</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>208</v>
+        <v>396</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>212</v>
+        <v>397</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>501</v>
+        <v>131</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>502</v>
+        <v>132</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>503</v>
+        <v>133</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>466</v>
+        <v>206</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>467</v>
+        <v>207</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>468</v>
+        <v>208</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>469</v>
+        <v>211</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>378</v>
+        <v>499</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>379</v>
+        <v>500</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>380</v>
+        <v>501</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>363</v>
+        <v>464</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>364</v>
+        <v>465</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>365</v>
+        <v>466</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>287</v>
+        <v>566</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>284</v>
+        <v>559</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>285</v>
+        <v>560</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>286</v>
+        <v>558</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>128</v>
+        <v>561</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>129</v>
+        <v>562</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>130</v>
+        <v>563</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>131</v>
+        <v>564</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>138</v>
+        <v>377</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>139</v>
+        <v>378</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>140</v>
+        <v>379</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>536</v>
+        <v>362</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>537</v>
+        <v>363</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>258</v>
+        <v>286</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>260</v>
+        <v>284</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>255</v>
+        <v>127</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>257</v>
+        <v>129</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>288</v>
+        <v>137</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>166</v>
+        <v>31</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>289</v>
+        <v>138</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>291</v>
+        <v>139</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>79</v>
+        <v>534</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>82</v>
+        <v>535</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>169</v>
+        <v>257</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>166</v>
+        <v>48</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>170</v>
+        <v>258</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>171</v>
+        <v>259</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>59</v>
+        <v>255</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>95</v>
+        <v>256</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>48</v>
+        <v>287</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>49</v>
+        <v>165</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>74</v>
+        <v>288</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>96</v>
+        <v>289</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>50</v>
+        <v>290</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>281</v>
+        <v>78</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>282</v>
+        <v>79</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>283</v>
+        <v>80</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>360</v>
+        <v>168</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>49</v>
+        <v>165</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>361</v>
+        <v>169</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>362</v>
+        <v>170</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>308</v>
+        <v>42</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>309</v>
+        <v>58</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>310</v>
+        <v>94</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>165</v>
+        <v>47</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>166</v>
+        <v>48</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>167</v>
+        <v>73</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>168</v>
+        <v>95</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>204</v>
+        <v>280</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>205</v>
+        <v>281</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>206</v>
+        <v>282</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>51</v>
+        <v>359</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>62</v>
+        <v>360</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>98</v>
+        <v>361</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>422</v>
+        <v>307</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>423</v>
+        <v>308</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>424</v>
+        <v>309</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>422</v>
+        <v>164</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>423</v>
+        <v>166</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>424</v>
+        <v>167</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>261</v>
+        <v>203</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>264</v>
+        <v>205</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>439</v>
+        <v>50</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>440</v>
+        <v>61</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>442</v>
+        <v>97</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>314</v>
+        <v>421</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>315</v>
+        <v>422</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>316</v>
+        <v>423</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>118</v>
+        <v>421</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>119</v>
+        <v>422</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>120</v>
+        <v>423</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>495</v>
+        <v>260</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>496</v>
+        <v>261</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>497</v>
+        <v>262</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>180</v>
+        <v>438</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>181</v>
+        <v>439</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>183</v>
+        <v>440</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>323</v>
+        <v>567</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>324</v>
+        <v>568</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>325</v>
+        <v>569</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>187</v>
+        <v>313</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>188</v>
+        <v>314</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>189</v>
+        <v>315</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>479</v>
+        <v>117</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>480</v>
+        <v>118</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>481</v>
+        <v>119</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>268</v>
+        <v>493</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>269</v>
+        <v>494</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>270</v>
+        <v>495</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>210</v>
+        <v>179</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>211</v>
+        <v>180</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>217</v>
+        <v>182</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>339</v>
+        <v>322</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>504</v>
+        <v>186</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>506</v>
+        <v>187</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>508</v>
+        <v>188</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>349</v>
+        <v>477</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>350</v>
+        <v>478</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>352</v>
+        <v>479</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>551</v>
+        <v>267</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>552</v>
+        <v>268</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>553</v>
+        <v>269</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>39</v>
+        <v>209</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>60</v>
+        <v>210</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>99</v>
+        <v>212</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>40</v>
+        <v>216</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>546</v>
+        <v>565</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>547</v>
+        <v>556</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>548</v>
+        <v>557</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>435</v>
+        <v>338</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>436</v>
+        <v>328</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>438</v>
+        <v>329</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>273</v>
+        <v>574</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>271</v>
+        <v>581</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>272</v>
+        <v>582</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>173</v>
+        <v>502</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>174</v>
+        <v>504</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>175</v>
+        <v>506</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>428</v>
+        <v>348</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>429</v>
+        <v>349</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>430</v>
+        <v>350</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>550</v>
+        <v>351</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>69</v>
+        <v>549</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>70</v>
+        <v>550</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>72</v>
+        <v>551</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>567</v>
+        <v>38</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>558</v>
+        <v>59</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>559</v>
+        <v>98</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>560</v>
+        <v>39</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>568</v>
+        <v>588</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>561</v>
+        <v>443</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>562</v>
+        <v>444</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>560</v>
+        <v>442</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>563</v>
+        <v>544</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>564</v>
+        <v>545</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>566</v>
+        <v>546</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>569</v>
+        <v>434</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>570</v>
+        <v>435</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>571</v>
+        <v>436</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>572</v>
+        <v>437</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>573</v>
+        <v>272</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>577</v>
+        <v>270</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>580</v>
+        <v>271</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>574</v>
+        <v>172</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>578</v>
+        <v>173</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>575</v>
+        <v>427</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>579</v>
+        <v>428</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>429</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>576</v>
+        <v>68</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>583</v>
+        <v>69</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>584</v>
+        <v>70</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A163" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A164" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>594</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F154">
-      <sortCondition ref="A1:A154"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F162">
+      <sortCondition ref="A1:A162"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="F1:F1048576">

</xml_diff>

<commit_message>
Updated tracking sheet with details from m111-2
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D4C878-F9B2-9E4B-8ABA-2264EA30C346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03ED427B-275B-F14D-B9C9-4C1F8D92013F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36040" yWindow="0" windowWidth="15160" windowHeight="28800" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="36040" yWindow="0" windowWidth="15160" windowHeight="28800" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="605">
   <si>
     <t>M-Number</t>
   </si>
@@ -1881,6 +1881,24 @@
   </si>
   <si>
     <t>transcriptions/m111-2.xml</t>
+  </si>
+  <si>
+    <t>Puritans</t>
+  </si>
+  <si>
+    <t>psn-puri</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-puri</t>
+  </si>
+  <si>
+    <t>Henry VI, The</t>
+  </si>
+  <si>
+    <t>lit-hen6</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-hen6</t>
   </si>
 </sst>
 </file>
@@ -2292,7 +2310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B19" sqref="B19"/>
     </sheetView>
@@ -2638,11 +2656,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F164"/>
+  <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D164" sqref="D164"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D166" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5086,6 +5104,34 @@
         <v>594</v>
       </c>
     </row>
+    <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A165" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A166" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>604</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F162">

</xml_diff>

<commit_message>
Added m111-3.xml information to tracking sheet
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03ED427B-275B-F14D-B9C9-4C1F8D92013F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B1CFDC-A377-D545-B804-9CBA9B709240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36040" yWindow="0" windowWidth="15160" windowHeight="28800" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="36040" yWindow="0" windowWidth="15160" windowHeight="28800" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="611">
   <si>
     <t>M-Number</t>
   </si>
@@ -1817,18 +1817,12 @@
     <t>psn-fals</t>
   </si>
   <si>
-    <t>psn-macb</t>
-  </si>
-  <si>
     <t>../resources/annotations.xml#psn-cleo</t>
   </si>
   <si>
     <t>../resources/annotations.xml#psn-fals</t>
   </si>
   <si>
-    <t>../resources/annotations.xml#psn-macb</t>
-  </si>
-  <si>
     <t>lit-temp</t>
   </si>
   <si>
@@ -1892,13 +1886,37 @@
     <t>../resources/annotations.xml#psn-puri</t>
   </si>
   <si>
-    <t>Henry VI, The</t>
-  </si>
-  <si>
     <t>lit-hen6</t>
   </si>
   <si>
     <t>../resources/annotations.xml#lit-hen6</t>
+  </si>
+  <si>
+    <t>King John</t>
+  </si>
+  <si>
+    <t>Henry VI</t>
+  </si>
+  <si>
+    <t>lit-john</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-john</t>
+  </si>
+  <si>
+    <t>lit-macb</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-macb</t>
+  </si>
+  <si>
+    <t>m111-3</t>
+  </si>
+  <si>
+    <t>transcriptions/m111-3.xml</t>
+  </si>
+  <si>
+    <t>M111 [The Reader]. Set 3 of 3. Typescript fragment, with the author's ms. corrections. 7p.</t>
   </si>
 </sst>
 </file>
@@ -2310,9 +2328,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B19" sqref="B19"/>
+      <selection pane="topRight" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2592,16 +2610,16 @@
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F17" s="5">
         <v>5</v>
@@ -2609,24 +2627,33 @@
     </row>
     <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>596</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>597</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>598</v>
       </c>
       <c r="F18" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>609</v>
       </c>
       <c r="F19" s="5">
         <v>5</v>
@@ -2656,11 +2683,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F166"/>
+  <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D166" sqref="D166"/>
+    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3178,7 +3205,7 @@
         <v>575</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3476,7 +3503,7 @@
         <v>576</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4133,13 +4160,13 @@
         <v>573</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>577</v>
+        <v>606</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>580</v>
+        <v>607</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4898,10 +4925,10 @@
         <v>44</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4968,7 +4995,7 @@
     </row>
     <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>31</v>
@@ -5078,58 +5105,72 @@
     </row>
     <row r="163" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="D163" s="1" t="s">
         <v>589</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="D164" s="1" t="s">
         <v>592</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="D165" s="1" t="s">
         <v>599</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="D166" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A167" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C167" s="1" t="s">
         <v>604</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to tracking sheet with details from m111-3
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B1CFDC-A377-D545-B804-9CBA9B709240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77079266-83C3-3443-868A-D8CDC65147EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36040" yWindow="0" windowWidth="15160" windowHeight="28800" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="36040" yWindow="0" windowWidth="15160" windowHeight="28800" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="615">
   <si>
     <t>M-Number</t>
   </si>
@@ -1917,6 +1917,18 @@
   </si>
   <si>
     <t>M111 [The Reader]. Set 3 of 3. Typescript fragment, with the author's ms. corrections. 7p.</t>
+  </si>
+  <si>
+    <t>Come back to additions on p. 1</t>
+  </si>
+  <si>
+    <t>Westmoreland</t>
+  </si>
+  <si>
+    <t>pla-west</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-west</t>
   </si>
 </sst>
 </file>
@@ -2328,9 +2340,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B24" sqref="B24"/>
+      <selection pane="topRight" activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2608,7 +2620,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>581</v>
       </c>
@@ -2624,8 +2636,11 @@
       <c r="F17" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G17" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>582</v>
       </c>
@@ -2641,8 +2656,11 @@
       <c r="F18" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G18" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>583</v>
       </c>
@@ -2656,15 +2674,21 @@
         <v>609</v>
       </c>
       <c r="F19" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -2683,11 +2707,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F167"/>
+  <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A169" sqref="A169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5173,6 +5197,20 @@
         <v>605</v>
       </c>
     </row>
+    <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>614</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F162">

</xml_diff>

<commit_message>
Further updates to tracking sheet with m111-3 details
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77079266-83C3-3443-868A-D8CDC65147EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5C48EB-740D-BA4A-9E72-113AE3078A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36040" yWindow="0" windowWidth="15160" windowHeight="28800" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="635">
   <si>
     <t>M-Number</t>
   </si>
@@ -1929,6 +1929,66 @@
   </si>
   <si>
     <t>../resources/annotations.xml#pla-west</t>
+  </si>
+  <si>
+    <t>Defense of Poesie</t>
+  </si>
+  <si>
+    <t>lit-defe</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-defe</t>
+  </si>
+  <si>
+    <t>Timber: Or, Discoveries</t>
+  </si>
+  <si>
+    <t>lit-timb</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-timb</t>
+  </si>
+  <si>
+    <t>Ghosts</t>
+  </si>
+  <si>
+    <t>lit-ghos</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-ghos</t>
+  </si>
+  <si>
+    <t>Surbiton</t>
+  </si>
+  <si>
+    <t>pla-surb</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-surb</t>
+  </si>
+  <si>
+    <t>Oliver, Giles</t>
+  </si>
+  <si>
+    <t>psn-gile</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-gile</t>
+  </si>
+  <si>
+    <t>Comma (Butterfly)</t>
+  </si>
+  <si>
+    <t>obj-comm</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#obj-comm</t>
+  </si>
+  <si>
+    <t>Oliver, Isa</t>
+  </si>
+  <si>
+    <t>psn-isa</t>
   </si>
 </sst>
 </file>
@@ -2707,11 +2767,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F168"/>
+  <dimension ref="A1:F175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A169" sqref="A169"/>
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D175" sqref="D175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3282,1939 +3342,2034 @@
     </row>
     <row r="39" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>242</v>
+        <v>630</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>44</v>
+        <v>165</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>243</v>
+        <v>631</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>244</v>
+        <v>632</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>41</v>
+        <v>242</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>55</v>
+        <v>243</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>96</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>310</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>311</v>
+        <v>55</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>312</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>484</v>
+        <v>310</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>485</v>
+        <v>311</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>486</v>
+        <v>312</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>365</v>
+        <v>615</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>366</v>
+        <v>616</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>367</v>
+        <v>617</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>160</v>
+        <v>484</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>161</v>
+        <v>485</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>162</v>
+        <v>486</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>417</v>
+        <v>365</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>418</v>
+        <v>366</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>420</v>
+        <v>367</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>417</v>
+        <v>160</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>418</v>
+        <v>161</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>473</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>539</v>
+        <v>417</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>540</v>
+        <v>418</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>541</v>
+        <v>419</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>264</v>
+        <v>417</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>265</v>
+        <v>418</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>266</v>
+        <v>419</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>250</v>
+        <v>539</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>248</v>
+        <v>540</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>251</v>
+        <v>541</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>461</v>
+        <v>264</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>462</v>
+        <v>265</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>468</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>140</v>
+        <v>250</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>141</v>
+        <v>248</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>142</v>
+        <v>249</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>318</v>
+        <v>461</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>319</v>
+        <v>462</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>321</v>
+        <v>463</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>193</v>
+        <v>140</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>165</v>
+        <v>48</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>194</v>
+        <v>141</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>195</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>253</v>
+        <v>318</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>115</v>
+        <v>319</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>116</v>
+        <v>321</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>572</v>
+        <v>193</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>31</v>
+        <v>165</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>576</v>
+        <v>194</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>578</v>
+        <v>195</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>325</v>
+        <v>253</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>326</v>
+        <v>115</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>327</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>404</v>
+        <v>572</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>405</v>
+        <v>576</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>406</v>
+        <v>578</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>487</v>
+        <v>325</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>488</v>
+        <v>326</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>489</v>
+        <v>327</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>525</v>
+        <v>404</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>526</v>
+        <v>405</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>527</v>
+        <v>406</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>516</v>
+        <v>487</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>517</v>
+        <v>488</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>518</v>
+        <v>489</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>514</v>
+        <v>525</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>513</v>
+        <v>526</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>158</v>
+        <v>516</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>159</v>
+        <v>517</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>163</v>
+        <v>518</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>512</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>304</v>
+        <v>158</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>305</v>
+        <v>159</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>306</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>411</v>
+        <v>519</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>412</v>
+        <v>521</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>413</v>
+        <v>522</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>411</v>
+        <v>621</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>412</v>
+        <v>622</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>413</v>
+        <v>623</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>109</v>
+        <v>304</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>110</v>
+        <v>305</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>111</v>
+        <v>306</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>37</v>
+        <v>411</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>56</v>
+        <v>412</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>90</v>
+        <v>413</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>547</v>
+        <v>411</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>542</v>
+        <v>412</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>543</v>
+        <v>413</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>454</v>
+        <v>109</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>398</v>
+        <v>110</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>400</v>
+        <v>111</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>330</v>
+        <v>37</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>331</v>
+        <v>56</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>332</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>273</v>
+        <v>547</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>274</v>
+        <v>542</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>276</v>
+        <v>543</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>45</v>
+        <v>454</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>60</v>
+        <v>398</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>91</v>
+        <v>399</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>46</v>
+        <v>400</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>469</v>
+        <v>330</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>470</v>
+        <v>331</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>472</v>
+        <v>332</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>228</v>
+        <v>274</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>229</v>
+        <v>275</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>293</v>
+        <v>45</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>294</v>
+        <v>60</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>295</v>
+        <v>91</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>296</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>352</v>
+        <v>469</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>353</v>
+        <v>470</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>354</v>
+        <v>471</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>508</v>
+        <v>603</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>509</v>
+        <v>600</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>511</v>
+        <v>601</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>223</v>
+        <v>293</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>224</v>
+        <v>294</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>225</v>
+        <v>295</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>226</v>
+        <v>296</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>316</v>
+        <v>352</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>317</v>
+        <v>353</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>320</v>
+        <v>354</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>106</v>
+        <v>508</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>107</v>
+        <v>509</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>108</v>
+        <v>510</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>490</v>
+        <v>219</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>491</v>
+        <v>220</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>492</v>
+        <v>221</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>496</v>
+        <v>223</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>497</v>
+        <v>224</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>498</v>
+        <v>225</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>297</v>
+        <v>316</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>292</v>
+        <v>320</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>528</v>
+        <v>590</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>529</v>
+        <v>591</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>530</v>
+        <v>592</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>451</v>
+        <v>106</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>452</v>
+        <v>107</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>453</v>
+        <v>108</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>175</v>
+        <v>490</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>191</v>
+        <v>491</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>176</v>
+        <v>492</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>196</v>
+        <v>496</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>197</v>
+        <v>497</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>199</v>
+        <v>498</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>149</v>
+        <v>602</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>150</v>
+        <v>604</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>151</v>
+        <v>605</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>356</v>
+        <v>528</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>357</v>
+        <v>529</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>358</v>
+        <v>530</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>382</v>
+        <v>451</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>333</v>
+        <v>452</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>334</v>
+        <v>453</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>424</v>
+        <v>175</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>425</v>
+        <v>191</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>426</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>100</v>
+        <v>196</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>102</v>
+        <v>198</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>401</v>
+        <v>298</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>402</v>
+        <v>299</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>403</v>
+        <v>300</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>301</v>
+        <v>149</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>302</v>
+        <v>150</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>303</v>
+        <v>151</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>480</v>
+        <v>356</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>481</v>
+        <v>357</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>482</v>
+        <v>358</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>63</v>
+        <v>382</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>64</v>
+        <v>333</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>65</v>
+        <v>334</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>573</v>
+        <v>424</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>606</v>
+        <v>425</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>607</v>
+        <v>426</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>152</v>
+        <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>155</v>
+        <v>102</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>430</v>
+        <v>401</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>431</v>
+        <v>402</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>433</v>
+        <v>403</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>51</v>
+        <v>301</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>62</v>
+        <v>302</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>92</v>
+        <v>303</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>277</v>
+        <v>480</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>278</v>
+        <v>481</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>279</v>
+        <v>482</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>245</v>
+        <v>63</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>247</v>
+        <v>64</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>246</v>
+        <v>67</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>252</v>
+        <v>65</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>189</v>
+        <v>573</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>190</v>
+        <v>606</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>192</v>
+        <v>607</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>239</v>
+        <v>152</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>240</v>
+        <v>153</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>241</v>
+        <v>154</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>40</v>
+        <v>430</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>57</v>
+        <v>431</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>93</v>
+        <v>432</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>395</v>
+        <v>51</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>165</v>
+        <v>31</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>396</v>
+        <v>62</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>397</v>
+        <v>92</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>131</v>
+        <v>277</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>132</v>
+        <v>278</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>133</v>
+        <v>279</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>206</v>
+        <v>245</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>207</v>
+        <v>247</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>208</v>
+        <v>246</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>211</v>
+        <v>252</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>499</v>
+        <v>189</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>500</v>
+        <v>190</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>501</v>
+        <v>192</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>464</v>
+        <v>239</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>465</v>
+        <v>240</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>467</v>
+        <v>241</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>566</v>
+        <v>40</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>559</v>
+        <v>57</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>560</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>558</v>
+        <v>93</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>561</v>
+        <v>395</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>44</v>
+        <v>165</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>562</v>
+        <v>396</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>564</v>
+        <v>397</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>377</v>
+        <v>131</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>378</v>
+        <v>132</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>379</v>
+        <v>133</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>362</v>
+        <v>206</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>363</v>
+        <v>207</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>364</v>
+        <v>208</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>286</v>
+        <v>499</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>283</v>
+        <v>500</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>285</v>
+        <v>501</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>127</v>
+        <v>464</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>128</v>
+        <v>465</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>129</v>
+        <v>466</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>130</v>
+        <v>467</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>137</v>
+        <v>566</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>138</v>
+        <v>559</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>139</v>
+        <v>560</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>534</v>
+        <v>627</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>628</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>257</v>
+        <v>633</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>259</v>
+        <v>634</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>254</v>
+        <v>561</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>255</v>
+        <v>562</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>256</v>
+        <v>563</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>287</v>
+        <v>377</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>165</v>
+        <v>48</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>288</v>
+        <v>378</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>290</v>
+        <v>379</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>78</v>
+        <v>362</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>79</v>
+        <v>363</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>81</v>
+        <v>364</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>168</v>
+        <v>286</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>165</v>
+        <v>44</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>169</v>
+        <v>283</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>170</v>
+        <v>284</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>42</v>
+        <v>127</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>58</v>
+        <v>128</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>94</v>
+        <v>129</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>73</v>
+        <v>138</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>49</v>
+        <v>139</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>280</v>
+        <v>534</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>282</v>
+        <v>535</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>359</v>
+        <v>257</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>360</v>
+        <v>258</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>361</v>
+        <v>259</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>307</v>
+        <v>254</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>308</v>
+        <v>255</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>309</v>
+        <v>256</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>164</v>
+        <v>287</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>165</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>166</v>
+        <v>288</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>167</v>
+        <v>289</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>203</v>
+        <v>78</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>204</v>
+        <v>79</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>205</v>
+        <v>80</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>50</v>
+        <v>168</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>31</v>
+        <v>165</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>61</v>
+        <v>169</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>97</v>
+        <v>170</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>421</v>
+        <v>42</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>422</v>
+        <v>58</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>423</v>
+        <v>94</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>421</v>
+        <v>597</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>422</v>
+        <v>598</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>423</v>
+        <v>599</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>260</v>
+        <v>47</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>261</v>
+        <v>73</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>262</v>
+        <v>95</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>263</v>
+        <v>49</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>438</v>
+        <v>280</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>439</v>
+        <v>281</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>441</v>
+        <v>282</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>567</v>
+        <v>359</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>568</v>
+        <v>360</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>570</v>
+        <v>361</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>117</v>
+        <v>164</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>31</v>
+        <v>165</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>493</v>
+        <v>203</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>494</v>
+        <v>204</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>495</v>
+        <v>205</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>179</v>
+        <v>50</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>180</v>
+        <v>61</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>182</v>
+        <v>97</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>322</v>
+        <v>421</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>323</v>
+        <v>422</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>324</v>
+        <v>423</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>186</v>
+        <v>421</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>187</v>
+        <v>422</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>188</v>
+        <v>423</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>477</v>
+        <v>260</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>478</v>
+        <v>261</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>479</v>
+        <v>262</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>267</v>
+        <v>438</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>268</v>
+        <v>439</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>269</v>
+        <v>440</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>209</v>
+        <v>567</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>210</v>
+        <v>568</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>212</v>
+        <v>569</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>216</v>
+        <v>570</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>565</v>
+        <v>313</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>556</v>
+        <v>314</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>558</v>
+        <v>315</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>338</v>
+        <v>117</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>328</v>
+        <v>118</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>329</v>
+        <v>119</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>574</v>
+        <v>493</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>579</v>
+        <v>494</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>580</v>
+        <v>495</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>502</v>
+        <v>179</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>504</v>
+        <v>180</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>506</v>
+        <v>182</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>348</v>
+        <v>322</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>349</v>
+        <v>323</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>351</v>
+        <v>324</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>549</v>
+        <v>186</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>550</v>
+        <v>187</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>551</v>
+        <v>188</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>38</v>
+        <v>587</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>59</v>
+        <v>588</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>39</v>
+        <v>589</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>586</v>
+        <v>477</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>443</v>
+        <v>478</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>442</v>
+        <v>479</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>544</v>
+        <v>267</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>545</v>
+        <v>268</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>546</v>
+        <v>269</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>434</v>
+        <v>624</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>435</v>
+        <v>625</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>437</v>
+        <v>626</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>272</v>
+        <v>209</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>270</v>
+        <v>210</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>271</v>
+        <v>212</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>172</v>
+        <v>565</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>173</v>
+        <v>556</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>174</v>
+        <v>557</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>427</v>
+        <v>338</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>428</v>
+        <v>328</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>548</v>
+        <v>329</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>68</v>
+        <v>574</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>69</v>
+        <v>579</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>71</v>
+        <v>580</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>587</v>
+        <v>502</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>588</v>
+        <v>504</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>589</v>
+        <v>506</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>590</v>
+        <v>618</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>591</v>
+        <v>619</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>592</v>
+        <v>620</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>597</v>
+        <v>348</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>598</v>
+        <v>349</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>599</v>
+        <v>350</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>603</v>
+        <v>549</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>601</v>
+        <v>551</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>602</v>
+        <v>38</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>604</v>
+        <v>59</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>605</v>
+        <v>98</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="B169" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C168" s="1" t="s">
+      <c r="C169" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="D168" s="1" t="s">
+      <c r="D169" s="1" t="s">
         <v>614</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A170" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A171" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A172" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A173" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A174" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A175" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F162">
-      <sortCondition ref="A1:A162"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F175">
+      <sortCondition ref="A1:A175"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="F1:F1048576">

</xml_diff>

<commit_message>
m112-1.xml: encoded p. 3 of 7
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65C0A2B-1FF1-E140-ADDF-9195F582168C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7537C7-B08A-8943-B178-251268A643DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36040" yWindow="0" windowWidth="15160" windowHeight="28800" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="669">
   <si>
     <t>M-Number</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>M110</t>
-  </si>
-  <si>
-    <t>M112</t>
   </si>
   <si>
     <t>M113</t>
@@ -1989,6 +1986,111 @@
   </si>
   <si>
     <t>psn-isa</t>
+  </si>
+  <si>
+    <t>M112-1</t>
+  </si>
+  <si>
+    <t>M112-2</t>
+  </si>
+  <si>
+    <t>M112-3</t>
+  </si>
+  <si>
+    <t>M112 [The Reader]. Typescript fragment with the author's ms. corrections, unsigned and undated. 5p.</t>
+  </si>
+  <si>
+    <t>m112-1.xml</t>
+  </si>
+  <si>
+    <t>transcriptions/m112-1.xml</t>
+  </si>
+  <si>
+    <t>Broadcast</t>
+  </si>
+  <si>
+    <t>lit-broa</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-broa</t>
+  </si>
+  <si>
+    <t>Johnson, Samuel</t>
+  </si>
+  <si>
+    <t>psn-sjoh</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-sjoh</t>
+  </si>
+  <si>
+    <t>Coleridge, Samuel Taylor</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-stco</t>
+  </si>
+  <si>
+    <t>psn-stco</t>
+  </si>
+  <si>
+    <t>psn-acbr</t>
+  </si>
+  <si>
+    <t>Bradley, A. C.</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-acbr</t>
+  </si>
+  <si>
+    <t>Frankland</t>
+  </si>
+  <si>
+    <t>Frankland's wife</t>
+  </si>
+  <si>
+    <t>Acton</t>
+  </si>
+  <si>
+    <t>Yorkshire</t>
+  </si>
+  <si>
+    <t>psn-franb</t>
+  </si>
+  <si>
+    <t>psn-frana</t>
+  </si>
+  <si>
+    <t>psn-wend</t>
+  </si>
+  <si>
+    <t>psn-acto</t>
+  </si>
+  <si>
+    <t>pla-york</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-york</t>
+  </si>
+  <si>
+    <t>Possibly reference to the Yorkshire Tragedy, attributed to Middleton</t>
+  </si>
+  <si>
+    <t>Wendoll</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-frana</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-franb</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-wend</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-acto</t>
+  </si>
+  <si>
+    <t>Oh, they're from A Woman Killed With Kindness, Thomas Heywood 1603, cf lit-woma</t>
   </si>
 </sst>
 </file>
@@ -2398,11 +2500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H40" sqref="H40"/>
+      <selection pane="topRight" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2433,10 +2535,10 @@
         <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>11</v>
@@ -2467,22 +2569,22 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F7" s="5">
         <v>2</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -2490,22 +2592,22 @@
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F8" s="5">
         <v>8</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2513,22 +2615,22 @@
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="F9" s="5">
         <v>9</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2536,22 +2638,22 @@
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F10" s="5">
         <v>9</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2559,19 +2661,19 @@
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F11" s="5">
         <v>19</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -2579,22 +2681,22 @@
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F12" s="5">
         <v>26</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -2602,19 +2704,19 @@
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>408</v>
       </c>
       <c r="F13" s="5">
         <v>35</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2622,19 +2724,19 @@
         <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>445</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>446</v>
       </c>
       <c r="F14" s="5">
         <v>7</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2642,22 +2744,22 @@
         <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>537</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>538</v>
       </c>
       <c r="F15" s="5">
         <v>9</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2665,92 +2767,117 @@
         <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>554</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>555</v>
       </c>
       <c r="F16" s="5">
         <v>5</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>584</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>585</v>
       </c>
       <c r="F17" s="5">
         <v>5</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>594</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>595</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>596</v>
       </c>
       <c r="F18" s="5">
         <v>4</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>608</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>609</v>
       </c>
       <c r="F19" s="5">
         <v>7</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>634</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="F20" s="5">
+        <v>5</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>635</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2767,11 +2894,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F175"/>
+  <dimension ref="A1:F184"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D175" sqref="D175"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E186" sqref="E186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2795,2575 +2922,2716 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>475</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="D27" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>523</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>532</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="E37" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>391</v>
-      </c>
       <c r="E38" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>631</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>616</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>419</v>
-      </c>
       <c r="E48" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>463</v>
-      </c>
       <c r="E52" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>319</v>
-      </c>
       <c r="D54" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C59" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>526</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C62" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>514</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="D64" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>521</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>622</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C67" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C68" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>412</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C69" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>412</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C70" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C73" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="E73" s="1" t="s">
         <v>399</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C74" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C75" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="E75" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C77" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="E77" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>600</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C79" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C80" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="E80" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C81" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C82" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="E82" s="1" t="s">
         <v>510</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C83" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="E83" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="E84" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D85" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>590</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C86" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>591</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C87" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C88" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C89" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>497</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>604</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C92" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>529</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C93" s="1" t="s">
+      <c r="D93" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C95" s="1" t="s">
+      <c r="D95" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="E95" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C96" s="1" t="s">
+      <c r="D96" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C97" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C98" s="1" t="s">
+      <c r="D98" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C99" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>333</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>425</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C101" s="1" t="s">
+      <c r="D101" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C102" s="1" t="s">
+      <c r="D102" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C103" s="1" t="s">
+      <c r="D103" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C104" s="1" t="s">
+      <c r="D104" s="1" t="s">
         <v>481</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C105" s="1" t="s">
+      <c r="D105" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E105" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C106" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>606</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B107" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C107" s="1" t="s">
+      <c r="D107" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="E107" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C108" s="1" t="s">
+      <c r="D108" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="E108" s="1" t="s">
         <v>432</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C110" s="1" t="s">
+      <c r="D110" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>246</v>
-      </c>
       <c r="E111" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="D112" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B113" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C113" s="1" t="s">
+      <c r="D113" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C115" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B116" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C116" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C117" s="1" t="s">
+      <c r="D117" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="D117" s="1" t="s">
-        <v>208</v>
-      </c>
       <c r="E117" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="B118" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C118" s="1" t="s">
+      <c r="D118" s="1" t="s">
         <v>500</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C119" s="1" t="s">
+      <c r="D119" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="E119" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C120" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="D120" s="1" t="s">
-        <v>560</v>
-      </c>
       <c r="E120" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C121" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>628</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>633</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="B123" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C123" s="1" t="s">
+      <c r="D123" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="E123" s="1" t="s">
         <v>563</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="B124" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C124" s="1" t="s">
+      <c r="D124" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C125" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B125" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C125" s="1" t="s">
+      <c r="D125" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C126" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="E126" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B127" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C127" s="1" t="s">
+      <c r="D127" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D127" s="1" t="s">
+      <c r="E127" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C128" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B128" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C128" s="1" t="s">
+      <c r="D128" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>534</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C130" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B130" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C130" s="1" t="s">
+      <c r="D130" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C131" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B131" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C131" s="1" t="s">
+      <c r="D131" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C132" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B132" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C132" s="1" t="s">
+      <c r="D132" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="E132" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C133" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B133" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C133" s="1" t="s">
+      <c r="D133" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D133" s="1" t="s">
+      <c r="E133" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C134" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C134" s="1" t="s">
+      <c r="D134" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C136" s="1" t="s">
+      <c r="D136" s="1" t="s">
         <v>598</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="C137" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E137" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C138" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C138" s="1" t="s">
+      <c r="D138" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C139" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B139" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C139" s="1" t="s">
+      <c r="D139" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C140" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B140" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C140" s="1" t="s">
+      <c r="D140" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="C141" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="D141" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C142" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B142" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C142" s="1" t="s">
+      <c r="D142" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C144" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="B144" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C144" s="1" t="s">
+      <c r="D144" s="1" t="s">
         <v>422</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C145" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="B145" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C145" s="1" t="s">
+      <c r="D145" s="1" t="s">
         <v>422</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C146" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B146" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C146" s="1" t="s">
+      <c r="D146" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="E146" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C147" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="B147" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C147" s="1" t="s">
+      <c r="D147" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="E147" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C148" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="B148" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C148" s="1" t="s">
+      <c r="D148" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="D148" s="1" t="s">
+      <c r="E148" s="1" t="s">
         <v>569</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C149" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C149" s="1" t="s">
+      <c r="D149" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C150" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B150" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C150" s="1" t="s">
+      <c r="D150" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C151" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="B151" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C151" s="1" t="s">
+      <c r="D151" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C152" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B152" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="D152" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C153" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C153" s="1" t="s">
+      <c r="D153" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C154" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B154" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C154" s="1" t="s">
+      <c r="D154" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C155" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="B155" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C155" s="1" t="s">
+      <c r="D155" s="1" t="s">
         <v>588</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C156" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="B156" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C156" s="1" t="s">
+      <c r="D156" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C157" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B157" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C157" s="1" t="s">
+      <c r="D157" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C158" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="B158" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C158" s="1" t="s">
+      <c r="D158" s="1" t="s">
         <v>625</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C159" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B159" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="D159" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C160" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="D160" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="D160" s="1" t="s">
+      <c r="E160" s="1" t="s">
         <v>557</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C161" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D161" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C162" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="D162" s="1" t="s">
         <v>579</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C164" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="B164" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C164" s="1" t="s">
+      <c r="D164" s="1" t="s">
         <v>619</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C165" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B165" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C165" s="1" t="s">
+      <c r="D165" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="D165" s="1" t="s">
+      <c r="E165" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C166" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="B166" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C166" s="1" t="s">
+      <c r="D166" s="1" t="s">
         <v>550</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E167" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E167" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C168" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D168" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="D168" s="1" t="s">
-        <v>444</v>
-      </c>
       <c r="E168" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C169" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="B169" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C169" s="1" t="s">
+      <c r="D169" s="1" t="s">
         <v>613</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C170" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="B170" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C170" s="1" t="s">
+      <c r="D170" s="1" t="s">
         <v>545</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C171" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="B171" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C171" s="1" t="s">
+      <c r="D171" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="D171" s="1" t="s">
+      <c r="E171" s="1" t="s">
         <v>436</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C172" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D172" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C173" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B173" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C173" s="1" t="s">
+      <c r="D173" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C174" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="B174" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C174" s="1" t="s">
+      <c r="D174" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="D174" s="1" t="s">
-        <v>429</v>
-      </c>
       <c r="E174" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C175" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B175" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C175" s="1" t="s">
+      <c r="D175" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D175" s="1" t="s">
+      <c r="E175" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E175" s="1" t="s">
-        <v>71</v>
+    </row>
+    <row r="176" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A176" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A177" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A178" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A179" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A180" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A181" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A182" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A183" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A184" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to tracking sheet with m112-3.xml info
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7537C7-B08A-8943-B178-251268A643DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0118C06-4772-A640-B1B2-DE9D4966A3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36040" yWindow="0" windowWidth="15160" windowHeight="28800" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="34640" yWindow="0" windowWidth="16560" windowHeight="28800" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="756">
   <si>
     <t>M-Number</t>
   </si>
@@ -2091,6 +2091,267 @@
   </si>
   <si>
     <t>Oh, they're from A Woman Killed With Kindness, Thomas Heywood 1603, cf lit-woma</t>
+  </si>
+  <si>
+    <t>Woman Killed with Kindness, A</t>
+  </si>
+  <si>
+    <t>lit-woma</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-woma</t>
+  </si>
+  <si>
+    <t>Heywood, Thomas</t>
+  </si>
+  <si>
+    <t>cf. psn-they</t>
+  </si>
+  <si>
+    <t>cf. lit-woma</t>
+  </si>
+  <si>
+    <t>psn-they</t>
+  </si>
+  <si>
+    <t>Marston, John</t>
+  </si>
+  <si>
+    <t>psn-jmar</t>
+  </si>
+  <si>
+    <t>Tourneur, Cecil</t>
+  </si>
+  <si>
+    <t>psn-ctou</t>
+  </si>
+  <si>
+    <t>Ford, John</t>
+  </si>
+  <si>
+    <t>psn-jfor</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-they</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-jmar</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-ctou</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-jfor</t>
+  </si>
+  <si>
+    <t>Stanley, Anne</t>
+  </si>
+  <si>
+    <t>psn-astan</t>
+  </si>
+  <si>
+    <t>Possibly Anne Stanley (1580-1647)</t>
+  </si>
+  <si>
+    <t>psn-arus</t>
+  </si>
+  <si>
+    <t>Russell, Anne</t>
+  </si>
+  <si>
+    <t>Herbert, Mary</t>
+  </si>
+  <si>
+    <t>psn-mher</t>
+  </si>
+  <si>
+    <t>Possibly Anne Dudley (1548-1604) nee Russell who served Queen Liz, was a patron of Spenser, sold Shakespeare his big house! And was a distant relative of Bertrand Russell and Winston Churchill</t>
+  </si>
+  <si>
+    <t>Possibly Mary Herbert (1580-1649), nee Talbot, granddaughter of Bess of Hardwick and courtier of Queen Liz</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-astan</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-arus</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-mher</t>
+  </si>
+  <si>
+    <t>Sheffield, Edmund</t>
+  </si>
+  <si>
+    <t>psn-eshe</t>
+  </si>
+  <si>
+    <t>Edmund Sheffield 1st earl of Mulgrave, 1564-1646</t>
+  </si>
+  <si>
+    <t>Erwin, Anne</t>
+  </si>
+  <si>
+    <t>psn-mirw</t>
+  </si>
+  <si>
+    <t>Mariana Irwin (or Anne Erwin here), able to find v little save her name</t>
+  </si>
+  <si>
+    <t>Grey, Elizabeth</t>
+  </si>
+  <si>
+    <t>psn-egre</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-eshe</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-mirw</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-egre</t>
+  </si>
+  <si>
+    <t>Possibly Elizabeth Grey (1582-1651), Countess of Kent and maid to Queen Liz</t>
+  </si>
+  <si>
+    <t>Arundel, Lord and Lady</t>
+  </si>
+  <si>
+    <t>psn-arun</t>
+  </si>
+  <si>
+    <t>Unknown, look up in diaries/letters of Ann Clifford</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-arun</t>
+  </si>
+  <si>
+    <t>Mad Lover, The</t>
+  </si>
+  <si>
+    <t>lit-madl</t>
+  </si>
+  <si>
+    <t>The Mad Lover, John Fletcher, 1647</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-madl</t>
+  </si>
+  <si>
+    <t>Ruthven, Lady</t>
+  </si>
+  <si>
+    <t>psn-ruth</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-ruth</t>
+  </si>
+  <si>
+    <t>Unknown, look up in diaries/letters of Ann Clifford. Maybe Lady Jane Ruthven, but that seems a stretch as she was Scottish nobility and then a courtier in Denmark/Sweden…</t>
+  </si>
+  <si>
+    <t>Morgann, Maurice</t>
+  </si>
+  <si>
+    <t>psn-mmor</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-mmor</t>
+  </si>
+  <si>
+    <t>m112-2.xml</t>
+  </si>
+  <si>
+    <t>transcriptions/m112-2.xml</t>
+  </si>
+  <si>
+    <t>Come back to additions on p. 2</t>
+  </si>
+  <si>
+    <t>M112-2 [The Reader]. Set 2 of 3. Typescript fragment, unsigned and undated with the author's ms. corrections. 2p.</t>
+  </si>
+  <si>
+    <t>Monotype</t>
+  </si>
+  <si>
+    <t>obj-mono</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#obj-mono</t>
+  </si>
+  <si>
+    <t>Henry V</t>
+  </si>
+  <si>
+    <t>lit-hen5</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-hen5</t>
+  </si>
+  <si>
+    <t>Midsummer Night's Dream, A</t>
+  </si>
+  <si>
+    <t>lit-mids</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-mids</t>
+  </si>
+  <si>
+    <t>Romeo and Juliet</t>
+  </si>
+  <si>
+    <t>lit-rome</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-rome</t>
+  </si>
+  <si>
+    <t>Magic Flute, The</t>
+  </si>
+  <si>
+    <t>Fidelio</t>
+  </si>
+  <si>
+    <t>lit-magi</t>
+  </si>
+  <si>
+    <t>lit-fide</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-magi</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-fide</t>
+  </si>
+  <si>
+    <t>m112-3.xml</t>
+  </si>
+  <si>
+    <t>transcriptions/m112-3.xml</t>
+  </si>
+  <si>
+    <t>M112 [The Reader]. Set 3 of 3. Typescript fragment, unsigned and undated. 3p.</t>
+  </si>
+  <si>
+    <t>Burton, Robert</t>
+  </si>
+  <si>
+    <t>psn-rbur</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-rbur</t>
+  </si>
+  <si>
+    <t>Anatomy of Melancholy, The</t>
+  </si>
+  <si>
+    <t>lit-anat</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-anat</t>
   </si>
 </sst>
 </file>
@@ -2502,9 +2763,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2865,14 +3126,47 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="F21" s="5">
+        <v>2</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>636</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="F22" s="5">
+        <v>3</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2894,11 +3188,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F184"/>
+  <dimension ref="A1:F207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E186" sqref="E186"/>
+    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D207" sqref="D207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2933,33 +3227,36 @@
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>654</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>75</v>
+        <v>659</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>76</v>
+        <v>667</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>119</v>
+        <v>668</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>413</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>414</v>
+        <v>75</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>415</v>
+        <v>76</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -2978,2666 +3275,3018 @@
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>473</v>
+        <v>413</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>474</v>
+        <v>414</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>475</v>
+        <v>415</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>473</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>51</v>
+        <v>474</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>88</v>
+        <v>475</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>334</v>
+        <v>753</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>335</v>
+        <v>754</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>336</v>
+        <v>755</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>182</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>183</v>
+        <v>51</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>380</v>
+        <v>334</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>155</v>
+        <v>335</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>156</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>111</v>
+        <v>182</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>112</v>
+        <v>183</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>199</v>
+        <v>380</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>200</v>
+        <v>155</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>214</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>456</v>
+        <v>710</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>454</v>
+        <v>711</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>455</v>
+        <v>713</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>391</v>
+        <v>111</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>392</v>
+        <v>112</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>393</v>
+        <v>113</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>382</v>
+        <v>199</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>383</v>
+        <v>200</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>384</v>
+        <v>201</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>133</v>
+        <v>382</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>134</v>
+        <v>383</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>135</v>
+        <v>384</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>367</v>
+        <v>447</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>369</v>
+        <v>449</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>375</v>
+        <v>387</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>84</v>
+        <v>133</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>85</v>
+        <v>134</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>502</v>
+        <v>367</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>504</v>
+        <v>368</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>232</v>
+        <v>373</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>233</v>
+        <v>374</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>234</v>
+        <v>375</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>370</v>
+        <v>650</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>371</v>
+        <v>649</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>372</v>
+        <v>651</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>229</v>
+        <v>640</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>230</v>
+        <v>641</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>231</v>
+        <v>642</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>142</v>
+        <v>86</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>502</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>52</v>
+        <v>504</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>98</v>
+        <v>506</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>176</v>
+        <v>750</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>146</v>
+        <v>233</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>147</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>354</v>
+        <v>370</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>71</v>
+        <v>371</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>73</v>
+        <v>372</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>229</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>53</v>
+        <v>230</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>65</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>519</v>
+        <v>144</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>522</v>
+        <v>143</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>523</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>530</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>531</v>
+        <v>52</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>532</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>81</v>
+        <v>176</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>82</v>
+        <v>177</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>83</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>457</v>
+        <v>145</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>458</v>
+        <v>146</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>459</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>570</v>
+        <v>354</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>574</v>
+        <v>71</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>576</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>235</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>236</v>
+        <v>53</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>237</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>102</v>
+        <v>519</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>103</v>
+        <v>522</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>212</v>
+        <v>523</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>388</v>
+        <v>530</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>389</v>
+        <v>531</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>482</v>
+        <v>532</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>629</v>
+        <v>81</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>630</v>
+        <v>82</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>631</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>241</v>
+        <v>457</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>242</v>
+        <v>458</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>243</v>
+        <v>459</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>570</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>54</v>
+        <v>574</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>95</v>
+        <v>576</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>309</v>
+        <v>235</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>310</v>
+        <v>236</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>311</v>
+        <v>237</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>614</v>
+        <v>102</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>615</v>
+        <v>103</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>616</v>
+        <v>104</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>483</v>
+        <v>388</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>484</v>
+        <v>389</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>485</v>
+        <v>390</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>364</v>
+        <v>646</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>365</v>
+        <v>648</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>366</v>
+        <v>647</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>159</v>
+        <v>629</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>160</v>
+        <v>630</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>161</v>
+        <v>631</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>416</v>
+        <v>241</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>417</v>
+        <v>242</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>419</v>
+        <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>416</v>
+        <v>40</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>417</v>
+        <v>54</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>472</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>538</v>
+        <v>309</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>539</v>
+        <v>310</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>540</v>
+        <v>311</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>263</v>
+        <v>614</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>264</v>
+        <v>615</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>265</v>
+        <v>616</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>249</v>
+        <v>483</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>247</v>
+        <v>484</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>250</v>
+        <v>485</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>460</v>
+        <v>364</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>461</v>
+        <v>365</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>467</v>
+        <v>366</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>317</v>
+        <v>416</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>318</v>
+        <v>417</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>320</v>
+        <v>418</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>192</v>
+        <v>416</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>193</v>
+        <v>417</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>194</v>
+        <v>418</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>252</v>
+        <v>538</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>114</v>
+        <v>539</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>115</v>
+        <v>540</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>571</v>
+        <v>263</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>575</v>
+        <v>264</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>577</v>
+        <v>265</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>324</v>
+        <v>701</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>325</v>
+        <v>702</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>326</v>
+        <v>707</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>703</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>403</v>
+        <v>249</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>404</v>
+        <v>247</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>405</v>
+        <v>248</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>487</v>
+        <v>461</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>488</v>
+        <v>462</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>524</v>
+        <v>139</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>525</v>
+        <v>140</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>526</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>515</v>
+        <v>317</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>516</v>
+        <v>318</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>517</v>
+        <v>320</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>513</v>
+        <v>192</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="C64" s="1" t="s">
-        <v>158</v>
+        <v>114</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>162</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>518</v>
+        <v>571</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>520</v>
+        <v>575</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>521</v>
+        <v>577</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>620</v>
+        <v>324</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>621</v>
+        <v>325</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>622</v>
+        <v>326</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>303</v>
+        <v>742</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>304</v>
+        <v>744</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>305</v>
+        <v>746</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>410</v>
+        <v>680</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>411</v>
+        <v>681</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>412</v>
+        <v>685</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>108</v>
+        <v>652</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>109</v>
+        <v>657</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>110</v>
+        <v>664</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>36</v>
+        <v>653</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>55</v>
+        <v>656</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>89</v>
+        <v>665</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>546</v>
+        <v>486</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>541</v>
+        <v>487</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>542</v>
+        <v>488</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>453</v>
+        <v>524</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>397</v>
+        <v>525</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>399</v>
+        <v>526</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>329</v>
+        <v>515</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>330</v>
+        <v>516</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>331</v>
+        <v>517</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>272</v>
+        <v>513</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>273</v>
+        <v>512</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>274</v>
+        <v>511</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>44</v>
+        <v>157</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>59</v>
+        <v>158</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>468</v>
+        <v>518</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>469</v>
+        <v>520</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>471</v>
+        <v>521</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>602</v>
+        <v>620</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>599</v>
+        <v>621</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>600</v>
+        <v>622</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>226</v>
+        <v>303</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>227</v>
+        <v>304</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>228</v>
+        <v>305</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>292</v>
+        <v>410</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>293</v>
+        <v>411</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>295</v>
+        <v>412</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>351</v>
+        <v>410</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>352</v>
+        <v>411</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>353</v>
+        <v>412</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>507</v>
+        <v>108</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>508</v>
+        <v>109</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>510</v>
+        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>218</v>
+        <v>36</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>219</v>
+        <v>55</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>221</v>
+        <v>89</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>222</v>
+        <v>546</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>223</v>
+        <v>541</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>225</v>
+        <v>542</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>315</v>
+        <v>453</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>316</v>
+        <v>397</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>319</v>
+        <v>398</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>589</v>
+        <v>704</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>590</v>
+        <v>705</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>591</v>
+        <v>708</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>105</v>
+        <v>329</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>106</v>
+        <v>330</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>107</v>
+        <v>331</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>489</v>
+        <v>272</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>490</v>
+        <v>273</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>491</v>
+        <v>274</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>495</v>
+        <v>44</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>496</v>
+        <v>59</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>497</v>
+        <v>90</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>296</v>
+        <v>468</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>290</v>
+        <v>469</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>291</v>
+        <v>470</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>601</v>
+        <v>732</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>603</v>
+        <v>733</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>604</v>
+        <v>734</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>527</v>
+        <v>602</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>528</v>
+        <v>599</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>529</v>
+        <v>600</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>450</v>
+        <v>226</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>451</v>
+        <v>227</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>452</v>
+        <v>228</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>174</v>
+        <v>292</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>190</v>
+        <v>293</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>175</v>
+        <v>294</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>195</v>
+        <v>691</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>196</v>
+        <v>692</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>197</v>
+        <v>697</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>198</v>
+        <v>694</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>297</v>
+        <v>672</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>298</v>
+        <v>675</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>299</v>
+        <v>682</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>148</v>
+        <v>351</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>149</v>
+        <v>352</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>150</v>
+        <v>353</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>355</v>
+        <v>507</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>356</v>
+        <v>508</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>357</v>
+        <v>509</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>381</v>
+        <v>218</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>332</v>
+        <v>219</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>333</v>
+        <v>220</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>423</v>
+        <v>222</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>424</v>
+        <v>223</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>425</v>
+        <v>224</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>99</v>
+        <v>315</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>100</v>
+        <v>316</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>101</v>
+        <v>319</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>400</v>
+        <v>589</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>401</v>
+        <v>590</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>402</v>
+        <v>591</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>300</v>
+        <v>105</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>301</v>
+        <v>106</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>302</v>
+        <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>479</v>
+        <v>643</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>480</v>
+        <v>644</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>481</v>
+        <v>645</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>62</v>
+        <v>489</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>63</v>
+        <v>490</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>64</v>
+        <v>491</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>572</v>
+        <v>495</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>605</v>
+        <v>496</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>606</v>
+        <v>497</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>151</v>
+        <v>296</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>152</v>
+        <v>290</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>154</v>
+        <v>291</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>429</v>
+        <v>601</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>430</v>
+        <v>603</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>432</v>
+        <v>604</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>50</v>
+        <v>527</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>61</v>
+        <v>528</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>91</v>
+        <v>529</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>276</v>
+        <v>450</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>277</v>
+        <v>451</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>278</v>
+        <v>452</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>244</v>
+        <v>174</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>246</v>
+        <v>190</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>251</v>
+        <v>175</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>191</v>
+        <v>197</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>238</v>
+        <v>297</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>239</v>
+        <v>298</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>240</v>
+        <v>299</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>39</v>
+        <v>148</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>56</v>
+        <v>149</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>394</v>
+        <v>355</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>164</v>
+        <v>47</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>395</v>
+        <v>356</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>396</v>
+        <v>357</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>130</v>
+        <v>381</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>131</v>
+        <v>332</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>132</v>
+        <v>333</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>205</v>
+        <v>423</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>206</v>
+        <v>424</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>210</v>
+        <v>425</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>498</v>
+        <v>99</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>499</v>
+        <v>100</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>500</v>
+        <v>101</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>463</v>
+        <v>400</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>464</v>
+        <v>401</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>466</v>
+        <v>402</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>565</v>
+        <v>300</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>558</v>
+        <v>301</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>557</v>
+        <v>302</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>626</v>
+        <v>479</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>627</v>
+        <v>480</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>632</v>
+        <v>62</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>633</v>
+        <v>63</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>560</v>
+        <v>572</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>561</v>
+        <v>605</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>563</v>
+        <v>606</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>376</v>
+        <v>714</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>377</v>
+        <v>715</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>378</v>
+        <v>717</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>361</v>
+        <v>741</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>362</v>
+        <v>743</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>363</v>
+        <v>745</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>285</v>
+        <v>151</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>282</v>
+        <v>152</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>283</v>
+        <v>153</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>284</v>
+        <v>154</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>126</v>
+        <v>429</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>127</v>
+        <v>430</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>128</v>
+        <v>431</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>129</v>
+        <v>432</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>136</v>
+        <v>50</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>137</v>
+        <v>61</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>533</v>
+        <v>676</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>534</v>
+        <v>677</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>253</v>
+        <v>735</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>254</v>
+        <v>736</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>255</v>
+        <v>737</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>286</v>
+        <v>729</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>287</v>
+        <v>730</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>289</v>
+        <v>731</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>77</v>
+        <v>244</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>78</v>
+        <v>246</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>79</v>
+        <v>245</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>80</v>
+        <v>251</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>169</v>
+        <v>191</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>41</v>
+        <v>722</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>57</v>
+        <v>723</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>93</v>
+        <v>724</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>596</v>
+        <v>238</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>597</v>
+        <v>239</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>598</v>
+        <v>240</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>279</v>
+        <v>394</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>280</v>
+        <v>395</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>281</v>
+        <v>396</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>358</v>
+        <v>130</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>359</v>
+        <v>131</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>360</v>
+        <v>132</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>306</v>
+        <v>205</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>307</v>
+        <v>206</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>308</v>
+        <v>207</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>163</v>
+        <v>498</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>164</v>
+        <v>47</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>165</v>
+        <v>499</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>166</v>
+        <v>500</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>202</v>
+        <v>463</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>203</v>
+        <v>464</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>204</v>
+        <v>465</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>49</v>
+        <v>565</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>60</v>
+        <v>558</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>96</v>
+        <v>559</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>420</v>
+        <v>626</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>421</v>
+        <v>627</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>420</v>
+        <v>632</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>422</v>
+        <v>633</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>259</v>
+        <v>560</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>260</v>
+        <v>561</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>261</v>
+        <v>562</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>262</v>
+        <v>563</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>437</v>
+        <v>376</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>438</v>
+        <v>377</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>440</v>
+        <v>378</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>566</v>
+        <v>361</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>567</v>
+        <v>362</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>569</v>
+        <v>363</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>312</v>
+        <v>285</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>314</v>
+        <v>283</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>118</v>
+        <v>128</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>492</v>
+        <v>136</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>493</v>
+        <v>137</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>494</v>
+        <v>138</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>178</v>
+        <v>533</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>181</v>
+        <v>534</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>321</v>
+        <v>256</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>322</v>
+        <v>257</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>323</v>
+        <v>258</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>185</v>
+        <v>253</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>186</v>
+        <v>254</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>187</v>
+        <v>255</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>586</v>
+        <v>286</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>587</v>
+        <v>287</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>588</v>
+        <v>288</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>476</v>
+        <v>77</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>477</v>
+        <v>78</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>478</v>
+        <v>79</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>266</v>
+        <v>167</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>267</v>
+        <v>168</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>268</v>
+        <v>169</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>623</v>
+        <v>41</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>624</v>
+        <v>57</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>625</v>
+        <v>93</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>208</v>
+        <v>596</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>209</v>
+        <v>597</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>215</v>
+        <v>598</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>564</v>
+        <v>46</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>555</v>
+        <v>72</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>556</v>
+        <v>94</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>557</v>
+        <v>48</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>337</v>
+        <v>279</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>327</v>
+        <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>328</v>
+        <v>281</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>573</v>
+        <v>358</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>578</v>
+        <v>359</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>579</v>
+        <v>360</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>501</v>
+        <v>738</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>503</v>
+        <v>739</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>505</v>
+        <v>740</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>617</v>
+        <v>306</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>618</v>
+        <v>307</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>619</v>
+        <v>308</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>347</v>
+        <v>163</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>348</v>
+        <v>165</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>548</v>
+        <v>690</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>549</v>
+        <v>689</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>550</v>
+        <v>696</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>37</v>
+        <v>718</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>58</v>
+        <v>719</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>97</v>
+        <v>720</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>38</v>
+        <v>721</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>585</v>
+        <v>202</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>442</v>
+        <v>203</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>441</v>
+        <v>204</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>611</v>
+        <v>49</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>612</v>
+        <v>60</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>613</v>
+        <v>96</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>543</v>
+        <v>698</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>544</v>
+        <v>699</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>545</v>
+        <v>706</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>271</v>
+        <v>420</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>269</v>
+        <v>421</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>270</v>
+        <v>422</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>171</v>
+        <v>259</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>172</v>
+        <v>260</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>173</v>
+        <v>261</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>426</v>
+        <v>437</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>427</v>
+        <v>438</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>428</v>
+        <v>439</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>547</v>
+        <v>440</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>67</v>
+        <v>566</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>68</v>
+        <v>567</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>69</v>
+        <v>568</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>70</v>
+        <v>569</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>640</v>
+        <v>312</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>641</v>
+        <v>313</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>642</v>
+        <v>314</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>643</v>
+        <v>116</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>644</v>
+        <v>117</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>645</v>
+        <v>118</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>646</v>
+        <v>492</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>648</v>
+        <v>493</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>647</v>
+        <v>494</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>650</v>
+        <v>178</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>649</v>
+        <v>179</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>651</v>
+        <v>181</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>652</v>
+        <v>321</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>657</v>
+        <v>322</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>668</v>
+        <v>323</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>653</v>
+        <v>185</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>656</v>
+        <v>186</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>668</v>
+        <v>187</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>663</v>
+        <v>686</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>658</v>
+        <v>687</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>666</v>
+        <v>695</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>668</v>
+        <v>688</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>654</v>
+        <v>586</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>659</v>
+        <v>587</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>668</v>
+        <v>588</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>655</v>
+        <v>476</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C184" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A185" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A186" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A187" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A188" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A189" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A190" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A191" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A192" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A193" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A194" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A195" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A196" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A197" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A198" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A199" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A200" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A201" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A202" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A203" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A204" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A205" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A206" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A207" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C207" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="D184" s="1" t="s">
+      <c r="D207" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="E184" s="1" t="s">
+      <c r="E207" s="1" t="s">
         <v>662</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F175">
-      <sortCondition ref="A1:A175"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F207">
+      <sortCondition ref="A1:A207"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="F1:F1048576">

</xml_diff>

<commit_message>
Not sure what the update is here...
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0895085C-79CC-A34C-AD95-B8F08C3A7198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A564CA0-C09B-4B45-9C8A-D9CFD38074FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35540" yWindow="0" windowWidth="15660" windowHeight="28800" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="34900" yWindow="0" windowWidth="16300" windowHeight="28800" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="781">
   <si>
     <t>M-Number</t>
   </si>
@@ -2352,6 +2352,81 @@
   </si>
   <si>
     <t>../resources/annotations.xml#lit-anat</t>
+  </si>
+  <si>
+    <t>M113 [The Reader]. Typescript fragments, one with the author's ms. corrections, unsigned and undated. 8p.</t>
+  </si>
+  <si>
+    <t>m113.xml</t>
+  </si>
+  <si>
+    <t>transcriptions/m113.xml</t>
+  </si>
+  <si>
+    <t>Westminster Abbey</t>
+  </si>
+  <si>
+    <t>pla-wmab</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-wmab</t>
+  </si>
+  <si>
+    <t>Tower of London</t>
+  </si>
+  <si>
+    <t>pla-towe</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-towe</t>
+  </si>
+  <si>
+    <t>psn-gcla</t>
+  </si>
+  <si>
+    <t>Clandon, Gilbert</t>
+  </si>
+  <si>
+    <t>Clandon, Angela</t>
+  </si>
+  <si>
+    <t>psn-acla</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-gcla</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-acla</t>
+  </si>
+  <si>
+    <t>Three Guineas</t>
+  </si>
+  <si>
+    <t>lit-3gui</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-3gui</t>
+  </si>
+  <si>
+    <t>Killed by psn-bjon</t>
+  </si>
+  <si>
+    <t>Dekker, Thomas</t>
+  </si>
+  <si>
+    <t>psn-tdek</t>
+  </si>
+  <si>
+    <t>La Trobe, Miss</t>
+  </si>
+  <si>
+    <t>psn-latr</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-tdek</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-latr</t>
   </si>
 </sst>
 </file>
@@ -2763,9 +2838,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C23" sqref="C23"/>
+    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3169,9 +3244,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>758</v>
       </c>
       <c r="F23" s="5">
         <v>8</v>
@@ -3191,11 +3275,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F207"/>
+  <dimension ref="A1:F214"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D207" sqref="D207"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B215" sqref="B215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3794,2502 +3878,2603 @@
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>570</v>
+        <v>767</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>574</v>
+        <v>768</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>576</v>
+        <v>770</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>235</v>
+        <v>766</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>236</v>
+        <v>765</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>237</v>
+        <v>769</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>102</v>
+        <v>570</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>103</v>
+        <v>574</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>212</v>
+        <v>576</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>388</v>
+        <v>235</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>482</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>646</v>
+        <v>102</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>648</v>
+        <v>103</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>647</v>
+        <v>104</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>629</v>
+        <v>388</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>164</v>
+        <v>47</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>630</v>
+        <v>389</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>631</v>
+        <v>390</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>241</v>
+        <v>646</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>242</v>
+        <v>648</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>243</v>
+        <v>647</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>40</v>
+        <v>629</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>54</v>
+        <v>630</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>95</v>
+        <v>631</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>309</v>
+        <v>241</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>310</v>
+        <v>242</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>311</v>
+        <v>243</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>614</v>
+        <v>40</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>615</v>
+        <v>54</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>616</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>483</v>
+        <v>309</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>484</v>
+        <v>310</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>485</v>
+        <v>311</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>364</v>
+        <v>614</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>365</v>
+        <v>615</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>366</v>
+        <v>616</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>159</v>
+        <v>775</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>160</v>
+        <v>776</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>161</v>
+        <v>779</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>416</v>
+        <v>483</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>417</v>
+        <v>484</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>419</v>
+        <v>485</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>416</v>
+        <v>364</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>417</v>
+        <v>365</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>472</v>
+        <v>366</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>538</v>
+        <v>159</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>539</v>
+        <v>160</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>540</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>263</v>
+        <v>416</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>264</v>
+        <v>417</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>265</v>
+        <v>418</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>701</v>
+        <v>416</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>702</v>
+        <v>417</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>707</v>
+        <v>418</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>703</v>
+        <v>472</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>249</v>
+        <v>538</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>247</v>
+        <v>539</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>250</v>
+        <v>540</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>460</v>
+        <v>263</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>461</v>
+        <v>264</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>467</v>
+        <v>265</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>139</v>
+        <v>701</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>140</v>
+        <v>702</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>141</v>
+        <v>707</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>703</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>317</v>
+        <v>249</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>318</v>
+        <v>247</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>320</v>
+        <v>248</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>192</v>
+        <v>460</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>193</v>
+        <v>461</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>194</v>
+        <v>462</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>252</v>
+        <v>139</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>571</v>
+        <v>317</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>575</v>
+        <v>318</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>577</v>
+        <v>320</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>324</v>
+        <v>192</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>43</v>
+        <v>164</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>325</v>
+        <v>193</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>326</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>742</v>
+        <v>252</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>744</v>
+        <v>114</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>746</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>680</v>
+        <v>571</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>681</v>
+        <v>575</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>685</v>
+        <v>577</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>403</v>
+        <v>324</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>404</v>
+        <v>325</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>405</v>
+        <v>326</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>652</v>
+        <v>742</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>657</v>
+        <v>744</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>668</v>
+        <v>746</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>653</v>
+        <v>680</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>656</v>
+        <v>681</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>668</v>
+        <v>685</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>486</v>
+        <v>403</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>487</v>
+        <v>404</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>488</v>
+        <v>405</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>524</v>
+        <v>652</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>525</v>
+        <v>657</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>526</v>
+        <v>664</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>515</v>
+        <v>653</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>516</v>
+        <v>656</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>517</v>
+        <v>665</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>513</v>
+        <v>486</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>512</v>
+        <v>487</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>157</v>
+        <v>524</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>158</v>
+        <v>525</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>162</v>
+        <v>526</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>620</v>
+        <v>513</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>621</v>
+        <v>512</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>511</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>303</v>
+        <v>157</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>304</v>
+        <v>158</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>305</v>
+        <v>162</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>410</v>
+        <v>518</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>411</v>
+        <v>520</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>412</v>
+        <v>521</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>410</v>
+        <v>620</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>411</v>
+        <v>621</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>412</v>
+        <v>622</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>108</v>
+        <v>303</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>109</v>
+        <v>304</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>110</v>
+        <v>305</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>36</v>
+        <v>410</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>55</v>
+        <v>411</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>89</v>
+        <v>412</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>546</v>
+        <v>410</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>541</v>
+        <v>411</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>542</v>
+        <v>412</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>453</v>
+        <v>108</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>397</v>
+        <v>109</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>399</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>704</v>
+        <v>36</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>705</v>
+        <v>55</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>708</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>709</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>329</v>
+        <v>546</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>330</v>
+        <v>541</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>331</v>
+        <v>542</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>272</v>
+        <v>453</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>273</v>
+        <v>397</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>274</v>
+        <v>398</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>275</v>
+        <v>399</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>44</v>
+        <v>704</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>59</v>
+        <v>705</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>90</v>
+        <v>708</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>45</v>
+        <v>709</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>468</v>
+        <v>329</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>469</v>
+        <v>330</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>471</v>
+        <v>331</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>732</v>
+        <v>272</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>733</v>
+        <v>273</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>734</v>
+        <v>274</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>602</v>
+        <v>44</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>599</v>
+        <v>59</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>600</v>
+        <v>90</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>226</v>
+        <v>468</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>227</v>
+        <v>469</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>228</v>
+        <v>470</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>292</v>
+        <v>732</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>293</v>
+        <v>733</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>295</v>
+        <v>734</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>691</v>
+        <v>602</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>692</v>
+        <v>599</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>697</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>694</v>
+        <v>600</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>672</v>
+        <v>226</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>675</v>
+        <v>227</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>674</v>
+        <v>228</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>351</v>
+        <v>292</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>352</v>
+        <v>293</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>353</v>
+        <v>294</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>507</v>
+        <v>691</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>508</v>
+        <v>692</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>509</v>
+        <v>697</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>510</v>
+        <v>694</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>218</v>
+        <v>672</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>219</v>
+        <v>675</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>220</v>
+        <v>682</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>221</v>
+        <v>674</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>222</v>
+        <v>351</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>223</v>
+        <v>352</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>225</v>
+        <v>353</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>315</v>
+        <v>507</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>316</v>
+        <v>508</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>319</v>
+        <v>509</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>589</v>
+        <v>218</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>590</v>
+        <v>219</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>591</v>
+        <v>220</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>105</v>
+        <v>222</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>106</v>
+        <v>223</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>107</v>
+        <v>224</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>643</v>
+        <v>315</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>644</v>
+        <v>316</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>645</v>
+        <v>319</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>489</v>
+        <v>589</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>490</v>
+        <v>590</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>491</v>
+        <v>591</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>495</v>
+        <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>496</v>
+        <v>106</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>497</v>
+        <v>107</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>296</v>
+        <v>643</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>290</v>
+        <v>644</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>291</v>
+        <v>645</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>601</v>
+        <v>489</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>603</v>
+        <v>490</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>604</v>
+        <v>491</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>527</v>
+        <v>495</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>528</v>
+        <v>496</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>529</v>
+        <v>497</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>450</v>
+        <v>296</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>451</v>
+        <v>290</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>452</v>
+        <v>291</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>174</v>
+        <v>601</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>190</v>
+        <v>603</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>175</v>
+        <v>604</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>195</v>
+        <v>527</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>196</v>
+        <v>528</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>198</v>
+        <v>529</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>297</v>
+        <v>450</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>298</v>
+        <v>451</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>299</v>
+        <v>452</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>148</v>
+        <v>777</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>149</v>
+        <v>778</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>150</v>
+        <v>780</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>355</v>
+        <v>174</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>356</v>
+        <v>190</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>357</v>
+        <v>175</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>381</v>
+        <v>195</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>332</v>
+        <v>196</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>333</v>
+        <v>197</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>423</v>
+        <v>297</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>424</v>
+        <v>298</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>425</v>
+        <v>299</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>100</v>
+        <v>149</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>101</v>
+        <v>150</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>400</v>
+        <v>355</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>401</v>
+        <v>356</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>402</v>
+        <v>357</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>300</v>
+        <v>381</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>301</v>
+        <v>332</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>302</v>
+        <v>333</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>479</v>
+        <v>423</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>480</v>
+        <v>424</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>481</v>
+        <v>425</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>572</v>
+        <v>400</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>605</v>
+        <v>401</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>606</v>
+        <v>402</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>714</v>
+        <v>300</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>715</v>
+        <v>301</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>717</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>716</v>
+        <v>302</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>741</v>
+        <v>479</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>743</v>
+        <v>480</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>745</v>
+        <v>481</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>151</v>
+        <v>62</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>152</v>
+        <v>63</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>153</v>
+        <v>66</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>154</v>
+        <v>64</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>429</v>
+        <v>572</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>430</v>
+        <v>605</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>432</v>
+        <v>606</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>50</v>
+        <v>714</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>61</v>
+        <v>715</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>91</v>
+        <v>717</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>676</v>
+        <v>741</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>677</v>
+        <v>743</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>683</v>
+        <v>745</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>276</v>
+        <v>151</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>277</v>
+        <v>152</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>278</v>
+        <v>153</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>735</v>
+        <v>429</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>736</v>
+        <v>430</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>737</v>
+        <v>431</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>729</v>
+        <v>50</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>730</v>
+        <v>61</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>731</v>
+        <v>91</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>244</v>
+        <v>676</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>246</v>
+        <v>677</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>251</v>
+        <v>683</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>188</v>
+        <v>276</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>189</v>
+        <v>277</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>191</v>
+        <v>278</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>723</v>
+        <v>736</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>724</v>
+        <v>737</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>238</v>
+        <v>729</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>239</v>
+        <v>730</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>240</v>
+        <v>731</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>39</v>
+        <v>244</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>56</v>
+        <v>246</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>92</v>
+        <v>245</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>394</v>
+        <v>188</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>395</v>
+        <v>189</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>396</v>
+        <v>191</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>130</v>
+        <v>722</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>131</v>
+        <v>723</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>132</v>
+        <v>724</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>205</v>
+        <v>238</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>206</v>
+        <v>239</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>498</v>
+        <v>39</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>499</v>
+        <v>56</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>500</v>
+        <v>92</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>463</v>
+        <v>394</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>43</v>
+        <v>164</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>464</v>
+        <v>395</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>466</v>
+        <v>396</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>565</v>
+        <v>130</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>558</v>
+        <v>131</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>557</v>
+        <v>132</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>626</v>
+        <v>205</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>627</v>
+        <v>206</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>632</v>
+        <v>498</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>633</v>
+        <v>499</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>560</v>
+        <v>463</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>561</v>
+        <v>464</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>562</v>
+        <v>465</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>563</v>
+        <v>466</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>376</v>
+        <v>565</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>377</v>
+        <v>558</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>378</v>
+        <v>559</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>361</v>
+        <v>626</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>362</v>
+        <v>627</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>285</v>
+        <v>632</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>284</v>
+        <v>633</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>126</v>
+        <v>560</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>127</v>
+        <v>561</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>128</v>
+        <v>562</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>129</v>
+        <v>563</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>136</v>
+        <v>376</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>137</v>
+        <v>377</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>138</v>
+        <v>378</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>533</v>
+        <v>361</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>534</v>
+        <v>362</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>256</v>
+        <v>285</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>257</v>
+        <v>282</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>258</v>
+        <v>283</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>253</v>
+        <v>126</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>254</v>
+        <v>127</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>255</v>
+        <v>128</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>286</v>
+        <v>136</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>287</v>
+        <v>137</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>289</v>
+        <v>138</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>77</v>
+        <v>533</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>80</v>
+        <v>534</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>167</v>
+        <v>256</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>164</v>
+        <v>47</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>168</v>
+        <v>257</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>169</v>
+        <v>258</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>41</v>
+        <v>253</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>93</v>
+        <v>255</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>596</v>
+        <v>286</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>597</v>
+        <v>287</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>598</v>
+        <v>288</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>279</v>
+        <v>167</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>280</v>
+        <v>168</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>281</v>
+        <v>169</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>358</v>
+        <v>41</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>359</v>
+        <v>57</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>360</v>
+        <v>93</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>738</v>
+        <v>596</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>739</v>
+        <v>597</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>740</v>
+        <v>598</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>306</v>
+        <v>46</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>307</v>
+        <v>72</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>308</v>
+        <v>94</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>163</v>
+        <v>279</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>165</v>
+        <v>280</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>690</v>
+        <v>358</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>689</v>
+        <v>359</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>693</v>
+        <v>360</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>718</v>
+        <v>738</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>719</v>
+        <v>739</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>720</v>
-      </c>
-      <c r="E167" s="1" t="s">
-        <v>721</v>
+        <v>740</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>202</v>
+        <v>306</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>203</v>
+        <v>307</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>204</v>
+        <v>308</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>49</v>
+        <v>163</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>699</v>
+        <v>689</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>706</v>
+        <v>696</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>420</v>
+        <v>718</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>421</v>
+        <v>719</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>422</v>
+        <v>720</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>721</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>420</v>
+        <v>202</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>421</v>
+        <v>203</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>422</v>
+        <v>204</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>259</v>
+        <v>49</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>260</v>
+        <v>60</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>262</v>
+        <v>96</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>437</v>
+        <v>698</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>438</v>
+        <v>699</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>439</v>
+        <v>706</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>440</v>
+        <v>700</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>566</v>
+        <v>420</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>567</v>
+        <v>421</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>569</v>
+        <v>422</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>312</v>
+        <v>420</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>313</v>
+        <v>421</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>314</v>
+        <v>422</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>116</v>
+        <v>259</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>117</v>
+        <v>260</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>118</v>
+        <v>261</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>492</v>
+        <v>437</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>493</v>
+        <v>438</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>494</v>
+        <v>439</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>178</v>
+        <v>566</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>179</v>
+        <v>567</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>181</v>
+        <v>568</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>185</v>
+        <v>116</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>186</v>
+        <v>117</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>187</v>
+        <v>118</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>686</v>
+        <v>492</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>687</v>
+        <v>493</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>695</v>
+        <v>494</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>688</v>
+        <v>774</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>586</v>
+        <v>178</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>587</v>
+        <v>179</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>588</v>
+        <v>181</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>476</v>
+        <v>321</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>477</v>
+        <v>322</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>478</v>
+        <v>323</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>266</v>
+        <v>185</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>267</v>
+        <v>186</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>268</v>
+        <v>187</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>623</v>
+        <v>686</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>624</v>
+        <v>687</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>625</v>
+        <v>695</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>688</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>208</v>
+        <v>586</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>209</v>
+        <v>587</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E187" s="1" t="s">
-        <v>215</v>
+        <v>588</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>564</v>
+        <v>476</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>555</v>
+        <v>477</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>557</v>
+        <v>478</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>337</v>
+        <v>266</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>327</v>
+        <v>267</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>328</v>
+        <v>268</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>573</v>
+        <v>623</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>578</v>
+        <v>624</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>579</v>
+        <v>625</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>501</v>
+        <v>208</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>503</v>
+        <v>209</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>505</v>
+        <v>211</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>617</v>
+        <v>564</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>618</v>
+        <v>555</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>619</v>
+        <v>556</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>678</v>
+        <v>337</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>679</v>
+        <v>327</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>684</v>
+        <v>328</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>347</v>
+        <v>573</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>348</v>
+        <v>578</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="E194" s="1" t="s">
-        <v>350</v>
+        <v>579</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>548</v>
+        <v>501</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>549</v>
+        <v>503</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>550</v>
+        <v>505</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>37</v>
+        <v>771</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>58</v>
+        <v>772</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E196" s="1" t="s">
-        <v>38</v>
+        <v>773</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>585</v>
+        <v>617</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>442</v>
+        <v>618</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="E197" s="1" t="s">
-        <v>441</v>
+        <v>619</v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>663</v>
+        <v>678</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>658</v>
+        <v>679</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="E198" s="1" t="s">
-        <v>668</v>
+        <v>684</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>611</v>
+        <v>762</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>612</v>
+        <v>763</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>613</v>
+        <v>764</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>543</v>
+        <v>347</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>544</v>
+        <v>348</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>545</v>
+        <v>349</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>433</v>
+        <v>548</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>434</v>
+        <v>549</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="E201" s="1" t="s">
-        <v>436</v>
+        <v>550</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>271</v>
+        <v>37</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>269</v>
+        <v>58</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>270</v>
+        <v>97</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>171</v>
+        <v>585</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>172</v>
+        <v>442</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>173</v>
+        <v>443</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>670</v>
+        <v>658</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>426</v>
+        <v>759</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>427</v>
+        <v>760</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="E205" s="1" t="s">
-        <v>547</v>
+        <v>761</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>67</v>
+        <v>611</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>68</v>
+        <v>612</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E206" s="1" t="s">
-        <v>70</v>
+        <v>613</v>
       </c>
     </row>
     <row r="207" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>655</v>
+        <v>543</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C207" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A208" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A209" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A210" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A211" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A212" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A213" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A214" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C214" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="D207" s="1" t="s">
+      <c r="D214" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="E207" s="1" t="s">
+      <c r="E214" s="1" t="s">
         <v>662</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F207">
-      <sortCondition ref="A1:A207"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F214">
+      <sortCondition ref="A1:A214"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="F1:F1048576">

</xml_diff>

<commit_message>
Latest updates to tracking sheet
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0895085C-79CC-A34C-AD95-B8F08C3A7198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F5BCD3-2C33-8F4E-800E-AF6C0947DCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35540" yWindow="0" windowWidth="15660" windowHeight="28800" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="34900" yWindow="0" windowWidth="16300" windowHeight="28800" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="781">
   <si>
     <t>M-Number</t>
   </si>
@@ -2352,6 +2352,81 @@
   </si>
   <si>
     <t>../resources/annotations.xml#lit-anat</t>
+  </si>
+  <si>
+    <t>M113 [The Reader]. Typescript fragments, one with the author's ms. corrections, unsigned and undated. 8p.</t>
+  </si>
+  <si>
+    <t>m113.xml</t>
+  </si>
+  <si>
+    <t>transcriptions/m113.xml</t>
+  </si>
+  <si>
+    <t>Westminster Abbey</t>
+  </si>
+  <si>
+    <t>pla-wmab</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-wmab</t>
+  </si>
+  <si>
+    <t>Tower of London</t>
+  </si>
+  <si>
+    <t>pla-towe</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-towe</t>
+  </si>
+  <si>
+    <t>psn-gcla</t>
+  </si>
+  <si>
+    <t>Clandon, Gilbert</t>
+  </si>
+  <si>
+    <t>Clandon, Angela</t>
+  </si>
+  <si>
+    <t>psn-acla</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-gcla</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-acla</t>
+  </si>
+  <si>
+    <t>Three Guineas</t>
+  </si>
+  <si>
+    <t>lit-3gui</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-3gui</t>
+  </si>
+  <si>
+    <t>Killed by psn-bjon</t>
+  </si>
+  <si>
+    <t>Dekker, Thomas</t>
+  </si>
+  <si>
+    <t>psn-tdek</t>
+  </si>
+  <si>
+    <t>La Trobe, Miss</t>
+  </si>
+  <si>
+    <t>psn-latr</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-tdek</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-latr</t>
   </si>
 </sst>
 </file>
@@ -2763,9 +2838,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C23" sqref="C23"/>
+    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3169,9 +3244,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>758</v>
       </c>
       <c r="F23" s="5">
         <v>8</v>
@@ -3191,11 +3275,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F207"/>
+  <dimension ref="A1:F214"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D207" sqref="D207"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3794,2502 +3878,2603 @@
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>570</v>
+        <v>767</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>574</v>
+        <v>768</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>576</v>
+        <v>770</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>235</v>
+        <v>766</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>236</v>
+        <v>765</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>237</v>
+        <v>769</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>102</v>
+        <v>570</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>103</v>
+        <v>574</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>212</v>
+        <v>576</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>388</v>
+        <v>235</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>482</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>646</v>
+        <v>102</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>648</v>
+        <v>103</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>647</v>
+        <v>104</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>629</v>
+        <v>388</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>164</v>
+        <v>47</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>630</v>
+        <v>389</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>631</v>
+        <v>390</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>241</v>
+        <v>646</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>242</v>
+        <v>648</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>243</v>
+        <v>647</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>40</v>
+        <v>629</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>54</v>
+        <v>630</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>95</v>
+        <v>631</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>309</v>
+        <v>241</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>310</v>
+        <v>242</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>311</v>
+        <v>243</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>614</v>
+        <v>40</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>615</v>
+        <v>54</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>616</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>483</v>
+        <v>309</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>484</v>
+        <v>310</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>485</v>
+        <v>311</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>364</v>
+        <v>614</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>365</v>
+        <v>615</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>366</v>
+        <v>616</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>159</v>
+        <v>775</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>160</v>
+        <v>776</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>161</v>
+        <v>779</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>416</v>
+        <v>483</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>417</v>
+        <v>484</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>419</v>
+        <v>485</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>416</v>
+        <v>364</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>417</v>
+        <v>365</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>472</v>
+        <v>366</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>538</v>
+        <v>159</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>539</v>
+        <v>160</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>540</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>263</v>
+        <v>416</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>264</v>
+        <v>417</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>265</v>
+        <v>418</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>701</v>
+        <v>416</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>702</v>
+        <v>417</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>707</v>
+        <v>418</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>703</v>
+        <v>472</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>249</v>
+        <v>538</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>247</v>
+        <v>539</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>250</v>
+        <v>540</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>460</v>
+        <v>263</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>461</v>
+        <v>264</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>467</v>
+        <v>265</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>139</v>
+        <v>701</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>140</v>
+        <v>702</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>141</v>
+        <v>707</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>703</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>317</v>
+        <v>249</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>318</v>
+        <v>247</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>320</v>
+        <v>248</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>192</v>
+        <v>460</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>193</v>
+        <v>461</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>194</v>
+        <v>462</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>252</v>
+        <v>139</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>571</v>
+        <v>317</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>575</v>
+        <v>318</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>577</v>
+        <v>320</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>324</v>
+        <v>192</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>43</v>
+        <v>164</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>325</v>
+        <v>193</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>326</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>742</v>
+        <v>252</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>744</v>
+        <v>114</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>746</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>680</v>
+        <v>571</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>681</v>
+        <v>575</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>685</v>
+        <v>577</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>403</v>
+        <v>324</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>404</v>
+        <v>325</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>405</v>
+        <v>326</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>652</v>
+        <v>742</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>657</v>
+        <v>744</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>668</v>
+        <v>746</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>653</v>
+        <v>680</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>656</v>
+        <v>681</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>668</v>
+        <v>685</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>486</v>
+        <v>403</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>487</v>
+        <v>404</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>488</v>
+        <v>405</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>524</v>
+        <v>652</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>525</v>
+        <v>657</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>526</v>
+        <v>664</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>515</v>
+        <v>653</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>516</v>
+        <v>656</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>517</v>
+        <v>665</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>513</v>
+        <v>486</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>512</v>
+        <v>487</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>157</v>
+        <v>524</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>158</v>
+        <v>525</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>162</v>
+        <v>526</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>620</v>
+        <v>513</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>621</v>
+        <v>512</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>511</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>303</v>
+        <v>157</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>304</v>
+        <v>158</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>305</v>
+        <v>162</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>410</v>
+        <v>518</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>411</v>
+        <v>520</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>412</v>
+        <v>521</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>410</v>
+        <v>620</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>411</v>
+        <v>621</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>412</v>
+        <v>622</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>108</v>
+        <v>303</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>109</v>
+        <v>304</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>110</v>
+        <v>305</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>36</v>
+        <v>410</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>55</v>
+        <v>411</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>89</v>
+        <v>412</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>546</v>
+        <v>410</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>541</v>
+        <v>411</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>542</v>
+        <v>412</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>453</v>
+        <v>108</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>397</v>
+        <v>109</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>399</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>704</v>
+        <v>36</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>705</v>
+        <v>55</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>708</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>709</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>329</v>
+        <v>546</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>330</v>
+        <v>541</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>331</v>
+        <v>542</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>272</v>
+        <v>453</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>273</v>
+        <v>397</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>274</v>
+        <v>398</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>275</v>
+        <v>399</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>44</v>
+        <v>704</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>59</v>
+        <v>705</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>90</v>
+        <v>708</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>45</v>
+        <v>709</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>468</v>
+        <v>329</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>469</v>
+        <v>330</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>471</v>
+        <v>331</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>732</v>
+        <v>272</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>733</v>
+        <v>273</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>734</v>
+        <v>274</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>602</v>
+        <v>44</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>599</v>
+        <v>59</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>600</v>
+        <v>90</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>226</v>
+        <v>468</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>227</v>
+        <v>469</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>228</v>
+        <v>470</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>292</v>
+        <v>732</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>293</v>
+        <v>733</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>295</v>
+        <v>734</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>691</v>
+        <v>602</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>692</v>
+        <v>599</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>697</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>694</v>
+        <v>600</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>672</v>
+        <v>226</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>675</v>
+        <v>227</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>674</v>
+        <v>228</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>351</v>
+        <v>292</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>352</v>
+        <v>293</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>353</v>
+        <v>294</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>507</v>
+        <v>691</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>508</v>
+        <v>692</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>509</v>
+        <v>697</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>510</v>
+        <v>694</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>218</v>
+        <v>672</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>219</v>
+        <v>675</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>220</v>
+        <v>682</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>221</v>
+        <v>674</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>222</v>
+        <v>351</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>223</v>
+        <v>352</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>225</v>
+        <v>353</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>315</v>
+        <v>507</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>316</v>
+        <v>508</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>319</v>
+        <v>509</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>589</v>
+        <v>218</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>590</v>
+        <v>219</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>591</v>
+        <v>220</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>105</v>
+        <v>222</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>106</v>
+        <v>223</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>107</v>
+        <v>224</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>643</v>
+        <v>315</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>644</v>
+        <v>316</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>645</v>
+        <v>319</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>489</v>
+        <v>589</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>490</v>
+        <v>590</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>491</v>
+        <v>591</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>495</v>
+        <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>496</v>
+        <v>106</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>497</v>
+        <v>107</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>296</v>
+        <v>643</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>290</v>
+        <v>644</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>291</v>
+        <v>645</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>601</v>
+        <v>489</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>603</v>
+        <v>490</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>604</v>
+        <v>491</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>527</v>
+        <v>495</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>528</v>
+        <v>496</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>529</v>
+        <v>497</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>450</v>
+        <v>296</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>451</v>
+        <v>290</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>452</v>
+        <v>291</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>174</v>
+        <v>601</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>190</v>
+        <v>603</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>175</v>
+        <v>604</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>195</v>
+        <v>527</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>196</v>
+        <v>528</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>198</v>
+        <v>529</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>297</v>
+        <v>450</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>298</v>
+        <v>451</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>299</v>
+        <v>452</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>148</v>
+        <v>777</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>149</v>
+        <v>778</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>150</v>
+        <v>780</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>355</v>
+        <v>174</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>356</v>
+        <v>190</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>357</v>
+        <v>175</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>381</v>
+        <v>195</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>332</v>
+        <v>196</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>333</v>
+        <v>197</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>423</v>
+        <v>297</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>424</v>
+        <v>298</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>425</v>
+        <v>299</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>100</v>
+        <v>149</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>101</v>
+        <v>150</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>400</v>
+        <v>355</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>401</v>
+        <v>356</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>402</v>
+        <v>357</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>300</v>
+        <v>381</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>301</v>
+        <v>332</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>302</v>
+        <v>333</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>479</v>
+        <v>423</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>480</v>
+        <v>424</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>481</v>
+        <v>425</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>572</v>
+        <v>400</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>605</v>
+        <v>401</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>606</v>
+        <v>402</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>714</v>
+        <v>300</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>715</v>
+        <v>301</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>717</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>716</v>
+        <v>302</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>741</v>
+        <v>479</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>743</v>
+        <v>480</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>745</v>
+        <v>481</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>151</v>
+        <v>62</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>152</v>
+        <v>63</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>153</v>
+        <v>66</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>154</v>
+        <v>64</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>429</v>
+        <v>572</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>430</v>
+        <v>605</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>432</v>
+        <v>606</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>50</v>
+        <v>714</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>61</v>
+        <v>715</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>91</v>
+        <v>717</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>676</v>
+        <v>741</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>677</v>
+        <v>743</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>683</v>
+        <v>745</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>276</v>
+        <v>151</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>277</v>
+        <v>152</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>278</v>
+        <v>153</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>735</v>
+        <v>429</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>736</v>
+        <v>430</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>737</v>
+        <v>431</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>729</v>
+        <v>50</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>730</v>
+        <v>61</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>731</v>
+        <v>91</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>244</v>
+        <v>676</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>246</v>
+        <v>677</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>251</v>
+        <v>683</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>188</v>
+        <v>276</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>189</v>
+        <v>277</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>191</v>
+        <v>278</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>723</v>
+        <v>736</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>724</v>
+        <v>737</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>238</v>
+        <v>729</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>239</v>
+        <v>730</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>240</v>
+        <v>731</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>39</v>
+        <v>244</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>56</v>
+        <v>246</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>92</v>
+        <v>245</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>394</v>
+        <v>188</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>395</v>
+        <v>189</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>396</v>
+        <v>191</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>130</v>
+        <v>722</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>131</v>
+        <v>723</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>132</v>
+        <v>724</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>205</v>
+        <v>238</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>206</v>
+        <v>239</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>498</v>
+        <v>39</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>499</v>
+        <v>56</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>500</v>
+        <v>92</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>463</v>
+        <v>394</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>43</v>
+        <v>164</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>464</v>
+        <v>395</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>466</v>
+        <v>396</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>565</v>
+        <v>130</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>558</v>
+        <v>131</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>557</v>
+        <v>132</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>626</v>
+        <v>205</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>627</v>
+        <v>206</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>632</v>
+        <v>498</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>633</v>
+        <v>499</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>560</v>
+        <v>463</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>561</v>
+        <v>464</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>562</v>
+        <v>465</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>563</v>
+        <v>466</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>376</v>
+        <v>565</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>377</v>
+        <v>558</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>378</v>
+        <v>559</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>361</v>
+        <v>626</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>362</v>
+        <v>627</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>285</v>
+        <v>632</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>284</v>
+        <v>633</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>126</v>
+        <v>560</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>127</v>
+        <v>561</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>128</v>
+        <v>562</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>129</v>
+        <v>563</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>136</v>
+        <v>376</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>137</v>
+        <v>377</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>138</v>
+        <v>378</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>533</v>
+        <v>361</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>534</v>
+        <v>362</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>256</v>
+        <v>285</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>257</v>
+        <v>282</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>258</v>
+        <v>283</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>253</v>
+        <v>126</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>254</v>
+        <v>127</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>255</v>
+        <v>128</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>286</v>
+        <v>136</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>287</v>
+        <v>137</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>289</v>
+        <v>138</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>77</v>
+        <v>533</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>80</v>
+        <v>534</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>167</v>
+        <v>256</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>164</v>
+        <v>47</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>168</v>
+        <v>257</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>169</v>
+        <v>258</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>41</v>
+        <v>253</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>93</v>
+        <v>255</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>596</v>
+        <v>286</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>597</v>
+        <v>287</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>598</v>
+        <v>288</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>279</v>
+        <v>167</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>280</v>
+        <v>168</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>281</v>
+        <v>169</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>358</v>
+        <v>41</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>359</v>
+        <v>57</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>360</v>
+        <v>93</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>738</v>
+        <v>596</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>739</v>
+        <v>597</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>740</v>
+        <v>598</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>306</v>
+        <v>46</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>307</v>
+        <v>72</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>308</v>
+        <v>94</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>163</v>
+        <v>279</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>165</v>
+        <v>280</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>690</v>
+        <v>358</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>689</v>
+        <v>359</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>693</v>
+        <v>360</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>718</v>
+        <v>738</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>719</v>
+        <v>739</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>720</v>
-      </c>
-      <c r="E167" s="1" t="s">
-        <v>721</v>
+        <v>740</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>202</v>
+        <v>306</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>203</v>
+        <v>307</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>204</v>
+        <v>308</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>49</v>
+        <v>163</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>699</v>
+        <v>689</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>706</v>
+        <v>696</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>420</v>
+        <v>718</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>421</v>
+        <v>719</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>422</v>
+        <v>720</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>721</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>420</v>
+        <v>202</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>421</v>
+        <v>203</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>422</v>
+        <v>204</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>259</v>
+        <v>49</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>260</v>
+        <v>60</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>262</v>
+        <v>96</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>437</v>
+        <v>698</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>438</v>
+        <v>699</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>439</v>
+        <v>706</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>440</v>
+        <v>700</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>566</v>
+        <v>420</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>567</v>
+        <v>421</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>569</v>
+        <v>422</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>312</v>
+        <v>420</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>313</v>
+        <v>421</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>314</v>
+        <v>422</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>116</v>
+        <v>259</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>117</v>
+        <v>260</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>118</v>
+        <v>261</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>492</v>
+        <v>437</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>493</v>
+        <v>438</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>494</v>
+        <v>439</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>178</v>
+        <v>566</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>179</v>
+        <v>567</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>181</v>
+        <v>568</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>185</v>
+        <v>116</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>186</v>
+        <v>117</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>187</v>
+        <v>118</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>686</v>
+        <v>492</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>687</v>
+        <v>493</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>695</v>
+        <v>494</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>688</v>
+        <v>774</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>586</v>
+        <v>178</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>587</v>
+        <v>179</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>588</v>
+        <v>181</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>476</v>
+        <v>321</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>477</v>
+        <v>322</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>478</v>
+        <v>323</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>266</v>
+        <v>185</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>267</v>
+        <v>186</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>268</v>
+        <v>187</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>623</v>
+        <v>686</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>624</v>
+        <v>687</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>625</v>
+        <v>695</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>688</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>208</v>
+        <v>586</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>209</v>
+        <v>587</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E187" s="1" t="s">
-        <v>215</v>
+        <v>588</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>564</v>
+        <v>476</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>555</v>
+        <v>477</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>557</v>
+        <v>478</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>337</v>
+        <v>266</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>327</v>
+        <v>267</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>328</v>
+        <v>268</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>573</v>
+        <v>623</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>578</v>
+        <v>624</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>579</v>
+        <v>625</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>501</v>
+        <v>208</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>503</v>
+        <v>209</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>505</v>
+        <v>211</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>617</v>
+        <v>564</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>618</v>
+        <v>555</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>619</v>
+        <v>556</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>678</v>
+        <v>337</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>679</v>
+        <v>327</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>684</v>
+        <v>328</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>347</v>
+        <v>573</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>348</v>
+        <v>578</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="E194" s="1" t="s">
-        <v>350</v>
+        <v>579</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>548</v>
+        <v>501</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>549</v>
+        <v>503</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>550</v>
+        <v>505</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>37</v>
+        <v>771</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>58</v>
+        <v>772</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E196" s="1" t="s">
-        <v>38</v>
+        <v>773</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>585</v>
+        <v>617</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>442</v>
+        <v>618</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="E197" s="1" t="s">
-        <v>441</v>
+        <v>619</v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>663</v>
+        <v>678</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>658</v>
+        <v>679</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="E198" s="1" t="s">
-        <v>668</v>
+        <v>684</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>611</v>
+        <v>762</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>612</v>
+        <v>763</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>613</v>
+        <v>764</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>543</v>
+        <v>347</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>544</v>
+        <v>348</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>545</v>
+        <v>349</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>433</v>
+        <v>548</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>434</v>
+        <v>549</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="E201" s="1" t="s">
-        <v>436</v>
+        <v>550</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>271</v>
+        <v>37</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>269</v>
+        <v>58</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>270</v>
+        <v>97</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>171</v>
+        <v>585</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>172</v>
+        <v>442</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>173</v>
+        <v>443</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>670</v>
+        <v>658</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>426</v>
+        <v>759</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>427</v>
+        <v>760</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="E205" s="1" t="s">
-        <v>547</v>
+        <v>761</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>67</v>
+        <v>611</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>68</v>
+        <v>612</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E206" s="1" t="s">
-        <v>70</v>
+        <v>613</v>
       </c>
     </row>
     <row r="207" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>655</v>
+        <v>543</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C207" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A208" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A209" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A210" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A211" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A212" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A213" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A214" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C214" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="D207" s="1" t="s">
+      <c r="D214" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="E207" s="1" t="s">
+      <c r="E214" s="1" t="s">
         <v>662</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F207">
-      <sortCondition ref="A1:A207"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F214">
+      <sortCondition ref="A1:A214"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="F1:F1048576">

</xml_diff>

<commit_message>
Update to tracking sheet with m45 data
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F5BCD3-2C33-8F4E-800E-AF6C0947DCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8270D8-BBD7-8345-A419-0D3F326E4B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34900" yWindow="0" windowWidth="16300" windowHeight="28800" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="24300" yWindow="500" windowWidth="16300" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="786">
   <si>
     <t>M-Number</t>
   </si>
@@ -2427,6 +2427,21 @@
   </si>
   <si>
     <t>../resources/annotations.xml#psn-latr</t>
+  </si>
+  <si>
+    <t>M45. Anon. Holograph fragment, unsigned, dated Nov. 24, 1940. 9p.</t>
+  </si>
+  <si>
+    <t>m45</t>
+  </si>
+  <si>
+    <t>Cheapside</t>
+  </si>
+  <si>
+    <t>pla-chea</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-chea</t>
   </si>
 </sst>
 </file>
@@ -2840,7 +2855,7 @@
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A23" sqref="A23"/>
+      <selection pane="topRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2889,6 +2904,12 @@
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>782</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -3275,11 +3296,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F214"/>
+  <dimension ref="A1:F215"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D212" sqref="D212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6471,6 +6492,20 @@
         <v>662</v>
       </c>
     </row>
+    <row r="215" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A215" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F214">

</xml_diff>

<commit_message>
Updates to tracking sheet for m45 data
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8270D8-BBD7-8345-A419-0D3F326E4B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BD1C83-B435-5148-BDDD-7D0629F0A7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24300" yWindow="500" windowWidth="16300" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="8940" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="789">
   <si>
     <t>M-Number</t>
   </si>
@@ -2442,6 +2442,15 @@
   </si>
   <si>
     <t>../resources/annotations.xml#pla-chea</t>
+  </si>
+  <si>
+    <t>Cato</t>
+  </si>
+  <si>
+    <t>psn-cato</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-cato</t>
   </si>
 </sst>
 </file>
@@ -3296,11 +3305,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F215"/>
+  <dimension ref="A1:F216"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D212" sqref="D212"/>
+      <pane ySplit="1" topLeftCell="A201" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6506,6 +6515,20 @@
         <v>785</v>
       </c>
     </row>
+    <row r="216" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A216" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F214">

</xml_diff>

<commit_message>
m47.xml: p. 1 of 11
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA0C20F-CEF8-8344-9180-89CBF6051F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36754EDA-412B-9042-8D1D-A9381BAEC5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8940" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="8940" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="802">
   <si>
     <t>M-Number</t>
   </si>
@@ -2470,6 +2470,27 @@
   </si>
   <si>
     <t>../resources/annotations.xml#pla-durh</t>
+  </si>
+  <si>
+    <t>Yeats, William Butler</t>
+  </si>
+  <si>
+    <t>psn-yeat</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-yeat</t>
+  </si>
+  <si>
+    <t>M47 [Anon]. Holograph fragments, undated. Some pages paginated 1-3. 11p.</t>
+  </si>
+  <si>
+    <t>m47</t>
+  </si>
+  <si>
+    <t>transcriptions/m45.xml</t>
+  </si>
+  <si>
+    <t>transcriptions/m46.xml</t>
   </si>
 </sst>
 </file>
@@ -2881,9 +2902,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H5" sqref="H5"/>
+      <selection pane="topRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2928,7 +2949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -2938,6 +2959,9 @@
       <c r="C4" s="1" t="s">
         <v>782</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>800</v>
+      </c>
       <c r="F4" s="5">
         <v>10</v>
       </c>
@@ -2948,7 +2972,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2958,13 +2982,25 @@
       <c r="C5" s="1" t="s">
         <v>790</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>801</v>
+      </c>
       <c r="F5" s="5">
         <v>9</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3345,11 +3381,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F217"/>
+  <dimension ref="A1:F218"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D165" sqref="D165"/>
+    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6583,6 +6619,20 @@
         <v>794</v>
       </c>
     </row>
+    <row r="218" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A218" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>797</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F214">

</xml_diff>

<commit_message>
m47.xml: p. 3 of 11
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36754EDA-412B-9042-8D1D-A9381BAEC5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8895BFD9-D3AD-A34B-9CA9-788DDC861040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8940" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="803">
   <si>
     <t>M-Number</t>
   </si>
@@ -673,9 +673,6 @@
     <t>psn-easu</t>
   </si>
   <si>
-    <t>Mother of Earl of Surrey (psn-easu)</t>
-  </si>
-  <si>
     <t>../resources/annotations.xml#psn-easu</t>
   </si>
   <si>
@@ -686,9 +683,6 @@
   </si>
   <si>
     <t>Son of Lady Anne Bacon (psn-abac)</t>
-  </si>
-  <si>
-    <t>Henry Howard? Son of Duchess of Norfolk (psn-duno)</t>
   </si>
   <si>
     <t>Find way to render blank lines on p. 2 and p. 9</t>
@@ -2491,6 +2485,15 @@
   </si>
   <si>
     <t>transcriptions/m46.xml</t>
+  </si>
+  <si>
+    <t>Henry Howard? Son of Duchess of Norfolk (psn-duno). Note m47 gets relation wrong - calls her his wife</t>
+  </si>
+  <si>
+    <t>Mother of Earl of Surrey (psn-easu), Elizabeth Howard</t>
+  </si>
+  <si>
+    <t>Get second (third, fourth) etc on that line even the hivemind couldn't parse</t>
   </si>
 </sst>
 </file>
@@ -2904,7 +2907,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D5" sqref="D5"/>
+      <selection pane="topRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2935,7 +2938,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>33</v>
@@ -2954,13 +2957,13 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F4" s="5">
         <v>10</v>
@@ -2969,7 +2972,7 @@
         <v>34</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2977,19 +2980,22 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F5" s="5">
         <v>9</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>34</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2997,10 +3003,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3008,7 +3014,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>25</v>
@@ -3031,7 +3037,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>26</v>
@@ -3069,7 +3075,7 @@
         <v>34</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3077,7 +3083,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -3092,7 +3098,7 @@
         <v>34</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3100,13 +3106,13 @@
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>340</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>342</v>
       </c>
       <c r="F11" s="5">
         <v>19</v>
@@ -3120,13 +3126,13 @@
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>343</v>
       </c>
       <c r="F12" s="5">
         <v>26</v>
@@ -3135,7 +3141,7 @@
         <v>34</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -3143,13 +3149,13 @@
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F13" s="5">
         <v>35</v>
@@ -3163,13 +3169,13 @@
         <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F14" s="5">
         <v>7</v>
@@ -3183,13 +3189,13 @@
         <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>535</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>537</v>
       </c>
       <c r="F15" s="5">
         <v>9</v>
@@ -3198,7 +3204,7 @@
         <v>34</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3206,13 +3212,13 @@
         <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>552</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>554</v>
       </c>
       <c r="F16" s="5">
         <v>5</v>
@@ -3223,16 +3229,16 @@
     </row>
     <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F17" s="5">
         <v>5</v>
@@ -3243,16 +3249,16 @@
     </row>
     <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>593</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>594</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>595</v>
       </c>
       <c r="F18" s="5">
         <v>4</v>
@@ -3263,16 +3269,16 @@
     </row>
     <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="F19" s="5">
         <v>7</v>
@@ -3281,21 +3287,21 @@
         <v>34</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>637</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>638</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>639</v>
       </c>
       <c r="F20" s="5">
         <v>5</v>
@@ -3306,16 +3312,16 @@
     </row>
     <row r="21" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="F21" s="5">
         <v>2</v>
@@ -3324,21 +3330,21 @@
         <v>34</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="F22" s="5">
         <v>3</v>
@@ -3352,13 +3358,13 @@
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>756</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>757</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>758</v>
       </c>
       <c r="F23" s="5">
         <v>8</v>
@@ -3384,8 +3390,8 @@
   <dimension ref="A1:F218"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E121" sqref="E121"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E144" sqref="E144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3420,19 +3426,19 @@
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3454,58 +3460,58 @@
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3524,16 +3530,16 @@
     </row>
     <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3552,7 +3558,7 @@
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>30</v>
@@ -3566,19 +3572,19 @@
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>710</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3595,7 +3601,7 @@
         <v>113</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3612,77 +3618,77 @@
         <v>201</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>447</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3701,58 +3707,58 @@
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>649</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3774,72 +3780,72 @@
     </row>
     <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>504</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>750</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3900,7 +3906,7 @@
     </row>
     <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>47</v>
@@ -3928,30 +3934,30 @@
     </row>
     <row r="37" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3970,72 +3976,72 @@
     </row>
     <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>768</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>574</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4052,66 +4058,66 @@
         <v>104</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>648</v>
-      </c>
       <c r="D47" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4130,72 +4136,72 @@
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4214,115 +4220,115 @@
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C57" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>418</v>
-      </c>
       <c r="E58" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>701</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>702</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D62" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4341,16 +4347,16 @@
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4369,7 +4375,7 @@
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>43</v>
@@ -4383,165 +4389,165 @@
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>575</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>744</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>486</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>512</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -4560,72 +4566,72 @@
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4658,81 +4664,81 @@
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C88" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E91" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4754,205 +4760,205 @@
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>469</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C97" s="1" t="s">
+      <c r="E97" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C98" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="E98" s="1" t="s">
         <v>692</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>697</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="E99" s="1" t="s">
         <v>672</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C101" s="1" t="s">
+      <c r="E101" s="1" t="s">
         <v>508</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C102" s="1" t="s">
+      <c r="E102" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C103" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E103" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>589</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4971,114 +4977,114 @@
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="D107" s="1" t="s">
         <v>643</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>489</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>495</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>527</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>450</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C114" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>778</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5114,16 +5120,16 @@
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5142,44 +5148,44 @@
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D121" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5198,44 +5204,44 @@
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5257,47 +5263,47 @@
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C128" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>715</v>
       </c>
-      <c r="D128" s="1" t="s">
-        <v>717</v>
-      </c>
       <c r="E128" s="1" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C129" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="D129" s="1" t="s">
         <v>743</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5319,19 +5325,19 @@
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="B131" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C131" s="1" t="s">
+      <c r="E131" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5350,75 +5356,75 @@
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D134" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C137" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B137" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>246</v>
-      </c>
       <c r="D137" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5437,30 +5443,30 @@
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="D139" s="1" t="s">
         <v>722</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>723</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D140" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5479,16 +5485,16 @@
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5519,142 +5525,142 @@
         <v>207</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>210</v>
+        <v>801</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C146" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="E146" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="D148" s="1" t="s">
         <v>626</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C150" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="E150" s="1" t="s">
         <v>561</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C153" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E153" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5690,58 +5696,58 @@
     </row>
     <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D158" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C159" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E159" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5791,16 +5797,16 @@
     </row>
     <row r="163" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="D163" s="1" t="s">
         <v>596</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>597</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5822,58 +5828,58 @@
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D165" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5892,36 +5898,36 @@
     </row>
     <row r="170" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="D171" s="1" t="s">
         <v>718</v>
       </c>
-      <c r="B171" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C171" s="1" t="s">
+      <c r="E171" s="1" t="s">
         <v>719</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>720</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5954,112 +5960,112 @@
     </row>
     <row r="174" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="E174" s="1" t="s">
         <v>698</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="D174" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D177" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B177" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C177" s="1" t="s">
+      <c r="E177" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="D177" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D178" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="B178" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C178" s="1" t="s">
+      <c r="E178" s="1" t="s">
         <v>438</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="D179" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="B179" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C179" s="1" t="s">
+      <c r="E179" s="1" t="s">
         <v>567</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6078,19 +6084,19 @@
     </row>
     <row r="182" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="D182" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="B182" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C182" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="D182" s="1" t="s">
-        <v>494</v>
-      </c>
       <c r="E182" s="1" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6109,16 +6115,16 @@
     </row>
     <row r="184" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D184" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C184" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="D184" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6137,75 +6143,75 @@
     </row>
     <row r="186" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="E186" s="1" t="s">
         <v>686</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C186" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="D186" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="D187" s="1" t="s">
         <v>586</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C187" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="D187" s="1" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D189" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C189" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6219,156 +6225,156 @@
         <v>209</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>215</v>
+        <v>800</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C192" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="E192" s="1" t="s">
         <v>555</v>
-      </c>
-      <c r="D192" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="E192" s="1" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C195" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="B195" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C195" s="1" t="s">
+      <c r="D195" s="1" t="s">
         <v>503</v>
-      </c>
-      <c r="D195" s="1" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D200" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="B200" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C200" s="1" t="s">
+      <c r="E200" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="D200" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="E200" s="1" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6390,109 +6396,109 @@
     </row>
     <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="D204" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="E204" s="1" t="s">
         <v>666</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="207" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="208" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D208" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="B208" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C208" s="1" t="s">
+      <c r="E208" s="1" t="s">
         <v>434</v>
-      </c>
-      <c r="D208" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="E208" s="1" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="209" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6511,36 +6517,36 @@
     </row>
     <row r="211" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="D211" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="E211" s="1" t="s">
         <v>671</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="212" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D212" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="B212" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C212" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="D212" s="1" t="s">
-        <v>428</v>
-      </c>
       <c r="E212" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="213" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6562,75 +6568,75 @@
     </row>
     <row r="214" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C214" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E214" s="1" t="s">
         <v>660</v>
-      </c>
-      <c r="D214" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="E214" s="1" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="D216" s="1" t="s">
         <v>786</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C216" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="D216" s="1" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="218" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="D218" s="1" t="s">
         <v>795</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C218" s="1" t="s">
-        <v>796</v>
-      </c>
-      <c r="D218" s="1" t="s">
-        <v>797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to tracking sheet with m1-8-1 info
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E505270-D2A7-CD43-8BB2-FD81BD3B3946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7B2A5B-6D32-4C42-ACE2-0BB2B8384F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8920" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="8920" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="834">
   <si>
     <t>M-Number</t>
   </si>
@@ -521,9 +521,6 @@
   </si>
   <si>
     <t>../resources/annotations.xml#pla-dove</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#gawa</t>
   </si>
   <si>
     <t>Round Table</t>
@@ -2539,6 +2536,57 @@
   </si>
   <si>
     <t>transcriptions/m1-8-1.xml</t>
+  </si>
+  <si>
+    <t>Berwick, North</t>
+  </si>
+  <si>
+    <t>pla-nber</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-nber</t>
+  </si>
+  <si>
+    <t>Lothian</t>
+  </si>
+  <si>
+    <t>pla-loth</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-loth</t>
+  </si>
+  <si>
+    <t>cf. pla-nber, obj-pill, m1-8-1.4</t>
+  </si>
+  <si>
+    <t>Denbigh, Earl of</t>
+  </si>
+  <si>
+    <t>psn-denb</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-denb</t>
+  </si>
+  <si>
+    <t>Spanish Tragedy, The</t>
+  </si>
+  <si>
+    <t>lit-span</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-span</t>
+  </si>
+  <si>
+    <t>Holy Grail (Sang Gral)</t>
+  </si>
+  <si>
+    <t>obj-gral</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#obj-gral</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-gawa</t>
   </si>
 </sst>
 </file>
@@ -2950,7 +2998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G3" sqref="G3"/>
     </sheetView>
@@ -2983,7 +3031,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>31</v>
@@ -2994,16 +3042,16 @@
     </row>
     <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>816</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>817</v>
       </c>
       <c r="F3" s="5">
         <v>9</v>
@@ -3011,37 +3059,37 @@
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3049,13 +3097,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>777</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>778</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="F11" s="5">
         <v>10</v>
@@ -3064,7 +3112,7 @@
         <v>32</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3072,13 +3120,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>786</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F12" s="5">
         <v>9</v>
@@ -3087,7 +3135,7 @@
         <v>32</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3095,13 +3143,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>794</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>795</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="F13" s="5">
         <v>11</v>
@@ -3115,7 +3163,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>23</v>
@@ -3138,7 +3186,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>24</v>
@@ -3176,7 +3224,7 @@
         <v>32</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3184,7 +3232,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>26</v>
@@ -3199,7 +3247,7 @@
         <v>32</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3207,13 +3255,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F18" s="5">
         <v>19</v>
@@ -3227,13 +3275,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F19" s="5">
         <v>26</v>
@@ -3242,7 +3290,7 @@
         <v>32</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -3250,13 +3298,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>403</v>
       </c>
       <c r="F20" s="5">
         <v>35</v>
@@ -3270,13 +3318,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>441</v>
       </c>
       <c r="F21" s="5">
         <v>7</v>
@@ -3290,13 +3338,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>532</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>533</v>
       </c>
       <c r="F22" s="5">
         <v>9</v>
@@ -3305,7 +3353,7 @@
         <v>32</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3313,13 +3361,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>549</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>550</v>
       </c>
       <c r="F23" s="5">
         <v>5</v>
@@ -3330,16 +3378,16 @@
     </row>
     <row r="24" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>579</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>580</v>
       </c>
       <c r="F24" s="5">
         <v>5</v>
@@ -3350,16 +3398,16 @@
     </row>
     <row r="25" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>589</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>590</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>591</v>
       </c>
       <c r="F25" s="5">
         <v>4</v>
@@ -3370,16 +3418,16 @@
     </row>
     <row r="26" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>603</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>604</v>
       </c>
       <c r="F26" s="5">
         <v>7</v>
@@ -3388,21 +3436,21 @@
         <v>32</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>634</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>635</v>
       </c>
       <c r="F27" s="5">
         <v>5</v>
@@ -3413,16 +3461,16 @@
     </row>
     <row r="28" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>721</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>722</v>
       </c>
       <c r="F28" s="5">
         <v>2</v>
@@ -3431,21 +3479,21 @@
         <v>32</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>743</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>744</v>
       </c>
       <c r="F29" s="5">
         <v>3</v>
@@ -3459,13 +3507,13 @@
         <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>753</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>754</v>
       </c>
       <c r="F30" s="5">
         <v>8</v>
@@ -3476,7 +3524,7 @@
     </row>
     <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="H32" s="1" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
   </sheetData>
@@ -3493,11 +3541,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F219"/>
+  <dimension ref="A1:F224"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D163" sqref="D163"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3515,13 +3563,13 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
@@ -3532,19 +3580,19 @@
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>663</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3566,58 +3614,58 @@
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>750</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3636,35 +3684,35 @@
     </row>
     <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>28</v>
@@ -3678,19 +3726,19 @@
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>707</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>709</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3707,94 +3755,94 @@
         <v>111</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>450</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>444</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3813,58 +3861,58 @@
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>646</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>645</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>637</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3886,72 +3934,72 @@
     </row>
     <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>747</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3984,30 +4032,30 @@
     </row>
     <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>783</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4026,7 +4074,7 @@
     </row>
     <row r="36" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>45</v>
@@ -4054,44 +4102,44 @@
     </row>
     <row r="38" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>780</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>518</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>527</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4110,72 +4158,72 @@
     </row>
     <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>454</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>764</v>
-      </c>
       <c r="D43" s="1" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4192,66 +4240,66 @@
         <v>102</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>386</v>
-      </c>
       <c r="E48" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>642</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>626</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4270,72 +4318,72 @@
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>611</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>771</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>772</v>
-      </c>
       <c r="D55" s="1" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>480</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4354,129 +4402,129 @@
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>789</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>414</v>
-      </c>
       <c r="E61" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>535</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C63" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>698</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>703</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>244</v>
-      </c>
       <c r="E65" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>458</v>
-      </c>
       <c r="E66" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4495,35 +4543,35 @@
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C69" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>41</v>
@@ -4537,168 +4585,168 @@
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>677</v>
-      </c>
       <c r="D74" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C78" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>483</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C79" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>521</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C80" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>512</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>155</v>
       </c>
@@ -4709,77 +4757,77 @@
         <v>156</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>160</v>
+        <v>833</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>516</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C84" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>617</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C85" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C86" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C87" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4812,81 +4860,81 @@
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>537</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="E91" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>701</v>
-      </c>
       <c r="D92" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>704</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C94" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="E94" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4908,205 +4956,205 @@
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="E96" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C97" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>729</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C98" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>595</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C99" s="1" t="s">
+      <c r="D99" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="E100" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>687</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>688</v>
-      </c>
       <c r="D101" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C103" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C104" s="1" t="s">
+      <c r="D104" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="E104" s="1" t="s">
         <v>505</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C105" s="1" t="s">
+      <c r="D105" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="E105" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C106" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="E106" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B107" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>312</v>
-      </c>
       <c r="D107" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C108" s="1" t="s">
+      <c r="D108" s="1" t="s">
         <v>586</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5125,159 +5173,159 @@
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C110" s="1" t="s">
+      <c r="D110" s="1" t="s">
         <v>640</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C111" s="1" t="s">
+      <c r="D111" s="1" t="s">
         <v>486</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C112" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C113" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C114" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>599</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C115" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="B116" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C116" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>447</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>773</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>774</v>
-      </c>
       <c r="D117" s="1" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C119" s="1" t="s">
+      <c r="D119" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="E119" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B120" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C120" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5296,44 +5344,44 @@
     </row>
     <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C122" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C123" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="B124" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C124" s="1" t="s">
+      <c r="D124" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5352,44 +5400,44 @@
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="B126" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C126" s="1" t="s">
+      <c r="D126" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C127" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D127" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C128" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>476</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5411,47 +5459,47 @@
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C130" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="D130" s="1" t="s">
         <v>601</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C131" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="E131" s="1" t="s">
         <v>711</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5473,19 +5521,19 @@
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C134" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C134" s="1" t="s">
+      <c r="D134" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="E134" s="1" t="s">
         <v>427</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5504,131 +5552,131 @@
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>673</v>
-      </c>
       <c r="D136" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C137" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B137" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C137" s="1" t="s">
+      <c r="D137" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C138" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D138" s="1" t="s">
         <v>732</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C139" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="B139" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C139" s="1" t="s">
+      <c r="D139" s="1" t="s">
         <v>726</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D140" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B140" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="E140" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B141" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="D141" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C142" s="1" t="s">
         <v>718</v>
       </c>
-      <c r="B142" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C142" s="1" t="s">
+      <c r="D142" s="1" t="s">
         <v>719</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C143" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="B143" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C143" s="1" t="s">
+      <c r="D143" s="1" t="s">
         <v>803</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C144" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B144" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C144" s="1" t="s">
+      <c r="D144" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5647,16 +5695,16 @@
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C146" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B146" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C146" s="1" t="s">
+      <c r="D146" s="1" t="s">
         <v>391</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5675,154 +5723,154 @@
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C148" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B148" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C148" s="1" t="s">
+      <c r="D148" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D148" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="E148" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C149" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D149" s="1" t="s">
         <v>495</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C150" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="D150" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="D150" s="1" t="s">
+      <c r="E150" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C151" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="D151" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="D151" s="1" t="s">
-        <v>555</v>
-      </c>
       <c r="E151" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C152" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="B152" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C152" s="1" t="s">
+      <c r="D152" s="1" t="s">
         <v>623</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C153" s="1" t="s">
         <v>628</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C154" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="D154" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="D154" s="1" t="s">
+      <c r="E154" s="1" t="s">
         <v>558</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C155" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D155" s="1" t="s">
         <v>373</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C156" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D156" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C157" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D157" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D157" s="1" t="s">
+      <c r="E157" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5858,58 +5906,58 @@
     </row>
     <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C160" s="1" t="s">
         <v>529</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C161" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D161" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C162" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B162" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C162" s="1" t="s">
+      <c r="D162" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C163" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B163" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C163" s="1" t="s">
+      <c r="D163" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="D163" s="1" t="s">
+      <c r="E163" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="E163" s="1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5931,16 +5979,16 @@
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C165" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B165" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C165" s="1" t="s">
+      <c r="D165" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5959,16 +6007,16 @@
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C167" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="B167" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C167" s="1" t="s">
+      <c r="D167" s="1" t="s">
         <v>593</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5990,120 +6038,120 @@
     </row>
     <row r="169" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C169" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B169" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C169" s="1" t="s">
+      <c r="D169" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C170" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D170" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C171" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="D171" s="1" t="s">
         <v>735</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C172" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D172" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B173" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B173" s="1" t="s">
+      <c r="C173" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C173" s="1" t="s">
+      <c r="D173" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C175" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="B175" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C175" s="1" t="s">
+      <c r="D175" s="1" t="s">
         <v>715</v>
       </c>
-      <c r="D175" s="1" t="s">
+      <c r="E175" s="1" t="s">
         <v>716</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C176" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B176" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C176" s="1" t="s">
+      <c r="D176" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="D176" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6122,112 +6170,112 @@
     </row>
     <row r="178" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C178" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="B178" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C178" s="1" t="s">
+      <c r="D178" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="E178" s="1" t="s">
         <v>695</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>702</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C179" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D179" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C180" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D180" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C181" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B181" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C181" s="1" t="s">
+      <c r="D181" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D181" s="1" t="s">
+      <c r="E181" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C182" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="B182" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C182" s="1" t="s">
+      <c r="D182" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="D182" s="1" t="s">
+      <c r="E182" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C183" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="B183" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C183" s="1" t="s">
+      <c r="D183" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="D183" s="1" t="s">
+      <c r="E183" s="1" t="s">
         <v>564</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C184" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D184" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="D184" s="1" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6246,297 +6294,297 @@
     </row>
     <row r="186" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C186" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="B186" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C186" s="1" t="s">
+      <c r="D186" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="D186" s="1" t="s">
-        <v>490</v>
-      </c>
       <c r="E186" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C188" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B188" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C188" s="1" t="s">
+      <c r="D188" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="D188" s="1" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C189" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D189" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C190" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="B190" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C190" s="1" t="s">
+      <c r="D190" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="E190" s="1" t="s">
         <v>683</v>
-      </c>
-      <c r="D190" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C191" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="B191" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C191" s="1" t="s">
+      <c r="D191" s="1" t="s">
         <v>583</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C192" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="D192" s="1" t="s">
         <v>473</v>
-      </c>
-      <c r="D192" s="1" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C193" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B193" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C193" s="1" t="s">
+      <c r="D193" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="D193" s="1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C194" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="D194" s="1" t="s">
         <v>620</v>
-      </c>
-      <c r="D194" s="1" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C195" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B195" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C195" s="1" t="s">
+      <c r="D195" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="D195" s="1" t="s">
-        <v>208</v>
-      </c>
       <c r="E195" s="1" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C196" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="D196" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="D196" s="1" t="s">
+      <c r="E196" s="1" t="s">
         <v>552</v>
-      </c>
-      <c r="E196" s="1" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C197" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D197" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="D197" s="1" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C198" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="D198" s="1" t="s">
         <v>574</v>
-      </c>
-      <c r="D198" s="1" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C200" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="D200" s="1" t="s">
         <v>768</v>
-      </c>
-      <c r="D200" s="1" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C201" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="D201" s="1" t="s">
         <v>614</v>
-      </c>
-      <c r="D201" s="1" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C202" s="1" t="s">
         <v>674</v>
       </c>
-      <c r="B202" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C202" s="1" t="s">
-        <v>675</v>
-      </c>
       <c r="D202" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C203" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="D203" s="1" t="s">
         <v>759</v>
-      </c>
-      <c r="D203" s="1" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C204" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="B204" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C204" s="1" t="s">
+      <c r="D204" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="D204" s="1" t="s">
+      <c r="E204" s="1" t="s">
         <v>345</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C205" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D205" s="1" t="s">
         <v>545</v>
-      </c>
-      <c r="D205" s="1" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6558,157 +6606,157 @@
     </row>
     <row r="207" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C207" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D207" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="D207" s="1" t="s">
-        <v>439</v>
-      </c>
       <c r="E207" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="208" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="209" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C209" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D209" s="1" t="s">
         <v>756</v>
-      </c>
-      <c r="D209" s="1" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C210" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="D210" s="1" t="s">
         <v>608</v>
-      </c>
-      <c r="D210" s="1" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="211" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C211" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="D211" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="D211" s="1" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="212" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C212" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="B212" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C212" s="1" t="s">
+      <c r="D212" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="D212" s="1" t="s">
+      <c r="E212" s="1" t="s">
         <v>431</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="213" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C213" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D213" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="D213" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="214" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C214" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D214" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="D214" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C215" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="D215" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="D215" s="1" t="s">
-        <v>667</v>
-      </c>
       <c r="E215" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C216" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="B216" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C216" s="1" t="s">
+      <c r="D216" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="D216" s="1" t="s">
-        <v>424</v>
-      </c>
       <c r="E216" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6730,33 +6778,109 @@
     </row>
     <row r="218" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C218" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="B218" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C218" s="1" t="s">
+      <c r="D218" s="1" t="s">
         <v>792</v>
-      </c>
-      <c r="D218" s="1" t="s">
-        <v>793</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C219" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="D219" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="D219" s="1" t="s">
+      <c r="E219" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="E219" s="1" t="s">
-        <v>658</v>
+    </row>
+    <row r="220" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A220" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A221" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A222" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A223" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A224" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>832</v>
       </c>
     </row>
   </sheetData>
@@ -6765,6 +6889,7 @@
       <sortCondition ref="A1:A219"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Y"</formula>

</xml_diff>

<commit_message>
m1-8-1.xml: p. 7 of 9
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7B2A5B-6D32-4C42-ACE2-0BB2B8384F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864ACDC7-C0F9-2C4B-8AEB-BB18D724193C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8920" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="837">
   <si>
     <t>M-Number</t>
   </si>
@@ -2587,6 +2587,15 @@
   </si>
   <si>
     <t>../resources/annotations.xml#psn-gawa</t>
+  </si>
+  <si>
+    <t>Merlin</t>
+  </si>
+  <si>
+    <t>psn-merl</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-merl</t>
   </si>
 </sst>
 </file>
@@ -3541,11 +3550,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F224"/>
+  <dimension ref="A1:F225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D82" sqref="D82"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6881,6 +6890,20 @@
       </c>
       <c r="D224" s="1" t="s">
         <v>832</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A225" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>836</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
m1-8-2.xml: completed draft. Need to get a second pair of eyes on it...
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC149E7-A550-214E-839A-425A568F77C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A0A748-8580-6344-A087-3EC8B3442D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8920" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="843">
   <si>
     <t>M-Number</t>
   </si>
@@ -1442,9 +1442,6 @@
   </si>
   <si>
     <t>A pun at end of m108.4, cf. psn-cmar</t>
-  </si>
-  <si>
-    <t>Is this actually Edward IV??? I'm guessing based on Latimer and the c16th but then again… Check against quotes! </t>
   </si>
   <si>
     <t>Amesbury</t>
@@ -2605,6 +2602,18 @@
   </si>
   <si>
     <t>transcriptions/m1-8-2.xml</t>
+  </si>
+  <si>
+    <t>Edward VI</t>
+  </si>
+  <si>
+    <t>psn-edw6</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-edw6</t>
+  </si>
+  <si>
+    <t>Is this a mistake for Edward IV perhaps?</t>
   </si>
 </sst>
 </file>
@@ -3016,7 +3025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
@@ -3060,16 +3069,16 @@
     </row>
     <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>815</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>816</v>
       </c>
       <c r="F3" s="5">
         <v>9</v>
@@ -3080,16 +3089,16 @@
     </row>
     <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>838</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>839</v>
       </c>
       <c r="F4" s="5">
         <v>13</v>
@@ -3097,32 +3106,32 @@
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3130,13 +3139,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>777</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="F11" s="5">
         <v>10</v>
@@ -3145,7 +3154,7 @@
         <v>32</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3153,13 +3162,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>785</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="F12" s="5">
         <v>9</v>
@@ -3168,7 +3177,7 @@
         <v>32</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3176,13 +3185,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>794</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="F13" s="5">
         <v>11</v>
@@ -3371,13 +3380,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>531</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>532</v>
       </c>
       <c r="F22" s="5">
         <v>9</v>
@@ -3386,7 +3395,7 @@
         <v>32</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3394,13 +3403,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>548</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>549</v>
       </c>
       <c r="F23" s="5">
         <v>5</v>
@@ -3411,16 +3420,16 @@
     </row>
     <row r="24" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>578</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>579</v>
       </c>
       <c r="F24" s="5">
         <v>5</v>
@@ -3431,16 +3440,16 @@
     </row>
     <row r="25" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>589</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>590</v>
       </c>
       <c r="F25" s="5">
         <v>4</v>
@@ -3451,16 +3460,16 @@
     </row>
     <row r="26" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>602</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>603</v>
       </c>
       <c r="F26" s="5">
         <v>7</v>
@@ -3469,21 +3478,21 @@
         <v>32</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>633</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>634</v>
       </c>
       <c r="F27" s="5">
         <v>5</v>
@@ -3494,16 +3503,16 @@
     </row>
     <row r="28" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>720</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>721</v>
       </c>
       <c r="F28" s="5">
         <v>2</v>
@@ -3512,21 +3521,21 @@
         <v>32</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>742</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>743</v>
       </c>
       <c r="F29" s="5">
         <v>3</v>
@@ -3540,13 +3549,13 @@
         <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>751</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>752</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>753</v>
       </c>
       <c r="F30" s="5">
         <v>8</v>
@@ -3557,7 +3566,7 @@
     </row>
     <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="H32" s="1" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
   </sheetData>
@@ -3576,9 +3585,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
   <dimension ref="A1:F225"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I130" sqref="I130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3596,7 +3605,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>4</v>
@@ -3613,19 +3622,19 @@
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>662</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3675,30 +3684,30 @@
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>469</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>749</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>750</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3759,19 +3768,19 @@
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>705</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>706</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>708</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3922,30 +3931,30 @@
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>645</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>636</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3967,30 +3976,30 @@
     </row>
     <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>746</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -4079,16 +4088,16 @@
     </row>
     <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>781</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>782</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4135,44 +4144,44 @@
     </row>
     <row r="38" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>779</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>526</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4205,44 +4214,44 @@
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>762</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>763</v>
-      </c>
       <c r="D43" s="1" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4290,35 +4299,35 @@
         <v>385</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>641</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>643</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>625</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4365,44 +4374,44 @@
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>610</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>770</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>771</v>
-      </c>
       <c r="D55" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4435,16 +4444,16 @@
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>788</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4466,33 +4475,33 @@
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>411</v>
+        <v>839</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>412</v>
+        <v>840</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>413</v>
+        <v>841</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>467</v>
+        <v>842</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>534</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4511,19 +4520,19 @@
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>697</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>702</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4618,16 +4627,16 @@
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4646,30 +4655,30 @@
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>676</v>
-      </c>
       <c r="D74" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4688,95 +4697,95 @@
     </row>
     <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C78" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>482</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C79" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>520</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C80" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>511</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4790,35 +4799,35 @@
         <v>156</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C84" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>616</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4893,16 +4902,16 @@
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>536</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4924,19 +4933,19 @@
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>700</v>
-      </c>
       <c r="D92" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>703</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5006,30 +5015,30 @@
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C97" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>728</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C98" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>594</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5065,36 +5074,36 @@
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>687</v>
-      </c>
       <c r="D101" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5113,19 +5122,19 @@
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C104" s="1" t="s">
+      <c r="D104" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="E104" s="1" t="s">
         <v>504</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5178,16 +5187,16 @@
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C108" s="1" t="s">
+      <c r="D108" s="1" t="s">
         <v>585</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5206,44 +5215,44 @@
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C110" s="1" t="s">
+      <c r="D110" s="1" t="s">
         <v>639</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C111" s="1" t="s">
+      <c r="D111" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C112" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5262,30 +5271,30 @@
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C114" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>598</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C115" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>523</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5304,16 +5313,16 @@
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>773</v>
-      </c>
       <c r="D117" s="1" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5461,16 +5470,16 @@
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C128" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>475</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5492,47 +5501,47 @@
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C130" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D130" s="1" t="s">
         <v>600</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C131" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E131" s="1" t="s">
         <v>710</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5585,16 +5594,16 @@
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>671</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>672</v>
-      </c>
       <c r="D136" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5613,30 +5622,30 @@
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C138" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="D138" s="1" t="s">
         <v>731</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C139" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="D139" s="1" t="s">
         <v>725</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5672,30 +5681,30 @@
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C142" s="1" t="s">
         <v>717</v>
       </c>
-      <c r="B142" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C142" s="1" t="s">
+      <c r="D142" s="1" t="s">
         <v>718</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C143" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="B143" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C143" s="1" t="s">
+      <c r="D143" s="1" t="s">
         <v>802</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5768,21 +5777,21 @@
         <v>204</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C149" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="D149" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5804,61 +5813,61 @@
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C151" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="D151" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="D151" s="1" t="s">
-        <v>554</v>
-      </c>
       <c r="E151" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C152" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="B152" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C152" s="1" t="s">
+      <c r="D152" s="1" t="s">
         <v>622</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C153" s="1" t="s">
         <v>627</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C154" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="D154" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="D154" s="1" t="s">
+      <c r="E154" s="1" t="s">
         <v>557</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5939,13 +5948,13 @@
     </row>
     <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C160" s="1" t="s">
         <v>528</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6040,16 +6049,16 @@
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C167" s="1" t="s">
         <v>591</v>
       </c>
-      <c r="B167" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C167" s="1" t="s">
+      <c r="D167" s="1" t="s">
         <v>592</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6099,16 +6108,16 @@
     </row>
     <row r="171" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C171" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="D171" s="1" t="s">
         <v>734</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6141,36 +6150,36 @@
     </row>
     <row r="174" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C175" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="B175" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C175" s="1" t="s">
+      <c r="D175" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="D175" s="1" t="s">
+      <c r="E175" s="1" t="s">
         <v>715</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6203,19 +6212,19 @@
     </row>
     <row r="178" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C178" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="B178" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C178" s="1" t="s">
+      <c r="D178" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="E178" s="1" t="s">
         <v>694</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6282,19 +6291,19 @@
     </row>
     <row r="183" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C183" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="B183" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C183" s="1" t="s">
+      <c r="D183" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="D183" s="1" t="s">
+      <c r="E183" s="1" t="s">
         <v>563</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6327,19 +6336,19 @@
     </row>
     <row r="186" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C186" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="B186" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C186" s="1" t="s">
+      <c r="D186" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="D186" s="1" t="s">
-        <v>489</v>
-      </c>
       <c r="E186" s="1" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6386,47 +6395,47 @@
     </row>
     <row r="190" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C190" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="B190" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C190" s="1" t="s">
+      <c r="D190" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="E190" s="1" t="s">
         <v>682</v>
-      </c>
-      <c r="D190" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C191" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="B191" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C191" s="1" t="s">
+      <c r="D191" s="1" t="s">
         <v>582</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C192" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D192" s="1" t="s">
         <v>472</v>
-      </c>
-      <c r="D192" s="1" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6445,16 +6454,16 @@
     </row>
     <row r="194" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C194" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="D194" s="1" t="s">
         <v>619</v>
-      </c>
-      <c r="D194" s="1" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6471,24 +6480,24 @@
         <v>207</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C196" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D196" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="D196" s="1" t="s">
+      <c r="E196" s="1" t="s">
         <v>551</v>
-      </c>
-      <c r="E196" s="1" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6507,86 +6516,86 @@
     </row>
     <row r="198" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C198" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="D198" s="1" t="s">
         <v>573</v>
-      </c>
-      <c r="D198" s="1" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C200" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="D200" s="1" t="s">
         <v>767</v>
-      </c>
-      <c r="D200" s="1" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C201" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="D201" s="1" t="s">
         <v>613</v>
-      </c>
-      <c r="D201" s="1" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C202" s="1" t="s">
         <v>673</v>
       </c>
-      <c r="B202" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C202" s="1" t="s">
-        <v>674</v>
-      </c>
       <c r="D202" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C203" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="D203" s="1" t="s">
         <v>758</v>
-      </c>
-      <c r="D203" s="1" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6608,16 +6617,16 @@
     </row>
     <row r="205" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C205" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D205" s="1" t="s">
         <v>544</v>
-      </c>
-      <c r="D205" s="1" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6639,7 +6648,7 @@
     </row>
     <row r="207" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>28</v>
@@ -6656,61 +6665,61 @@
     </row>
     <row r="208" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="209" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C209" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="D209" s="1" t="s">
         <v>755</v>
-      </c>
-      <c r="D209" s="1" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C210" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="D210" s="1" t="s">
         <v>607</v>
-      </c>
-      <c r="D210" s="1" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="211" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C211" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="D211" s="1" t="s">
         <v>539</v>
-      </c>
-      <c r="D211" s="1" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="212" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6760,19 +6769,19 @@
     </row>
     <row r="215" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C215" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="D215" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="D215" s="1" t="s">
-        <v>666</v>
-      </c>
       <c r="E215" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6789,7 +6798,7 @@
         <v>423</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6811,123 +6820,123 @@
     </row>
     <row r="218" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C218" s="1" t="s">
         <v>790</v>
       </c>
-      <c r="B218" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C218" s="1" t="s">
+      <c r="D218" s="1" t="s">
         <v>791</v>
-      </c>
-      <c r="D218" s="1" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C219" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="D219" s="1" t="s">
         <v>655</v>
       </c>
-      <c r="D219" s="1" t="s">
+      <c r="E219" s="1" t="s">
         <v>656</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C220" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="D220" s="1" t="s">
         <v>818</v>
       </c>
-      <c r="D220" s="1" t="s">
-        <v>819</v>
-      </c>
       <c r="E220" s="1" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="221" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C221" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="D221" s="1" t="s">
         <v>821</v>
       </c>
-      <c r="D221" s="1" t="s">
+      <c r="E221" s="1" t="s">
         <v>822</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="222" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C222" s="1" t="s">
         <v>824</v>
       </c>
-      <c r="B222" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C222" s="1" t="s">
+      <c r="D222" s="1" t="s">
         <v>825</v>
-      </c>
-      <c r="D222" s="1" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C223" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="D223" s="1" t="s">
         <v>828</v>
-      </c>
-      <c r="D223" s="1" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C224" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="D224" s="1" t="s">
         <v>831</v>
-      </c>
-      <c r="D224" s="1" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C225" s="1" t="s">
         <v>834</v>
       </c>
-      <c r="B225" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C225" s="1" t="s">
+      <c r="D225" s="1" t="s">
         <v>835</v>
-      </c>
-      <c r="D225" s="1" t="s">
-        <v>836</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
m1-8-3.xml: p. 9 of 15
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD955C3-73F5-3644-B3E6-8D5151A91550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874297D5-8D71-A24A-AFE3-D94E89BBE495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="849">
   <si>
     <t>M-Number</t>
   </si>
@@ -2622,7 +2622,16 @@
     <t>m1-8-3</t>
   </si>
   <si>
-    <t>M1-8. 2 of 8. [Anon]. Holograph. In [Articles, essays, fiction and reviews], vol. 8 [1938-39], pp. 106-134. 15p.</t>
+    <t>M1-8. 3 of 8. [Anon: For the long poem is luminous, radiant...]. Holograph. In [Articles, essays, fiction and reviews], vol. 8 [1938-39], pp. 106-134. 15p.</t>
+  </si>
+  <si>
+    <t>Raleigh, Sir Walter</t>
+  </si>
+  <si>
+    <t>psn-wral</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-wral</t>
   </si>
 </sst>
 </file>
@@ -3034,9 +3043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B11" sqref="B11"/>
+      <selection pane="topRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3607,11 +3616,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F225"/>
+  <dimension ref="A1:F226"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E228" sqref="E228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6961,6 +6970,20 @@
       </c>
       <c r="D225" s="1" t="s">
         <v>835</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A226" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>848</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
m1-8-3.xml: p. 12 of 15
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874297D5-8D71-A24A-AFE3-D94E89BBE495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB448F96-9257-0845-AB00-2E7A59ACB5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="858">
   <si>
     <t>M-Number</t>
   </si>
@@ -2632,6 +2632,33 @@
   </si>
   <si>
     <t>../resources/annotations.xml#psn-wral</t>
+  </si>
+  <si>
+    <t>Swan, The</t>
+  </si>
+  <si>
+    <t>pla-swan</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-swan</t>
+  </si>
+  <si>
+    <t>Comedy of Errors</t>
+  </si>
+  <si>
+    <t>lit-come</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-come</t>
+  </si>
+  <si>
+    <t>Gray's Inn</t>
+  </si>
+  <si>
+    <t>pla-gray</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-gray</t>
   </si>
 </sst>
 </file>
@@ -3616,11 +3643,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F226"/>
+  <dimension ref="A1:F229"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E228" sqref="E228"/>
+      <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E238" sqref="E238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3922,3074 +3949,3116 @@
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>131</v>
+        <v>816</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>132</v>
+        <v>817</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>133</v>
+        <v>818</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>822</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>362</v>
+        <v>131</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>363</v>
+        <v>132</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>364</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>644</v>
+        <v>368</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>643</v>
+        <v>369</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>645</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>634</v>
+        <v>644</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>635</v>
+        <v>643</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>636</v>
+        <v>645</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>82</v>
+        <v>634</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>83</v>
+        <v>635</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>85</v>
+        <v>636</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>496</v>
+        <v>82</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>498</v>
+        <v>83</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>500</v>
+        <v>84</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>365</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>366</v>
+        <v>228</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>367</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>224</v>
+        <v>365</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>225</v>
+        <v>366</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>226</v>
+        <v>367</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>142</v>
+        <v>224</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>140</v>
+        <v>226</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>142</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>50</v>
+        <v>141</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>173</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>174</v>
+        <v>50</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>177</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>780</v>
+        <v>173</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>781</v>
+        <v>174</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>782</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>143</v>
+        <v>780</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>144</v>
+        <v>781</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>145</v>
+        <v>782</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>349</v>
+        <v>143</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>33</v>
+        <v>349</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>777</v>
+        <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>778</v>
+        <v>51</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>779</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>513</v>
+        <v>777</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>516</v>
+        <v>778</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>517</v>
+        <v>779</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>524</v>
+        <v>513</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>525</v>
+        <v>516</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>79</v>
+        <v>524</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>80</v>
+        <v>525</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>81</v>
+        <v>526</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>452</v>
+        <v>79</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>453</v>
+        <v>80</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>454</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>761</v>
+        <v>452</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>762</v>
+        <v>453</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>764</v>
+        <v>454</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>564</v>
+        <v>760</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>568</v>
+        <v>759</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>570</v>
+        <v>763</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>230</v>
+        <v>564</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>231</v>
+        <v>568</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>232</v>
+        <v>570</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>101</v>
+        <v>231</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>383</v>
+        <v>100</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>384</v>
+        <v>101</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>385</v>
+        <v>102</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>476</v>
+        <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>640</v>
+        <v>383</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>642</v>
+        <v>384</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>641</v>
+        <v>385</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>623</v>
+        <v>640</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>624</v>
+        <v>642</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>625</v>
+        <v>641</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>236</v>
+        <v>623</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>237</v>
+        <v>624</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>238</v>
+        <v>625</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>38</v>
+        <v>236</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>52</v>
+        <v>237</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>93</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>304</v>
+        <v>38</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>305</v>
+        <v>52</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>306</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>608</v>
+        <v>304</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>609</v>
+        <v>305</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>610</v>
+        <v>306</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>769</v>
+        <v>608</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>770</v>
+        <v>609</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>773</v>
+        <v>610</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>477</v>
+        <v>769</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>478</v>
+        <v>770</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>479</v>
+        <v>773</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>359</v>
+        <v>823</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>360</v>
+        <v>824</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>361</v>
+        <v>825</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>157</v>
+        <v>477</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>158</v>
+        <v>478</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>159</v>
+        <v>479</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>786</v>
+        <v>359</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>787</v>
+        <v>360</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>788</v>
+        <v>361</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>411</v>
+        <v>157</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>412</v>
+        <v>158</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>414</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>839</v>
+        <v>786</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>840</v>
+        <v>787</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>841</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>842</v>
+        <v>788</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>532</v>
+        <v>411</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>533</v>
+        <v>412</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>534</v>
+        <v>413</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>258</v>
+        <v>839</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>259</v>
+        <v>840</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>260</v>
+        <v>841</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>842</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>695</v>
+        <v>532</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>696</v>
+        <v>533</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>697</v>
+        <v>534</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>455</v>
+        <v>695</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>456</v>
+        <v>696</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>457</v>
+        <v>701</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>462</v>
+        <v>697</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>137</v>
+        <v>244</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>138</v>
+        <v>242</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>139</v>
+        <v>243</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>312</v>
+        <v>455</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>313</v>
+        <v>456</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>315</v>
+        <v>457</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>189</v>
+        <v>137</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>161</v>
+        <v>45</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>190</v>
+        <v>138</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>247</v>
+        <v>312</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>112</v>
+        <v>313</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>113</v>
+        <v>315</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>565</v>
+        <v>189</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>569</v>
+        <v>190</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>571</v>
+        <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>319</v>
+        <v>247</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>320</v>
+        <v>112</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>321</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>736</v>
+        <v>565</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>738</v>
+        <v>569</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>740</v>
+        <v>571</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>674</v>
+        <v>319</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>675</v>
+        <v>320</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>679</v>
+        <v>321</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>398</v>
+        <v>736</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>399</v>
+        <v>738</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>400</v>
+        <v>740</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>646</v>
+        <v>674</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>651</v>
+        <v>675</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>662</v>
+        <v>679</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>647</v>
+        <v>398</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>650</v>
+        <v>399</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>662</v>
+        <v>400</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>480</v>
+        <v>646</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>481</v>
+        <v>651</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>482</v>
+        <v>658</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>518</v>
+        <v>647</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>519</v>
+        <v>650</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>520</v>
+        <v>659</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>509</v>
+        <v>480</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>510</v>
+        <v>481</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>511</v>
+        <v>482</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>507</v>
+        <v>518</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>506</v>
+        <v>519</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>508</v>
+        <v>520</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>155</v>
+        <v>509</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>156</v>
+        <v>510</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>832</v>
+        <v>511</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>515</v>
+        <v>505</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>614</v>
+        <v>155</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>615</v>
+        <v>156</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>616</v>
+        <v>832</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>298</v>
+        <v>512</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>299</v>
+        <v>514</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>300</v>
+        <v>515</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>405</v>
+        <v>614</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>406</v>
+        <v>615</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>407</v>
+        <v>616</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>405</v>
+        <v>298</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>406</v>
+        <v>299</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>407</v>
+        <v>300</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>106</v>
+        <v>405</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>107</v>
+        <v>406</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>108</v>
+        <v>407</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>34</v>
+        <v>405</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>53</v>
+        <v>406</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>87</v>
+        <v>407</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>540</v>
+        <v>106</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>535</v>
+        <v>107</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>536</v>
+        <v>108</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>448</v>
+        <v>34</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>392</v>
+        <v>53</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>394</v>
+        <v>87</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>698</v>
+        <v>540</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>699</v>
+        <v>535</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>702</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>703</v>
+        <v>536</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>324</v>
+        <v>448</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>325</v>
+        <v>392</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>326</v>
+        <v>393</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>267</v>
+        <v>698</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>268</v>
+        <v>699</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>269</v>
+        <v>702</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>270</v>
+        <v>703</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>42</v>
+        <v>324</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>57</v>
+        <v>325</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>43</v>
+        <v>326</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>463</v>
+        <v>267</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>464</v>
+        <v>268</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>465</v>
+        <v>269</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>466</v>
+        <v>270</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>726</v>
+        <v>42</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>727</v>
+        <v>57</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>728</v>
+        <v>88</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>596</v>
+        <v>463</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>593</v>
+        <v>464</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>594</v>
+        <v>465</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>221</v>
+        <v>726</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>222</v>
+        <v>727</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>223</v>
+        <v>728</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>287</v>
+        <v>596</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>288</v>
+        <v>593</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>290</v>
+        <v>594</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>685</v>
+        <v>221</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>686</v>
+        <v>222</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>688</v>
+        <v>223</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>666</v>
+        <v>287</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>669</v>
+        <v>288</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>676</v>
+        <v>289</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>668</v>
+        <v>290</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>346</v>
+        <v>685</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>347</v>
+        <v>686</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>348</v>
+        <v>691</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>688</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>501</v>
+        <v>666</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>502</v>
+        <v>669</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>503</v>
+        <v>676</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>504</v>
+        <v>668</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>213</v>
+        <v>346</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>214</v>
+        <v>347</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>216</v>
+        <v>348</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>217</v>
+        <v>501</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>218</v>
+        <v>502</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>219</v>
+        <v>503</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>220</v>
+        <v>504</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>310</v>
+        <v>213</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>311</v>
+        <v>214</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>314</v>
+        <v>215</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>583</v>
+        <v>217</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>584</v>
+        <v>218</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>585</v>
+        <v>219</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>103</v>
+        <v>829</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>104</v>
+        <v>830</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>105</v>
+        <v>831</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>637</v>
+        <v>310</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>638</v>
+        <v>311</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>639</v>
+        <v>314</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>483</v>
+        <v>583</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>484</v>
+        <v>584</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>485</v>
+        <v>585</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>489</v>
+        <v>103</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>490</v>
+        <v>104</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>491</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>291</v>
+        <v>637</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>285</v>
+        <v>638</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>286</v>
+        <v>639</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>595</v>
+        <v>483</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>597</v>
+        <v>484</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>598</v>
+        <v>485</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>521</v>
+        <v>489</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>522</v>
+        <v>490</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>523</v>
+        <v>491</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>445</v>
+        <v>291</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>446</v>
+        <v>285</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>447</v>
+        <v>286</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>771</v>
+        <v>595</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>772</v>
+        <v>597</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>774</v>
+        <v>598</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>171</v>
+        <v>521</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>187</v>
+        <v>522</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>172</v>
+        <v>523</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>192</v>
+        <v>445</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>193</v>
+        <v>446</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>195</v>
+        <v>447</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>292</v>
+        <v>771</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>293</v>
+        <v>772</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>294</v>
+        <v>774</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>350</v>
+        <v>192</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>351</v>
+        <v>193</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>352</v>
+        <v>194</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>376</v>
+        <v>292</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>327</v>
+        <v>293</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>328</v>
+        <v>294</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>418</v>
+        <v>146</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>419</v>
+        <v>147</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>420</v>
+        <v>148</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>97</v>
+        <v>350</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>98</v>
+        <v>351</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>99</v>
+        <v>352</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>396</v>
+        <v>327</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>397</v>
+        <v>328</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>295</v>
+        <v>418</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>296</v>
+        <v>419</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>297</v>
+        <v>420</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>473</v>
+        <v>97</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>474</v>
+        <v>98</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>475</v>
+        <v>99</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>60</v>
+        <v>395</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>61</v>
+        <v>396</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>62</v>
+        <v>397</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>566</v>
+        <v>295</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>599</v>
+        <v>296</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>600</v>
+        <v>297</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>708</v>
+        <v>819</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>709</v>
+        <v>820</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>711</v>
+        <v>821</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>710</v>
+        <v>822</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>735</v>
+        <v>473</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>737</v>
+        <v>474</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>739</v>
+        <v>475</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>149</v>
+        <v>60</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>150</v>
+        <v>61</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>151</v>
+        <v>64</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>152</v>
+        <v>62</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>424</v>
+        <v>566</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>425</v>
+        <v>599</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>427</v>
+        <v>600</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>48</v>
+        <v>708</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>59</v>
+        <v>709</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>89</v>
+        <v>711</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>670</v>
+        <v>735</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>671</v>
+        <v>737</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>677</v>
+        <v>739</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>271</v>
+        <v>149</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>272</v>
+        <v>150</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>273</v>
+        <v>151</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>729</v>
+        <v>424</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>730</v>
+        <v>425</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>731</v>
+        <v>426</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>723</v>
+        <v>48</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>724</v>
+        <v>59</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>725</v>
+        <v>89</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>239</v>
+        <v>670</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>241</v>
+        <v>671</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>246</v>
+        <v>677</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>185</v>
+        <v>833</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>186</v>
+        <v>834</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>188</v>
+        <v>835</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>716</v>
+        <v>271</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>717</v>
+        <v>272</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>718</v>
+        <v>273</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>800</v>
+        <v>729</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>801</v>
+        <v>730</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>802</v>
+        <v>731</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>233</v>
+        <v>723</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>234</v>
+        <v>724</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>235</v>
+        <v>725</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>37</v>
+        <v>239</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>54</v>
+        <v>241</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>90</v>
+        <v>240</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>389</v>
+        <v>185</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>390</v>
+        <v>186</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>391</v>
+        <v>188</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>128</v>
+        <v>716</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>129</v>
+        <v>717</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>130</v>
+        <v>718</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>202</v>
+        <v>800</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>203</v>
+        <v>801</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>797</v>
+        <v>802</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>492</v>
+        <v>233</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>493</v>
+        <v>234</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>494</v>
+        <v>235</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>458</v>
+        <v>37</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>459</v>
+        <v>54</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>461</v>
+        <v>90</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>559</v>
+        <v>389</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>552</v>
+        <v>390</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>551</v>
+        <v>391</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>620</v>
+        <v>128</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>621</v>
+        <v>129</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>626</v>
+        <v>202</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>627</v>
+        <v>203</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>554</v>
+        <v>492</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>555</v>
+        <v>493</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>557</v>
+        <v>494</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>371</v>
+        <v>458</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>372</v>
+        <v>459</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>373</v>
+        <v>460</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>356</v>
+        <v>559</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>357</v>
+        <v>552</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>358</v>
+        <v>553</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>280</v>
+        <v>620</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>277</v>
+        <v>621</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>124</v>
+        <v>626</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>127</v>
+        <v>627</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>134</v>
+        <v>554</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>135</v>
+        <v>555</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>136</v>
+        <v>556</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>527</v>
+        <v>371</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>528</v>
+        <v>372</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>251</v>
+        <v>356</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>252</v>
+        <v>357</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>253</v>
+        <v>358</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>249</v>
+        <v>277</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>250</v>
+        <v>278</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>281</v>
+        <v>124</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>282</v>
+        <v>125</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>283</v>
+        <v>126</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>284</v>
+        <v>127</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>75</v>
+        <v>134</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>164</v>
+        <v>527</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>166</v>
+        <v>528</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>55</v>
+        <v>252</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>91</v>
+        <v>253</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>590</v>
+        <v>248</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>591</v>
+        <v>249</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>592</v>
+        <v>250</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>44</v>
+        <v>281</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>70</v>
+        <v>282</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>92</v>
+        <v>283</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>46</v>
+        <v>284</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>274</v>
+        <v>75</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>275</v>
+        <v>76</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>276</v>
+        <v>77</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>353</v>
+        <v>164</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>354</v>
+        <v>165</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>355</v>
+        <v>166</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>732</v>
+        <v>39</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>733</v>
+        <v>55</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>734</v>
+        <v>91</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>301</v>
+        <v>590</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>302</v>
+        <v>591</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>303</v>
+        <v>592</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>160</v>
+        <v>44</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>161</v>
+        <v>45</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>162</v>
+        <v>70</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>684</v>
+        <v>846</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>683</v>
+        <v>847</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>687</v>
+        <v>848</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>712</v>
+        <v>274</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>713</v>
+        <v>275</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>715</v>
+        <v>276</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>199</v>
+        <v>353</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>200</v>
+        <v>354</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>201</v>
+        <v>355</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>47</v>
+        <v>732</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>58</v>
+        <v>733</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>94</v>
+        <v>734</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>692</v>
+        <v>301</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>693</v>
+        <v>302</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>694</v>
+        <v>303</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>415</v>
+        <v>160</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>416</v>
+        <v>162</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>415</v>
+        <v>684</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>416</v>
+        <v>683</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>417</v>
+        <v>690</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>687</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>254</v>
+        <v>712</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>255</v>
+        <v>713</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>256</v>
+        <v>714</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>257</v>
+        <v>715</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>432</v>
+        <v>199</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>433</v>
+        <v>200</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>435</v>
+        <v>201</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>560</v>
+        <v>47</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>561</v>
+        <v>58</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>563</v>
+        <v>94</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>307</v>
+        <v>692</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>308</v>
+        <v>693</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>309</v>
+        <v>700</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>114</v>
+        <v>415</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>115</v>
+        <v>416</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>116</v>
+        <v>417</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>486</v>
+        <v>415</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>487</v>
+        <v>416</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>768</v>
+        <v>417</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>175</v>
+        <v>254</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>176</v>
+        <v>255</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>178</v>
+        <v>256</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>316</v>
+        <v>432</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>317</v>
+        <v>433</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>318</v>
+        <v>434</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>182</v>
+        <v>560</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>183</v>
+        <v>561</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>184</v>
+        <v>562</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>680</v>
+        <v>307</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>681</v>
+        <v>308</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>682</v>
+        <v>309</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>580</v>
+        <v>826</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>581</v>
+        <v>827</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>582</v>
+        <v>828</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>470</v>
+        <v>114</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>471</v>
+        <v>115</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>472</v>
+        <v>116</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>261</v>
+        <v>486</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>262</v>
+        <v>487</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>263</v>
+        <v>488</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>617</v>
+        <v>175</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>618</v>
+        <v>176</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>619</v>
+        <v>178</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>205</v>
+        <v>316</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>206</v>
+        <v>317</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E195" s="1" t="s">
-        <v>796</v>
+        <v>318</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>558</v>
+        <v>182</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>549</v>
+        <v>183</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="E196" s="1" t="s">
-        <v>551</v>
+        <v>184</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>332</v>
+        <v>680</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>322</v>
+        <v>681</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>323</v>
+        <v>689</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>567</v>
+        <v>580</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>572</v>
+        <v>581</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>573</v>
+        <v>582</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>495</v>
+        <v>470</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>497</v>
+        <v>471</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>499</v>
+        <v>472</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>765</v>
+        <v>261</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>766</v>
+        <v>262</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>767</v>
+        <v>263</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>611</v>
+        <v>617</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>612</v>
+        <v>618</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>613</v>
+        <v>619</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>672</v>
+        <v>205</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>673</v>
+        <v>206</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>678</v>
+        <v>207</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>796</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>756</v>
+        <v>558</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>757</v>
+        <v>549</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>758</v>
+        <v>550</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>343</v>
+        <v>322</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>345</v>
+        <v>323</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>542</v>
+        <v>567</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>543</v>
+        <v>572</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>544</v>
+        <v>573</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>35</v>
+        <v>495</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>56</v>
+        <v>497</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E206" s="1" t="s">
-        <v>36</v>
+        <v>499</v>
       </c>
     </row>
     <row r="207" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>579</v>
+        <v>765</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>437</v>
+        <v>766</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="E207" s="1" t="s">
-        <v>436</v>
+        <v>767</v>
       </c>
     </row>
     <row r="208" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>657</v>
+        <v>611</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>652</v>
+        <v>612</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>660</v>
-      </c>
-      <c r="E208" s="1" t="s">
-        <v>662</v>
+        <v>613</v>
       </c>
     </row>
     <row r="209" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>753</v>
+        <v>672</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>754</v>
+        <v>673</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>755</v>
+        <v>678</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>605</v>
+        <v>756</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>606</v>
+        <v>757</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>607</v>
+        <v>758</v>
       </c>
     </row>
     <row r="211" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>537</v>
+        <v>342</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>538</v>
+        <v>343</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>539</v>
+        <v>344</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="212" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>428</v>
+        <v>542</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>429</v>
+        <v>543</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>431</v>
+        <v>544</v>
       </c>
     </row>
     <row r="213" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>266</v>
+        <v>35</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>264</v>
+        <v>56</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>265</v>
+        <v>95</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="214" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>168</v>
+        <v>579</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>169</v>
+        <v>437</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>170</v>
+        <v>438</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>664</v>
+        <v>652</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>421</v>
+        <v>753</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>422</v>
+        <v>754</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>541</v>
+        <v>755</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>65</v>
+        <v>605</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>66</v>
+        <v>606</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E217" s="1" t="s">
-        <v>68</v>
+        <v>607</v>
       </c>
     </row>
     <row r="218" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>789</v>
+        <v>537</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>790</v>
+        <v>538</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>791</v>
+        <v>539</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>649</v>
+        <v>428</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>654</v>
+        <v>429</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>655</v>
+        <v>430</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>656</v>
+        <v>431</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>816</v>
+        <v>266</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>817</v>
+        <v>264</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>818</v>
-      </c>
-      <c r="E220" s="1" t="s">
-        <v>822</v>
+        <v>265</v>
       </c>
     </row>
     <row r="221" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>819</v>
+        <v>168</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>820</v>
+        <v>169</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>821</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>822</v>
+        <v>170</v>
       </c>
     </row>
     <row r="222" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>823</v>
+        <v>663</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>824</v>
+        <v>664</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>825</v>
+        <v>665</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>826</v>
+        <v>421</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>827</v>
+        <v>422</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>828</v>
+        <v>423</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>829</v>
+        <v>65</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>830</v>
+        <v>66</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>833</v>
+        <v>789</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>834</v>
+        <v>790</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>846</v>
+        <v>649</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>847</v>
+        <v>654</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>848</v>
+        <v>655</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A227" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A228" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A229" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>857</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F219">
-      <sortCondition ref="A1:A219"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F226">
+      <sortCondition ref="A1:A226"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
m1-8-4.1 p. 1 of 9
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD8DC9D-997A-E840-8C47-862F27731D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3370395-3CD9-9045-B550-93274C4C3B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Annotations!$A$1:$F$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="862">
   <si>
     <t>M-Number</t>
   </si>
@@ -2668,6 +2667,9 @@
   </si>
   <si>
     <t>transcriptions/m1-8-4.xml</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-wpem</t>
   </si>
 </sst>
 </file>
@@ -3079,9 +3081,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7"/>
+      <selection pane="topRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3669,9 +3671,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
   <dimension ref="A1:F229"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6115,6 +6117,9 @@
       </c>
       <c r="C165" s="1" t="s">
         <v>527</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>861</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
m1-8-4.xml: p. 4 of 9
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3370395-3CD9-9045-B550-93274C4C3B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D0D402-A1DD-3545-BA87-C08925C5EAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Annotations" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Annotations!$A$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Annotations!$A$1:$F$229</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2492,9 +2492,6 @@
     <t>../resources/annotations.xml#psn-wmor</t>
   </si>
   <si>
-    <t>trea</t>
-  </si>
-  <si>
     <t>transcriptions/m47.xml</t>
   </si>
   <si>
@@ -2670,6 +2667,9 @@
   </si>
   <si>
     <t>../resources/annotations.xml#psn-wpem</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -3125,16 +3125,16 @@
     </row>
     <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>813</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>814</v>
       </c>
       <c r="F3" s="5">
         <v>9</v>
@@ -3145,16 +3145,16 @@
     </row>
     <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>835</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>836</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>837</v>
       </c>
       <c r="F4" s="5">
         <v>12</v>
@@ -3165,16 +3165,16 @@
     </row>
     <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="F5" s="5">
         <v>15</v>
@@ -3185,16 +3185,16 @@
     </row>
     <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>858</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>859</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>860</v>
       </c>
       <c r="F6" s="5">
         <v>9</v>
@@ -3202,22 +3202,22 @@
     </row>
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3277,7 +3277,7 @@
         <v>792</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F13" s="5">
         <v>11</v>
@@ -3672,8 +3672,8 @@
   <dimension ref="A1:F229"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E165" sqref="E165"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3691,7 +3691,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>802</v>
+        <v>861</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>4</v>
@@ -3975,19 +3975,19 @@
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>817</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4505,16 +4505,16 @@
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>823</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4592,19 +4592,19 @@
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C63" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>839</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>840</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4916,7 +4916,7 @@
         <v>156</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5127,7 +5127,7 @@
         <v>465</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5290,16 +5290,16 @@
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C109" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>829</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5601,19 +5601,19 @@
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C131" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>819</v>
       </c>
-      <c r="D131" s="1" t="s">
+      <c r="E131" s="1" t="s">
         <v>820</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5756,16 +5756,16 @@
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="B141" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C141" s="1" t="s">
+      <c r="D141" s="1" t="s">
         <v>833</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6119,7 +6119,7 @@
         <v>527</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6245,16 +6245,16 @@
     </row>
     <row r="174" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C174" s="1" t="s">
         <v>845</v>
       </c>
-      <c r="B174" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C174" s="1" t="s">
+      <c r="D174" s="1" t="s">
         <v>846</v>
-      </c>
-      <c r="D174" s="1" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6501,16 +6501,16 @@
     </row>
     <row r="191" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C191" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="D191" s="1" t="s">
         <v>826</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7044,48 +7044,48 @@
     </row>
     <row r="227" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C227" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="D227" s="1" t="s">
         <v>849</v>
-      </c>
-      <c r="D227" s="1" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="228" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C228" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="D228" s="1" t="s">
         <v>852</v>
-      </c>
-      <c r="D228" s="1" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="229" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C229" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="D229" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="D229" s="1" t="s">
-        <v>856</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F27" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
+  <autoFilter ref="A1:F229" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F226">
       <sortCondition ref="A1:A226"/>
     </sortState>

</xml_diff>

<commit_message>
m1-8-4.xml: p. 5 of 9
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D0D402-A1DD-3545-BA87-C08925C5EAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF460A3-0463-E949-9B5B-21E99EC76782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -3672,8 +3672,8 @@
   <dimension ref="A1:F229"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
m1-8-4.xml: p. 9 of 9
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF460A3-0463-E949-9B5B-21E99EC76782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B736873-4339-384E-8B9C-CE7E28F5AFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
     <sheet name="Annotations" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Annotations!$A$1:$F$229</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Annotations!$A$1:$F$230</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="867">
   <si>
     <t>M-Number</t>
   </si>
@@ -2670,6 +2670,21 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Beethoven, Ludwig van</t>
+  </si>
+  <si>
+    <t>psn-lvbe</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-lbve</t>
+  </si>
+  <si>
+    <t>cf. lit-fide</t>
+  </si>
+  <si>
+    <t>cf. psn-lbve</t>
   </si>
 </sst>
 </file>
@@ -3081,7 +3096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G7" sqref="G7"/>
     </sheetView>
@@ -3199,6 +3214,9 @@
       <c r="F6" s="5">
         <v>9</v>
       </c>
+      <c r="G6" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -3669,11 +3687,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F229"/>
+  <dimension ref="A1:F230"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D78" sqref="D78"/>
+    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E240" sqref="E240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4421,426 +4439,426 @@
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>622</v>
+        <v>850</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>161</v>
+        <v>41</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>623</v>
+        <v>851</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>624</v>
+        <v>852</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>236</v>
+        <v>622</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>237</v>
+        <v>623</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>238</v>
+        <v>624</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>38</v>
+        <v>236</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>52</v>
+        <v>237</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>93</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>304</v>
+        <v>38</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>305</v>
+        <v>52</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>306</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>607</v>
+        <v>304</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>608</v>
+        <v>305</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>609</v>
+        <v>306</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>768</v>
+        <v>607</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>769</v>
+        <v>608</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>772</v>
+        <v>609</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>821</v>
+        <v>768</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>822</v>
+        <v>769</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>823</v>
+        <v>772</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>476</v>
+        <v>821</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>477</v>
+        <v>822</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>478</v>
+        <v>823</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>157</v>
+        <v>359</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>158</v>
+        <v>360</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>159</v>
+        <v>361</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>785</v>
+        <v>157</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>786</v>
+        <v>158</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>787</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>411</v>
+        <v>785</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>412</v>
+        <v>786</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>414</v>
+        <v>787</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>837</v>
+        <v>411</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>838</v>
+        <v>412</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>839</v>
+        <v>413</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>840</v>
+        <v>414</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>531</v>
+        <v>837</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>532</v>
+        <v>838</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>533</v>
+        <v>839</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>840</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>258</v>
+        <v>531</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>259</v>
+        <v>532</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>260</v>
+        <v>533</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>694</v>
+        <v>258</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>695</v>
+        <v>259</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>696</v>
+        <v>260</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>244</v>
+        <v>694</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>242</v>
+        <v>695</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>243</v>
+        <v>700</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>245</v>
+        <v>696</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>455</v>
+        <v>244</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>456</v>
+        <v>242</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>457</v>
+        <v>243</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>462</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>137</v>
+        <v>455</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>138</v>
+        <v>456</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>139</v>
+        <v>457</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>312</v>
+        <v>137</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>313</v>
+        <v>138</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>315</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>189</v>
+        <v>312</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>161</v>
+        <v>41</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>190</v>
+        <v>313</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>191</v>
+        <v>315</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>247</v>
+        <v>189</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>112</v>
+        <v>190</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>113</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>564</v>
+        <v>247</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>568</v>
+        <v>112</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>570</v>
+        <v>113</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>319</v>
+        <v>564</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>320</v>
+        <v>568</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>321</v>
+        <v>570</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>735</v>
+        <v>319</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>737</v>
+        <v>320</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>739</v>
+        <v>321</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>673</v>
+        <v>735</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>674</v>
+        <v>737</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>678</v>
+        <v>739</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>866</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>398</v>
+        <v>673</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>399</v>
+        <v>674</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>400</v>
+        <v>678</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>645</v>
+        <v>398</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>650</v>
+        <v>399</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>657</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>661</v>
+        <v>400</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>661</v>
@@ -4848,131 +4866,134 @@
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>479</v>
+        <v>646</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>480</v>
+        <v>649</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>481</v>
+        <v>658</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>517</v>
+        <v>479</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>518</v>
+        <v>480</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>519</v>
+        <v>481</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>508</v>
+        <v>517</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>509</v>
+        <v>518</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>510</v>
+        <v>519</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>155</v>
+        <v>506</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>156</v>
+        <v>505</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>830</v>
+        <v>504</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>511</v>
+        <v>155</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>513</v>
+        <v>156</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>514</v>
+        <v>830</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>613</v>
+        <v>511</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>614</v>
+        <v>513</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>615</v>
+        <v>514</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>298</v>
+        <v>613</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>299</v>
+        <v>614</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>300</v>
+        <v>615</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>405</v>
+        <v>298</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>406</v>
+        <v>299</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>407</v>
+        <v>300</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4991,2103 +5012,2120 @@
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>106</v>
+        <v>405</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>107</v>
+        <v>406</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>108</v>
+        <v>407</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>539</v>
+        <v>34</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>534</v>
+        <v>53</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>535</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>448</v>
+        <v>853</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>392</v>
+        <v>854</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>394</v>
+        <v>855</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>697</v>
+        <v>539</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>698</v>
+        <v>534</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>702</v>
+        <v>535</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>324</v>
+        <v>448</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>325</v>
+        <v>392</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>326</v>
+        <v>393</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>267</v>
+        <v>697</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>268</v>
+        <v>698</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>269</v>
+        <v>701</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>270</v>
+        <v>702</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>42</v>
+        <v>324</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>57</v>
+        <v>325</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>43</v>
+        <v>326</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>463</v>
+        <v>267</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>464</v>
+        <v>268</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>465</v>
+        <v>269</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>856</v>
+        <v>270</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>725</v>
+        <v>42</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>726</v>
+        <v>57</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>727</v>
+        <v>88</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>595</v>
+        <v>463</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>592</v>
+        <v>464</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>593</v>
+        <v>465</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>856</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>221</v>
+        <v>725</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>222</v>
+        <v>726</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>223</v>
+        <v>727</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>287</v>
+        <v>595</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>288</v>
+        <v>592</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>290</v>
+        <v>593</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>684</v>
+        <v>221</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>685</v>
+        <v>222</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>687</v>
+        <v>223</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>665</v>
+        <v>287</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>668</v>
+        <v>288</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>675</v>
+        <v>289</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>667</v>
+        <v>290</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>346</v>
+        <v>684</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>347</v>
+        <v>685</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>348</v>
+        <v>690</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>687</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>500</v>
+        <v>665</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>501</v>
+        <v>668</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>502</v>
+        <v>675</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>503</v>
+        <v>667</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>213</v>
+        <v>346</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>214</v>
+        <v>347</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>216</v>
+        <v>348</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>217</v>
+        <v>500</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>218</v>
+        <v>501</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>219</v>
+        <v>502</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>220</v>
+        <v>503</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>827</v>
+        <v>213</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>828</v>
+        <v>214</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>829</v>
+        <v>215</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>310</v>
+        <v>217</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>311</v>
+        <v>218</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>314</v>
+        <v>219</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>582</v>
+        <v>827</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>583</v>
+        <v>828</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>584</v>
+        <v>829</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>103</v>
+        <v>310</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>104</v>
+        <v>311</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>105</v>
+        <v>314</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>636</v>
+        <v>582</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>637</v>
+        <v>583</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>638</v>
+        <v>584</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>482</v>
+        <v>103</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>483</v>
+        <v>104</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>484</v>
+        <v>105</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>488</v>
+        <v>636</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>489</v>
+        <v>637</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>490</v>
+        <v>638</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>291</v>
+        <v>482</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>285</v>
+        <v>483</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>286</v>
+        <v>484</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>594</v>
+        <v>488</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>596</v>
+        <v>489</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>597</v>
+        <v>490</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>520</v>
+        <v>291</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>521</v>
+        <v>285</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>522</v>
+        <v>286</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>445</v>
+        <v>594</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>446</v>
+        <v>596</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>447</v>
+        <v>597</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>770</v>
+        <v>520</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>771</v>
+        <v>521</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>773</v>
+        <v>522</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>171</v>
+        <v>445</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>187</v>
+        <v>446</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>172</v>
+        <v>447</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>192</v>
+        <v>770</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>193</v>
+        <v>771</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>195</v>
+        <v>773</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>292</v>
+        <v>171</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>293</v>
+        <v>187</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>294</v>
+        <v>172</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>146</v>
+        <v>192</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>147</v>
+        <v>193</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>148</v>
+        <v>194</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>350</v>
+        <v>292</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>351</v>
+        <v>293</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>352</v>
+        <v>294</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>376</v>
+        <v>146</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>327</v>
+        <v>147</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>328</v>
+        <v>148</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>418</v>
+        <v>350</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>419</v>
+        <v>351</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>420</v>
+        <v>352</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>97</v>
+        <v>376</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>98</v>
+        <v>327</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>99</v>
+        <v>328</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>395</v>
+        <v>418</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>396</v>
+        <v>419</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>397</v>
+        <v>420</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>295</v>
+        <v>97</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>296</v>
+        <v>98</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>297</v>
+        <v>99</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>817</v>
+        <v>395</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>818</v>
+        <v>396</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>819</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>820</v>
+        <v>397</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>472</v>
+        <v>295</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>473</v>
+        <v>296</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>474</v>
+        <v>297</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>60</v>
+        <v>817</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>61</v>
+        <v>818</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>64</v>
+        <v>819</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>62</v>
+        <v>820</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>565</v>
+        <v>472</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>598</v>
+        <v>473</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>599</v>
+        <v>474</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>707</v>
+        <v>60</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>708</v>
+        <v>61</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>710</v>
+        <v>64</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>709</v>
+        <v>62</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>734</v>
+        <v>565</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>736</v>
+        <v>598</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>738</v>
+        <v>599</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>149</v>
+        <v>707</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>150</v>
+        <v>708</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>151</v>
+        <v>710</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>152</v>
+        <v>709</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>424</v>
+        <v>734</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>425</v>
+        <v>736</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>427</v>
+        <v>738</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>48</v>
+        <v>149</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>59</v>
+        <v>150</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>89</v>
+        <v>151</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>669</v>
+        <v>424</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>670</v>
+        <v>425</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>676</v>
+        <v>426</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>831</v>
+        <v>48</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>832</v>
+        <v>59</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>833</v>
+        <v>89</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>271</v>
+        <v>669</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>272</v>
+        <v>670</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>273</v>
+        <v>676</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>728</v>
+        <v>831</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>729</v>
+        <v>832</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>730</v>
+        <v>833</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>722</v>
+        <v>271</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>723</v>
+        <v>272</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>724</v>
+        <v>273</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>239</v>
+        <v>728</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>241</v>
+        <v>729</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>246</v>
+        <v>730</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>185</v>
+        <v>722</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>186</v>
+        <v>723</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>188</v>
+        <v>724</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>715</v>
+        <v>239</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>716</v>
+        <v>241</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>717</v>
+        <v>240</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>799</v>
+        <v>185</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>800</v>
+        <v>186</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>801</v>
+        <v>188</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>233</v>
+        <v>715</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>234</v>
+        <v>716</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>235</v>
+        <v>717</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>37</v>
+        <v>799</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>54</v>
+        <v>800</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>90</v>
+        <v>801</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>389</v>
+        <v>233</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>390</v>
+        <v>234</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>391</v>
+        <v>235</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>128</v>
+        <v>37</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>129</v>
+        <v>54</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>202</v>
+        <v>389</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>203</v>
+        <v>390</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>796</v>
+        <v>391</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>491</v>
+        <v>128</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>492</v>
+        <v>129</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>493</v>
+        <v>130</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>458</v>
+        <v>202</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>459</v>
+        <v>203</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>460</v>
+        <v>204</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>461</v>
+        <v>796</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>558</v>
+        <v>491</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>551</v>
+        <v>492</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>550</v>
+        <v>493</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>619</v>
+        <v>458</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>620</v>
+        <v>459</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>460</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>625</v>
+        <v>558</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>626</v>
+        <v>551</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>553</v>
+        <v>619</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>554</v>
+        <v>620</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>371</v>
+        <v>625</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>373</v>
+        <v>626</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>356</v>
+        <v>553</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>357</v>
+        <v>554</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>358</v>
+        <v>555</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>280</v>
+        <v>371</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>277</v>
+        <v>372</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>279</v>
+        <v>373</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>124</v>
+        <v>356</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>125</v>
+        <v>357</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E163" s="1" t="s">
-        <v>127</v>
+        <v>358</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>134</v>
+        <v>280</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>135</v>
+        <v>277</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>136</v>
+        <v>278</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>526</v>
+        <v>124</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>527</v>
+        <v>125</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>860</v>
+        <v>126</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>251</v>
+        <v>134</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>252</v>
+        <v>135</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>253</v>
+        <v>136</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>248</v>
+        <v>526</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>249</v>
+        <v>527</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>250</v>
+        <v>860</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>281</v>
+        <v>251</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>161</v>
+        <v>45</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>282</v>
+        <v>252</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>75</v>
+        <v>248</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>76</v>
+        <v>249</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>78</v>
+        <v>250</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>164</v>
+        <v>281</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>165</v>
+        <v>282</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>166</v>
+        <v>283</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>589</v>
+        <v>164</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>590</v>
+        <v>165</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>591</v>
+        <v>166</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>844</v>
+        <v>589</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>845</v>
+        <v>590</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>846</v>
+        <v>591</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>274</v>
+        <v>44</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>275</v>
+        <v>70</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>276</v>
+        <v>92</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>353</v>
+        <v>844</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>354</v>
+        <v>845</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>355</v>
+        <v>846</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>731</v>
+        <v>274</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>732</v>
+        <v>275</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>733</v>
+        <v>276</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>301</v>
+        <v>353</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>302</v>
+        <v>354</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>303</v>
+        <v>355</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>160</v>
+        <v>731</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>161</v>
+        <v>41</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>162</v>
+        <v>732</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>683</v>
+        <v>301</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>682</v>
+        <v>302</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>686</v>
+        <v>303</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>711</v>
+        <v>160</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>712</v>
+        <v>162</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>199</v>
+        <v>683</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>200</v>
+        <v>682</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>201</v>
+        <v>689</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>47</v>
+        <v>711</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>58</v>
+        <v>712</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>94</v>
+        <v>713</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>691</v>
+        <v>199</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>692</v>
+        <v>200</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="E184" s="1" t="s">
-        <v>693</v>
+        <v>201</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>415</v>
+        <v>47</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>416</v>
+        <v>58</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>417</v>
+        <v>94</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>415</v>
+        <v>691</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>416</v>
+        <v>692</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>417</v>
+        <v>699</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>254</v>
+        <v>415</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>255</v>
+        <v>416</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="E187" s="1" t="s">
-        <v>257</v>
+        <v>417</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>435</v>
+        <v>417</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>559</v>
+        <v>254</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>560</v>
+        <v>255</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>561</v>
+        <v>256</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>562</v>
+        <v>257</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>307</v>
+        <v>432</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>308</v>
+        <v>433</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>309</v>
+        <v>434</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>824</v>
+        <v>559</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>825</v>
+        <v>560</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>826</v>
+        <v>561</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>114</v>
+        <v>307</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>115</v>
+        <v>308</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>116</v>
+        <v>309</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>485</v>
+        <v>824</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>486</v>
+        <v>825</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="E193" s="1" t="s">
-        <v>767</v>
+        <v>826</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>175</v>
+        <v>114</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>176</v>
+        <v>115</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>316</v>
+        <v>485</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>317</v>
+        <v>486</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>318</v>
+        <v>487</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>767</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>679</v>
+        <v>316</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>680</v>
+        <v>317</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="E197" s="1" t="s">
-        <v>681</v>
+        <v>318</v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>579</v>
+        <v>182</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>580</v>
+        <v>183</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>581</v>
+        <v>184</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>469</v>
+        <v>679</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>470</v>
+        <v>680</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>471</v>
+        <v>688</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>261</v>
+        <v>579</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>262</v>
+        <v>580</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>263</v>
+        <v>581</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>616</v>
+        <v>469</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>617</v>
+        <v>470</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>618</v>
+        <v>471</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>205</v>
+        <v>261</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>206</v>
+        <v>262</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E202" s="1" t="s">
-        <v>795</v>
+        <v>263</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>557</v>
+        <v>616</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>548</v>
+        <v>617</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="E203" s="1" t="s">
-        <v>550</v>
+        <v>618</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>332</v>
+        <v>205</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>322</v>
+        <v>206</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>323</v>
+        <v>207</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>566</v>
+        <v>847</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>571</v>
+        <v>848</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>572</v>
+        <v>849</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>494</v>
+        <v>557</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>496</v>
+        <v>548</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>498</v>
+        <v>549</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="207" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>764</v>
+        <v>332</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>765</v>
+        <v>322</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>766</v>
+        <v>323</v>
       </c>
     </row>
     <row r="208" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>610</v>
+        <v>566</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>611</v>
+        <v>571</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>612</v>
+        <v>572</v>
       </c>
     </row>
     <row r="209" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>671</v>
+        <v>494</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>672</v>
+        <v>496</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>677</v>
+        <v>498</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>755</v>
+        <v>764</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>756</v>
+        <v>765</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
     </row>
     <row r="211" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>342</v>
+        <v>610</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>343</v>
+        <v>611</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>345</v>
+        <v>612</v>
       </c>
     </row>
     <row r="212" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>541</v>
+        <v>671</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>542</v>
+        <v>672</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>543</v>
+        <v>677</v>
       </c>
     </row>
     <row r="213" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>35</v>
+        <v>755</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>56</v>
+        <v>756</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>36</v>
+        <v>757</v>
       </c>
     </row>
     <row r="214" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>578</v>
+        <v>342</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>437</v>
+        <v>343</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>438</v>
+        <v>344</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>436</v>
+        <v>345</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>656</v>
+        <v>541</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>651</v>
+        <v>542</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E215" s="1" t="s">
-        <v>661</v>
+        <v>543</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>752</v>
+        <v>35</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>753</v>
+        <v>56</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>754</v>
+        <v>95</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>605</v>
+        <v>437</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>606</v>
+        <v>438</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="218" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>536</v>
+        <v>656</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>537</v>
+        <v>651</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>538</v>
+        <v>659</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>428</v>
+        <v>752</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>429</v>
+        <v>753</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>431</v>
+        <v>754</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>266</v>
+        <v>604</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>264</v>
+        <v>605</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>265</v>
+        <v>606</v>
       </c>
     </row>
     <row r="221" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>168</v>
+        <v>536</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>169</v>
+        <v>537</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>170</v>
+        <v>538</v>
       </c>
     </row>
     <row r="222" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>662</v>
+        <v>428</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>663</v>
+        <v>429</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>664</v>
+        <v>430</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>666</v>
+        <v>431</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>421</v>
+        <v>266</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>422</v>
+        <v>264</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>540</v>
+        <v>265</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>65</v>
+        <v>168</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>66</v>
+        <v>169</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>68</v>
+        <v>170</v>
       </c>
     </row>
     <row r="225" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>788</v>
+        <v>662</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>789</v>
+        <v>663</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>790</v>
+        <v>664</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>666</v>
       </c>
     </row>
     <row r="226" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>648</v>
+        <v>421</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>653</v>
+        <v>422</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>654</v>
+        <v>423</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>655</v>
+        <v>540</v>
       </c>
     </row>
     <row r="227" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>847</v>
+        <v>65</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>848</v>
+        <v>66</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>849</v>
+        <v>67</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="228" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>850</v>
+        <v>788</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>851</v>
+        <v>789</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>852</v>
+        <v>790</v>
       </c>
     </row>
     <row r="229" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>853</v>
+        <v>648</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>854</v>
+        <v>653</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>855</v>
+        <v>654</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A230" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>865</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F229" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F226">
-      <sortCondition ref="A1:A226"/>
+  <autoFilter ref="A1:F230" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F229">
+      <sortCondition ref="A1:A229"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
m1-8-5.xml: p. 2 of 16
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F4CA9D-05D3-2D4A-B5E1-FA5DE1F40F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C56F58-0543-0A4F-9772-72C0EA1A50A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="873">
   <si>
     <t>M-Number</t>
   </si>
@@ -2694,6 +2694,15 @@
   </si>
   <si>
     <t>transcriptions/m1-8-5.xml</t>
+  </si>
+  <si>
+    <t>Revenger's Tragedy, The</t>
+  </si>
+  <si>
+    <t>lit-reve</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-reve</t>
   </si>
 </sst>
 </file>
@@ -3105,7 +3114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B8" sqref="B8"/>
     </sheetView>
@@ -3708,11 +3717,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F230"/>
+  <dimension ref="A1:F231"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E240" sqref="E240"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7141,6 +7150,20 @@
       </c>
       <c r="E230" s="1" t="s">
         <v>865</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A231" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
m1-8-5.xml: p. 4 of ...4
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C56F58-0543-0A4F-9772-72C0EA1A50A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47AD68E-A72E-FF49-8F21-C63AF67A0608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="874">
   <si>
     <t>M-Number</t>
   </si>
@@ -2687,9 +2687,6 @@
     <t>cf. psn-lbve</t>
   </si>
   <si>
-    <t>M1-8-5. The Reader. Holograph. In back [Articles, essays, fiction and reviews], vol. 8 [1938-39], pp. 17-32. 16p.</t>
-  </si>
-  <si>
     <t>m1-8-5</t>
   </si>
   <si>
@@ -2703,6 +2700,12 @@
   </si>
   <si>
     <t>../resources/annotations.xml#lit-reve</t>
+  </si>
+  <si>
+    <t>p. 3 - Scramble the plays together!!! - and note, this is shorter than anticipated - 4pp. Instead of 16.</t>
+  </si>
+  <si>
+    <t>M1-8-5. The Reader. Holograph. In back [Articles, essays, fiction and reviews], vol. 8 [1938-39], pp. 17-20. 4p.</t>
   </si>
 </sst>
 </file>
@@ -3114,7 +3117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B8" sqref="B8"/>
     </sheetView>
@@ -3241,16 +3244,19 @@
         <v>807</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>868</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>869</v>
       </c>
       <c r="F7" s="5">
         <v>16</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>872</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3719,9 +3725,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
   <dimension ref="A1:F231"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D106" sqref="D106"/>
+    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7154,16 +7160,16 @@
     </row>
     <row r="231" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C231" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="D231" s="1" t="s">
         <v>871</v>
-      </c>
-      <c r="D231" s="1" t="s">
-        <v>872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
m1-8-5.xml: p. 4 of ?
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C3F4B8-5E8A-BA4D-908D-1FFA84D5ACA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055B9B39-F1D0-A14B-AA03-D47B200600C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -3742,7 +3742,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K215" sqref="K215"/>
+      <selection pane="bottomLeft" activeCell="H229" sqref="H229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
m1-8-7.xml: p. 1 of 6
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055B9B39-F1D0-A14B-AA03-D47B200600C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DCC759-0B74-E94A-A5BD-1353C6262C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="887">
   <si>
     <t>M-Number</t>
   </si>
@@ -2721,6 +2721,30 @@
   </si>
   <si>
     <t>pla-merm</t>
+  </si>
+  <si>
+    <t>Gammer Gurton's Needle</t>
+  </si>
+  <si>
+    <t>lit-gamme</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-merm</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#lit-gamme</t>
+  </si>
+  <si>
+    <t>M1-8-6. [The readers faculty is a queer one...]. Holograph. In back [Articles, essays, fiction and reviews], vol. 8 [1938-39], pp. 21-26. 6p</t>
+  </si>
+  <si>
+    <t>m1-8-6</t>
+  </si>
+  <si>
+    <t>transcriptions/m1-8-6.xml</t>
+  </si>
+  <si>
+    <t>A little short for a stormtrooper</t>
   </si>
 </sst>
 </file>
@@ -3132,9 +3156,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B8" sqref="B8"/>
+      <selection pane="topRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3268,15 +3292,36 @@
         <v>868</v>
       </c>
       <c r="F7" s="5">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>872</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>808</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="F8" s="5">
+        <v>6</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>886</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3738,11 +3783,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F233"/>
+  <dimension ref="A1:F234"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H229" sqref="H229"/>
+    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7201,7 +7246,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="233" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>877</v>
       </c>
@@ -7210,6 +7255,23 @@
       </c>
       <c r="C233" s="1" t="s">
         <v>878</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A234" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
m1-8-8.xml: initial (and final :) commit)
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DCC759-0B74-E94A-A5BD-1353C6262C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3246C4A9-9CC9-4946-9EA0-594418912673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="898">
   <si>
     <t>M-Number</t>
   </si>
@@ -2745,6 +2745,39 @@
   </si>
   <si>
     <t>A little short for a stormtrooper</t>
+  </si>
+  <si>
+    <t>Middleton, Thomas</t>
+  </si>
+  <si>
+    <t>psn-tmid</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-tmid</t>
+  </si>
+  <si>
+    <t>London Bridge</t>
+  </si>
+  <si>
+    <t>pla-lobr</t>
+  </si>
+  <si>
+    <t>M1-8-7. [If you have read this brittle &amp;amp; imperfect sketch...]. Holograph. In back [Articles, essays, fiction and reviews], vol. 8 [1938-39], pp. 27-32. 6p.</t>
+  </si>
+  <si>
+    <t>m1-8-7</t>
+  </si>
+  <si>
+    <t>transcriptions/m1-8-7.xml</t>
+  </si>
+  <si>
+    <t>M1-8-8. The Reader. In back [Articles, essays, fiction and reviews], vol. 8 [1938-39], p. 31. 1p.</t>
+  </si>
+  <si>
+    <t>m1-8-8</t>
+  </si>
+  <si>
+    <t>transcriptions/m1-8-8.xml</t>
   </si>
 </sst>
 </file>
@@ -3154,11 +3187,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H8" sqref="H8"/>
+      <selection pane="topRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3324,163 +3357,170 @@
         <v>886</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="F9" s="5">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>774</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>793</v>
-      </c>
-      <c r="F11" s="5">
-        <v>10</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="B10" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="F12" s="5">
         <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>783</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>794</v>
-      </c>
-      <c r="F12" s="5">
-        <v>9</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>797</v>
+        <v>784</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>791</v>
+        <v>782</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>792</v>
+        <v>783</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
       <c r="F13" s="5">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="H13" s="1" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>339</v>
+        <v>791</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>792</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>118</v>
+        <v>802</v>
       </c>
       <c r="F14" s="5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F15" s="5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>120</v>
+        <v>340</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F16" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>334</v>
+        <v>120</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F17" s="5">
         <v>9</v>
@@ -3489,87 +3529,90 @@
         <v>32</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>335</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>337</v>
+        <v>122</v>
       </c>
       <c r="F18" s="5">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="H18" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F19" s="5">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>374</v>
-      </c>
     </row>
     <row r="20" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>404</v>
+        <v>341</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>401</v>
+        <v>336</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>402</v>
+        <v>338</v>
       </c>
       <c r="F20" s="5">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="H20" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>441</v>
+        <v>404</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>439</v>
+        <v>401</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>440</v>
+        <v>402</v>
       </c>
       <c r="F21" s="5">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>32</v>
@@ -3577,59 +3620,59 @@
     </row>
     <row r="22" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>528</v>
+        <v>441</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>529</v>
+        <v>439</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>530</v>
+        <v>440</v>
       </c>
       <c r="F22" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>544</v>
-      </c>
     </row>
     <row r="23" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>546</v>
+        <v>528</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>545</v>
+        <v>529</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>547</v>
+        <v>530</v>
       </c>
       <c r="F23" s="5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="H23" s="1" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="24" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>573</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>585</v>
+        <v>546</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>576</v>
+        <v>545</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>577</v>
+        <v>547</v>
       </c>
       <c r="F24" s="5">
         <v>5</v>
@@ -3640,19 +3683,19 @@
     </row>
     <row r="25" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>587</v>
+        <v>576</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>588</v>
+        <v>577</v>
       </c>
       <c r="F25" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>32</v>
@@ -3660,112 +3703,132 @@
     </row>
     <row r="26" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>602</v>
+        <v>586</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>600</v>
+        <v>587</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>601</v>
+        <v>588</v>
       </c>
       <c r="F26" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>603</v>
-      </c>
     </row>
     <row r="27" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>627</v>
+        <v>575</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>630</v>
+        <v>602</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>631</v>
+        <v>600</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>632</v>
+        <v>601</v>
       </c>
       <c r="F27" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="H27" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>721</v>
+        <v>630</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>718</v>
+        <v>631</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>719</v>
+        <v>632</v>
       </c>
       <c r="F28" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>720</v>
-      </c>
     </row>
     <row r="29" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>742</v>
+        <v>721</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>740</v>
+        <v>718</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>741</v>
+        <v>719</v>
       </c>
       <c r="F29" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="H29" s="1" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>22</v>
+        <v>629</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>749</v>
+        <v>742</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>750</v>
+        <v>740</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>751</v>
+        <v>741</v>
       </c>
       <c r="F30" s="5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H32" s="1" t="s">
+    <row r="31" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="F31" s="5">
+        <v>8</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H33" s="1" t="s">
         <v>798</v>
       </c>
     </row>
@@ -3783,11 +3846,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F234"/>
+  <dimension ref="A1:F236"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C236" sqref="C236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7272,6 +7335,31 @@
       </c>
       <c r="D234" s="1" t="s">
         <v>882</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A235" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A236" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
m1-8-9.xml: p. 1 of 9
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3246C4A9-9CC9-4946-9EA0-594418912673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECDD597-FFE5-CA49-8FE7-63B7856194ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="902">
   <si>
     <t>M-Number</t>
   </si>
@@ -2778,6 +2778,18 @@
   </si>
   <si>
     <t>transcriptions/m1-8-8.xml</t>
+  </si>
+  <si>
+    <t>M1-8-9</t>
+  </si>
+  <si>
+    <t>m1-8-9</t>
+  </si>
+  <si>
+    <t>transcriptions/m1-8-9.xml</t>
+  </si>
+  <si>
+    <t>M1-8, 9 of 9. The Reader. In back [Articles, essays, fiction and reviews], vol. 8 [1938-39], pp. 34-42. 9p</t>
   </si>
 </sst>
 </file>
@@ -3191,7 +3203,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B13" sqref="B13"/>
+      <selection pane="topRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3395,6 +3407,23 @@
       </c>
       <c r="G10" s="5" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="F11" s="5">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
m1-8-9.xml: p. 2 of 9
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECDD597-FFE5-CA49-8FE7-63B7856194ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F784F07F-2954-3345-AE7A-AA3764FB3AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -3201,7 +3201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B14" sqref="B14"/>
     </sheetView>
@@ -3877,9 +3877,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
   <dimension ref="A1:F236"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C236" sqref="C236"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
m1-8-10.xml: p. 2 of 3
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FFEF77-E677-B54E-B469-DF28B0B09913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFEAAC9-252F-CE48-93CC-FC3D56E7CCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="910">
   <si>
     <t>M-Number</t>
   </si>
@@ -2802,6 +2802,18 @@
   </si>
   <si>
     <t>transcriptions/m1-8-10.xml</t>
+  </si>
+  <si>
+    <t>James I of England and VI of Scotland</t>
+  </si>
+  <si>
+    <t>psn-kjam</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-kjam</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-lobr</t>
   </si>
 </sst>
 </file>
@@ -3211,11 +3223,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G12" sqref="G12"/>
+      <selection pane="topRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3458,285 +3470,242 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>774</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>793</v>
-      </c>
-      <c r="F13" s="5">
-        <v>10</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>783</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>794</v>
-      </c>
-      <c r="F14" s="5">
-        <v>9</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>797</v>
-      </c>
-    </row>
     <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>791</v>
+        <v>774</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>792</v>
+        <v>775</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>802</v>
+        <v>793</v>
       </c>
       <c r="F15" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="H15" s="1" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>339</v>
+        <v>782</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>23</v>
+        <v>783</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>118</v>
+        <v>794</v>
       </c>
       <c r="F16" s="5">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>340</v>
+        <v>791</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>792</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>123</v>
+        <v>802</v>
       </c>
       <c r="F17" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>120</v>
+        <v>339</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F18" s="5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F19" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>212</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>333</v>
+        <v>120</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>335</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>337</v>
+        <v>121</v>
       </c>
       <c r="F20" s="5">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="H20" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>336</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>338</v>
+        <v>122</v>
       </c>
       <c r="F21" s="5">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>404</v>
+        <v>333</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>401</v>
+        <v>335</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>402</v>
+        <v>337</v>
       </c>
       <c r="F22" s="5">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>441</v>
+        <v>341</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>439</v>
+        <v>336</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>440</v>
+        <v>338</v>
       </c>
       <c r="F23" s="5">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="H23" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>528</v>
+        <v>404</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>529</v>
+        <v>401</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>530</v>
+        <v>402</v>
       </c>
       <c r="F24" s="5">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>544</v>
-      </c>
     </row>
     <row r="25" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>546</v>
+        <v>441</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>545</v>
+        <v>439</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>547</v>
+        <v>440</v>
       </c>
       <c r="F25" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>32</v>
@@ -3744,39 +3713,42 @@
     </row>
     <row r="26" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>573</v>
+        <v>20</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>585</v>
+        <v>528</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>576</v>
+        <v>529</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>577</v>
+        <v>530</v>
       </c>
       <c r="F26" s="5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="H26" s="1" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>574</v>
+        <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>586</v>
+        <v>546</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>587</v>
+        <v>545</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>588</v>
+        <v>547</v>
       </c>
       <c r="F27" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>32</v>
@@ -3784,42 +3756,39 @@
     </row>
     <row r="28" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>602</v>
+        <v>585</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>600</v>
+        <v>576</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>601</v>
+        <v>577</v>
       </c>
       <c r="F28" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>603</v>
-      </c>
     </row>
     <row r="29" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>627</v>
+        <v>574</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>630</v>
+        <v>586</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>631</v>
+        <v>587</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>632</v>
+        <v>588</v>
       </c>
       <c r="F29" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>32</v>
@@ -3827,42 +3796,42 @@
     </row>
     <row r="30" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>628</v>
+        <v>575</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>721</v>
+        <v>602</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>718</v>
+        <v>600</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>719</v>
+        <v>601</v>
       </c>
       <c r="F30" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>720</v>
+        <v>603</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>742</v>
+        <v>630</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>740</v>
+        <v>631</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>741</v>
+        <v>632</v>
       </c>
       <c r="F31" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>32</v>
@@ -3870,26 +3839,69 @@
     </row>
     <row r="32" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>22</v>
+        <v>628</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>749</v>
+        <v>721</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>750</v>
+        <v>718</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>751</v>
+        <v>719</v>
       </c>
       <c r="F32" s="5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H34" s="1" t="s">
+      <c r="H32" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="F33" s="5">
+        <v>3</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="F34" s="5">
+        <v>8</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H36" s="1" t="s">
         <v>798</v>
       </c>
     </row>
@@ -3907,11 +3919,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F236"/>
+  <dimension ref="A1:F237"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D237" sqref="D237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7412,7 +7424,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="236" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>890</v>
       </c>
@@ -7421,6 +7433,23 @@
       </c>
       <c r="C236" s="1" t="s">
         <v>891</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A237" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>908</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
m1-8-10.xml: p. 4 of 6. Decided it\'s one longer fragment instead of two shorter ones
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFEAAC9-252F-CE48-93CC-FC3D56E7CCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1421FC13-F323-4240-B1C3-DD50B0564663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="919">
   <si>
     <t>M-Number</t>
   </si>
@@ -2814,6 +2814,33 @@
   </si>
   <si>
     <t>../resources/annotations.xml#pla-lobr</t>
+  </si>
+  <si>
+    <t>Knole</t>
+  </si>
+  <si>
+    <t>pla-knol</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#pla-knol</t>
+  </si>
+  <si>
+    <t>Nashe, Thomas</t>
+  </si>
+  <si>
+    <t>psn-tnas</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-tnas</t>
+  </si>
+  <si>
+    <t>Cf. lit-trav</t>
+  </si>
+  <si>
+    <t>Cf psn-tnas, n.b. in m1-8-10 title is presumably misremembered</t>
+  </si>
+  <si>
+    <t>Literary Work+B193</t>
   </si>
 </sst>
 </file>
@@ -3227,7 +3254,7 @@
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B18" sqref="B18"/>
+      <selection pane="topRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3467,7 +3494,7 @@
         <v>905</v>
       </c>
       <c r="F12" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3919,11 +3946,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F237"/>
+  <dimension ref="A1:F239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D237" sqref="D237"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7035,7 +7062,7 @@
         <v>764</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>41</v>
+        <v>918</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>765</v>
@@ -7116,6 +7143,9 @@
       <c r="D215" s="1" t="s">
         <v>543</v>
       </c>
+      <c r="E215" s="1" t="s">
+        <v>917</v>
+      </c>
     </row>
     <row r="216" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
@@ -7450,6 +7480,37 @@
       </c>
       <c r="D237" s="1" t="s">
         <v>908</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A238" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A239" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "update to tracking sheet"
This reverts commit 3e6e5282e576ad8a448ebce5d67b5d609d194128.
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EF7758-7BD4-BD44-9ED6-D7CED91E3091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1421FC13-F323-4240-B1C3-DD50B0564663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="919">
   <si>
     <t>M-Number</t>
   </si>
@@ -2841,18 +2841,6 @@
   </si>
   <si>
     <t>Literary Work+B193</t>
-  </si>
-  <si>
-    <t>cf psn-rbur</t>
-  </si>
-  <si>
-    <t>Miller, Sissy</t>
-  </si>
-  <si>
-    <t>psn-smil</t>
-  </si>
-  <si>
-    <t>../resources/annotations.xml#psn-smil</t>
   </si>
 </sst>
 </file>
@@ -3262,11 +3250,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G19" sqref="G19"/>
+      <selection pane="topRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3508,9 +3496,6 @@
       <c r="F12" s="5">
         <v>6</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -3945,12 +3930,6 @@
     <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="H36" s="1" t="s">
         <v>798</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F37" s="5">
-        <f>SUM(F3:F34)</f>
-        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -3967,11 +3946,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F240"/>
+  <dimension ref="A1:F239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D240" sqref="D240"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4093,9 +4072,6 @@
       <c r="D7" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>919</v>
-      </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -4262,3299 +4238,3285 @@
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>862</v>
+        <v>380</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>863</v>
+        <v>381</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>864</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>865</v>
+        <v>382</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>380</v>
+        <v>814</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>381</v>
+        <v>815</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>382</v>
+        <v>816</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>814</v>
+        <v>131</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>815</v>
+        <v>132</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>820</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>131</v>
+        <v>362</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>132</v>
+        <v>363</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>133</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>874</v>
+        <v>643</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>875</v>
+        <v>642</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>876</v>
+        <v>644</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>368</v>
+        <v>633</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>369</v>
+        <v>634</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>370</v>
+        <v>635</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>643</v>
+        <v>82</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>642</v>
+        <v>83</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>644</v>
+        <v>84</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>633</v>
+        <v>495</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>634</v>
+        <v>497</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>635</v>
+        <v>499</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>82</v>
+        <v>743</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>83</v>
+        <v>744</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>495</v>
+        <v>227</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>497</v>
+        <v>228</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>499</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>743</v>
+        <v>365</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>744</v>
+        <v>366</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>365</v>
+        <v>142</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>366</v>
+        <v>141</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>224</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>225</v>
+        <v>50</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>40</v>
+        <v>779</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>50</v>
+        <v>780</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>779</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>780</v>
+        <v>69</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>143</v>
+        <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>144</v>
+        <v>51</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>349</v>
+        <v>776</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>69</v>
+        <v>777</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>33</v>
+        <v>512</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>51</v>
+        <v>515</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>776</v>
+        <v>523</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>777</v>
+        <v>524</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>512</v>
+        <v>79</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>515</v>
+        <v>80</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>523</v>
+        <v>452</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>524</v>
+        <v>453</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>79</v>
+        <v>760</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>80</v>
+        <v>761</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>452</v>
+        <v>759</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>453</v>
+        <v>758</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>760</v>
+        <v>563</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>761</v>
+        <v>567</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>759</v>
+        <v>230</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>758</v>
+        <v>231</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>563</v>
+        <v>100</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>567</v>
+        <v>101</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>569</v>
+        <v>102</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>230</v>
+        <v>383</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>231</v>
+        <v>384</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>232</v>
+        <v>385</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>100</v>
+        <v>639</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>101</v>
+        <v>641</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>208</v>
+        <v>640</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>383</v>
+        <v>850</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>384</v>
+        <v>851</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>475</v>
+        <v>852</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>639</v>
+        <v>622</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>641</v>
+        <v>623</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>640</v>
+        <v>624</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>850</v>
+        <v>236</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>851</v>
+        <v>237</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>852</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>622</v>
+        <v>38</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>623</v>
+        <v>52</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>624</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>236</v>
+        <v>304</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>237</v>
+        <v>305</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>238</v>
+        <v>306</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>38</v>
+        <v>607</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>52</v>
+        <v>608</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>93</v>
+        <v>609</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>304</v>
+        <v>768</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>305</v>
+        <v>769</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>306</v>
+        <v>772</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>607</v>
+        <v>821</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>608</v>
+        <v>822</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>609</v>
+        <v>823</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>768</v>
+        <v>476</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>769</v>
+        <v>477</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>772</v>
+        <v>478</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>821</v>
+        <v>359</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>822</v>
+        <v>360</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>823</v>
+        <v>361</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>476</v>
+        <v>157</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>477</v>
+        <v>158</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>478</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>359</v>
+        <v>785</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>360</v>
+        <v>786</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>361</v>
+        <v>787</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>157</v>
+        <v>411</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>158</v>
+        <v>412</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>159</v>
+        <v>413</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>785</v>
+        <v>837</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>786</v>
+        <v>838</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>787</v>
+        <v>839</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>840</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>411</v>
+        <v>531</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>412</v>
+        <v>532</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>414</v>
+        <v>533</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>837</v>
+        <v>258</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>838</v>
+        <v>259</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>839</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>840</v>
+        <v>260</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>531</v>
+        <v>694</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>532</v>
+        <v>695</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>533</v>
+        <v>700</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>260</v>
+        <v>243</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>694</v>
+        <v>455</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>695</v>
+        <v>456</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>700</v>
+        <v>457</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>696</v>
+        <v>462</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>244</v>
+        <v>137</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>242</v>
+        <v>138</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>245</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>455</v>
+        <v>312</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>456</v>
+        <v>313</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>462</v>
+        <v>315</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>137</v>
+        <v>189</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>138</v>
+        <v>190</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>312</v>
+        <v>247</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>313</v>
+        <v>112</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>315</v>
+        <v>113</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>189</v>
+        <v>564</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>190</v>
+        <v>568</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>191</v>
+        <v>570</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>247</v>
+        <v>319</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>112</v>
+        <v>320</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>113</v>
+        <v>321</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>564</v>
+        <v>735</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>568</v>
+        <v>737</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>570</v>
+        <v>739</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>866</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>319</v>
+        <v>673</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>320</v>
+        <v>674</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>321</v>
+        <v>678</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>735</v>
+        <v>398</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>737</v>
+        <v>399</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>866</v>
+        <v>400</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>673</v>
+        <v>645</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>674</v>
+        <v>650</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>678</v>
+        <v>657</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>398</v>
+        <v>646</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>399</v>
+        <v>649</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>400</v>
+        <v>658</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>645</v>
+        <v>479</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>650</v>
+        <v>480</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>657</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>661</v>
+        <v>481</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>646</v>
+        <v>517</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>649</v>
+        <v>518</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>661</v>
+        <v>519</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>479</v>
+        <v>508</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>480</v>
+        <v>509</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>481</v>
+        <v>510</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>518</v>
+        <v>505</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>519</v>
+        <v>504</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>508</v>
+        <v>155</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>509</v>
+        <v>156</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>510</v>
+        <v>830</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>879</v>
+        <v>511</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>880</v>
+        <v>513</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>882</v>
+        <v>514</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>506</v>
+        <v>613</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>505</v>
+        <v>614</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>507</v>
+        <v>615</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>155</v>
+        <v>298</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>156</v>
+        <v>299</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>830</v>
+        <v>300</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>511</v>
+        <v>405</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>513</v>
+        <v>406</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>514</v>
+        <v>407</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>613</v>
+        <v>405</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>614</v>
+        <v>406</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>615</v>
+        <v>407</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>298</v>
+        <v>106</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>299</v>
+        <v>107</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>300</v>
+        <v>108</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>405</v>
+        <v>34</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>406</v>
+        <v>53</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>407</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>405</v>
+        <v>853</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>406</v>
+        <v>854</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>407</v>
+        <v>855</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>106</v>
+        <v>539</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>107</v>
+        <v>534</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>108</v>
+        <v>535</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>34</v>
+        <v>448</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>53</v>
+        <v>392</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>87</v>
+        <v>393</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>853</v>
+        <v>697</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>854</v>
+        <v>698</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>855</v>
+        <v>701</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>702</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>539</v>
+        <v>324</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>534</v>
+        <v>325</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>535</v>
+        <v>326</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>448</v>
+        <v>267</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>392</v>
+        <v>268</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>393</v>
+        <v>269</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>394</v>
+        <v>270</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>697</v>
+        <v>42</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>698</v>
+        <v>57</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>701</v>
+        <v>88</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>702</v>
+        <v>43</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>324</v>
+        <v>463</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>325</v>
+        <v>464</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>326</v>
+        <v>465</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>856</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>267</v>
+        <v>725</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>268</v>
+        <v>726</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>270</v>
+        <v>727</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>42</v>
+        <v>595</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>57</v>
+        <v>592</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>43</v>
+        <v>593</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>463</v>
+        <v>221</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>464</v>
+        <v>222</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>856</v>
+        <v>223</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>725</v>
+        <v>287</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>726</v>
+        <v>288</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>727</v>
+        <v>289</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>595</v>
+        <v>684</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>592</v>
+        <v>685</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>593</v>
+        <v>690</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>687</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>221</v>
+        <v>665</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>222</v>
+        <v>668</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>223</v>
+        <v>675</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>287</v>
+        <v>346</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>288</v>
+        <v>347</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>290</v>
+        <v>348</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>684</v>
+        <v>500</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>685</v>
+        <v>501</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>690</v>
+        <v>502</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>687</v>
+        <v>503</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>665</v>
+        <v>213</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>668</v>
+        <v>214</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>675</v>
+        <v>215</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>667</v>
+        <v>216</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>346</v>
+        <v>217</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>347</v>
+        <v>218</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>348</v>
+        <v>219</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>500</v>
+        <v>827</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>501</v>
+        <v>828</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>503</v>
+        <v>829</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>213</v>
+        <v>310</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>214</v>
+        <v>311</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>216</v>
+        <v>314</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>217</v>
+        <v>582</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>218</v>
+        <v>583</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>220</v>
+        <v>584</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>827</v>
+        <v>103</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>828</v>
+        <v>104</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>829</v>
+        <v>105</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>310</v>
+        <v>636</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>311</v>
+        <v>637</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>314</v>
+        <v>638</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>582</v>
+        <v>482</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>583</v>
+        <v>483</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>584</v>
+        <v>484</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>906</v>
+        <v>488</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>907</v>
+        <v>489</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>908</v>
+        <v>490</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>103</v>
+        <v>291</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>104</v>
+        <v>285</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>105</v>
+        <v>286</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>636</v>
+        <v>594</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>637</v>
+        <v>596</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>638</v>
+        <v>597</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>482</v>
+        <v>520</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>483</v>
+        <v>521</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>484</v>
+        <v>522</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>488</v>
+        <v>445</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>489</v>
+        <v>446</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>490</v>
+        <v>447</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>291</v>
+        <v>770</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>285</v>
+        <v>771</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>286</v>
+        <v>773</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>594</v>
+        <v>171</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>596</v>
+        <v>187</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>597</v>
+        <v>172</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>910</v>
+        <v>192</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>911</v>
+        <v>193</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>912</v>
+        <v>194</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>520</v>
+        <v>292</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>521</v>
+        <v>293</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>522</v>
+        <v>294</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>445</v>
+        <v>146</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>446</v>
+        <v>147</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>447</v>
+        <v>148</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>770</v>
+        <v>350</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>771</v>
+        <v>351</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>773</v>
+        <v>352</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>171</v>
+        <v>376</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>187</v>
+        <v>327</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>172</v>
+        <v>328</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>192</v>
+        <v>418</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>193</v>
+        <v>419</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>195</v>
+        <v>420</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>292</v>
+        <v>97</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>293</v>
+        <v>98</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>294</v>
+        <v>99</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>146</v>
+        <v>395</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>147</v>
+        <v>396</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>148</v>
+        <v>397</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>350</v>
+        <v>295</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>351</v>
+        <v>296</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>352</v>
+        <v>297</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>376</v>
+        <v>817</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>327</v>
+        <v>818</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>328</v>
+        <v>819</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>418</v>
+        <v>472</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>419</v>
+        <v>473</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>420</v>
+        <v>474</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>99</v>
+        <v>64</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>890</v>
+        <v>565</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>891</v>
+        <v>598</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>909</v>
+        <v>599</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>395</v>
+        <v>707</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>396</v>
+        <v>708</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>397</v>
+        <v>710</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>295</v>
+        <v>734</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>296</v>
+        <v>736</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>297</v>
+        <v>738</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>817</v>
+        <v>149</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>818</v>
+        <v>150</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>819</v>
+        <v>151</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>820</v>
+        <v>152</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>472</v>
+        <v>424</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>473</v>
+        <v>425</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>474</v>
+        <v>426</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>565</v>
+        <v>669</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>598</v>
+        <v>670</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>599</v>
+        <v>676</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>707</v>
+        <v>831</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>708</v>
+        <v>832</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>709</v>
+        <v>833</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>734</v>
+        <v>271</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>736</v>
+        <v>272</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>738</v>
+        <v>273</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>149</v>
+        <v>728</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>150</v>
+        <v>729</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>152</v>
+        <v>730</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>424</v>
+        <v>722</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>425</v>
+        <v>723</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>427</v>
+        <v>724</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>48</v>
+        <v>239</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>59</v>
+        <v>241</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>89</v>
+        <v>240</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>669</v>
+        <v>185</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>670</v>
+        <v>186</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>676</v>
+        <v>188</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>831</v>
+        <v>715</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>832</v>
+        <v>716</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>833</v>
+        <v>717</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>877</v>
+        <v>799</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>878</v>
+        <v>800</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>881</v>
+        <v>801</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>272</v>
+        <v>234</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>887</v>
+        <v>37</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>888</v>
+        <v>54</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>889</v>
+        <v>90</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>728</v>
+        <v>389</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>729</v>
+        <v>390</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>730</v>
+        <v>391</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>722</v>
+        <v>128</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>161</v>
+        <v>45</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>723</v>
+        <v>129</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>724</v>
+        <v>130</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>241</v>
+        <v>203</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>240</v>
+        <v>204</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>246</v>
+        <v>796</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>185</v>
+        <v>491</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>186</v>
+        <v>492</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>188</v>
+        <v>493</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>715</v>
+        <v>458</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>716</v>
+        <v>459</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>717</v>
+        <v>460</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>799</v>
+        <v>558</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>800</v>
+        <v>551</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>801</v>
+        <v>552</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>913</v>
+        <v>619</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>914</v>
+        <v>620</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>915</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>233</v>
+        <v>625</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>235</v>
+        <v>626</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>37</v>
+        <v>553</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>54</v>
+        <v>554</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>90</v>
+        <v>555</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>161</v>
+        <v>45</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>128</v>
+        <v>356</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>129</v>
+        <v>357</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>130</v>
+        <v>358</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>202</v>
+        <v>280</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>203</v>
+        <v>277</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>204</v>
+        <v>278</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>796</v>
+        <v>279</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>491</v>
+        <v>124</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>492</v>
+        <v>125</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>493</v>
+        <v>126</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>458</v>
+        <v>134</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>459</v>
+        <v>135</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>461</v>
+        <v>136</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>558</v>
+        <v>526</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>551</v>
+        <v>527</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="E167" s="1" t="s">
-        <v>550</v>
+        <v>860</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>619</v>
+        <v>251</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>620</v>
+        <v>252</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>625</v>
+        <v>248</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>626</v>
+        <v>249</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>553</v>
+        <v>281</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>554</v>
+        <v>282</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>555</v>
+        <v>283</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>556</v>
+        <v>284</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>371</v>
+        <v>75</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>372</v>
+        <v>76</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>373</v>
+        <v>77</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>356</v>
+        <v>164</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>357</v>
+        <v>165</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>358</v>
+        <v>166</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>280</v>
+        <v>39</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>277</v>
+        <v>55</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>279</v>
+        <v>91</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>124</v>
+        <v>589</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>125</v>
+        <v>590</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>127</v>
+        <v>591</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>134</v>
+        <v>44</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>136</v>
+        <v>92</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>526</v>
+        <v>844</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>527</v>
+        <v>845</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>860</v>
+        <v>846</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>248</v>
+        <v>353</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>249</v>
+        <v>354</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>250</v>
+        <v>355</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>281</v>
+        <v>731</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>161</v>
+        <v>41</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>282</v>
+        <v>732</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>284</v>
+        <v>733</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>75</v>
+        <v>301</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>76</v>
+        <v>302</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>78</v>
+        <v>303</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>39</v>
+        <v>683</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>55</v>
+        <v>682</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>91</v>
+        <v>689</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>589</v>
+        <v>711</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>590</v>
+        <v>712</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>591</v>
+        <v>713</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>44</v>
+        <v>199</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E184" s="1" t="s">
-        <v>46</v>
+        <v>201</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>844</v>
+        <v>47</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>845</v>
+        <v>58</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>846</v>
+        <v>94</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>274</v>
+        <v>691</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>275</v>
+        <v>692</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>276</v>
+        <v>699</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>869</v>
+        <v>415</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>870</v>
+        <v>416</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>871</v>
+        <v>417</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>353</v>
+        <v>415</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>354</v>
+        <v>416</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>355</v>
+        <v>417</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>731</v>
+        <v>254</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>732</v>
+        <v>255</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>733</v>
+        <v>256</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>301</v>
+        <v>432</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>302</v>
+        <v>433</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>303</v>
+        <v>434</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>160</v>
+        <v>559</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>162</v>
+        <v>560</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>561</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>683</v>
+        <v>307</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>682</v>
+        <v>308</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="E192" s="1" t="s">
-        <v>686</v>
+        <v>309</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>711</v>
+        <v>824</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>712</v>
+        <v>825</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="E193" s="1" t="s">
-        <v>714</v>
+        <v>826</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>199</v>
+        <v>114</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>200</v>
+        <v>115</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>201</v>
+        <v>116</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>47</v>
+        <v>485</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>58</v>
+        <v>486</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>94</v>
+        <v>487</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>767</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>691</v>
+        <v>175</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>692</v>
+        <v>176</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="E196" s="1" t="s">
-        <v>693</v>
+        <v>178</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>415</v>
+        <v>316</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>416</v>
+        <v>317</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>417</v>
+        <v>318</v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>415</v>
+        <v>182</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>416</v>
+        <v>183</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>417</v>
+        <v>184</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>254</v>
+        <v>679</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>255</v>
+        <v>680</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>256</v>
+        <v>688</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>257</v>
+        <v>681</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>432</v>
+        <v>579</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>433</v>
+        <v>580</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="E200" s="1" t="s">
-        <v>435</v>
+        <v>581</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>559</v>
+        <v>469</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>560</v>
+        <v>470</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="E201" s="1" t="s">
-        <v>562</v>
+        <v>471</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>307</v>
+        <v>261</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>308</v>
+        <v>262</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>309</v>
+        <v>263</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>824</v>
+        <v>616</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>825</v>
+        <v>617</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>826</v>
+        <v>618</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>114</v>
+        <v>205</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>115</v>
+        <v>206</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>116</v>
+        <v>207</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>485</v>
+        <v>847</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>486</v>
+        <v>848</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="E205" s="1" t="s">
-        <v>767</v>
+        <v>849</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>175</v>
+        <v>557</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>176</v>
+        <v>548</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>178</v>
+        <v>549</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="207" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>316</v>
+        <v>332</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="208" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>182</v>
+        <v>566</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>183</v>
+        <v>571</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>184</v>
+        <v>572</v>
       </c>
     </row>
     <row r="209" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>679</v>
+        <v>494</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>680</v>
+        <v>496</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="E209" s="1" t="s">
-        <v>681</v>
+        <v>498</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>579</v>
+        <v>764</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>28</v>
+        <v>918</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>580</v>
+        <v>765</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>581</v>
+        <v>766</v>
       </c>
     </row>
     <row r="211" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>469</v>
+        <v>610</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>470</v>
+        <v>611</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>471</v>
+        <v>612</v>
       </c>
     </row>
     <row r="212" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>261</v>
+        <v>671</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>262</v>
+        <v>672</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>263</v>
+        <v>677</v>
       </c>
     </row>
     <row r="213" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>616</v>
+        <v>755</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>617</v>
+        <v>756</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>618</v>
+        <v>757</v>
       </c>
     </row>
     <row r="214" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>206</v>
+        <v>343</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>207</v>
+        <v>344</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>795</v>
+        <v>345</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>847</v>
+        <v>541</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>848</v>
+        <v>542</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>849</v>
+        <v>543</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>917</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>557</v>
+        <v>35</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>548</v>
+        <v>56</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>549</v>
+        <v>95</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>550</v>
+        <v>36</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>332</v>
+        <v>578</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>322</v>
+        <v>437</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>323</v>
+        <v>438</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="218" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>566</v>
+        <v>656</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>571</v>
+        <v>651</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>572</v>
+        <v>659</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>494</v>
+        <v>752</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>496</v>
+        <v>753</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>498</v>
+        <v>754</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>764</v>
+        <v>604</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>918</v>
+        <v>45</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>765</v>
+        <v>605</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>766</v>
+        <v>606</v>
       </c>
     </row>
     <row r="221" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>610</v>
+        <v>536</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>611</v>
+        <v>537</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>612</v>
+        <v>538</v>
       </c>
     </row>
     <row r="222" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>671</v>
+        <v>428</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>672</v>
+        <v>429</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>677</v>
+        <v>430</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>755</v>
+        <v>266</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>756</v>
+        <v>264</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>757</v>
+        <v>265</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>342</v>
+        <v>168</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>343</v>
+        <v>169</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>345</v>
+        <v>170</v>
       </c>
     </row>
     <row r="225" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>541</v>
+        <v>662</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>542</v>
+        <v>663</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>543</v>
+        <v>664</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>917</v>
+        <v>666</v>
       </c>
     </row>
     <row r="226" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>35</v>
+        <v>421</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>56</v>
+        <v>422</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>95</v>
+        <v>423</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>36</v>
+        <v>540</v>
       </c>
     </row>
     <row r="227" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>578</v>
+        <v>65</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>437</v>
+        <v>66</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>438</v>
+        <v>67</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>436</v>
+        <v>68</v>
       </c>
     </row>
     <row r="228" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>656</v>
+        <v>788</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>651</v>
+        <v>789</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>661</v>
+        <v>790</v>
       </c>
     </row>
     <row r="229" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>752</v>
+        <v>648</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>753</v>
+        <v>653</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>754</v>
+        <v>654</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="230" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>604</v>
+        <v>862</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>605</v>
+        <v>863</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>606</v>
+        <v>864</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>865</v>
       </c>
     </row>
     <row r="231" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>536</v>
+        <v>869</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>537</v>
+        <v>870</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>538</v>
+        <v>871</v>
       </c>
     </row>
     <row r="232" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>428</v>
+        <v>874</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>429</v>
+        <v>875</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>431</v>
+        <v>876</v>
       </c>
     </row>
     <row r="233" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>266</v>
+        <v>877</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>264</v>
+        <v>878</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>265</v>
+        <v>881</v>
       </c>
     </row>
     <row r="234" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>168</v>
+        <v>879</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>169</v>
+        <v>880</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>170</v>
+        <v>882</v>
       </c>
     </row>
     <row r="235" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>662</v>
+        <v>887</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>663</v>
+        <v>888</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>666</v>
+        <v>889</v>
       </c>
     </row>
     <row r="236" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
-        <v>421</v>
+        <v>890</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>422</v>
+        <v>891</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>540</v>
+        <v>909</v>
       </c>
     </row>
     <row r="237" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
-        <v>65</v>
+        <v>906</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>66</v>
+        <v>907</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E237" s="1" t="s">
-        <v>68</v>
+        <v>908</v>
       </c>
     </row>
     <row r="238" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
-        <v>788</v>
+        <v>910</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>789</v>
+        <v>911</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>790</v>
+        <v>912</v>
       </c>
     </row>
     <row r="239" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>648</v>
+        <v>913</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>653</v>
+        <v>914</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>654</v>
+        <v>915</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A240" s="1" t="s">
-        <v>920</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>921</v>
-      </c>
-      <c r="D240" s="1" t="s">
-        <v>922</v>
+        <v>916</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F230" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F239">
-      <sortCondition ref="A1:A239"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F229">
+      <sortCondition ref="A1:A229"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Revert "Revert "update to tracking sheet""
This reverts commit 5dbc501a8b2917363ff9e1452d5d2ac04fb16963.
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1421FC13-F323-4240-B1C3-DD50B0564663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EF7758-7BD4-BD44-9ED6-D7CED91E3091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="923">
   <si>
     <t>M-Number</t>
   </si>
@@ -2841,6 +2841,18 @@
   </si>
   <si>
     <t>Literary Work+B193</t>
+  </si>
+  <si>
+    <t>cf psn-rbur</t>
+  </si>
+  <si>
+    <t>Miller, Sissy</t>
+  </si>
+  <si>
+    <t>psn-smil</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-smil</t>
   </si>
 </sst>
 </file>
@@ -3250,11 +3262,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B14" sqref="B14"/>
+      <selection pane="topRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3496,6 +3508,9 @@
       <c r="F12" s="5">
         <v>6</v>
       </c>
+      <c r="G12" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -3930,6 +3945,12 @@
     <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="H36" s="1" t="s">
         <v>798</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F37" s="5">
+        <f>SUM(F3:F34)</f>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -3946,11 +3967,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
-  <dimension ref="A1:F239"/>
+  <dimension ref="A1:F240"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D240" sqref="D240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4072,6 +4093,9 @@
       <c r="D7" s="1" t="s">
         <v>748</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>919</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -4238,3285 +4262,3299 @@
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>380</v>
+        <v>862</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>381</v>
+        <v>863</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>382</v>
+        <v>864</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>865</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>814</v>
+        <v>380</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>815</v>
+        <v>381</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>820</v>
+        <v>382</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>131</v>
+        <v>814</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>132</v>
+        <v>815</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>133</v>
+        <v>816</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>362</v>
+        <v>131</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>363</v>
+        <v>132</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>364</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>643</v>
+        <v>874</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>642</v>
+        <v>875</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>644</v>
+        <v>876</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>633</v>
+        <v>368</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>634</v>
+        <v>369</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>635</v>
+        <v>370</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>82</v>
+        <v>643</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>83</v>
+        <v>642</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>85</v>
+        <v>644</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>495</v>
+        <v>633</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>497</v>
+        <v>634</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>499</v>
+        <v>635</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>743</v>
+        <v>82</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>744</v>
+        <v>83</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>227</v>
+        <v>495</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>228</v>
+        <v>497</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>229</v>
+        <v>499</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>365</v>
+        <v>743</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>366</v>
+        <v>744</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>142</v>
+        <v>365</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>141</v>
+        <v>366</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>224</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>779</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="B37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="38" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="B38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>776</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>777</v>
+        <v>69</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>512</v>
+        <v>33</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>515</v>
+        <v>51</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>523</v>
+        <v>776</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="B46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="47" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="B47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>758</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>762</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="B48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>569</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>475</v>
+        <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>639</v>
+        <v>100</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>641</v>
+        <v>101</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>640</v>
+        <v>102</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>850</v>
+        <v>383</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>851</v>
+        <v>384</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>852</v>
+        <v>385</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>622</v>
+        <v>639</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>623</v>
+        <v>641</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>624</v>
+        <v>640</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>236</v>
+        <v>850</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>237</v>
+        <v>851</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>238</v>
+        <v>852</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>38</v>
+        <v>622</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>52</v>
+        <v>623</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>93</v>
+        <v>624</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>304</v>
+        <v>236</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>305</v>
+        <v>237</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>306</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>607</v>
+        <v>38</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>608</v>
+        <v>52</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>609</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>768</v>
+        <v>304</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>769</v>
+        <v>305</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>772</v>
+        <v>306</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>821</v>
+        <v>607</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>822</v>
+        <v>608</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>823</v>
+        <v>609</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>476</v>
+        <v>768</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>477</v>
+        <v>769</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>478</v>
+        <v>772</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>359</v>
+        <v>821</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>360</v>
+        <v>822</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>361</v>
+        <v>823</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>157</v>
+        <v>476</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>158</v>
+        <v>477</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>159</v>
+        <v>478</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>785</v>
+        <v>359</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>786</v>
+        <v>360</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>787</v>
+        <v>361</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>411</v>
+        <v>157</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>412</v>
+        <v>158</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>414</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>837</v>
+        <v>785</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>838</v>
+        <v>786</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>839</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>840</v>
+        <v>787</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>531</v>
+        <v>411</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>532</v>
+        <v>412</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>533</v>
+        <v>413</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>258</v>
+        <v>837</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>259</v>
+        <v>838</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>260</v>
+        <v>839</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>840</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>694</v>
+        <v>531</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>695</v>
+        <v>532</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>696</v>
+        <v>533</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>455</v>
+        <v>694</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>456</v>
+        <v>695</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>457</v>
+        <v>700</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>462</v>
+        <v>696</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>137</v>
+        <v>244</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>138</v>
+        <v>242</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>139</v>
+        <v>243</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>312</v>
+        <v>455</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>313</v>
+        <v>456</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>315</v>
+        <v>457</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>189</v>
+        <v>137</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>161</v>
+        <v>45</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>190</v>
+        <v>138</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>247</v>
+        <v>312</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>112</v>
+        <v>313</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>113</v>
+        <v>315</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>564</v>
+        <v>189</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>568</v>
+        <v>190</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>570</v>
+        <v>191</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>319</v>
+        <v>247</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>320</v>
+        <v>112</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>321</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>735</v>
+        <v>564</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>737</v>
+        <v>568</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>866</v>
+        <v>570</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>673</v>
+        <v>319</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>674</v>
+        <v>320</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>678</v>
+        <v>321</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>398</v>
+        <v>735</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>399</v>
+        <v>737</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>400</v>
+        <v>739</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>866</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>645</v>
+        <v>673</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>650</v>
+        <v>674</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>657</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>661</v>
+        <v>678</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>646</v>
+        <v>398</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>649</v>
+        <v>399</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>661</v>
+        <v>400</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>479</v>
+        <v>645</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>480</v>
+        <v>650</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>481</v>
+        <v>657</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>517</v>
+        <v>646</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>518</v>
+        <v>649</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>519</v>
+        <v>658</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>508</v>
+        <v>479</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>509</v>
+        <v>480</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>510</v>
+        <v>481</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>505</v>
+        <v>518</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>155</v>
+        <v>508</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>156</v>
+        <v>509</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>830</v>
+        <v>510</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>511</v>
+        <v>879</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>513</v>
+        <v>880</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>514</v>
+        <v>882</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>613</v>
+        <v>506</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>614</v>
+        <v>505</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>615</v>
+        <v>504</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>298</v>
+        <v>155</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>299</v>
+        <v>156</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>300</v>
+        <v>830</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>405</v>
+        <v>511</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>406</v>
+        <v>513</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>407</v>
+        <v>514</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>405</v>
+        <v>613</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>406</v>
+        <v>614</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>407</v>
+        <v>615</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>106</v>
+        <v>298</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>107</v>
+        <v>299</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>108</v>
+        <v>300</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>34</v>
+        <v>405</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>53</v>
+        <v>406</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>87</v>
+        <v>407</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>853</v>
+        <v>405</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>854</v>
+        <v>406</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>855</v>
+        <v>407</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>539</v>
+        <v>106</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>534</v>
+        <v>107</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>535</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>448</v>
+        <v>34</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>392</v>
+        <v>53</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>394</v>
+        <v>87</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>697</v>
+        <v>853</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>698</v>
+        <v>854</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>702</v>
+        <v>855</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>324</v>
+        <v>539</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>325</v>
+        <v>534</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>326</v>
+        <v>535</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>267</v>
+        <v>448</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>268</v>
+        <v>392</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>269</v>
+        <v>393</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>270</v>
+        <v>394</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>42</v>
+        <v>697</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>57</v>
+        <v>698</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>88</v>
+        <v>701</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>43</v>
+        <v>702</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>463</v>
+        <v>324</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>464</v>
+        <v>325</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>856</v>
+        <v>326</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>725</v>
+        <v>267</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>726</v>
+        <v>268</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>727</v>
+        <v>269</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>595</v>
+        <v>42</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>592</v>
+        <v>57</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>593</v>
+        <v>88</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>221</v>
+        <v>463</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>222</v>
+        <v>464</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>223</v>
+        <v>465</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>856</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>287</v>
+        <v>725</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>288</v>
+        <v>726</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>290</v>
+        <v>727</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>684</v>
+        <v>595</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>685</v>
+        <v>592</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>687</v>
+        <v>593</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>665</v>
+        <v>221</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>668</v>
+        <v>222</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>667</v>
+        <v>223</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>346</v>
+        <v>287</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>347</v>
+        <v>288</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>348</v>
+        <v>289</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>500</v>
+        <v>684</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>501</v>
+        <v>685</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>502</v>
+        <v>690</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>503</v>
+        <v>687</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>213</v>
+        <v>665</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>214</v>
+        <v>668</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>215</v>
+        <v>675</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>216</v>
+        <v>667</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>217</v>
+        <v>346</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>218</v>
+        <v>347</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>220</v>
+        <v>348</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>827</v>
+        <v>500</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>828</v>
+        <v>501</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>829</v>
+        <v>502</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>310</v>
+        <v>213</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>311</v>
+        <v>214</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>314</v>
+        <v>215</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>582</v>
+        <v>217</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>583</v>
+        <v>218</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>584</v>
+        <v>219</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>103</v>
+        <v>827</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>104</v>
+        <v>828</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>105</v>
+        <v>829</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>636</v>
+        <v>310</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>637</v>
+        <v>311</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>638</v>
+        <v>314</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>482</v>
+        <v>582</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>483</v>
+        <v>583</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>484</v>
+        <v>584</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>488</v>
+        <v>906</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>489</v>
+        <v>907</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>490</v>
+        <v>908</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>291</v>
+        <v>103</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>285</v>
+        <v>104</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>286</v>
+        <v>105</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>594</v>
+        <v>636</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>596</v>
+        <v>637</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>597</v>
+        <v>638</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>520</v>
+        <v>482</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>521</v>
+        <v>483</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>522</v>
+        <v>484</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>445</v>
+        <v>488</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>446</v>
+        <v>489</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>447</v>
+        <v>490</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>770</v>
+        <v>291</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>771</v>
+        <v>285</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>773</v>
+        <v>286</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>171</v>
+        <v>594</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>187</v>
+        <v>596</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>172</v>
+        <v>597</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>192</v>
+        <v>910</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>193</v>
+        <v>911</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>195</v>
+        <v>912</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>292</v>
+        <v>520</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>293</v>
+        <v>521</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>294</v>
+        <v>522</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>146</v>
+        <v>445</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>147</v>
+        <v>446</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>148</v>
+        <v>447</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>350</v>
+        <v>770</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>351</v>
+        <v>771</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>352</v>
+        <v>773</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>376</v>
+        <v>171</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>327</v>
+        <v>187</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>328</v>
+        <v>172</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>418</v>
+        <v>192</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>419</v>
+        <v>193</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>420</v>
+        <v>194</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>97</v>
+        <v>292</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>98</v>
+        <v>293</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>99</v>
+        <v>294</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>395</v>
+        <v>146</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>396</v>
+        <v>147</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>397</v>
+        <v>148</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>295</v>
+        <v>350</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>296</v>
+        <v>351</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>297</v>
+        <v>352</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>817</v>
+        <v>376</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>818</v>
+        <v>327</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>819</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>820</v>
+        <v>328</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>472</v>
+        <v>418</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>473</v>
+        <v>419</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>474</v>
+        <v>420</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>565</v>
+        <v>890</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>598</v>
+        <v>891</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>599</v>
+        <v>909</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>707</v>
+        <v>395</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>708</v>
+        <v>396</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>709</v>
+        <v>397</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>734</v>
+        <v>295</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>736</v>
+        <v>296</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>738</v>
+        <v>297</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>149</v>
+        <v>817</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>150</v>
+        <v>818</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>151</v>
+        <v>819</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>152</v>
+        <v>820</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>424</v>
+        <v>472</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>425</v>
+        <v>473</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>427</v>
+        <v>474</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>89</v>
+        <v>64</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>669</v>
+        <v>565</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>670</v>
+        <v>598</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>676</v>
+        <v>599</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>831</v>
+        <v>707</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>832</v>
+        <v>708</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>833</v>
+        <v>710</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>271</v>
+        <v>734</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>272</v>
+        <v>736</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>273</v>
+        <v>738</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>728</v>
+        <v>149</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>729</v>
+        <v>150</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>730</v>
+        <v>151</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>722</v>
+        <v>424</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>723</v>
+        <v>425</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>724</v>
+        <v>426</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>239</v>
+        <v>48</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>241</v>
+        <v>59</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>246</v>
+        <v>89</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>185</v>
+        <v>669</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>186</v>
+        <v>670</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>188</v>
+        <v>676</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>715</v>
+        <v>831</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>716</v>
+        <v>832</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>717</v>
+        <v>833</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>799</v>
+        <v>877</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>800</v>
+        <v>878</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>801</v>
+        <v>881</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>233</v>
+        <v>271</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>234</v>
+        <v>272</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>37</v>
+        <v>887</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>54</v>
+        <v>888</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>90</v>
+        <v>889</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>389</v>
+        <v>728</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>161</v>
+        <v>41</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>390</v>
+        <v>729</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>391</v>
+        <v>730</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>128</v>
+        <v>722</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>129</v>
+        <v>723</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>130</v>
+        <v>724</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>202</v>
+        <v>239</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>203</v>
+        <v>241</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>204</v>
+        <v>240</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>796</v>
+        <v>246</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>491</v>
+        <v>185</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>492</v>
+        <v>186</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>493</v>
+        <v>188</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>458</v>
+        <v>715</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>459</v>
+        <v>716</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>461</v>
+        <v>717</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>558</v>
+        <v>799</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>551</v>
+        <v>800</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>550</v>
+        <v>801</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>619</v>
+        <v>913</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>620</v>
+        <v>914</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>915</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>625</v>
+        <v>233</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>626</v>
+        <v>234</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>553</v>
+        <v>37</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>554</v>
+        <v>54</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>556</v>
+        <v>90</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>371</v>
+        <v>389</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>372</v>
+        <v>390</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>373</v>
+        <v>391</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>356</v>
+        <v>128</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>357</v>
+        <v>129</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>358</v>
+        <v>130</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>280</v>
+        <v>202</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>277</v>
+        <v>203</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>278</v>
+        <v>204</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>279</v>
+        <v>796</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>124</v>
+        <v>491</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>125</v>
+        <v>492</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>127</v>
+        <v>493</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>134</v>
+        <v>458</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>135</v>
+        <v>459</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>136</v>
+        <v>460</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>526</v>
+        <v>558</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>527</v>
+        <v>551</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>860</v>
+        <v>552</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>251</v>
+        <v>619</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>252</v>
+        <v>620</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>248</v>
+        <v>625</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>250</v>
+        <v>626</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>281</v>
+        <v>553</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>161</v>
+        <v>41</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>282</v>
+        <v>554</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>283</v>
+        <v>555</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>284</v>
+        <v>556</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>75</v>
+        <v>371</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>76</v>
+        <v>372</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>78</v>
+        <v>373</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>164</v>
+        <v>356</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>161</v>
+        <v>45</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>165</v>
+        <v>357</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>166</v>
+        <v>358</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>39</v>
+        <v>280</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>55</v>
+        <v>277</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>91</v>
+        <v>278</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>589</v>
+        <v>124</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>590</v>
+        <v>125</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>591</v>
+        <v>126</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>844</v>
+        <v>526</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>845</v>
+        <v>527</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>846</v>
+        <v>860</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>353</v>
+        <v>248</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>354</v>
+        <v>249</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>355</v>
+        <v>250</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>731</v>
+        <v>281</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>732</v>
+        <v>282</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>733</v>
+        <v>283</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>301</v>
+        <v>75</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>302</v>
+        <v>76</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>303</v>
+        <v>77</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>683</v>
+        <v>39</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>682</v>
+        <v>55</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>686</v>
+        <v>91</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>711</v>
+        <v>589</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>712</v>
+        <v>590</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>714</v>
+        <v>591</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>199</v>
+        <v>44</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>201</v>
+        <v>92</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>47</v>
+        <v>844</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>58</v>
+        <v>845</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>94</v>
+        <v>846</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>691</v>
+        <v>274</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>692</v>
+        <v>275</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>693</v>
+        <v>276</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>415</v>
+        <v>869</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>416</v>
+        <v>870</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>417</v>
+        <v>871</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>416</v>
+        <v>354</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>417</v>
+        <v>355</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>254</v>
+        <v>731</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>255</v>
+        <v>732</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="E189" s="1" t="s">
-        <v>257</v>
+        <v>733</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>432</v>
+        <v>301</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>433</v>
+        <v>302</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>435</v>
+        <v>303</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>559</v>
+        <v>160</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>560</v>
+        <v>162</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="E191" s="1" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>307</v>
+        <v>683</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>308</v>
+        <v>682</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>309</v>
+        <v>689</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>824</v>
+        <v>711</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>825</v>
+        <v>712</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>826</v>
+        <v>713</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>114</v>
+        <v>199</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>115</v>
+        <v>200</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>116</v>
+        <v>201</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>485</v>
+        <v>47</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>486</v>
+        <v>58</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="E195" s="1" t="s">
-        <v>767</v>
+        <v>94</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>175</v>
+        <v>691</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>176</v>
+        <v>692</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>178</v>
+        <v>699</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>316</v>
+        <v>415</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>317</v>
+        <v>416</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>318</v>
+        <v>417</v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>182</v>
+        <v>415</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>183</v>
+        <v>416</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>184</v>
+        <v>417</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>679</v>
+        <v>254</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>680</v>
+        <v>255</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>688</v>
+        <v>256</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>681</v>
+        <v>257</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>579</v>
+        <v>432</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>580</v>
+        <v>433</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>581</v>
+        <v>434</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>469</v>
+        <v>559</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>470</v>
+        <v>560</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>471</v>
+        <v>561</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>261</v>
+        <v>307</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>262</v>
+        <v>308</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>263</v>
+        <v>309</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>616</v>
+        <v>824</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>617</v>
+        <v>825</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>618</v>
+        <v>826</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>205</v>
+        <v>114</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>206</v>
+        <v>115</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>795</v>
+        <v>116</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>847</v>
+        <v>485</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>848</v>
+        <v>486</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>849</v>
+        <v>487</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>767</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>557</v>
+        <v>175</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>548</v>
+        <v>176</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="E206" s="1" t="s">
-        <v>550</v>
+        <v>178</v>
       </c>
     </row>
     <row r="207" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="208" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>566</v>
+        <v>182</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>571</v>
+        <v>183</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>572</v>
+        <v>184</v>
       </c>
     </row>
     <row r="209" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>494</v>
+        <v>679</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>496</v>
+        <v>680</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>498</v>
+        <v>688</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>764</v>
+        <v>579</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>918</v>
+        <v>28</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>765</v>
+        <v>580</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>766</v>
+        <v>581</v>
       </c>
     </row>
     <row r="211" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>610</v>
+        <v>469</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>611</v>
+        <v>470</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>612</v>
+        <v>471</v>
       </c>
     </row>
     <row r="212" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>671</v>
+        <v>261</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>672</v>
+        <v>262</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>677</v>
+        <v>263</v>
       </c>
     </row>
     <row r="213" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>755</v>
+        <v>616</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>756</v>
+        <v>617</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>757</v>
+        <v>618</v>
       </c>
     </row>
     <row r="214" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>342</v>
+        <v>205</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>343</v>
+        <v>206</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>344</v>
+        <v>207</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>345</v>
+        <v>795</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>541</v>
+        <v>847</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>542</v>
+        <v>848</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="E215" s="1" t="s">
-        <v>917</v>
+        <v>849</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>35</v>
+        <v>557</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>56</v>
+        <v>548</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>95</v>
+        <v>549</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>36</v>
+        <v>550</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>578</v>
+        <v>332</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>437</v>
+        <v>322</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="E217" s="1" t="s">
-        <v>436</v>
+        <v>323</v>
       </c>
     </row>
     <row r="218" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>656</v>
+        <v>566</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>651</v>
+        <v>571</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E218" s="1" t="s">
-        <v>661</v>
+        <v>572</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>752</v>
+        <v>494</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>753</v>
+        <v>496</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>754</v>
+        <v>498</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>604</v>
+        <v>764</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>45</v>
+        <v>918</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>605</v>
+        <v>765</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>606</v>
+        <v>766</v>
       </c>
     </row>
     <row r="221" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>536</v>
+        <v>610</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>537</v>
+        <v>611</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>538</v>
+        <v>612</v>
       </c>
     </row>
     <row r="222" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>428</v>
+        <v>671</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>429</v>
+        <v>672</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="E222" s="1" t="s">
-        <v>431</v>
+        <v>677</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>266</v>
+        <v>755</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>264</v>
+        <v>756</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>265</v>
+        <v>757</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>168</v>
+        <v>342</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>169</v>
+        <v>343</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>170</v>
+        <v>344</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="225" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>662</v>
+        <v>541</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>663</v>
+        <v>542</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>664</v>
+        <v>543</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>666</v>
+        <v>917</v>
       </c>
     </row>
     <row r="226" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>421</v>
+        <v>35</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>422</v>
+        <v>56</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>423</v>
+        <v>95</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>540</v>
+        <v>36</v>
       </c>
     </row>
     <row r="227" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>65</v>
+        <v>578</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>66</v>
+        <v>437</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>67</v>
+        <v>438</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>68</v>
+        <v>436</v>
       </c>
     </row>
     <row r="228" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>788</v>
+        <v>656</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>789</v>
+        <v>651</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>790</v>
+        <v>659</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="229" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>648</v>
+        <v>752</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>653</v>
+        <v>753</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="E229" s="1" t="s">
-        <v>655</v>
+        <v>754</v>
       </c>
     </row>
     <row r="230" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>862</v>
+        <v>604</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>863</v>
+        <v>605</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>864</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>865</v>
+        <v>606</v>
       </c>
     </row>
     <row r="231" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>869</v>
+        <v>536</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>870</v>
+        <v>537</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>871</v>
+        <v>538</v>
       </c>
     </row>
     <row r="232" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>874</v>
+        <v>428</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>875</v>
+        <v>429</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>876</v>
+        <v>430</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="233" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>877</v>
+        <v>266</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>878</v>
+        <v>264</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>881</v>
+        <v>265</v>
       </c>
     </row>
     <row r="234" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>879</v>
+        <v>168</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>880</v>
+        <v>169</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>882</v>
+        <v>170</v>
       </c>
     </row>
     <row r="235" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>887</v>
+        <v>662</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>888</v>
+        <v>663</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>889</v>
+        <v>664</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>666</v>
       </c>
     </row>
     <row r="236" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
-        <v>890</v>
+        <v>421</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>891</v>
+        <v>422</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>909</v>
+        <v>423</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="237" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
-        <v>906</v>
+        <v>65</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>907</v>
+        <v>66</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>908</v>
+        <v>67</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="238" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
-        <v>910</v>
+        <v>788</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>911</v>
+        <v>789</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>912</v>
+        <v>790</v>
       </c>
     </row>
     <row r="239" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>913</v>
+        <v>648</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>914</v>
+        <v>653</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>915</v>
+        <v>654</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>916</v>
+        <v>655</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A240" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>922</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F230" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F229">
-      <sortCondition ref="A1:A229"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F239">
+      <sortCondition ref="A1:A239"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
m1-8-7 through -10: update with @facs attribs for each paragraph-like textual unit
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C990E0-FE58-0147-A555-DF073FEF3D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933500A0-B2F8-784D-BDE8-5DAB21FF4071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="935">
   <si>
     <t>M-Number</t>
   </si>
@@ -3315,7 +3315,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H7" sqref="H7"/>
+      <selection pane="topRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3517,6 +3517,9 @@
       <c r="G8" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="H8" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="J8" s="1" t="s">
         <v>885</v>
       </c>
@@ -3543,6 +3546,9 @@
       <c r="G9" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="H9" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -3566,6 +3572,9 @@
       <c r="G10" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="H10" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -3589,6 +3598,9 @@
       <c r="G11" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="H11" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -3610,6 +3622,9 @@
         <v>6</v>
       </c>
       <c r="G12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
m47 and m48.xml: update with @facs attribs for each paragraph-like textual unitand minor update to m45.xml
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF0FE1B-9B9C-6849-90F1-A48318E57851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B95B886-33F9-6C40-B003-79494CC999C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="945">
   <si>
     <t>M-Number</t>
   </si>
@@ -3345,7 +3345,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G12" sqref="G12"/>
+      <selection pane="topRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3709,6 +3709,9 @@
       <c r="G16" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="H16" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="J16" s="1" t="s">
         <v>796</v>
       </c>
@@ -3735,6 +3738,9 @@
       <c r="G17" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="H17" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -3753,9 +3759,12 @@
         <v>938</v>
       </c>
       <c r="F18" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>31</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -4129,7 +4138,7 @@
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F37" s="5">
         <f>SUM(F3:F34)</f>
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -4171,8 +4180,8 @@
   <dimension ref="A1:F240"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A241" sqref="A241"/>
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E240" sqref="E240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
m50.xml: adding @facs attributes
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B95B886-33F9-6C40-B003-79494CC999C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CAA0AA-9034-FB42-BABD-F5E2AD54D46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="945">
   <si>
     <t>M-Number</t>
   </si>
@@ -3345,7 +3345,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F19" sqref="F19"/>
+      <selection pane="topRight" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3767,6 +3767,9 @@
       <c r="H18" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="I18" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="J18" s="1" t="s">
         <v>29</v>
       </c>
@@ -3791,6 +3794,9 @@
         <v>8</v>
       </c>
       <c r="G19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>31</v>
       </c>
       <c r="J19" s="1" t="s">

</xml_diff>

<commit_message>
m51.xml: added @facs attributes
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CAA0AA-9034-FB42-BABD-F5E2AD54D46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D197B10F-873B-1240-A7D6-67C250FDCB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="948">
   <si>
     <t>M-Number</t>
   </si>
@@ -2919,6 +2919,15 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m54-manifest.json</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m108-manifest.json</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m109-manifest.json</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m110-manifest.json</t>
   </si>
 </sst>
 </file>
@@ -3343,9 +3352,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I19" sqref="I19"/>
+      <selection pane="topRight" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3825,6 +3834,9 @@
       <c r="G20" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="H20" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="J20" s="1" t="s">
         <v>210</v>
       </c>
@@ -3851,6 +3863,9 @@
       <c r="G21" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="H21" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="J21" s="1" t="s">
         <v>211</v>
       </c>
@@ -3940,6 +3955,9 @@
       <c r="D25" s="1" t="s">
         <v>439</v>
       </c>
+      <c r="E25" s="6" t="s">
+        <v>945</v>
+      </c>
       <c r="F25" s="5">
         <v>7</v>
       </c>
@@ -3960,6 +3978,9 @@
       <c r="D26" s="1" t="s">
         <v>529</v>
       </c>
+      <c r="E26" s="6" t="s">
+        <v>946</v>
+      </c>
       <c r="F26" s="5">
         <v>9</v>
       </c>
@@ -3982,6 +4003,9 @@
       </c>
       <c r="D27" s="1" t="s">
         <v>546</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>947</v>
       </c>
       <c r="F27" s="5">
         <v>5</v>
@@ -4175,9 +4199,13 @@
     <hyperlink ref="E23" r:id="rId18" xr:uid="{A1667000-7830-844E-9086-11CF3B4D55B2}"/>
     <hyperlink ref="E24" r:id="rId19" xr:uid="{904D1463-1E2F-3240-BB21-D1122114E897}"/>
     <hyperlink ref="E15" r:id="rId20" xr:uid="{F41C189A-7D88-9040-97D1-0CBF3500C2F0}"/>
+    <hyperlink ref="E25" r:id="rId21" xr:uid="{320A6C45-ED98-644E-A93B-A086FC794F4F}"/>
+    <hyperlink ref="E26:E27" r:id="rId22" display="https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m108-manifest.json" xr:uid="{5FDF83DE-B05E-6648-83B6-79117939C2BD}"/>
+    <hyperlink ref="E26" r:id="rId23" xr:uid="{DDBE96EE-FA90-E444-B89A-BB7CF5AE1D03}"/>
+    <hyperlink ref="E27" r:id="rId24" xr:uid="{E4B7B736-B87B-BB46-8F24-C9894D56EA25}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId25"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
m54-3.xml: adding text from original transcription and @facs
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D197B10F-873B-1240-A7D6-67C250FDCB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC9F3D6-46F4-7F49-9253-E5B4D63EC319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="500" windowWidth="32340" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="2280" yWindow="500" windowWidth="38160" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="960">
   <si>
     <t>M-Number</t>
   </si>
@@ -2929,12 +2929,48 @@
   <si>
     <t>https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m110-manifest.json</t>
   </si>
+  <si>
+    <t>M54-1</t>
+  </si>
+  <si>
+    <t>M54-2</t>
+  </si>
+  <si>
+    <t>M54-3</t>
+  </si>
+  <si>
+    <t>M54-4</t>
+  </si>
+  <si>
+    <t>M54-5</t>
+  </si>
+  <si>
+    <t>M54-6</t>
+  </si>
+  <si>
+    <t>M54-7</t>
+  </si>
+  <si>
+    <t>M54-8</t>
+  </si>
+  <si>
+    <t>M54-9</t>
+  </si>
+  <si>
+    <t>M54-10</t>
+  </si>
+  <si>
+    <t>M54-11</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2972,13 +3008,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2990,11 +3038,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3014,8 +3063,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3350,11 +3403,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H22" sqref="H22"/>
+      <selection pane="topRight" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3935,240 +3988,318 @@
       <c r="E24" s="6" t="s">
         <v>944</v>
       </c>
-      <c r="F24" s="5">
-        <v>35</v>
-      </c>
       <c r="G24" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="H24" s="7" t="s">
+        <v>959</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>945</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F36" s="5">
         <v>7</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="H36" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E37" s="6" t="s">
         <v>946</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F37" s="5">
         <v>9</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G37" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="H37" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J37" s="1" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="38" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E38" s="6" t="s">
         <v>947</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F38" s="5">
         <v>5</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G38" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="H38" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F39" s="5">
         <v>5</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G39" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="40" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F40" s="5">
         <v>4</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G40" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="41" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F41" s="5">
         <v>7</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G41" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="42" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F42" s="5">
         <v>5</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G42" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="43" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>720</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>717</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>718</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F43" s="5">
         <v>2</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G43" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="44" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>741</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F44" s="5">
         <v>3</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G44" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="45" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>750</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F45" s="5">
         <v>8</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G45" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="J36" s="1" t="s">
+    <row r="47" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J47" s="1" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F37" s="5">
-        <f>SUM(F3:F34)</f>
-        <v>265</v>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F48" s="5">
+        <f>SUM(F3:F45)</f>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -4199,10 +4330,10 @@
     <hyperlink ref="E23" r:id="rId18" xr:uid="{A1667000-7830-844E-9086-11CF3B4D55B2}"/>
     <hyperlink ref="E24" r:id="rId19" xr:uid="{904D1463-1E2F-3240-BB21-D1122114E897}"/>
     <hyperlink ref="E15" r:id="rId20" xr:uid="{F41C189A-7D88-9040-97D1-0CBF3500C2F0}"/>
-    <hyperlink ref="E25" r:id="rId21" xr:uid="{320A6C45-ED98-644E-A93B-A086FC794F4F}"/>
-    <hyperlink ref="E26:E27" r:id="rId22" display="https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m108-manifest.json" xr:uid="{5FDF83DE-B05E-6648-83B6-79117939C2BD}"/>
-    <hyperlink ref="E26" r:id="rId23" xr:uid="{DDBE96EE-FA90-E444-B89A-BB7CF5AE1D03}"/>
-    <hyperlink ref="E27" r:id="rId24" xr:uid="{E4B7B736-B87B-BB46-8F24-C9894D56EA25}"/>
+    <hyperlink ref="E36" r:id="rId21" xr:uid="{320A6C45-ED98-644E-A93B-A086FC794F4F}"/>
+    <hyperlink ref="E37:E38" r:id="rId22" display="https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m108-manifest.json" xr:uid="{5FDF83DE-B05E-6648-83B6-79117939C2BD}"/>
+    <hyperlink ref="E37" r:id="rId23" xr:uid="{DDBE96EE-FA90-E444-B89A-BB7CF5AE1D03}"/>
+    <hyperlink ref="E38" r:id="rId24" xr:uid="{E4B7B736-B87B-BB46-8F24-C9894D56EA25}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId25"/>

</xml_diff>

<commit_message>
m54-8 and -9.xml: text and @facs
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B113D1B6-1B78-B144-9F41-E8409A3B7AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3B08D3-F5DE-C941-B8FF-5D8E47474640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="500" windowWidth="38160" windowHeight="26600" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="947">
   <si>
     <t>M-Number</t>
   </si>
@@ -2919,6 +2919,12 @@
   </si>
   <si>
     <t>M54, 6 of 11. [Anon: the pear shaped lute; on which the Queen herself once played...]. Typescript fragment, 1 fol.</t>
+  </si>
+  <si>
+    <t>M54, 8 of 11. [Anon: With that a joyous fellow issued]. Typescript fragment, 3 fols.</t>
+  </si>
+  <si>
+    <t>M54, 9 of 11. [Anon: The road led to the old graves...]. Typescript fragment, 8 fols.</t>
   </si>
 </sst>
 </file>
@@ -3360,9 +3366,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B30" sqref="B30"/>
+      <selection pane="topRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4011,24 +4017,42 @@
       <c r="E30" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="F30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>922</v>
       </c>
+      <c r="B31" s="1" t="s">
+        <v>945</v>
+      </c>
       <c r="C31" s="1" t="s">
         <v>934</v>
       </c>
       <c r="D31" s="6"/>
+      <c r="E31" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>923</v>
       </c>
+      <c r="B32" s="1" t="s">
+        <v>946</v>
+      </c>
       <c r="C32" s="1" t="s">
         <v>935</v>
       </c>
       <c r="D32" s="6"/>
+      <c r="E32" s="5">
+        <v>8</v>
+      </c>
     </row>
     <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
@@ -4259,7 +4283,7 @@
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E48" s="5">
         <f>SUM(E3:E45)</f>
-        <v>247</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
m1-8-1 and -2: v3 with key attributes for refs
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3B08D3-F5DE-C941-B8FF-5D8E47474640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674376BA-EF04-ED42-90B0-735314F715D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="947">
   <si>
     <t>M-Number</t>
   </si>
@@ -1141,12 +1141,6 @@
   </si>
   <si>
     <t>Check deletions on p. 14 - second para of deletions doesn't appear to be deleted on preview but perhaps this is just a limitation of the preview engine</t>
-  </si>
-  <si>
-    <t>Arthur, King</t>
-  </si>
-  <si>
-    <t>Lear, King</t>
   </si>
   <si>
     <t>Barge, The</t>
@@ -2925,6 +2919,12 @@
   </si>
   <si>
     <t>M54, 9 of 11. [Anon: The road led to the old graves...]. Typescript fragment, 8 fols.</t>
+  </si>
+  <si>
+    <t>Arthur (King)</t>
+  </si>
+  <si>
+    <t>King Lear</t>
   </si>
 </sst>
 </file>
@@ -3366,9 +3366,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D32" sqref="D32"/>
+      <selection pane="topRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3393,19 +3393,19 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>7</v>
@@ -3413,16 +3413,16 @@
     </row>
     <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E3" s="5">
         <v>9</v>
@@ -3436,16 +3436,16 @@
     </row>
     <row r="4" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E4" s="5">
         <v>12</v>
@@ -3459,16 +3459,16 @@
     </row>
     <row r="5" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E5" s="5">
         <v>15</v>
@@ -3482,16 +3482,16 @@
     </row>
     <row r="6" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E6" s="5">
         <v>9</v>
@@ -3505,16 +3505,16 @@
     </row>
     <row r="7" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E7" s="5">
         <v>4</v>
@@ -3526,21 +3526,21 @@
         <v>30</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E8" s="5">
         <v>6</v>
@@ -3552,21 +3552,21 @@
         <v>30</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="E9" s="5">
         <v>6</v>
@@ -3580,16 +3580,16 @@
     </row>
     <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
@@ -3603,16 +3603,16 @@
     </row>
     <row r="11" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>868</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>870</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E11" s="5">
         <v>3</v>
@@ -3626,16 +3626,16 @@
     </row>
     <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="E12" s="5">
         <v>6</v>
@@ -3652,13 +3652,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="E15" s="5">
         <v>10</v>
@@ -3670,7 +3670,7 @@
         <v>30</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -3678,13 +3678,13 @@
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="E16" s="5">
         <v>9</v>
@@ -3696,7 +3696,7 @@
         <v>30</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -3704,13 +3704,13 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="E17" s="5">
         <v>11</v>
@@ -3733,7 +3733,7 @@
         <v>21</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="E18" s="5">
         <v>3</v>
@@ -3762,7 +3762,7 @@
         <v>22</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="E19" s="5">
         <v>8</v>
@@ -3788,7 +3788,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="E20" s="5">
         <v>9</v>
@@ -3814,7 +3814,7 @@
         <v>24</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="E21" s="5">
         <v>9</v>
@@ -3840,7 +3840,7 @@
         <v>329</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="E22" s="5">
         <v>19</v>
@@ -3863,7 +3863,7 @@
         <v>330</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="E23" s="5">
         <v>26</v>
@@ -3880,33 +3880,33 @@
         <v>16</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="5">
@@ -3921,13 +3921,13 @@
     </row>
     <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="5">
@@ -3942,13 +3942,13 @@
     </row>
     <row r="27" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="5">
@@ -3963,13 +3963,13 @@
     </row>
     <row r="28" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="5">
@@ -3984,13 +3984,13 @@
     </row>
     <row r="29" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="5">
@@ -4005,13 +4005,13 @@
     </row>
     <row r="30" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="5">
@@ -4026,13 +4026,13 @@
     </row>
     <row r="31" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="5">
@@ -4041,13 +4041,13 @@
     </row>
     <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="5">
@@ -4056,28 +4056,28 @@
     </row>
     <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="D35" s="6"/>
     </row>
@@ -4086,13 +4086,13 @@
         <v>17</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="E36" s="5">
         <v>7</v>
@@ -4109,13 +4109,13 @@
         <v>18</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="E37" s="5">
         <v>9</v>
@@ -4132,13 +4132,13 @@
         <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="E38" s="5">
         <v>5</v>
@@ -4152,13 +4152,13 @@
     </row>
     <row r="39" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E39" s="5">
         <v>5</v>
@@ -4166,16 +4166,19 @@
       <c r="F39" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="G39" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E40" s="5">
         <v>4</v>
@@ -4183,16 +4186,19 @@
       <c r="F40" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="G40" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="41" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E41" s="5">
         <v>7</v>
@@ -4200,19 +4206,22 @@
       <c r="F41" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="G41" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="I41" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E42" s="5">
         <v>5</v>
@@ -4220,16 +4229,19 @@
       <c r="F42" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="G42" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="43" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="E43" s="5">
         <v>2</v>
@@ -4237,24 +4249,30 @@
       <c r="F43" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="G43" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="I43" s="1" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E44" s="5">
         <v>3</v>
       </c>
       <c r="F44" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4263,10 +4281,10 @@
         <v>20</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="E45" s="5">
         <v>8</v>
@@ -4274,10 +4292,13 @@
       <c r="F45" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="G45" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="I47" s="1" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -4328,9 +4349,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
   <dimension ref="A1:F240"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E240" sqref="E240"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4348,7 +4369,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
@@ -4365,19 +4386,19 @@
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4399,61 +4420,61 @@
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4500,7 +4521,7 @@
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>367</v>
+        <v>945</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>26</v>
@@ -4514,19 +4535,19 @@
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>686</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4565,106 +4586,106 @@
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>432</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>835</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>836</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>837</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4697,16 +4718,16 @@
     </row>
     <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4725,30 +4746,30 @@
     </row>
     <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>625</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4770,30 +4791,30 @@
     </row>
     <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>487</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>724</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>725</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -4882,16 +4903,16 @@
     </row>
     <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>759</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>760</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -4938,44 +4959,44 @@
     </row>
     <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -4994,58 +5015,58 @@
     </row>
     <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>741</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>554</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5081,61 +5102,61 @@
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>624</v>
-      </c>
       <c r="D52" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5182,58 +5203,58 @@
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>797</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>798</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5266,64 +5287,64 @@
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C65" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C66" s="1" t="s">
+      <c r="E66" s="1" t="s">
         <v>813</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>814</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5342,19 +5363,19 @@
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>677</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5376,19 +5397,19 @@
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5449,16 +5470,16 @@
     </row>
     <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>555</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5477,154 +5498,154 @@
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>721</v>
-      </c>
       <c r="E78" s="1" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>469</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>507</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C86" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>852</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C87" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="E87" s="1" t="s">
         <v>495</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5638,35 +5659,35 @@
         <v>150</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5685,30 +5706,30 @@
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5741,64 +5762,64 @@
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C98" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E98" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5851,47 +5872,47 @@
     </row>
     <row r="103" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5927,36 +5948,36 @@
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C108" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="E108" s="1" t="s">
         <v>668</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="E109" s="1" t="s">
         <v>648</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>651</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5975,19 +5996,19 @@
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C111" s="1" t="s">
+      <c r="E111" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6026,16 +6047,16 @@
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6054,30 +6075,30 @@
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>568</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>873</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>874</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6096,44 +6117,44 @@
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>619</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>472</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="D121" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6152,72 +6173,72 @@
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>510</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C127" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="D127" s="1" t="s">
         <v>751</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6295,7 +6316,7 @@
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>368</v>
+        <v>946</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>39</v>
@@ -6309,16 +6330,16 @@
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="D134" s="1" t="s">
         <v>409</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6337,30 +6358,30 @@
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D137" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6379,33 +6400,33 @@
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C139" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="E139" s="1" t="s">
         <v>794</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>795</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6427,47 +6448,47 @@
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C143" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="D143" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="D143" s="1" t="s">
-        <v>693</v>
-      </c>
       <c r="E143" s="1" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C144" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="D144" s="1" t="s">
         <v>718</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6489,19 +6510,19 @@
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D146" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="B146" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C146" s="1" t="s">
+      <c r="E146" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6520,44 +6541,44 @@
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D149" s="1" t="s">
         <v>807</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>808</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6576,44 +6597,44 @@
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="D152" s="1" t="s">
         <v>858</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6649,47 +6670,47 @@
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="D157" s="1" t="s">
         <v>698</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="D158" s="1" t="s">
         <v>777</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>778</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="D159" s="1" t="s">
         <v>880</v>
       </c>
-      <c r="B159" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C159" s="1" t="s">
+      <c r="E159" s="1" t="s">
         <v>881</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>882</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6722,16 +6743,16 @@
     </row>
     <row r="162" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6762,97 +6783,97 @@
         <v>198</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C166" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="E166" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="D168" s="1" t="s">
         <v>603</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>604</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C170" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="E170" s="1" t="s">
         <v>541</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6933,16 +6954,16 @@
     </row>
     <row r="176" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7037,16 +7058,16 @@
     </row>
     <row r="183" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="D183" s="1" t="s">
         <v>574</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C183" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7068,16 +7089,16 @@
     </row>
     <row r="185" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="D185" s="1" t="s">
         <v>818</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C185" s="1" t="s">
-        <v>819</v>
-      </c>
-      <c r="D185" s="1" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7096,16 +7117,16 @@
     </row>
     <row r="187" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7124,16 +7145,16 @@
     </row>
     <row r="189" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7166,36 +7187,36 @@
     </row>
     <row r="192" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="D193" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="B193" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C193" s="1" t="s">
+      <c r="E193" s="1" t="s">
         <v>695</v>
-      </c>
-      <c r="D193" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="E193" s="1" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7228,47 +7249,47 @@
     </row>
     <row r="196" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="E196" s="1" t="s">
         <v>674</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C196" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="D196" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="E196" s="1" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7290,36 +7311,36 @@
     </row>
     <row r="200" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D200" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="B200" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C200" s="1" t="s">
+      <c r="E200" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="D200" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="E200" s="1" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D201" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="B201" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C201" s="1" t="s">
+      <c r="E201" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="D201" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="E201" s="1" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7338,16 +7359,16 @@
     </row>
     <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7366,19 +7387,19 @@
     </row>
     <row r="205" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="D205" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="B205" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="D205" s="1" t="s">
-        <v>477</v>
-      </c>
       <c r="E205" s="1" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7425,47 +7446,47 @@
     </row>
     <row r="209" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="E209" s="1" t="s">
         <v>662</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C209" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="D209" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="E209" s="1" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D210" s="1" t="s">
         <v>565</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C210" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="D210" s="1" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="211" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="212" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7484,16 +7505,16 @@
     </row>
     <row r="213" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="214" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7510,38 +7531,38 @@
         <v>201</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C216" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="E216" s="1" t="s">
         <v>535</v>
-      </c>
-      <c r="D216" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7560,86 +7581,86 @@
     </row>
     <row r="218" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C219" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="B219" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C219" s="1" t="s">
+      <c r="D219" s="1" t="s">
         <v>486</v>
-      </c>
-      <c r="D219" s="1" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="D220" s="1" t="s">
         <v>744</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>885</v>
-      </c>
-      <c r="C220" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="D220" s="1" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="221" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="222" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7661,19 +7682,19 @@
     </row>
     <row r="225" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="226" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7695,95 +7716,95 @@
     </row>
     <row r="227" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="228" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D228" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="E228" s="1" t="s">
         <v>642</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="229" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="230" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="231" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="232" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D232" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="B232" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C232" s="1" t="s">
+      <c r="E232" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="D232" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="233" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7816,36 +7837,36 @@
     </row>
     <row r="235" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="D235" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="E235" s="1" t="s">
         <v>647</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="236" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D236" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="B236" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="D236" s="1" t="s">
-        <v>414</v>
-      </c>
       <c r="E236" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="237" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7867,47 +7888,47 @@
     </row>
     <row r="238" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="D238" s="1" t="s">
         <v>768</v>
-      </c>
-      <c r="B238" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C238" s="1" t="s">
-        <v>769</v>
-      </c>
-      <c r="D238" s="1" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="239" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C239" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="E239" s="1" t="s">
         <v>636</v>
-      </c>
-      <c r="D239" s="1" t="s">
-        <v>637</v>
-      </c>
-      <c r="E239" s="1" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="240" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="D240" s="1" t="s">
         <v>887</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>888</v>
-      </c>
-      <c r="D240" s="1" t="s">
-        <v>889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
m1-8-3 and -4: v3 with key for refs
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674376BA-EF04-ED42-90B0-735314F715D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7412A31-2EA2-7346-B1AE-9CDF2FFCD64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="947">
   <si>
     <t>M-Number</t>
   </si>
@@ -1582,9 +1582,6 @@
   </si>
   <si>
     <t>../resources/annotations.xml/pla-chop</t>
-  </si>
-  <si>
-    <t>Pembroke, Lord William</t>
   </si>
   <si>
     <t>psn-wpem</t>
@@ -2925,6 +2922,9 @@
   </si>
   <si>
     <t>King Lear</t>
+  </si>
+  <si>
+    <t>Pembroke, William (Lord)</t>
   </si>
 </sst>
 </file>
@@ -3366,9 +3366,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B25" sqref="B25"/>
+      <selection pane="topRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3393,7 +3393,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>392</v>
@@ -3402,10 +3402,10 @@
         <v>29</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>7</v>
@@ -3413,16 +3413,16 @@
     </row>
     <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>787</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E3" s="5">
         <v>9</v>
@@ -3433,19 +3433,22 @@
       <c r="G3" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H3" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>808</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>809</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E4" s="5">
         <v>12</v>
@@ -3456,19 +3459,22 @@
       <c r="G4" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H4" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="E5" s="5">
         <v>15</v>
@@ -3479,19 +3485,22 @@
       <c r="G5" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H5" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>830</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E6" s="5">
         <v>9</v>
@@ -3505,16 +3514,16 @@
     </row>
     <row r="7" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E7" s="5">
         <v>4</v>
@@ -3526,21 +3535,21 @@
         <v>30</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>853</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>854</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="E8" s="5">
         <v>6</v>
@@ -3552,21 +3561,21 @@
         <v>30</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>861</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>862</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="E9" s="5">
         <v>6</v>
@@ -3580,16 +3589,16 @@
     </row>
     <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>863</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>864</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
@@ -3603,16 +3612,16 @@
     </row>
     <row r="11" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>868</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>867</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="E11" s="5">
         <v>3</v>
@@ -3626,16 +3635,16 @@
     </row>
     <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>870</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E12" s="5">
         <v>6</v>
@@ -3652,13 +3661,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>753</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E15" s="5">
         <v>10</v>
@@ -3670,7 +3679,7 @@
         <v>30</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -3678,13 +3687,13 @@
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>761</v>
-      </c>
       <c r="D16" s="6" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E16" s="5">
         <v>9</v>
@@ -3696,7 +3705,7 @@
         <v>30</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -3704,13 +3713,13 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>770</v>
-      </c>
       <c r="D17" s="6" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E17" s="5">
         <v>11</v>
@@ -3733,7 +3742,7 @@
         <v>21</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E18" s="5">
         <v>3</v>
@@ -3762,7 +3771,7 @@
         <v>22</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E19" s="5">
         <v>8</v>
@@ -3788,7 +3797,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E20" s="5">
         <v>9</v>
@@ -3814,7 +3823,7 @@
         <v>24</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E21" s="5">
         <v>9</v>
@@ -3840,7 +3849,7 @@
         <v>329</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E22" s="5">
         <v>19</v>
@@ -3863,7 +3872,7 @@
         <v>330</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E23" s="5">
         <v>26</v>
@@ -3886,27 +3895,27 @@
         <v>391</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="5">
@@ -3921,13 +3930,13 @@
     </row>
     <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="5">
@@ -3942,13 +3951,13 @@
     </row>
     <row r="27" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="5">
@@ -3963,13 +3972,13 @@
     </row>
     <row r="28" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="5">
@@ -3984,13 +3993,13 @@
     </row>
     <row r="29" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="5">
@@ -4005,13 +4014,13 @@
     </row>
     <row r="30" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="5">
@@ -4026,13 +4035,13 @@
     </row>
     <row r="31" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="5">
@@ -4041,13 +4050,13 @@
     </row>
     <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="5">
@@ -4056,28 +4065,28 @@
     </row>
     <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="D35" s="6"/>
     </row>
@@ -4092,7 +4101,7 @@
         <v>428</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="E36" s="5">
         <v>7</v>
@@ -4109,13 +4118,13 @@
         <v>18</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>517</v>
-      </c>
       <c r="D37" s="6" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="E37" s="5">
         <v>9</v>
@@ -4132,13 +4141,13 @@
         <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="E38" s="5">
         <v>5</v>
@@ -4152,13 +4161,13 @@
     </row>
     <row r="39" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E39" s="5">
         <v>5</v>
@@ -4172,13 +4181,13 @@
     </row>
     <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>570</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>571</v>
       </c>
       <c r="E40" s="5">
         <v>4</v>
@@ -4192,13 +4201,13 @@
     </row>
     <row r="41" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E41" s="5">
         <v>7</v>
@@ -4210,18 +4219,18 @@
         <v>30</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>612</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>613</v>
       </c>
       <c r="E42" s="5">
         <v>5</v>
@@ -4235,13 +4244,13 @@
     </row>
     <row r="43" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E43" s="5">
         <v>2</v>
@@ -4253,18 +4262,18 @@
         <v>30</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E44" s="5">
         <v>3</v>
@@ -4281,10 +4290,10 @@
         <v>20</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>728</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>729</v>
       </c>
       <c r="E45" s="5">
         <v>8</v>
@@ -4298,7 +4307,7 @@
     </row>
     <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="I47" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -4350,8 +4359,8 @@
   <dimension ref="A1:F240"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E135" sqref="E135"/>
+      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4369,7 +4378,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
@@ -4386,19 +4395,19 @@
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>641</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4462,19 +4471,19 @@
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>726</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>727</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4521,7 +4530,7 @@
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>26</v>
@@ -4535,19 +4544,19 @@
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>684</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>685</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4642,19 +4651,19 @@
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>833</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>834</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>835</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4673,19 +4682,19 @@
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>789</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>790</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4718,16 +4727,16 @@
     </row>
     <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>845</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4746,30 +4755,30 @@
     </row>
     <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>624</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>623</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>615</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4805,16 +4814,16 @@
     </row>
     <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>722</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>723</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -4903,16 +4912,16 @@
     </row>
     <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>758</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -4959,16 +4968,16 @@
     </row>
     <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>755</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -5029,44 +5038,44 @@
     </row>
     <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>739</v>
-      </c>
       <c r="D46" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5119,44 +5128,44 @@
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>620</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>823</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>605</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5203,44 +5212,44 @@
     </row>
     <row r="58" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>590</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>747</v>
-      </c>
       <c r="D59" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>795</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>796</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>797</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5287,16 +5296,16 @@
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>764</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5318,33 +5327,33 @@
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="E66" s="1" t="s">
         <v>812</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>519</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5363,19 +5372,19 @@
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C69" s="1" t="s">
+      <c r="D69" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>676</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>681</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5470,16 +5479,16 @@
     </row>
     <row r="76" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5498,33 +5507,33 @@
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>654</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>655</v>
-      </c>
       <c r="D79" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5543,36 +5552,36 @@
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5619,16 +5628,16 @@
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5659,7 +5668,7 @@
         <v>150</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5678,16 +5687,16 @@
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>596</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5762,30 +5771,30 @@
     </row>
     <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>826</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C97" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>521</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5807,19 +5816,19 @@
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>679</v>
-      </c>
       <c r="D99" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="E99" s="1" t="s">
         <v>682</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5884,35 +5893,35 @@
         <v>453</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C104" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>706</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>575</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5948,36 +5957,36 @@
     </row>
     <row r="108" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>666</v>
-      </c>
       <c r="D108" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6047,16 +6056,16 @@
     </row>
     <row r="114" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C114" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>802</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6075,30 +6084,30 @@
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="B116" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C116" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>567</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>871</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C117" s="1" t="s">
+      <c r="D117" s="1" t="s">
         <v>872</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6117,16 +6126,16 @@
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C119" s="1" t="s">
+      <c r="D119" s="1" t="s">
         <v>618</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6173,30 +6182,30 @@
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C123" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>579</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C124" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>876</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>877</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6229,16 +6238,16 @@
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="B127" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>749</v>
-      </c>
       <c r="D127" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6316,7 +6325,7 @@
     </row>
     <row r="133" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>39</v>
@@ -6358,16 +6367,16 @@
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6400,19 +6409,19 @@
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C139" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="D139" s="1" t="s">
         <v>792</v>
       </c>
-      <c r="D139" s="1" t="s">
+      <c r="E139" s="1" t="s">
         <v>793</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6448,47 +6457,47 @@
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C142" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="D142" s="1" t="s">
         <v>581</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C143" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="E143" s="1" t="s">
         <v>689</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6541,44 +6550,44 @@
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C148" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="B148" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>651</v>
-      </c>
       <c r="D148" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C149" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C149" s="1" t="s">
+      <c r="D149" s="1" t="s">
         <v>806</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6597,44 +6606,44 @@
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C152" s="1" t="s">
         <v>856</v>
       </c>
-      <c r="B152" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C152" s="1" t="s">
+      <c r="D152" s="1" t="s">
         <v>857</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C153" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D153" s="1" t="s">
         <v>709</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C154" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="D154" s="1" t="s">
         <v>703</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6670,47 +6679,47 @@
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C157" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="B157" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C157" s="1" t="s">
+      <c r="D157" s="1" t="s">
         <v>697</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C158" s="1" t="s">
         <v>775</v>
       </c>
-      <c r="B158" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C158" s="1" t="s">
+      <c r="D158" s="1" t="s">
         <v>776</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C159" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="B159" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C159" s="1" t="s">
+      <c r="D159" s="1" t="s">
         <v>879</v>
       </c>
-      <c r="D159" s="1" t="s">
+      <c r="E159" s="1" t="s">
         <v>880</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6783,7 +6792,7 @@
         <v>198</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6819,61 +6828,61 @@
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C167" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D167" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="D167" s="1" t="s">
-        <v>537</v>
-      </c>
       <c r="E167" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C168" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="B168" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C168" s="1" t="s">
+      <c r="D168" s="1" t="s">
         <v>602</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C169" s="1" t="s">
         <v>607</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C170" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="D170" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="D170" s="1" t="s">
+      <c r="E170" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6954,16 +6963,16 @@
     </row>
     <row r="176" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C176" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="B176" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>515</v>
-      </c>
       <c r="D176" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7058,16 +7067,16 @@
     </row>
     <row r="183" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C183" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="B183" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C183" s="1" t="s">
+      <c r="D183" s="1" t="s">
         <v>573</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7089,16 +7098,16 @@
     </row>
     <row r="185" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C185" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="B185" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C185" s="1" t="s">
+      <c r="D185" s="1" t="s">
         <v>817</v>
-      </c>
-      <c r="D185" s="1" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7117,16 +7126,16 @@
     </row>
     <row r="187" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C187" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="D187" s="1" t="s">
         <v>840</v>
-      </c>
-      <c r="D187" s="1" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7145,16 +7154,16 @@
     </row>
     <row r="189" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C189" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="D189" s="1" t="s">
         <v>712</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7187,36 +7196,36 @@
     </row>
     <row r="192" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C193" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="B193" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C193" s="1" t="s">
+      <c r="D193" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="D193" s="1" t="s">
+      <c r="E193" s="1" t="s">
         <v>694</v>
-      </c>
-      <c r="E193" s="1" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7249,19 +7258,19 @@
     </row>
     <row r="196" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C196" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="B196" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C196" s="1" t="s">
+      <c r="D196" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="E196" s="1" t="s">
         <v>673</v>
-      </c>
-      <c r="D196" s="1" t="s">
-        <v>680</v>
-      </c>
-      <c r="E196" s="1" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7328,19 +7337,19 @@
     </row>
     <row r="201" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C201" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="B201" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C201" s="1" t="s">
+      <c r="D201" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="D201" s="1" t="s">
+      <c r="E201" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="E201" s="1" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7359,16 +7368,16 @@
     </row>
     <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C203" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="D203" s="1" t="s">
         <v>799</v>
-      </c>
-      <c r="D203" s="1" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7399,7 +7408,7 @@
         <v>475</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7446,33 +7455,33 @@
     </row>
     <row r="209" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C209" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="B209" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C209" s="1" t="s">
+      <c r="D209" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="E209" s="1" t="s">
         <v>661</v>
-      </c>
-      <c r="D209" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="E209" s="1" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C210" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="B210" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C210" s="1" t="s">
+      <c r="D210" s="1" t="s">
         <v>564</v>
-      </c>
-      <c r="D210" s="1" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="211" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7505,16 +7514,16 @@
     </row>
     <row r="213" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C213" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="D213" s="1" t="s">
         <v>599</v>
-      </c>
-      <c r="D213" s="1" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="214" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7531,38 +7540,38 @@
         <v>201</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C215" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="D215" s="1" t="s">
         <v>820</v>
-      </c>
-      <c r="D215" s="1" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C216" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="D216" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D216" s="1" t="s">
+      <c r="E216" s="1" t="s">
         <v>534</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7581,16 +7590,16 @@
     </row>
     <row r="218" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C218" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="D218" s="1" t="s">
         <v>556</v>
-      </c>
-      <c r="D218" s="1" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7609,58 +7618,58 @@
     </row>
     <row r="220" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="C220" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="B220" s="1" t="s">
-        <v>883</v>
-      </c>
-      <c r="C220" s="1" t="s">
+      <c r="D220" s="1" t="s">
         <v>743</v>
-      </c>
-      <c r="D220" s="1" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="221" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C221" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="D221" s="1" t="s">
         <v>593</v>
-      </c>
-      <c r="D221" s="1" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="222" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C222" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="B222" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C222" s="1" t="s">
-        <v>653</v>
-      </c>
       <c r="D222" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C223" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="D223" s="1" t="s">
         <v>734</v>
-      </c>
-      <c r="D223" s="1" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7682,19 +7691,19 @@
     </row>
     <row r="225" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C225" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D225" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="D225" s="1" t="s">
-        <v>530</v>
-      </c>
       <c r="E225" s="1" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="226" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7716,7 +7725,7 @@
     </row>
     <row r="227" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>26</v>
@@ -7733,61 +7742,61 @@
     </row>
     <row r="228" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="229" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C229" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="D229" s="1" t="s">
         <v>731</v>
-      </c>
-      <c r="D229" s="1" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="230" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C230" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="D230" s="1" t="s">
         <v>587</v>
-      </c>
-      <c r="D230" s="1" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="231" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C231" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="D231" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="D231" s="1" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="232" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7837,19 +7846,19 @@
     </row>
     <row r="235" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C235" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="D235" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="D235" s="1" t="s">
-        <v>645</v>
-      </c>
       <c r="E235" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="236" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7866,7 +7875,7 @@
         <v>412</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="237" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7888,47 +7897,47 @@
     </row>
     <row r="238" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C238" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="B238" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C238" s="1" t="s">
+      <c r="D238" s="1" t="s">
         <v>767</v>
-      </c>
-      <c r="D238" s="1" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="239" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C239" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="D239" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="D239" s="1" t="s">
+      <c r="E239" s="1" t="s">
         <v>635</v>
-      </c>
-      <c r="E239" s="1" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="240" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C240" s="1" t="s">
         <v>885</v>
       </c>
-      <c r="B240" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C240" s="1" t="s">
+      <c r="D240" s="1" t="s">
         <v>886</v>
-      </c>
-      <c r="D240" s="1" t="s">
-        <v>887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
m1-8-5 to -10: v3 updates to <rs> tags
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6271370-A4AD-5347-A963-B6EA35BA0CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2494D263-9E46-3F44-8C81-CFC9D967A609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -3033,7 +3033,17 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3366,9 +3376,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F30" sqref="F30:G30"/>
+      <selection pane="topRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4322,7 +4332,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="F1:H1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7951,7 +7961,7 @@
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
m48-52.xml: v3 update with key attribs for references
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012E769C-2EA5-794D-B6D4-14EDF0CC8107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79302FE7-1870-5D4E-8017-F1CE80159578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="954">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="955">
   <si>
     <t>M-Number</t>
   </si>
@@ -2786,9 +2786,6 @@
     <t>https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m45-manifest.json</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m65-manifest.json</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m47-manifest.json</t>
   </si>
   <si>
@@ -2946,6 +2943,12 @@
   </si>
   <si>
     <t>Tennyson, Alfred</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m46-manifest.json</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m113-manifest.json</t>
   </si>
 </sst>
 </file>
@@ -3387,9 +3390,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H18" sqref="H18"/>
+      <selection pane="topRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3738,7 +3741,7 @@
         <v>759</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>900</v>
+        <v>953</v>
       </c>
       <c r="E16" s="5">
         <v>9</v>
@@ -3767,7 +3770,7 @@
         <v>768</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E17" s="5">
         <v>11</v>
@@ -3793,7 +3796,7 @@
         <v>21</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E18" s="5">
         <v>3</v>
@@ -3802,6 +3805,9 @@
         <v>30</v>
       </c>
       <c r="G18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>30</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -3819,7 +3825,7 @@
         <v>22</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E19" s="5">
         <v>8</v>
@@ -3828,6 +3834,9 @@
         <v>30</v>
       </c>
       <c r="G19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>30</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -3845,7 +3854,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E20" s="5">
         <v>9</v>
@@ -3854,6 +3863,9 @@
         <v>30</v>
       </c>
       <c r="G20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>30</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -3871,7 +3883,7 @@
         <v>24</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E21" s="5">
         <v>9</v>
@@ -3897,7 +3909,7 @@
         <v>329</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E22" s="5">
         <v>19</v>
@@ -3920,7 +3932,7 @@
         <v>330</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E23" s="5">
         <v>26</v>
@@ -3943,27 +3955,27 @@
         <v>391</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="5">
@@ -3978,13 +3990,13 @@
     </row>
     <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="5">
@@ -3999,13 +4011,13 @@
     </row>
     <row r="27" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="5">
@@ -4020,13 +4032,13 @@
     </row>
     <row r="28" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="5">
@@ -4041,13 +4053,13 @@
     </row>
     <row r="29" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="5">
@@ -4062,13 +4074,13 @@
     </row>
     <row r="30" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="5">
@@ -4083,13 +4095,13 @@
     </row>
     <row r="31" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="5">
@@ -4098,13 +4110,13 @@
     </row>
     <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="5">
@@ -4113,28 +4125,28 @@
     </row>
     <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D35" s="6"/>
     </row>
@@ -4149,7 +4161,7 @@
         <v>428</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E36" s="5">
         <v>7</v>
@@ -4172,7 +4184,7 @@
         <v>515</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E37" s="5">
         <v>9</v>
@@ -4195,7 +4207,7 @@
         <v>529</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="E38" s="5">
         <v>5</v>
@@ -4217,6 +4229,9 @@
       <c r="C39" s="1" t="s">
         <v>559</v>
       </c>
+      <c r="D39" s="6" t="s">
+        <v>910</v>
+      </c>
       <c r="E39" s="5">
         <v>5</v>
       </c>
@@ -4227,7 +4242,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>557</v>
       </c>
@@ -4236,6 +4251,9 @@
       </c>
       <c r="C40" s="1" t="s">
         <v>569</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>910</v>
       </c>
       <c r="E40" s="5">
         <v>4</v>
@@ -4257,6 +4275,9 @@
       <c r="C41" s="1" t="s">
         <v>581</v>
       </c>
+      <c r="D41" s="6" t="s">
+        <v>910</v>
+      </c>
       <c r="E41" s="5">
         <v>7</v>
       </c>
@@ -4280,6 +4301,9 @@
       <c r="C42" s="1" t="s">
         <v>611</v>
       </c>
+      <c r="D42" s="6" t="s">
+        <v>910</v>
+      </c>
       <c r="E42" s="5">
         <v>5</v>
       </c>
@@ -4300,6 +4324,9 @@
       <c r="C43" s="1" t="s">
         <v>697</v>
       </c>
+      <c r="D43" s="6" t="s">
+        <v>910</v>
+      </c>
       <c r="E43" s="5">
         <v>2</v>
       </c>
@@ -4323,6 +4350,9 @@
       <c r="C44" s="1" t="s">
         <v>718</v>
       </c>
+      <c r="D44" s="6" t="s">
+        <v>910</v>
+      </c>
       <c r="E44" s="5">
         <v>3</v>
       </c>
@@ -4342,6 +4372,9 @@
       </c>
       <c r="C45" s="1" t="s">
         <v>727</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>954</v>
       </c>
       <c r="E45" s="5">
         <v>8</v>
@@ -4396,9 +4429,11 @@
     <hyperlink ref="D37:D38" r:id="rId22" display="https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m108-manifest.json" xr:uid="{5FDF83DE-B05E-6648-83B6-79117939C2BD}"/>
     <hyperlink ref="D37" r:id="rId23" xr:uid="{DDBE96EE-FA90-E444-B89A-BB7CF5AE1D03}"/>
     <hyperlink ref="D38" r:id="rId24" xr:uid="{E4B7B736-B87B-BB46-8F24-C9894D56EA25}"/>
+    <hyperlink ref="D39:D45" r:id="rId25" display="https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m108-manifest.json" xr:uid="{A88FA7C4-88CC-374D-9FB9-785AA74D1C8D}"/>
+    <hyperlink ref="D45" r:id="rId26" xr:uid="{C721C539-C5A2-C144-9780-C15E8452E338}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId25"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId27"/>
 </worksheet>
 </file>
 
@@ -4406,9 +4441,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9177BC3-9C2F-4FB7-BC81-8F81FE0107BA}">
   <dimension ref="A1:F242"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4578,7 +4613,7 @@
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>26</v>
@@ -5176,19 +5211,19 @@
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>946</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>947</v>
-      </c>
       <c r="D52" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6261,7 +6296,7 @@
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>39</v>
@@ -7042,7 +7077,7 @@
     </row>
     <row r="178" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>26</v>
@@ -7416,19 +7451,19 @@
     </row>
     <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C203" s="1" t="s">
         <v>950</v>
       </c>
-      <c r="B203" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C203" s="1" t="s">
-        <v>951</v>
-      </c>
       <c r="D203" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="E203" s="1" t="s">
         <v>948</v>
-      </c>
-      <c r="E203" s="1" t="s">
-        <v>949</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7700,7 +7735,7 @@
     </row>
     <row r="222" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
m53, 54-1 and 54-2.xml: v3 updates
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79302FE7-1870-5D4E-8017-F1CE80159578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E706CB-AC9B-E247-9573-CFF9DE25E048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="955">
   <si>
     <t>M-Number</t>
   </si>
@@ -979,9 +979,6 @@
   </si>
   <si>
     <t>../resources/annotations.xml#psn-stge</t>
-  </si>
-  <si>
-    <t>Faust</t>
   </si>
   <si>
     <t>lit-faus</t>
@@ -2949,6 +2946,9 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/JoshuaAPhillips/digital-anon/main/manifests/m113-manifest.json</t>
+  </si>
+  <si>
+    <t>Doctor Faustus</t>
   </si>
 </sst>
 </file>
@@ -3392,7 +3392,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H20" sqref="H20"/>
+      <selection pane="topRight" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3417,19 +3417,19 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>7</v>
@@ -3437,16 +3437,16 @@
     </row>
     <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>785</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E3" s="5">
         <v>9</v>
@@ -3463,16 +3463,16 @@
     </row>
     <row r="4" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>807</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="E4" s="5">
         <v>12</v>
@@ -3489,16 +3489,16 @@
     </row>
     <row r="5" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E5" s="5">
         <v>15</v>
@@ -3515,16 +3515,16 @@
     </row>
     <row r="6" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>828</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E6" s="5">
         <v>9</v>
@@ -3541,16 +3541,16 @@
     </row>
     <row r="7" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="E7" s="5">
         <v>4</v>
@@ -3565,21 +3565,21 @@
         <v>30</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>851</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>852</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E8" s="5">
         <v>6</v>
@@ -3594,21 +3594,21 @@
         <v>30</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>859</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>860</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E9" s="5">
         <v>6</v>
@@ -3625,16 +3625,16 @@
     </row>
     <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>861</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>862</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
@@ -3651,16 +3651,16 @@
     </row>
     <row r="11" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>866</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>865</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="E11" s="5">
         <v>3</v>
@@ -3677,16 +3677,16 @@
     </row>
     <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>868</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E12" s="5">
         <v>6</v>
@@ -3706,13 +3706,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>750</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>751</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E15" s="5">
         <v>10</v>
@@ -3727,7 +3727,7 @@
         <v>30</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -3735,13 +3735,13 @@
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>758</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>759</v>
-      </c>
       <c r="D16" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="E16" s="5">
         <v>9</v>
@@ -3756,7 +3756,7 @@
         <v>30</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -3764,13 +3764,13 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>767</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>768</v>
-      </c>
       <c r="D17" s="6" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="E17" s="5">
         <v>11</v>
@@ -3790,13 +3790,13 @@
         <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E18" s="5">
         <v>3</v>
@@ -3819,13 +3819,13 @@
         <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E19" s="5">
         <v>8</v>
@@ -3854,7 +3854,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E20" s="5">
         <v>9</v>
@@ -3877,13 +3877,13 @@
         <v>13</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E21" s="5">
         <v>9</v>
@@ -3892,6 +3892,9 @@
         <v>30</v>
       </c>
       <c r="G21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>30</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -3903,13 +3906,13 @@
         <v>14</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E22" s="5">
         <v>19</v>
@@ -3918,6 +3921,9 @@
         <v>30</v>
       </c>
       <c r="G22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3926,13 +3932,13 @@
         <v>15</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E23" s="5">
         <v>26</v>
@@ -3940,8 +3946,11 @@
       <c r="F23" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H23" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="I23" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.2">
@@ -3949,33 +3958,33 @@
         <v>16</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="5">
@@ -3987,16 +3996,19 @@
       <c r="G25" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H25" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="5">
@@ -4008,16 +4020,19 @@
       <c r="G26" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H26" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="5">
@@ -4032,13 +4047,13 @@
     </row>
     <row r="28" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="5">
@@ -4053,13 +4068,13 @@
     </row>
     <row r="29" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="5">
@@ -4074,13 +4089,13 @@
     </row>
     <row r="30" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="5">
@@ -4095,13 +4110,13 @@
     </row>
     <row r="31" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="5">
@@ -4110,13 +4125,13 @@
     </row>
     <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="5">
@@ -4125,28 +4140,28 @@
     </row>
     <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D35" s="6"/>
     </row>
@@ -4155,13 +4170,13 @@
         <v>17</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E36" s="5">
         <v>7</v>
@@ -4178,13 +4193,13 @@
         <v>18</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>515</v>
-      </c>
       <c r="D37" s="6" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E37" s="5">
         <v>9</v>
@@ -4201,13 +4216,13 @@
         <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E38" s="5">
         <v>5</v>
@@ -4221,16 +4236,16 @@
     </row>
     <row r="39" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E39" s="5">
         <v>5</v>
@@ -4244,16 +4259,16 @@
     </row>
     <row r="40" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>569</v>
-      </c>
       <c r="D40" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E40" s="5">
         <v>4</v>
@@ -4267,16 +4282,16 @@
     </row>
     <row r="41" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E41" s="5">
         <v>7</v>
@@ -4288,21 +4303,21 @@
         <v>30</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>611</v>
-      </c>
       <c r="D42" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E42" s="5">
         <v>5</v>
@@ -4316,16 +4331,16 @@
     </row>
     <row r="43" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E43" s="5">
         <v>2</v>
@@ -4337,21 +4352,21 @@
         <v>30</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E44" s="5">
         <v>3</v>
@@ -4368,13 +4383,13 @@
         <v>20</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>726</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>727</v>
-      </c>
       <c r="D45" s="6" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="E45" s="5">
         <v>8</v>
@@ -4388,7 +4403,7 @@
     </row>
     <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="I47" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -4442,8 +4457,8 @@
   <dimension ref="A1:F242"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A217" sqref="A217"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4461,7 +4476,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
@@ -4478,19 +4493,19 @@
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>639</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4512,61 +4527,61 @@
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>724</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>725</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4585,16 +4600,16 @@
     </row>
     <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4613,7 +4628,7 @@
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>26</v>
@@ -4627,19 +4642,19 @@
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>683</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4678,106 +4693,106 @@
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>437</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>431</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>831</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>833</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>371</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>788</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4796,72 +4811,72 @@
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>843</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>622</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>613</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -4883,30 +4898,30 @@
     </row>
     <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>720</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>721</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -4925,16 +4940,16 @@
     </row>
     <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -4995,16 +5010,16 @@
     </row>
     <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>755</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>756</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -5023,7 +5038,7 @@
     </row>
     <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>43</v>
@@ -5051,44 +5066,44 @@
     </row>
     <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>753</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>502</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>511</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -5107,58 +5122,58 @@
     </row>
     <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>441</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>737</v>
-      </c>
       <c r="D46" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5194,78 +5209,78 @@
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>375</v>
-      </c>
       <c r="E51" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>945</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>946</v>
-      </c>
       <c r="D52" s="1" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>618</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>821</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>603</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5312,72 +5327,72 @@
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>588</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>745</v>
-      </c>
       <c r="D60" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>794</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>465</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5396,64 +5411,64 @@
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>762</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="E66" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>808</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C67" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>810</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>811</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5472,19 +5487,19 @@
     </row>
     <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>673</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C70" s="1" t="s">
+      <c r="D70" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>674</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>679</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5506,19 +5521,19 @@
     </row>
     <row r="72" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>445</v>
-      </c>
       <c r="E72" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5579,182 +5594,182 @@
     </row>
     <row r="77" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>313</v>
+        <v>954</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>653</v>
-      </c>
       <c r="D80" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C81" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C85" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>505</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C86" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>496</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5768,35 +5783,35 @@
         <v>150</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>500</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>594</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5815,30 +5830,30 @@
     </row>
     <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C94" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5871,78 +5886,78 @@
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C97" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>824</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C98" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>519</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C99" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="E99" s="1" t="s">
         <v>383</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>677</v>
-      </c>
       <c r="D100" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="E100" s="1" t="s">
         <v>680</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C101" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -5981,47 +5996,47 @@
     </row>
     <row r="104" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C104" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="D104" s="1" t="s">
-        <v>453</v>
-      </c>
       <c r="E104" s="1" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>704</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C106" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>573</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6057,67 +6072,67 @@
     </row>
     <row r="109" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>664</v>
-      </c>
       <c r="D109" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C111" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C112" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="E112" s="1" t="s">
         <v>489</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6156,16 +6171,16 @@
     </row>
     <row r="115" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C115" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>800</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6184,30 +6199,30 @@
     </row>
     <row r="117" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C117" s="1" t="s">
+      <c r="D117" s="1" t="s">
         <v>565</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="B118" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C118" s="1" t="s">
+      <c r="D118" s="1" t="s">
         <v>870</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>871</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6226,44 +6241,44 @@
     </row>
     <row r="120" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="B120" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C120" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>616</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C121" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="B122" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C122" s="1" t="s">
+      <c r="D122" s="1" t="s">
         <v>477</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6282,86 +6297,86 @@
     </row>
     <row r="124" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C124" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>577</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C125" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C126" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>874</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="B127" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C127" s="1" t="s">
+      <c r="D127" s="1" t="s">
         <v>508</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C128" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="B128" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C128" s="1" t="s">
+      <c r="D128" s="1" t="s">
         <v>434</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="B129" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>747</v>
-      </c>
       <c r="D129" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6425,30 +6440,30 @@
     </row>
     <row r="134" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C134" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D134" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C135" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C135" s="1" t="s">
+      <c r="D135" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6467,30 +6482,30 @@
     </row>
     <row r="137" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C138" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C138" s="1" t="s">
+      <c r="D138" s="1" t="s">
         <v>386</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6509,33 +6524,33 @@
     </row>
     <row r="140" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C140" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="D140" s="1" t="s">
         <v>790</v>
       </c>
-      <c r="D140" s="1" t="s">
+      <c r="E140" s="1" t="s">
         <v>791</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C141" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="D141" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6557,47 +6572,47 @@
     </row>
     <row r="143" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C143" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="D143" s="1" t="s">
         <v>579</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C144" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="E144" s="1" t="s">
         <v>687</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6619,19 +6634,19 @@
     </row>
     <row r="147" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C147" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="B147" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C147" s="1" t="s">
+      <c r="D147" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="E147" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6650,44 +6665,44 @@
     </row>
     <row r="149" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C149" s="1" t="s">
         <v>648</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>649</v>
-      </c>
       <c r="D149" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C150" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="B150" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C150" s="1" t="s">
+      <c r="D150" s="1" t="s">
         <v>804</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6706,58 +6721,58 @@
     </row>
     <row r="153" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C153" s="1" t="s">
         <v>854</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C153" s="1" t="s">
+      <c r="D153" s="1" t="s">
         <v>855</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C154" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="D154" s="1" t="s">
         <v>707</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C155" s="1" t="s">
         <v>883</v>
       </c>
-      <c r="B155" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C155" s="1" t="s">
+      <c r="D155" s="1" t="s">
         <v>884</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C156" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="D156" s="1" t="s">
         <v>701</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6793,47 +6808,47 @@
     </row>
     <row r="159" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C159" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="B159" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C159" s="1" t="s">
+      <c r="D159" s="1" t="s">
         <v>695</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C160" s="1" t="s">
         <v>773</v>
       </c>
-      <c r="B160" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C160" s="1" t="s">
+      <c r="D160" s="1" t="s">
         <v>774</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C161" s="1" t="s">
         <v>876</v>
       </c>
-      <c r="B161" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C161" s="1" t="s">
+      <c r="D161" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="D161" s="1" t="s">
+      <c r="E161" s="1" t="s">
         <v>878</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>879</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6866,16 +6881,16 @@
     </row>
     <row r="164" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C164" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="D164" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -6906,125 +6921,125 @@
         <v>198</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C167" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D167" s="1" t="s">
         <v>480</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C168" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D168" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="D168" s="1" t="s">
+      <c r="E168" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C169" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="D169" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="D169" s="1" t="s">
-        <v>535</v>
-      </c>
       <c r="E169" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C170" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="B170" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C170" s="1" t="s">
+      <c r="D170" s="1" t="s">
         <v>600</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C171" s="1" t="s">
         <v>605</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C172" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="D172" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="D172" s="1" t="s">
+      <c r="E172" s="1" t="s">
         <v>538</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C173" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D173" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C174" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D174" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="D174" s="1" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7077,16 +7092,16 @@
     </row>
     <row r="178" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7181,16 +7196,16 @@
     </row>
     <row r="185" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C185" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="B185" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C185" s="1" t="s">
+      <c r="D185" s="1" t="s">
         <v>571</v>
-      </c>
-      <c r="D185" s="1" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7212,16 +7227,16 @@
     </row>
     <row r="187" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C187" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="B187" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C187" s="1" t="s">
+      <c r="D187" s="1" t="s">
         <v>815</v>
-      </c>
-      <c r="D187" s="1" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7240,44 +7255,44 @@
     </row>
     <row r="189" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C189" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="D189" s="1" t="s">
         <v>838</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C190" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D190" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="D190" s="1" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C191" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="D191" s="1" t="s">
         <v>710</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7310,36 +7325,36 @@
     </row>
     <row r="194" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C195" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="B195" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C195" s="1" t="s">
+      <c r="D195" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="D195" s="1" t="s">
+      <c r="E195" s="1" t="s">
         <v>692</v>
-      </c>
-      <c r="E195" s="1" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7372,47 +7387,47 @@
     </row>
     <row r="198" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C198" s="1" t="s">
         <v>670</v>
       </c>
-      <c r="B198" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C198" s="1" t="s">
+      <c r="D198" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="E198" s="1" t="s">
         <v>671</v>
-      </c>
-      <c r="D198" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="E198" s="1" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C199" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D199" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="D199" s="1" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C200" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D200" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="D200" s="1" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7434,53 +7449,53 @@
     </row>
     <row r="202" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C202" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="B202" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C202" s="1" t="s">
+      <c r="D202" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="D202" s="1" t="s">
+      <c r="E202" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="E202" s="1" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C203" s="1" t="s">
         <v>949</v>
       </c>
-      <c r="B203" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C203" s="1" t="s">
-        <v>950</v>
-      </c>
       <c r="D203" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="E203" s="1" t="s">
         <v>947</v>
-      </c>
-      <c r="E203" s="1" t="s">
-        <v>948</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C204" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="B204" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C204" s="1" t="s">
+      <c r="D204" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="D204" s="1" t="s">
+      <c r="E204" s="1" t="s">
         <v>544</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7499,16 +7514,16 @@
     </row>
     <row r="206" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C206" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="D206" s="1" t="s">
         <v>797</v>
-      </c>
-      <c r="D206" s="1" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="207" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7527,19 +7542,19 @@
     </row>
     <row r="208" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C208" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="B208" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C208" s="1" t="s">
+      <c r="D208" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="D208" s="1" t="s">
-        <v>475</v>
-      </c>
       <c r="E208" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="209" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7586,47 +7601,47 @@
     </row>
     <row r="212" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C212" s="1" t="s">
         <v>658</v>
       </c>
-      <c r="B212" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C212" s="1" t="s">
+      <c r="D212" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="E212" s="1" t="s">
         <v>659</v>
-      </c>
-      <c r="D212" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="213" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C213" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="B213" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C213" s="1" t="s">
+      <c r="D213" s="1" t="s">
         <v>562</v>
-      </c>
-      <c r="D213" s="1" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="214" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C214" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="D214" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="D214" s="1" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7645,16 +7660,16 @@
     </row>
     <row r="216" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C216" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="D216" s="1" t="s">
         <v>597</v>
-      </c>
-      <c r="D216" s="1" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7671,170 +7686,170 @@
         <v>201</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="218" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C218" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="D218" s="1" t="s">
         <v>818</v>
-      </c>
-      <c r="D218" s="1" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C219" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="D219" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D219" s="1" t="s">
+      <c r="E219" s="1" t="s">
         <v>532</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C220" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D220" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="D220" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="221" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C221" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="D221" s="1" t="s">
         <v>554</v>
-      </c>
-      <c r="D221" s="1" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="222" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="C223" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="B223" s="1" t="s">
-        <v>881</v>
-      </c>
-      <c r="C223" s="1" t="s">
+      <c r="D223" s="1" t="s">
         <v>741</v>
-      </c>
-      <c r="D223" s="1" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C224" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="D224" s="1" t="s">
         <v>591</v>
-      </c>
-      <c r="D224" s="1" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="225" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C225" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="B225" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C225" s="1" t="s">
-        <v>651</v>
-      </c>
       <c r="D225" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="226" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C226" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D226" s="1" t="s">
         <v>732</v>
-      </c>
-      <c r="D226" s="1" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="227" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C227" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B227" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C227" s="1" t="s">
+      <c r="D227" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D227" s="1" t="s">
+      <c r="E227" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="228" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C228" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D228" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="D228" s="1" t="s">
-        <v>528</v>
-      </c>
       <c r="E228" s="1" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="229" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7856,95 +7871,95 @@
     </row>
     <row r="230" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C230" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D230" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="D230" s="1" t="s">
-        <v>427</v>
-      </c>
       <c r="E230" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="231" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="232" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C232" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="D232" s="1" t="s">
         <v>729</v>
-      </c>
-      <c r="D232" s="1" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="233" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C233" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="D233" s="1" t="s">
         <v>585</v>
-      </c>
-      <c r="D233" s="1" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="234" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C234" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="D234" s="1" t="s">
         <v>522</v>
-      </c>
-      <c r="D234" s="1" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="235" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C235" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="B235" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C235" s="1" t="s">
+      <c r="D235" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="D235" s="1" t="s">
+      <c r="E235" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="236" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -7977,36 +7992,36 @@
     </row>
     <row r="238" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C238" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="D238" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="D238" s="1" t="s">
-        <v>643</v>
-      </c>
       <c r="E238" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="239" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C239" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="B239" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C239" s="1" t="s">
+      <c r="D239" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="D239" s="1" t="s">
-        <v>412</v>
-      </c>
       <c r="E239" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="240" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -8028,33 +8043,33 @@
     </row>
     <row r="241" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C241" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="B241" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C241" s="1" t="s">
+      <c r="D241" s="1" t="s">
         <v>765</v>
-      </c>
-      <c r="D241" s="1" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="242" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C242" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="D242" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="D242" s="1" t="s">
+      <c r="E242" s="1" t="s">
         <v>633</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
m54 subfragments: v3 with key attribs
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E706CB-AC9B-E247-9573-CFF9DE25E048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F329806-ECAB-4248-BAF3-A07F7D32BFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Annotations" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Annotations!$A$1:$F$230</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Annotations!$A$1:$F$229</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="959">
   <si>
     <t>M-Number</t>
   </si>
@@ -2949,6 +2949,18 @@
   </si>
   <si>
     <t>Doctor Faustus</t>
+  </si>
+  <si>
+    <t>Melancthon, Philipp</t>
+  </si>
+  <si>
+    <t>psn-pmel</t>
+  </si>
+  <si>
+    <t>../resources/annotations.xml#psn-pmel</t>
+  </si>
+  <si>
+    <t>M54, 7 of 11. [Anon: distinct from the minstrel, whose words are printed.]. Typescript fragment, 2 fols.</t>
   </si>
 </sst>
 </file>
@@ -3390,9 +3402,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H27" sqref="H27"/>
+      <selection pane="topRight" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4044,6 +4056,9 @@
       <c r="G27" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H27" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
@@ -4065,6 +4080,9 @@
       <c r="G28" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H28" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
@@ -4086,6 +4104,9 @@
       <c r="G29" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H29" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -4107,13 +4128,16 @@
       <c r="G30" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H30" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="31" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>916</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>939</v>
+        <v>958</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>928</v>
@@ -4122,13 +4146,22 @@
       <c r="E31" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="F31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>917</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>929</v>
@@ -4137,15 +4170,24 @@
       <c r="E32" s="5">
         <v>8</v>
       </c>
+      <c r="F32" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>918</v>
       </c>
+      <c r="B33" s="1" t="s">
+        <v>940</v>
+      </c>
       <c r="C33" s="1" t="s">
         <v>930</v>
       </c>
       <c r="D33" s="6"/>
+      <c r="F33" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
@@ -4155,6 +4197,9 @@
         <v>931</v>
       </c>
       <c r="D34" s="6"/>
+      <c r="F34" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -4164,6 +4209,9 @@
         <v>932</v>
       </c>
       <c r="D35" s="6"/>
+      <c r="F35" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="36" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
@@ -4457,8 +4505,8 @@
   <dimension ref="A1:F242"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A200" sqref="A200:XFD200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7418,664 +7466,664 @@
     </row>
     <row r="200" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>403</v>
+        <v>248</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>404</v>
+        <v>249</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>405</v>
+        <v>250</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>248</v>
+        <v>420</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>249</v>
+        <v>421</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>250</v>
+        <v>422</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>251</v>
+        <v>423</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>420</v>
+        <v>948</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>421</v>
+        <v>949</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>422</v>
+        <v>946</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>423</v>
+        <v>947</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>948</v>
+        <v>541</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>949</v>
+        <v>542</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>946</v>
+        <v>543</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>947</v>
+        <v>544</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>541</v>
+        <v>301</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>542</v>
+        <v>302</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>544</v>
+        <v>303</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>301</v>
+        <v>795</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>302</v>
+        <v>796</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>303</v>
+        <v>797</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>795</v>
+        <v>112</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>796</v>
+        <v>113</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>797</v>
+        <v>114</v>
       </c>
     </row>
     <row r="207" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>112</v>
+        <v>472</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>113</v>
+        <v>473</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>114</v>
+        <v>474</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>742</v>
       </c>
     </row>
     <row r="208" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>472</v>
+        <v>169</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>473</v>
+        <v>170</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="E208" s="1" t="s">
-        <v>742</v>
+        <v>172</v>
       </c>
     </row>
     <row r="209" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>169</v>
+        <v>310</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>170</v>
+        <v>311</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>172</v>
+        <v>312</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>310</v>
+        <v>176</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>311</v>
+        <v>177</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>312</v>
+        <v>178</v>
       </c>
     </row>
     <row r="211" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>176</v>
+        <v>657</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>177</v>
+        <v>658</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>178</v>
+        <v>666</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>659</v>
       </c>
     </row>
     <row r="212" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>657</v>
+        <v>560</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>658</v>
+        <v>561</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>659</v>
+        <v>562</v>
       </c>
     </row>
     <row r="213" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>560</v>
+        <v>456</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>561</v>
+        <v>457</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>562</v>
+        <v>458</v>
       </c>
     </row>
     <row r="214" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>456</v>
+        <v>255</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>457</v>
+        <v>256</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>458</v>
+        <v>257</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>255</v>
+        <v>595</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>256</v>
+        <v>596</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>257</v>
+        <v>597</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>595</v>
+        <v>199</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>596</v>
+        <v>200</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>597</v>
+        <v>201</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>199</v>
+        <v>816</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>200</v>
+        <v>817</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E217" s="1" t="s">
-        <v>768</v>
+        <v>818</v>
       </c>
     </row>
     <row r="218" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>816</v>
+        <v>539</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>817</v>
+        <v>530</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>818</v>
+        <v>531</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>539</v>
+        <v>325</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>530</v>
+        <v>315</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>532</v>
+        <v>316</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>325</v>
+        <v>548</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>315</v>
+        <v>553</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>316</v>
+        <v>554</v>
       </c>
     </row>
     <row r="221" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>548</v>
+        <v>951</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>553</v>
+        <v>482</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>554</v>
+        <v>484</v>
       </c>
     </row>
     <row r="222" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>951</v>
+        <v>739</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>26</v>
+        <v>880</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>482</v>
+        <v>740</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>484</v>
+        <v>741</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>739</v>
+        <v>589</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>880</v>
+        <v>39</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>740</v>
+        <v>590</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>741</v>
+        <v>591</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>589</v>
+        <v>649</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>590</v>
+        <v>650</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>591</v>
+        <v>655</v>
       </c>
     </row>
     <row r="225" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>649</v>
+        <v>730</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>650</v>
+        <v>731</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>655</v>
+        <v>732</v>
       </c>
     </row>
     <row r="226" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>730</v>
+        <v>333</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>731</v>
+        <v>334</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>732</v>
+        <v>335</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="227" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>333</v>
+        <v>525</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>334</v>
+        <v>526</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>335</v>
+        <v>527</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>336</v>
+        <v>879</v>
       </c>
     </row>
     <row r="228" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>525</v>
+        <v>33</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>526</v>
+        <v>54</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>527</v>
+        <v>93</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>879</v>
+        <v>34</v>
       </c>
     </row>
     <row r="229" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>33</v>
+        <v>559</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>54</v>
+        <v>425</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>93</v>
+        <v>426</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>34</v>
+        <v>424</v>
       </c>
     </row>
     <row r="230" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>559</v>
+        <v>634</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>425</v>
+        <v>629</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>426</v>
+        <v>637</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>424</v>
+        <v>639</v>
       </c>
     </row>
     <row r="231" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>634</v>
+        <v>727</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>629</v>
+        <v>728</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>637</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>639</v>
+        <v>729</v>
       </c>
     </row>
     <row r="232" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>727</v>
+        <v>583</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>728</v>
+        <v>584</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>729</v>
+        <v>585</v>
       </c>
     </row>
     <row r="233" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>583</v>
+        <v>520</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>584</v>
+        <v>521</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>585</v>
+        <v>522</v>
       </c>
     </row>
     <row r="234" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>520</v>
+        <v>416</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>521</v>
+        <v>417</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>522</v>
+        <v>418</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="235" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>416</v>
+        <v>260</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>417</v>
+        <v>258</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>419</v>
+        <v>259</v>
       </c>
     </row>
     <row r="236" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
-        <v>260</v>
+        <v>162</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>258</v>
+        <v>163</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>259</v>
+        <v>164</v>
       </c>
     </row>
     <row r="237" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
-        <v>162</v>
+        <v>640</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>163</v>
+        <v>641</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>164</v>
+        <v>642</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>644</v>
       </c>
     </row>
     <row r="238" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
-        <v>640</v>
+        <v>409</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>641</v>
+        <v>410</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>642</v>
+        <v>411</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>644</v>
+        <v>524</v>
       </c>
     </row>
     <row r="239" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>409</v>
+        <v>63</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>410</v>
+        <v>64</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>411</v>
+        <v>65</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>524</v>
+        <v>66</v>
       </c>
     </row>
     <row r="240" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
-        <v>63</v>
+        <v>763</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>64</v>
+        <v>764</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E240" s="1" t="s">
-        <v>66</v>
+        <v>765</v>
       </c>
     </row>
     <row r="241" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
-        <v>763</v>
+        <v>626</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>764</v>
+        <v>631</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>765</v>
+        <v>632</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="242" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
-        <v>626</v>
+        <v>955</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>631</v>
+        <v>956</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>633</v>
+        <v>957</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F230" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F242">
-      <sortCondition ref="A1:A242"/>
+  <autoFilter ref="A1:F229" xr:uid="{D77021C4-16C3-4387-961E-B82FE813C9FE}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F241">
+      <sortCondition ref="A1:A241"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Reader fragments: v3 edits with key attribs
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F329806-ECAB-4248-BAF3-A07F7D32BFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ACF349-2192-A84A-AAEA-796E6DD02599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="961">
   <si>
     <t>M-Number</t>
   </si>
@@ -2961,6 +2961,12 @@
   </si>
   <si>
     <t>M54, 7 of 11. [Anon: distinct from the minstrel, whose words are printed.]. Typescript fragment, 2 fols.</t>
+  </si>
+  <si>
+    <t>M54, 10 of 11. [Anon: and the peasants to respect their mother tongue...]. Typescript fragment, 2 fols.</t>
+  </si>
+  <si>
+    <t>M54, 11 of 11. [Anon: there is a jolt at the points...]. Typescript fragment, 1 fol.</t>
   </si>
 </sst>
 </file>
@@ -3402,9 +3408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B37" sqref="B37"/>
+      <selection pane="topRight" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4144,7 +4150,7 @@
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>30</v>
@@ -4168,9 +4174,15 @@
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4185,19 +4197,40 @@
         <v>930</v>
       </c>
       <c r="D33" s="6"/>
+      <c r="E33" s="5">
+        <v>8</v>
+      </c>
       <c r="F33" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="G33" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>919</v>
       </c>
+      <c r="B34" s="1" t="s">
+        <v>959</v>
+      </c>
       <c r="C34" s="1" t="s">
         <v>931</v>
       </c>
       <c r="D34" s="6"/>
+      <c r="E34" s="5">
+        <v>2</v>
+      </c>
       <c r="F34" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4205,11 +4238,23 @@
       <c r="A35" s="1" t="s">
         <v>920</v>
       </c>
+      <c r="B35" s="1" t="s">
+        <v>960</v>
+      </c>
       <c r="C35" s="1" t="s">
         <v>932</v>
       </c>
       <c r="D35" s="6"/>
+      <c r="E35" s="5">
+        <v>1</v>
+      </c>
       <c r="F35" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4457,7 +4502,7 @@
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E48" s="5">
         <f>SUM(E3:E45)</f>
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -4505,8 +4550,8 @@
   <dimension ref="A1:F242"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A200" sqref="A200:XFD200"/>
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
m50-2.xml: edits based on time in Berg
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ACF349-2192-A84A-AAEA-796E6DD02599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D2ED2F-8EFD-4642-B683-83ECD784280F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="961">
   <si>
     <t>M-Number</t>
   </si>
@@ -3408,9 +3408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55FE68-D4A2-46EA-B841-9A4287A5B051}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B38" sqref="B38"/>
+      <selection pane="topRight" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4280,6 +4280,9 @@
       <c r="G36" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H36" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="37" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
@@ -4303,6 +4306,9 @@
       <c r="G37" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H37" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="38" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
@@ -4326,6 +4332,9 @@
       <c r="G38" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H38" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="39" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
@@ -4349,6 +4358,9 @@
       <c r="G39" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H39" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="40" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
@@ -4372,6 +4384,9 @@
       <c r="G40" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H40" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="41" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
@@ -4395,6 +4410,9 @@
       <c r="G41" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H41" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="I41" s="1" t="s">
         <v>582</v>
       </c>
@@ -4421,6 +4439,9 @@
       <c r="G42" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H42" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="43" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
@@ -4444,6 +4465,9 @@
       <c r="G43" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H43" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="I43" s="1" t="s">
         <v>697</v>
       </c>
@@ -4470,6 +4494,9 @@
       <c r="G44" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H44" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="45" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
@@ -4491,6 +4518,9 @@
         <v>30</v>
       </c>
       <c r="G45" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="5" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tracking-sheet.xlsx: updates concerning annotations?
</commit_message>
<xml_diff>
--- a/tracking-sheet.xlsx
+++ b/tracking-sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/digital-anon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joshua/Documents/digital-anon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48EC01F-B0C2-304D-98A1-3513E71B5BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB93C877-BCF2-F64A-9677-7764B3278744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="-1440" windowWidth="21600" windowHeight="37900" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15700" activeTab="1" xr2:uid="{E1328B9C-38E5-4F5D-92FF-3C87A9111859}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptions" sheetId="1" r:id="rId1"/>
@@ -2081,9 +2081,6 @@
     <t>Possibly Anne Dudley (1548-1604) nee Russell who served Queen Liz, was a patron of Spenser, sold Shakespeare his big house! And was a distant relative of Bertrand Russell and Winston Churchill</t>
   </si>
   <si>
-    <t>Possibly Mary Herbert (1580-1649), nee Talbot, granddaughter of Bess of Hardwick and courtier of Queen Liz</t>
-  </si>
-  <si>
     <t>../resources/annotations.xml#psn-astan</t>
   </si>
   <si>
@@ -2964,6 +2961,9 @@
   </si>
   <si>
     <t>M54, 11 of 11. [Anon: there is a jolt at the points...]. Typescript fragment, 1 fol.</t>
+  </si>
+  <si>
+    <t>Possibly Mary Herbert (1580-1649), nee Talbot, granddaughter of Bess of Hardwick and courtier of Queen Liz or Mary</t>
   </si>
 </sst>
 </file>
@@ -3432,7 +3432,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>391</v>
@@ -3441,10 +3441,10 @@
         <v>29</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>7</v>
@@ -3452,16 +3452,16 @@
     </row>
     <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>784</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E3" s="5">
         <v>9</v>
@@ -3478,16 +3478,16 @@
     </row>
     <row r="4" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>806</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E4" s="5">
         <v>12</v>
@@ -3504,16 +3504,16 @@
     </row>
     <row r="5" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E5" s="5">
         <v>15</v>
@@ -3530,16 +3530,16 @@
     </row>
     <row r="6" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>826</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>827</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="E6" s="5">
         <v>9</v>
@@ -3556,16 +3556,16 @@
     </row>
     <row r="7" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E7" s="5">
         <v>4</v>
@@ -3580,21 +3580,21 @@
         <v>30</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>850</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>851</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E8" s="5">
         <v>6</v>
@@ -3609,21 +3609,21 @@
         <v>30</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="32" x14ac:dyDescent="0.2